<commit_message>
036 : added blueprnt driver
</commit_message>
<xml_diff>
--- a/0.36/compatibility.xlsx
+++ b/0.36/compatibility.xlsx
@@ -16,8 +16,8 @@
     <sheet name="ALL" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ALL!$A$1:$M$2031</definedName>
-    <definedName name="LIST" localSheetId="1">ALL!$B$1:$M$2031</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ALL!$A$1:$M$2028</definedName>
+    <definedName name="LIST" localSheetId="1">ALL!$B$1:$M$2028</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -14068,10 +14068,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14480,6 +14480,75 @@
         <v>689</v>
       </c>
     </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3770</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3771</v>
+      </c>
+      <c r="D19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" t="s">
+        <v>172</v>
+      </c>
+      <c r="M19" t="s">
+        <v>3772</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3773</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3771</v>
+      </c>
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" t="s">
+        <v>172</v>
+      </c>
+      <c r="M20" t="s">
+        <v>3774</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3775</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3771</v>
+      </c>
+      <c r="D21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" t="s">
+        <v>172</v>
+      </c>
+      <c r="M21" t="s">
+        <v>3776</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14487,10 +14556,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2031"/>
+  <dimension ref="A1:M2028"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A320" workbookViewId="0">
-      <selection activeCell="F331" sqref="F331"/>
+    <sheetView tabSelected="1" topLeftCell="A2001" workbookViewId="0">
+      <selection activeCell="D2029" sqref="D2029"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -60100,22 +60169,22 @@
         <v>1870</v>
       </c>
       <c r="B1864" t="s">
-        <v>3770</v>
+        <v>3777</v>
       </c>
       <c r="C1864" t="s">
-        <v>3771</v>
+        <v>3778</v>
       </c>
       <c r="D1864" t="s">
         <v>14</v>
       </c>
       <c r="E1864" t="s">
-        <v>14</v>
+        <v>154</v>
       </c>
       <c r="H1864" t="s">
         <v>172</v>
       </c>
       <c r="M1864" t="s">
-        <v>3772</v>
+        <v>3779</v>
       </c>
     </row>
     <row r="1865" spans="1:13" x14ac:dyDescent="0.3">
@@ -60123,22 +60192,19 @@
         <v>1871</v>
       </c>
       <c r="B1865" t="s">
-        <v>3773</v>
+        <v>3780</v>
       </c>
       <c r="C1865" t="s">
-        <v>3771</v>
+        <v>3781</v>
       </c>
       <c r="D1865" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1865" t="s">
         <v>14</v>
       </c>
       <c r="H1865" t="s">
         <v>172</v>
       </c>
       <c r="M1865" t="s">
-        <v>3774</v>
+        <v>3782</v>
       </c>
     </row>
     <row r="1866" spans="1:13" x14ac:dyDescent="0.3">
@@ -60146,22 +60212,19 @@
         <v>1872</v>
       </c>
       <c r="B1866" t="s">
-        <v>3775</v>
+        <v>3783</v>
       </c>
       <c r="C1866" t="s">
-        <v>3771</v>
+        <v>3781</v>
       </c>
       <c r="D1866" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1866" t="s">
         <v>14</v>
       </c>
       <c r="H1866" t="s">
         <v>172</v>
       </c>
       <c r="M1866" t="s">
-        <v>3776</v>
+        <v>3784</v>
       </c>
     </row>
     <row r="1867" spans="1:13" x14ac:dyDescent="0.3">
@@ -60169,22 +60232,19 @@
         <v>1873</v>
       </c>
       <c r="B1867" t="s">
-        <v>3777</v>
+        <v>3785</v>
       </c>
       <c r="C1867" t="s">
-        <v>3778</v>
+        <v>3786</v>
       </c>
       <c r="D1867" t="s">
         <v>14</v>
       </c>
-      <c r="E1867" t="s">
-        <v>154</v>
-      </c>
       <c r="H1867" t="s">
-        <v>172</v>
+        <v>336</v>
       </c>
       <c r="M1867" t="s">
-        <v>3779</v>
+        <v>3787</v>
       </c>
     </row>
     <row r="1868" spans="1:13" x14ac:dyDescent="0.3">
@@ -60192,19 +60252,19 @@
         <v>1874</v>
       </c>
       <c r="B1868" t="s">
-        <v>3780</v>
+        <v>3788</v>
       </c>
       <c r="C1868" t="s">
-        <v>3781</v>
+        <v>3786</v>
       </c>
       <c r="D1868" t="s">
         <v>14</v>
       </c>
       <c r="H1868" t="s">
-        <v>172</v>
+        <v>336</v>
       </c>
       <c r="M1868" t="s">
-        <v>3782</v>
+        <v>3789</v>
       </c>
     </row>
     <row r="1869" spans="1:13" x14ac:dyDescent="0.3">
@@ -60212,19 +60272,19 @@
         <v>1875</v>
       </c>
       <c r="B1869" t="s">
-        <v>3783</v>
+        <v>3790</v>
       </c>
       <c r="C1869" t="s">
-        <v>3781</v>
+        <v>3786</v>
       </c>
       <c r="D1869" t="s">
         <v>14</v>
       </c>
       <c r="H1869" t="s">
-        <v>172</v>
+        <v>336</v>
       </c>
       <c r="M1869" t="s">
-        <v>3784</v>
+        <v>3791</v>
       </c>
     </row>
     <row r="1870" spans="1:13" x14ac:dyDescent="0.3">
@@ -60232,7 +60292,7 @@
         <v>1876</v>
       </c>
       <c r="B1870" t="s">
-        <v>3785</v>
+        <v>3792</v>
       </c>
       <c r="C1870" t="s">
         <v>3786</v>
@@ -60244,7 +60304,7 @@
         <v>336</v>
       </c>
       <c r="M1870" t="s">
-        <v>3787</v>
+        <v>3793</v>
       </c>
     </row>
     <row r="1871" spans="1:13" x14ac:dyDescent="0.3">
@@ -60252,19 +60312,22 @@
         <v>1877</v>
       </c>
       <c r="B1871" t="s">
-        <v>3788</v>
+        <v>3794</v>
       </c>
       <c r="C1871" t="s">
-        <v>3786</v>
+        <v>3795</v>
       </c>
       <c r="D1871" t="s">
-        <v>14</v>
+        <v>405</v>
+      </c>
+      <c r="E1871" t="s">
+        <v>1187</v>
       </c>
       <c r="H1871" t="s">
-        <v>336</v>
+        <v>71</v>
       </c>
       <c r="M1871" t="s">
-        <v>3789</v>
+        <v>3796</v>
       </c>
     </row>
     <row r="1872" spans="1:13" x14ac:dyDescent="0.3">
@@ -60272,19 +60335,22 @@
         <v>1878</v>
       </c>
       <c r="B1872" t="s">
-        <v>3790</v>
+        <v>3797</v>
       </c>
       <c r="C1872" t="s">
-        <v>3786</v>
+        <v>3795</v>
       </c>
       <c r="D1872" t="s">
-        <v>14</v>
+        <v>405</v>
+      </c>
+      <c r="E1872" t="s">
+        <v>1187</v>
       </c>
       <c r="H1872" t="s">
-        <v>336</v>
+        <v>71</v>
       </c>
       <c r="M1872" t="s">
-        <v>3791</v>
+        <v>3798</v>
       </c>
     </row>
     <row r="1873" spans="1:13" x14ac:dyDescent="0.3">
@@ -60292,19 +60358,19 @@
         <v>1879</v>
       </c>
       <c r="B1873" t="s">
-        <v>3792</v>
+        <v>3799</v>
       </c>
       <c r="C1873" t="s">
-        <v>3786</v>
+        <v>3800</v>
       </c>
       <c r="D1873" t="s">
         <v>14</v>
       </c>
       <c r="H1873" t="s">
-        <v>336</v>
+        <v>71</v>
       </c>
       <c r="M1873" t="s">
-        <v>3793</v>
+        <v>3801</v>
       </c>
     </row>
     <row r="1874" spans="1:13" x14ac:dyDescent="0.3">
@@ -60312,10 +60378,10 @@
         <v>1880</v>
       </c>
       <c r="B1874" t="s">
-        <v>3794</v>
+        <v>3802</v>
       </c>
       <c r="C1874" t="s">
-        <v>3795</v>
+        <v>3803</v>
       </c>
       <c r="D1874" t="s">
         <v>405</v>
@@ -60323,11 +60389,14 @@
       <c r="E1874" t="s">
         <v>1187</v>
       </c>
+      <c r="F1874" t="s">
+        <v>3804</v>
+      </c>
       <c r="H1874" t="s">
         <v>71</v>
       </c>
       <c r="M1874" t="s">
-        <v>3796</v>
+        <v>3805</v>
       </c>
     </row>
     <row r="1875" spans="1:13" x14ac:dyDescent="0.3">
@@ -60335,22 +60404,19 @@
         <v>1881</v>
       </c>
       <c r="B1875" t="s">
-        <v>3797</v>
+        <v>3806</v>
       </c>
       <c r="C1875" t="s">
-        <v>3795</v>
+        <v>3807</v>
       </c>
       <c r="D1875" t="s">
-        <v>405</v>
-      </c>
-      <c r="E1875" t="s">
-        <v>1187</v>
+        <v>473</v>
       </c>
       <c r="H1875" t="s">
-        <v>71</v>
+        <v>2939</v>
       </c>
       <c r="M1875" t="s">
-        <v>3798</v>
+        <v>3808</v>
       </c>
     </row>
     <row r="1876" spans="1:13" x14ac:dyDescent="0.3">
@@ -60358,19 +60424,16 @@
         <v>1882</v>
       </c>
       <c r="B1876" t="s">
-        <v>3799</v>
+        <v>3809</v>
       </c>
       <c r="C1876" t="s">
-        <v>3800</v>
+        <v>3810</v>
       </c>
       <c r="D1876" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1876" t="s">
-        <v>71</v>
+        <v>473</v>
       </c>
       <c r="M1876" t="s">
-        <v>3801</v>
+        <v>3811</v>
       </c>
     </row>
     <row r="1877" spans="1:13" x14ac:dyDescent="0.3">
@@ -60378,25 +60441,16 @@
         <v>1883</v>
       </c>
       <c r="B1877" t="s">
-        <v>3802</v>
+        <v>3812</v>
       </c>
       <c r="C1877" t="s">
-        <v>3803</v>
+        <v>3810</v>
       </c>
       <c r="D1877" t="s">
-        <v>405</v>
-      </c>
-      <c r="E1877" t="s">
-        <v>1187</v>
-      </c>
-      <c r="F1877" t="s">
-        <v>3804</v>
-      </c>
-      <c r="H1877" t="s">
-        <v>71</v>
+        <v>473</v>
       </c>
       <c r="M1877" t="s">
-        <v>3805</v>
+        <v>3813</v>
       </c>
     </row>
     <row r="1878" spans="1:13" x14ac:dyDescent="0.3">
@@ -60404,19 +60458,16 @@
         <v>1884</v>
       </c>
       <c r="B1878" t="s">
-        <v>3806</v>
+        <v>3814</v>
       </c>
       <c r="C1878" t="s">
-        <v>3807</v>
-      </c>
-      <c r="D1878" t="s">
-        <v>473</v>
-      </c>
-      <c r="H1878" t="s">
-        <v>2939</v>
+        <v>3815</v>
+      </c>
+      <c r="D1878">
+        <v>8080</v>
       </c>
       <c r="M1878" t="s">
-        <v>3808</v>
+        <v>3816</v>
       </c>
     </row>
     <row r="1879" spans="1:13" x14ac:dyDescent="0.3">
@@ -60424,16 +60475,31 @@
         <v>1885</v>
       </c>
       <c r="B1879" t="s">
-        <v>3809</v>
+        <v>3817</v>
       </c>
       <c r="C1879" t="s">
-        <v>3810</v>
+        <v>3818</v>
       </c>
       <c r="D1879" t="s">
-        <v>473</v>
+        <v>3439</v>
+      </c>
+      <c r="E1879" t="s">
+        <v>3439</v>
+      </c>
+      <c r="F1879" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G1879" t="s">
+        <v>1187</v>
+      </c>
+      <c r="H1879" t="s">
+        <v>333</v>
+      </c>
+      <c r="I1879" t="s">
+        <v>551</v>
       </c>
       <c r="M1879" t="s">
-        <v>3811</v>
+        <v>3819</v>
       </c>
     </row>
     <row r="1880" spans="1:13" x14ac:dyDescent="0.3">
@@ -60441,16 +60507,19 @@
         <v>1886</v>
       </c>
       <c r="B1880" t="s">
-        <v>3812</v>
+        <v>3820</v>
       </c>
       <c r="C1880" t="s">
-        <v>3810</v>
+        <v>3821</v>
       </c>
       <c r="D1880" t="s">
-        <v>473</v>
+        <v>14</v>
+      </c>
+      <c r="H1880" t="s">
+        <v>172</v>
       </c>
       <c r="M1880" t="s">
-        <v>3813</v>
+        <v>3822</v>
       </c>
     </row>
     <row r="1881" spans="1:13" x14ac:dyDescent="0.3">
@@ -60458,16 +60527,31 @@
         <v>1887</v>
       </c>
       <c r="B1881" t="s">
-        <v>3814</v>
+        <v>3823</v>
       </c>
       <c r="C1881" t="s">
-        <v>3815</v>
-      </c>
-      <c r="D1881">
-        <v>8080</v>
+        <v>3824</v>
+      </c>
+      <c r="D1881" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1881" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1881" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1881" t="s">
+        <v>154</v>
+      </c>
+      <c r="H1881" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1881" t="s">
+        <v>166</v>
       </c>
       <c r="M1881" t="s">
-        <v>3816</v>
+        <v>3825</v>
       </c>
     </row>
     <row r="1882" spans="1:13" x14ac:dyDescent="0.3">
@@ -60475,31 +60559,31 @@
         <v>1888</v>
       </c>
       <c r="B1882" t="s">
-        <v>3817</v>
+        <v>3826</v>
       </c>
       <c r="C1882" t="s">
-        <v>3818</v>
+        <v>3824</v>
       </c>
       <c r="D1882" t="s">
-        <v>3439</v>
+        <v>14</v>
       </c>
       <c r="E1882" t="s">
-        <v>3439</v>
+        <v>14</v>
       </c>
       <c r="F1882" t="s">
-        <v>1187</v>
+        <v>14</v>
       </c>
       <c r="G1882" t="s">
-        <v>1187</v>
+        <v>154</v>
       </c>
       <c r="H1882" t="s">
-        <v>333</v>
+        <v>71</v>
       </c>
       <c r="I1882" t="s">
-        <v>551</v>
+        <v>166</v>
       </c>
       <c r="M1882" t="s">
-        <v>3819</v>
+        <v>3827</v>
       </c>
     </row>
     <row r="1883" spans="1:13" x14ac:dyDescent="0.3">
@@ -60507,19 +60591,31 @@
         <v>1889</v>
       </c>
       <c r="B1883" t="s">
-        <v>3820</v>
+        <v>3828</v>
       </c>
       <c r="C1883" t="s">
-        <v>3821</v>
+        <v>3824</v>
       </c>
       <c r="D1883" t="s">
         <v>14</v>
       </c>
+      <c r="E1883" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1883" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1883" t="s">
+        <v>154</v>
+      </c>
       <c r="H1883" t="s">
-        <v>172</v>
+        <v>71</v>
+      </c>
+      <c r="I1883" t="s">
+        <v>166</v>
       </c>
       <c r="M1883" t="s">
-        <v>3822</v>
+        <v>3829</v>
       </c>
     </row>
     <row r="1884" spans="1:13" x14ac:dyDescent="0.3">
@@ -60527,7 +60623,7 @@
         <v>1890</v>
       </c>
       <c r="B1884" t="s">
-        <v>3823</v>
+        <v>3830</v>
       </c>
       <c r="C1884" t="s">
         <v>3824</v>
@@ -60551,7 +60647,7 @@
         <v>166</v>
       </c>
       <c r="M1884" t="s">
-        <v>3825</v>
+        <v>3831</v>
       </c>
     </row>
     <row r="1885" spans="1:13" x14ac:dyDescent="0.3">
@@ -60559,31 +60655,22 @@
         <v>1891</v>
       </c>
       <c r="B1885" t="s">
-        <v>3826</v>
+        <v>3832</v>
       </c>
       <c r="C1885" t="s">
-        <v>3824</v>
-      </c>
-      <c r="D1885" t="s">
-        <v>14</v>
+        <v>3833</v>
+      </c>
+      <c r="D1885">
+        <v>68000</v>
       </c>
       <c r="E1885" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1885" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1885" t="s">
         <v>154</v>
       </c>
       <c r="H1885" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1885" t="s">
-        <v>166</v>
+        <v>1495</v>
       </c>
       <c r="M1885" t="s">
-        <v>3827</v>
+        <v>3834</v>
       </c>
     </row>
     <row r="1886" spans="1:13" x14ac:dyDescent="0.3">
@@ -60591,10 +60678,10 @@
         <v>1892</v>
       </c>
       <c r="B1886" t="s">
-        <v>3828</v>
+        <v>3835</v>
       </c>
       <c r="C1886" t="s">
-        <v>3824</v>
+        <v>3836</v>
       </c>
       <c r="D1886" t="s">
         <v>14</v>
@@ -60602,20 +60689,14 @@
       <c r="E1886" t="s">
         <v>14</v>
       </c>
-      <c r="F1886" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1886" t="s">
-        <v>154</v>
-      </c>
       <c r="H1886" t="s">
-        <v>71</v>
+        <v>1239</v>
       </c>
       <c r="I1886" t="s">
-        <v>166</v>
+        <v>333</v>
       </c>
       <c r="M1886" t="s">
-        <v>3829</v>
+        <v>3837</v>
       </c>
     </row>
     <row r="1887" spans="1:13" x14ac:dyDescent="0.3">
@@ -60623,10 +60704,10 @@
         <v>1893</v>
       </c>
       <c r="B1887" t="s">
-        <v>3830</v>
+        <v>3838</v>
       </c>
       <c r="C1887" t="s">
-        <v>3824</v>
+        <v>3836</v>
       </c>
       <c r="D1887" t="s">
         <v>14</v>
@@ -60634,20 +60715,14 @@
       <c r="E1887" t="s">
         <v>14</v>
       </c>
-      <c r="F1887" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1887" t="s">
-        <v>154</v>
-      </c>
       <c r="H1887" t="s">
-        <v>71</v>
+        <v>1239</v>
       </c>
       <c r="I1887" t="s">
-        <v>166</v>
+        <v>333</v>
       </c>
       <c r="M1887" t="s">
-        <v>3831</v>
+        <v>4494</v>
       </c>
     </row>
     <row r="1888" spans="1:13" x14ac:dyDescent="0.3">
@@ -60655,22 +60730,25 @@
         <v>1894</v>
       </c>
       <c r="B1888" t="s">
-        <v>3832</v>
+        <v>3839</v>
       </c>
       <c r="C1888" t="s">
-        <v>3833</v>
-      </c>
-      <c r="D1888">
-        <v>68000</v>
+        <v>3836</v>
+      </c>
+      <c r="D1888" t="s">
+        <v>14</v>
       </c>
       <c r="E1888" t="s">
-        <v>154</v>
+        <v>14</v>
       </c>
       <c r="H1888" t="s">
-        <v>1495</v>
+        <v>71</v>
+      </c>
+      <c r="I1888" t="s">
+        <v>166</v>
       </c>
       <c r="M1888" t="s">
-        <v>3834</v>
+        <v>4495</v>
       </c>
     </row>
     <row r="1889" spans="1:13" x14ac:dyDescent="0.3">
@@ -60678,7 +60756,7 @@
         <v>1895</v>
       </c>
       <c r="B1889" t="s">
-        <v>3835</v>
+        <v>3840</v>
       </c>
       <c r="C1889" t="s">
         <v>3836</v>
@@ -60696,7 +60774,7 @@
         <v>333</v>
       </c>
       <c r="M1889" t="s">
-        <v>3837</v>
+        <v>3841</v>
       </c>
     </row>
     <row r="1890" spans="1:13" x14ac:dyDescent="0.3">
@@ -60704,10 +60782,10 @@
         <v>1896</v>
       </c>
       <c r="B1890" t="s">
-        <v>3838</v>
+        <v>3842</v>
       </c>
       <c r="C1890" t="s">
-        <v>3836</v>
+        <v>3843</v>
       </c>
       <c r="D1890" t="s">
         <v>14</v>
@@ -60716,13 +60794,10 @@
         <v>14</v>
       </c>
       <c r="H1890" t="s">
-        <v>1239</v>
-      </c>
-      <c r="I1890" t="s">
-        <v>333</v>
+        <v>349</v>
       </c>
       <c r="M1890" t="s">
-        <v>4494</v>
+        <v>3844</v>
       </c>
     </row>
     <row r="1891" spans="1:13" x14ac:dyDescent="0.3">
@@ -60730,25 +60805,22 @@
         <v>1897</v>
       </c>
       <c r="B1891" t="s">
-        <v>3839</v>
+        <v>3845</v>
       </c>
       <c r="C1891" t="s">
-        <v>3836</v>
+        <v>3846</v>
       </c>
       <c r="D1891" t="s">
         <v>14</v>
       </c>
       <c r="E1891" t="s">
-        <v>14</v>
+        <v>154</v>
       </c>
       <c r="H1891" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1891" t="s">
-        <v>166</v>
+        <v>349</v>
       </c>
       <c r="M1891" t="s">
-        <v>4495</v>
+        <v>3847</v>
       </c>
     </row>
     <row r="1892" spans="1:13" x14ac:dyDescent="0.3">
@@ -60756,25 +60828,19 @@
         <v>1898</v>
       </c>
       <c r="B1892" t="s">
-        <v>3840</v>
+        <v>3848</v>
       </c>
       <c r="C1892" t="s">
-        <v>3836</v>
+        <v>3849</v>
       </c>
       <c r="D1892" t="s">
         <v>14</v>
       </c>
-      <c r="E1892" t="s">
-        <v>14</v>
-      </c>
       <c r="H1892" t="s">
-        <v>1239</v>
-      </c>
-      <c r="I1892" t="s">
-        <v>333</v>
+        <v>172</v>
       </c>
       <c r="M1892" t="s">
-        <v>3841</v>
+        <v>3850</v>
       </c>
     </row>
     <row r="1893" spans="1:13" x14ac:dyDescent="0.3">
@@ -60782,22 +60848,19 @@
         <v>1899</v>
       </c>
       <c r="B1893" t="s">
-        <v>3842</v>
+        <v>3851</v>
       </c>
       <c r="C1893" t="s">
-        <v>3843</v>
-      </c>
-      <c r="D1893" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1893" t="s">
-        <v>14</v>
+        <v>3852</v>
+      </c>
+      <c r="D1893">
+        <v>8080</v>
       </c>
       <c r="H1893" t="s">
-        <v>349</v>
+        <v>406</v>
       </c>
       <c r="M1893" t="s">
-        <v>3844</v>
+        <v>3853</v>
       </c>
     </row>
     <row r="1894" spans="1:13" x14ac:dyDescent="0.3">
@@ -60805,22 +60868,19 @@
         <v>1900</v>
       </c>
       <c r="B1894" t="s">
-        <v>3845</v>
+        <v>3854</v>
       </c>
       <c r="C1894" t="s">
-        <v>3846</v>
+        <v>3855</v>
       </c>
       <c r="D1894" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1894" t="s">
-        <v>154</v>
+        <v>1108</v>
       </c>
       <c r="H1894" t="s">
-        <v>349</v>
+        <v>336</v>
       </c>
       <c r="M1894" t="s">
-        <v>3847</v>
+        <v>3856</v>
       </c>
     </row>
     <row r="1895" spans="1:13" x14ac:dyDescent="0.3">
@@ -60828,19 +60888,22 @@
         <v>1901</v>
       </c>
       <c r="B1895" t="s">
-        <v>3848</v>
+        <v>3857</v>
       </c>
       <c r="C1895" t="s">
-        <v>3849</v>
+        <v>3858</v>
       </c>
       <c r="D1895" t="s">
         <v>14</v>
       </c>
+      <c r="E1895" t="s">
+        <v>154</v>
+      </c>
       <c r="H1895" t="s">
-        <v>172</v>
+        <v>336</v>
       </c>
       <c r="M1895" t="s">
-        <v>3850</v>
+        <v>3859</v>
       </c>
     </row>
     <row r="1896" spans="1:13" x14ac:dyDescent="0.3">
@@ -60848,19 +60911,22 @@
         <v>1902</v>
       </c>
       <c r="B1896" t="s">
-        <v>3851</v>
+        <v>3860</v>
       </c>
       <c r="C1896" t="s">
-        <v>3852</v>
-      </c>
-      <c r="D1896">
-        <v>8080</v>
+        <v>3858</v>
+      </c>
+      <c r="D1896" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1896" t="s">
+        <v>154</v>
       </c>
       <c r="H1896" t="s">
-        <v>406</v>
+        <v>336</v>
       </c>
       <c r="M1896" t="s">
-        <v>3853</v>
+        <v>3861</v>
       </c>
     </row>
     <row r="1897" spans="1:13" x14ac:dyDescent="0.3">
@@ -60868,19 +60934,22 @@
         <v>1903</v>
       </c>
       <c r="B1897" t="s">
-        <v>3854</v>
+        <v>3862</v>
       </c>
       <c r="C1897" t="s">
-        <v>3855</v>
+        <v>3863</v>
       </c>
       <c r="D1897" t="s">
-        <v>1108</v>
+        <v>3864</v>
+      </c>
+      <c r="E1897" t="s">
+        <v>728</v>
       </c>
       <c r="H1897" t="s">
-        <v>336</v>
+        <v>2073</v>
       </c>
       <c r="M1897" t="s">
-        <v>3856</v>
+        <v>3865</v>
       </c>
     </row>
     <row r="1898" spans="1:13" x14ac:dyDescent="0.3">
@@ -60888,22 +60957,19 @@
         <v>1904</v>
       </c>
       <c r="B1898" t="s">
-        <v>3857</v>
+        <v>3866</v>
       </c>
       <c r="C1898" t="s">
-        <v>3858</v>
-      </c>
-      <c r="D1898" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1898" t="s">
-        <v>154</v>
+        <v>3867</v>
+      </c>
+      <c r="D1898">
+        <v>68000</v>
       </c>
       <c r="H1898" t="s">
-        <v>336</v>
+        <v>2378</v>
       </c>
       <c r="M1898" t="s">
-        <v>3859</v>
+        <v>3868</v>
       </c>
     </row>
     <row r="1899" spans="1:13" x14ac:dyDescent="0.3">
@@ -60911,22 +60977,22 @@
         <v>1905</v>
       </c>
       <c r="B1899" t="s">
-        <v>3860</v>
+        <v>3869</v>
       </c>
       <c r="C1899" t="s">
-        <v>3858</v>
-      </c>
-      <c r="D1899" t="s">
-        <v>14</v>
+        <v>3870</v>
+      </c>
+      <c r="D1899">
+        <v>68000</v>
       </c>
       <c r="E1899" t="s">
         <v>154</v>
       </c>
       <c r="H1899" t="s">
-        <v>336</v>
+        <v>1239</v>
       </c>
       <c r="M1899" t="s">
-        <v>3861</v>
+        <v>3871</v>
       </c>
     </row>
     <row r="1900" spans="1:13" x14ac:dyDescent="0.3">
@@ -60934,22 +61000,19 @@
         <v>1906</v>
       </c>
       <c r="B1900" t="s">
-        <v>3862</v>
+        <v>3872</v>
       </c>
       <c r="C1900" t="s">
-        <v>3863</v>
+        <v>3873</v>
       </c>
       <c r="D1900" t="s">
-        <v>3864</v>
-      </c>
-      <c r="E1900" t="s">
-        <v>728</v>
+        <v>405</v>
       </c>
       <c r="H1900" t="s">
-        <v>2073</v>
+        <v>71</v>
       </c>
       <c r="M1900" t="s">
-        <v>3865</v>
+        <v>3874</v>
       </c>
     </row>
     <row r="1901" spans="1:13" x14ac:dyDescent="0.3">
@@ -60957,19 +61020,16 @@
         <v>1907</v>
       </c>
       <c r="B1901" t="s">
-        <v>3866</v>
+        <v>3875</v>
       </c>
       <c r="C1901" t="s">
-        <v>3867</v>
-      </c>
-      <c r="D1901">
-        <v>68000</v>
-      </c>
-      <c r="H1901" t="s">
-        <v>2378</v>
+        <v>3876</v>
+      </c>
+      <c r="D1901" t="s">
+        <v>14</v>
       </c>
       <c r="M1901" t="s">
-        <v>3868</v>
+        <v>4496</v>
       </c>
     </row>
     <row r="1902" spans="1:13" x14ac:dyDescent="0.3">
@@ -60977,10 +61037,10 @@
         <v>1908</v>
       </c>
       <c r="B1902" t="s">
-        <v>3869</v>
+        <v>3877</v>
       </c>
       <c r="C1902" t="s">
-        <v>3870</v>
+        <v>3878</v>
       </c>
       <c r="D1902">
         <v>68000</v>
@@ -60989,10 +61049,10 @@
         <v>154</v>
       </c>
       <c r="H1902" t="s">
-        <v>1239</v>
+        <v>1356</v>
       </c>
       <c r="M1902" t="s">
-        <v>3871</v>
+        <v>3879</v>
       </c>
     </row>
     <row r="1903" spans="1:13" x14ac:dyDescent="0.3">
@@ -61000,19 +61060,22 @@
         <v>1909</v>
       </c>
       <c r="B1903" t="s">
-        <v>3872</v>
+        <v>3880</v>
       </c>
       <c r="C1903" t="s">
-        <v>3873</v>
-      </c>
-      <c r="D1903" t="s">
-        <v>405</v>
+        <v>3878</v>
+      </c>
+      <c r="D1903">
+        <v>68000</v>
+      </c>
+      <c r="E1903" t="s">
+        <v>154</v>
       </c>
       <c r="H1903" t="s">
-        <v>71</v>
+        <v>1356</v>
       </c>
       <c r="M1903" t="s">
-        <v>3874</v>
+        <v>4497</v>
       </c>
     </row>
     <row r="1904" spans="1:13" x14ac:dyDescent="0.3">
@@ -61020,16 +61083,22 @@
         <v>1910</v>
       </c>
       <c r="B1904" t="s">
-        <v>3875</v>
+        <v>3881</v>
       </c>
       <c r="C1904" t="s">
-        <v>3876</v>
-      </c>
-      <c r="D1904" t="s">
-        <v>14</v>
+        <v>3878</v>
+      </c>
+      <c r="D1904">
+        <v>68000</v>
+      </c>
+      <c r="E1904" t="s">
+        <v>154</v>
+      </c>
+      <c r="H1904" t="s">
+        <v>1356</v>
       </c>
       <c r="M1904" t="s">
-        <v>4496</v>
+        <v>3882</v>
       </c>
     </row>
     <row r="1905" spans="1:13" x14ac:dyDescent="0.3">
@@ -61037,7 +61106,7 @@
         <v>1911</v>
       </c>
       <c r="B1905" t="s">
-        <v>3877</v>
+        <v>3883</v>
       </c>
       <c r="C1905" t="s">
         <v>3878</v>
@@ -61052,7 +61121,7 @@
         <v>1356</v>
       </c>
       <c r="M1905" t="s">
-        <v>3879</v>
+        <v>3884</v>
       </c>
     </row>
     <row r="1906" spans="1:13" x14ac:dyDescent="0.3">
@@ -61060,7 +61129,7 @@
         <v>1912</v>
       </c>
       <c r="B1906" t="s">
-        <v>3880</v>
+        <v>3885</v>
       </c>
       <c r="C1906" t="s">
         <v>3878</v>
@@ -61075,7 +61144,7 @@
         <v>1356</v>
       </c>
       <c r="M1906" t="s">
-        <v>4497</v>
+        <v>3886</v>
       </c>
     </row>
     <row r="1907" spans="1:13" x14ac:dyDescent="0.3">
@@ -61083,7 +61152,7 @@
         <v>1913</v>
       </c>
       <c r="B1907" t="s">
-        <v>3881</v>
+        <v>3887</v>
       </c>
       <c r="C1907" t="s">
         <v>3878</v>
@@ -61098,7 +61167,7 @@
         <v>1356</v>
       </c>
       <c r="M1907" t="s">
-        <v>3882</v>
+        <v>3888</v>
       </c>
     </row>
     <row r="1908" spans="1:13" x14ac:dyDescent="0.3">
@@ -61106,7 +61175,7 @@
         <v>1914</v>
       </c>
       <c r="B1908" t="s">
-        <v>3883</v>
+        <v>3889</v>
       </c>
       <c r="C1908" t="s">
         <v>3878</v>
@@ -61121,7 +61190,7 @@
         <v>1356</v>
       </c>
       <c r="M1908" t="s">
-        <v>3884</v>
+        <v>3890</v>
       </c>
     </row>
     <row r="1909" spans="1:13" x14ac:dyDescent="0.3">
@@ -61129,7 +61198,7 @@
         <v>1915</v>
       </c>
       <c r="B1909" t="s">
-        <v>3885</v>
+        <v>3891</v>
       </c>
       <c r="C1909" t="s">
         <v>3878</v>
@@ -61144,7 +61213,7 @@
         <v>1356</v>
       </c>
       <c r="M1909" t="s">
-        <v>3886</v>
+        <v>4498</v>
       </c>
     </row>
     <row r="1910" spans="1:13" x14ac:dyDescent="0.3">
@@ -61152,7 +61221,7 @@
         <v>1916</v>
       </c>
       <c r="B1910" t="s">
-        <v>3887</v>
+        <v>3892</v>
       </c>
       <c r="C1910" t="s">
         <v>3878</v>
@@ -61167,7 +61236,7 @@
         <v>1356</v>
       </c>
       <c r="M1910" t="s">
-        <v>3888</v>
+        <v>3893</v>
       </c>
     </row>
     <row r="1911" spans="1:13" x14ac:dyDescent="0.3">
@@ -61175,7 +61244,7 @@
         <v>1917</v>
       </c>
       <c r="B1911" t="s">
-        <v>3889</v>
+        <v>3894</v>
       </c>
       <c r="C1911" t="s">
         <v>3878</v>
@@ -61190,7 +61259,7 @@
         <v>1356</v>
       </c>
       <c r="M1911" t="s">
-        <v>3890</v>
+        <v>3895</v>
       </c>
     </row>
     <row r="1912" spans="1:13" x14ac:dyDescent="0.3">
@@ -61198,7 +61267,7 @@
         <v>1918</v>
       </c>
       <c r="B1912" t="s">
-        <v>3891</v>
+        <v>3896</v>
       </c>
       <c r="C1912" t="s">
         <v>3878</v>
@@ -61213,7 +61282,7 @@
         <v>1356</v>
       </c>
       <c r="M1912" t="s">
-        <v>4498</v>
+        <v>3897</v>
       </c>
     </row>
     <row r="1913" spans="1:13" x14ac:dyDescent="0.3">
@@ -61221,7 +61290,7 @@
         <v>1919</v>
       </c>
       <c r="B1913" t="s">
-        <v>3892</v>
+        <v>3898</v>
       </c>
       <c r="C1913" t="s">
         <v>3878</v>
@@ -61236,7 +61305,7 @@
         <v>1356</v>
       </c>
       <c r="M1913" t="s">
-        <v>3893</v>
+        <v>3899</v>
       </c>
     </row>
     <row r="1914" spans="1:13" x14ac:dyDescent="0.3">
@@ -61244,7 +61313,7 @@
         <v>1920</v>
       </c>
       <c r="B1914" t="s">
-        <v>3894</v>
+        <v>3900</v>
       </c>
       <c r="C1914" t="s">
         <v>3878</v>
@@ -61259,7 +61328,7 @@
         <v>1356</v>
       </c>
       <c r="M1914" t="s">
-        <v>3895</v>
+        <v>3901</v>
       </c>
     </row>
     <row r="1915" spans="1:13" x14ac:dyDescent="0.3">
@@ -61267,7 +61336,7 @@
         <v>1921</v>
       </c>
       <c r="B1915" t="s">
-        <v>3896</v>
+        <v>3902</v>
       </c>
       <c r="C1915" t="s">
         <v>3878</v>
@@ -61282,7 +61351,7 @@
         <v>1356</v>
       </c>
       <c r="M1915" t="s">
-        <v>3897</v>
+        <v>4499</v>
       </c>
     </row>
     <row r="1916" spans="1:13" x14ac:dyDescent="0.3">
@@ -61290,7 +61359,7 @@
         <v>1922</v>
       </c>
       <c r="B1916" t="s">
-        <v>3898</v>
+        <v>3903</v>
       </c>
       <c r="C1916" t="s">
         <v>3878</v>
@@ -61305,7 +61374,7 @@
         <v>1356</v>
       </c>
       <c r="M1916" t="s">
-        <v>3899</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="1917" spans="1:13" x14ac:dyDescent="0.3">
@@ -61313,7 +61382,7 @@
         <v>1923</v>
       </c>
       <c r="B1917" t="s">
-        <v>3900</v>
+        <v>3904</v>
       </c>
       <c r="C1917" t="s">
         <v>3878</v>
@@ -61328,7 +61397,7 @@
         <v>1356</v>
       </c>
       <c r="M1917" t="s">
-        <v>3901</v>
+        <v>3905</v>
       </c>
     </row>
     <row r="1918" spans="1:13" x14ac:dyDescent="0.3">
@@ -61336,7 +61405,7 @@
         <v>1924</v>
       </c>
       <c r="B1918" t="s">
-        <v>3902</v>
+        <v>3906</v>
       </c>
       <c r="C1918" t="s">
         <v>3878</v>
@@ -61351,7 +61420,7 @@
         <v>1356</v>
       </c>
       <c r="M1918" t="s">
-        <v>4499</v>
+        <v>3907</v>
       </c>
     </row>
     <row r="1919" spans="1:13" x14ac:dyDescent="0.3">
@@ -61359,7 +61428,7 @@
         <v>1925</v>
       </c>
       <c r="B1919" t="s">
-        <v>3903</v>
+        <v>3908</v>
       </c>
       <c r="C1919" t="s">
         <v>3878</v>
@@ -61374,7 +61443,7 @@
         <v>1356</v>
       </c>
       <c r="M1919" t="s">
-        <v>4500</v>
+        <v>3909</v>
       </c>
     </row>
     <row r="1920" spans="1:13" x14ac:dyDescent="0.3">
@@ -61382,7 +61451,7 @@
         <v>1926</v>
       </c>
       <c r="B1920" t="s">
-        <v>3904</v>
+        <v>3910</v>
       </c>
       <c r="C1920" t="s">
         <v>3878</v>
@@ -61397,7 +61466,7 @@
         <v>1356</v>
       </c>
       <c r="M1920" t="s">
-        <v>3905</v>
+        <v>3911</v>
       </c>
     </row>
     <row r="1921" spans="1:13" x14ac:dyDescent="0.3">
@@ -61405,7 +61474,7 @@
         <v>1927</v>
       </c>
       <c r="B1921" t="s">
-        <v>3906</v>
+        <v>3912</v>
       </c>
       <c r="C1921" t="s">
         <v>3878</v>
@@ -61420,7 +61489,7 @@
         <v>1356</v>
       </c>
       <c r="M1921" t="s">
-        <v>3907</v>
+        <v>3913</v>
       </c>
     </row>
     <row r="1922" spans="1:13" x14ac:dyDescent="0.3">
@@ -61428,7 +61497,7 @@
         <v>1928</v>
       </c>
       <c r="B1922" t="s">
-        <v>3908</v>
+        <v>3914</v>
       </c>
       <c r="C1922" t="s">
         <v>3878</v>
@@ -61443,7 +61512,7 @@
         <v>1356</v>
       </c>
       <c r="M1922" t="s">
-        <v>3909</v>
+        <v>3915</v>
       </c>
     </row>
     <row r="1923" spans="1:13" x14ac:dyDescent="0.3">
@@ -61451,7 +61520,7 @@
         <v>1929</v>
       </c>
       <c r="B1923" t="s">
-        <v>3910</v>
+        <v>3916</v>
       </c>
       <c r="C1923" t="s">
         <v>3878</v>
@@ -61466,7 +61535,7 @@
         <v>1356</v>
       </c>
       <c r="M1923" t="s">
-        <v>3911</v>
+        <v>4501</v>
       </c>
     </row>
     <row r="1924" spans="1:13" x14ac:dyDescent="0.3">
@@ -61474,7 +61543,7 @@
         <v>1930</v>
       </c>
       <c r="B1924" t="s">
-        <v>3912</v>
+        <v>3917</v>
       </c>
       <c r="C1924" t="s">
         <v>3878</v>
@@ -61489,7 +61558,7 @@
         <v>1356</v>
       </c>
       <c r="M1924" t="s">
-        <v>3913</v>
+        <v>3918</v>
       </c>
     </row>
     <row r="1925" spans="1:13" x14ac:dyDescent="0.3">
@@ -61497,7 +61566,7 @@
         <v>1931</v>
       </c>
       <c r="B1925" t="s">
-        <v>3914</v>
+        <v>3919</v>
       </c>
       <c r="C1925" t="s">
         <v>3878</v>
@@ -61512,7 +61581,7 @@
         <v>1356</v>
       </c>
       <c r="M1925" t="s">
-        <v>3915</v>
+        <v>3920</v>
       </c>
     </row>
     <row r="1926" spans="1:13" x14ac:dyDescent="0.3">
@@ -61520,7 +61589,7 @@
         <v>1932</v>
       </c>
       <c r="B1926" t="s">
-        <v>3916</v>
+        <v>3921</v>
       </c>
       <c r="C1926" t="s">
         <v>3878</v>
@@ -61535,7 +61604,7 @@
         <v>1356</v>
       </c>
       <c r="M1926" t="s">
-        <v>4501</v>
+        <v>3922</v>
       </c>
     </row>
     <row r="1927" spans="1:13" x14ac:dyDescent="0.3">
@@ -61543,7 +61612,7 @@
         <v>1933</v>
       </c>
       <c r="B1927" t="s">
-        <v>3917</v>
+        <v>3923</v>
       </c>
       <c r="C1927" t="s">
         <v>3878</v>
@@ -61558,7 +61627,7 @@
         <v>1356</v>
       </c>
       <c r="M1927" t="s">
-        <v>3918</v>
+        <v>4502</v>
       </c>
     </row>
     <row r="1928" spans="1:13" x14ac:dyDescent="0.3">
@@ -61566,7 +61635,7 @@
         <v>1934</v>
       </c>
       <c r="B1928" t="s">
-        <v>3919</v>
+        <v>3924</v>
       </c>
       <c r="C1928" t="s">
         <v>3878</v>
@@ -61581,7 +61650,7 @@
         <v>1356</v>
       </c>
       <c r="M1928" t="s">
-        <v>3920</v>
+        <v>4503</v>
       </c>
     </row>
     <row r="1929" spans="1:13" x14ac:dyDescent="0.3">
@@ -61589,7 +61658,7 @@
         <v>1935</v>
       </c>
       <c r="B1929" t="s">
-        <v>3921</v>
+        <v>3925</v>
       </c>
       <c r="C1929" t="s">
         <v>3878</v>
@@ -61604,7 +61673,7 @@
         <v>1356</v>
       </c>
       <c r="M1929" t="s">
-        <v>3922</v>
+        <v>4504</v>
       </c>
     </row>
     <row r="1930" spans="1:13" x14ac:dyDescent="0.3">
@@ -61612,7 +61681,7 @@
         <v>1936</v>
       </c>
       <c r="B1930" t="s">
-        <v>3923</v>
+        <v>3926</v>
       </c>
       <c r="C1930" t="s">
         <v>3878</v>
@@ -61627,7 +61696,7 @@
         <v>1356</v>
       </c>
       <c r="M1930" t="s">
-        <v>4502</v>
+        <v>3927</v>
       </c>
     </row>
     <row r="1931" spans="1:13" x14ac:dyDescent="0.3">
@@ -61635,7 +61704,7 @@
         <v>1937</v>
       </c>
       <c r="B1931" t="s">
-        <v>3924</v>
+        <v>3928</v>
       </c>
       <c r="C1931" t="s">
         <v>3878</v>
@@ -61650,7 +61719,7 @@
         <v>1356</v>
       </c>
       <c r="M1931" t="s">
-        <v>4503</v>
+        <v>3929</v>
       </c>
     </row>
     <row r="1932" spans="1:13" x14ac:dyDescent="0.3">
@@ -61658,7 +61727,7 @@
         <v>1938</v>
       </c>
       <c r="B1932" t="s">
-        <v>3925</v>
+        <v>3930</v>
       </c>
       <c r="C1932" t="s">
         <v>3878</v>
@@ -61673,7 +61742,7 @@
         <v>1356</v>
       </c>
       <c r="M1932" t="s">
-        <v>4504</v>
+        <v>4505</v>
       </c>
     </row>
     <row r="1933" spans="1:13" x14ac:dyDescent="0.3">
@@ -61681,7 +61750,7 @@
         <v>1939</v>
       </c>
       <c r="B1933" t="s">
-        <v>3926</v>
+        <v>3931</v>
       </c>
       <c r="C1933" t="s">
         <v>3878</v>
@@ -61696,7 +61765,7 @@
         <v>1356</v>
       </c>
       <c r="M1933" t="s">
-        <v>3927</v>
+        <v>3932</v>
       </c>
     </row>
     <row r="1934" spans="1:13" x14ac:dyDescent="0.3">
@@ -61704,7 +61773,7 @@
         <v>1940</v>
       </c>
       <c r="B1934" t="s">
-        <v>3928</v>
+        <v>3933</v>
       </c>
       <c r="C1934" t="s">
         <v>3878</v>
@@ -61719,7 +61788,7 @@
         <v>1356</v>
       </c>
       <c r="M1934" t="s">
-        <v>3929</v>
+        <v>4506</v>
       </c>
     </row>
     <row r="1935" spans="1:13" x14ac:dyDescent="0.3">
@@ -61727,7 +61796,7 @@
         <v>1941</v>
       </c>
       <c r="B1935" t="s">
-        <v>3930</v>
+        <v>3934</v>
       </c>
       <c r="C1935" t="s">
         <v>3878</v>
@@ -61742,7 +61811,7 @@
         <v>1356</v>
       </c>
       <c r="M1935" t="s">
-        <v>4505</v>
+        <v>3935</v>
       </c>
     </row>
     <row r="1936" spans="1:13" x14ac:dyDescent="0.3">
@@ -61750,7 +61819,7 @@
         <v>1942</v>
       </c>
       <c r="B1936" t="s">
-        <v>3931</v>
+        <v>3936</v>
       </c>
       <c r="C1936" t="s">
         <v>3878</v>
@@ -61765,7 +61834,7 @@
         <v>1356</v>
       </c>
       <c r="M1936" t="s">
-        <v>3932</v>
+        <v>3937</v>
       </c>
     </row>
     <row r="1937" spans="1:13" x14ac:dyDescent="0.3">
@@ -61773,7 +61842,7 @@
         <v>1943</v>
       </c>
       <c r="B1937" t="s">
-        <v>3933</v>
+        <v>3938</v>
       </c>
       <c r="C1937" t="s">
         <v>3878</v>
@@ -61788,7 +61857,7 @@
         <v>1356</v>
       </c>
       <c r="M1937" t="s">
-        <v>4506</v>
+        <v>4507</v>
       </c>
     </row>
     <row r="1938" spans="1:13" x14ac:dyDescent="0.3">
@@ -61796,7 +61865,7 @@
         <v>1944</v>
       </c>
       <c r="B1938" t="s">
-        <v>3934</v>
+        <v>3939</v>
       </c>
       <c r="C1938" t="s">
         <v>3878</v>
@@ -61811,7 +61880,7 @@
         <v>1356</v>
       </c>
       <c r="M1938" t="s">
-        <v>3935</v>
+        <v>4508</v>
       </c>
     </row>
     <row r="1939" spans="1:13" x14ac:dyDescent="0.3">
@@ -61819,7 +61888,7 @@
         <v>1945</v>
       </c>
       <c r="B1939" t="s">
-        <v>3936</v>
+        <v>3940</v>
       </c>
       <c r="C1939" t="s">
         <v>3878</v>
@@ -61834,7 +61903,7 @@
         <v>1356</v>
       </c>
       <c r="M1939" t="s">
-        <v>3937</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="1940" spans="1:13" x14ac:dyDescent="0.3">
@@ -61842,7 +61911,7 @@
         <v>1946</v>
       </c>
       <c r="B1940" t="s">
-        <v>3938</v>
+        <v>3942</v>
       </c>
       <c r="C1940" t="s">
         <v>3878</v>
@@ -61857,7 +61926,7 @@
         <v>1356</v>
       </c>
       <c r="M1940" t="s">
-        <v>4507</v>
+        <v>4509</v>
       </c>
     </row>
     <row r="1941" spans="1:13" x14ac:dyDescent="0.3">
@@ -61865,7 +61934,7 @@
         <v>1947</v>
       </c>
       <c r="B1941" t="s">
-        <v>3939</v>
+        <v>3943</v>
       </c>
       <c r="C1941" t="s">
         <v>3878</v>
@@ -61880,7 +61949,7 @@
         <v>1356</v>
       </c>
       <c r="M1941" t="s">
-        <v>4508</v>
+        <v>4510</v>
       </c>
     </row>
     <row r="1942" spans="1:13" x14ac:dyDescent="0.3">
@@ -61888,7 +61957,7 @@
         <v>1948</v>
       </c>
       <c r="B1942" t="s">
-        <v>3940</v>
+        <v>3944</v>
       </c>
       <c r="C1942" t="s">
         <v>3878</v>
@@ -61903,7 +61972,7 @@
         <v>1356</v>
       </c>
       <c r="M1942" t="s">
-        <v>3941</v>
+        <v>4511</v>
       </c>
     </row>
     <row r="1943" spans="1:13" x14ac:dyDescent="0.3">
@@ -61911,7 +61980,7 @@
         <v>1949</v>
       </c>
       <c r="B1943" t="s">
-        <v>3942</v>
+        <v>3945</v>
       </c>
       <c r="C1943" t="s">
         <v>3878</v>
@@ -61926,7 +61995,7 @@
         <v>1356</v>
       </c>
       <c r="M1943" t="s">
-        <v>4509</v>
+        <v>4512</v>
       </c>
     </row>
     <row r="1944" spans="1:13" x14ac:dyDescent="0.3">
@@ -61934,7 +62003,7 @@
         <v>1950</v>
       </c>
       <c r="B1944" t="s">
-        <v>3943</v>
+        <v>3946</v>
       </c>
       <c r="C1944" t="s">
         <v>3878</v>
@@ -61949,7 +62018,7 @@
         <v>1356</v>
       </c>
       <c r="M1944" t="s">
-        <v>4510</v>
+        <v>4513</v>
       </c>
     </row>
     <row r="1945" spans="1:13" x14ac:dyDescent="0.3">
@@ -61957,7 +62026,7 @@
         <v>1951</v>
       </c>
       <c r="B1945" t="s">
-        <v>3944</v>
+        <v>3947</v>
       </c>
       <c r="C1945" t="s">
         <v>3878</v>
@@ -61972,7 +62041,7 @@
         <v>1356</v>
       </c>
       <c r="M1945" t="s">
-        <v>4511</v>
+        <v>4514</v>
       </c>
     </row>
     <row r="1946" spans="1:13" x14ac:dyDescent="0.3">
@@ -61980,7 +62049,7 @@
         <v>1952</v>
       </c>
       <c r="B1946" t="s">
-        <v>3945</v>
+        <v>3948</v>
       </c>
       <c r="C1946" t="s">
         <v>3878</v>
@@ -61995,7 +62064,7 @@
         <v>1356</v>
       </c>
       <c r="M1946" t="s">
-        <v>4512</v>
+        <v>4515</v>
       </c>
     </row>
     <row r="1947" spans="1:13" x14ac:dyDescent="0.3">
@@ -62003,7 +62072,7 @@
         <v>1953</v>
       </c>
       <c r="B1947" t="s">
-        <v>3946</v>
+        <v>3949</v>
       </c>
       <c r="C1947" t="s">
         <v>3878</v>
@@ -62018,7 +62087,7 @@
         <v>1356</v>
       </c>
       <c r="M1947" t="s">
-        <v>4513</v>
+        <v>3950</v>
       </c>
     </row>
     <row r="1948" spans="1:13" x14ac:dyDescent="0.3">
@@ -62026,7 +62095,7 @@
         <v>1954</v>
       </c>
       <c r="B1948" t="s">
-        <v>3947</v>
+        <v>3951</v>
       </c>
       <c r="C1948" t="s">
         <v>3878</v>
@@ -62041,7 +62110,7 @@
         <v>1356</v>
       </c>
       <c r="M1948" t="s">
-        <v>4514</v>
+        <v>3952</v>
       </c>
     </row>
     <row r="1949" spans="1:13" x14ac:dyDescent="0.3">
@@ -62049,7 +62118,7 @@
         <v>1955</v>
       </c>
       <c r="B1949" t="s">
-        <v>3948</v>
+        <v>3953</v>
       </c>
       <c r="C1949" t="s">
         <v>3878</v>
@@ -62064,7 +62133,7 @@
         <v>1356</v>
       </c>
       <c r="M1949" t="s">
-        <v>4515</v>
+        <v>3954</v>
       </c>
     </row>
     <row r="1950" spans="1:13" x14ac:dyDescent="0.3">
@@ -62072,7 +62141,7 @@
         <v>1956</v>
       </c>
       <c r="B1950" t="s">
-        <v>3949</v>
+        <v>3955</v>
       </c>
       <c r="C1950" t="s">
         <v>3878</v>
@@ -62087,7 +62156,7 @@
         <v>1356</v>
       </c>
       <c r="M1950" t="s">
-        <v>3950</v>
+        <v>4516</v>
       </c>
     </row>
     <row r="1951" spans="1:13" x14ac:dyDescent="0.3">
@@ -62095,7 +62164,7 @@
         <v>1957</v>
       </c>
       <c r="B1951" t="s">
-        <v>3951</v>
+        <v>3956</v>
       </c>
       <c r="C1951" t="s">
         <v>3878</v>
@@ -62110,7 +62179,7 @@
         <v>1356</v>
       </c>
       <c r="M1951" t="s">
-        <v>3952</v>
+        <v>3957</v>
       </c>
     </row>
     <row r="1952" spans="1:13" x14ac:dyDescent="0.3">
@@ -62118,7 +62187,7 @@
         <v>1958</v>
       </c>
       <c r="B1952" t="s">
-        <v>3953</v>
+        <v>3958</v>
       </c>
       <c r="C1952" t="s">
         <v>3878</v>
@@ -62133,7 +62202,7 @@
         <v>1356</v>
       </c>
       <c r="M1952" t="s">
-        <v>3954</v>
+        <v>3959</v>
       </c>
     </row>
     <row r="1953" spans="1:13" x14ac:dyDescent="0.3">
@@ -62141,7 +62210,7 @@
         <v>1959</v>
       </c>
       <c r="B1953" t="s">
-        <v>3955</v>
+        <v>3960</v>
       </c>
       <c r="C1953" t="s">
         <v>3878</v>
@@ -62156,7 +62225,7 @@
         <v>1356</v>
       </c>
       <c r="M1953" t="s">
-        <v>4516</v>
+        <v>4517</v>
       </c>
     </row>
     <row r="1954" spans="1:13" x14ac:dyDescent="0.3">
@@ -62164,7 +62233,7 @@
         <v>1960</v>
       </c>
       <c r="B1954" t="s">
-        <v>3956</v>
+        <v>3961</v>
       </c>
       <c r="C1954" t="s">
         <v>3878</v>
@@ -62179,7 +62248,7 @@
         <v>1356</v>
       </c>
       <c r="M1954" t="s">
-        <v>3957</v>
+        <v>3962</v>
       </c>
     </row>
     <row r="1955" spans="1:13" x14ac:dyDescent="0.3">
@@ -62187,7 +62256,7 @@
         <v>1961</v>
       </c>
       <c r="B1955" t="s">
-        <v>3958</v>
+        <v>3963</v>
       </c>
       <c r="C1955" t="s">
         <v>3878</v>
@@ -62202,7 +62271,7 @@
         <v>1356</v>
       </c>
       <c r="M1955" t="s">
-        <v>3959</v>
+        <v>4518</v>
       </c>
     </row>
     <row r="1956" spans="1:13" x14ac:dyDescent="0.3">
@@ -62210,7 +62279,7 @@
         <v>1962</v>
       </c>
       <c r="B1956" t="s">
-        <v>3960</v>
+        <v>3964</v>
       </c>
       <c r="C1956" t="s">
         <v>3878</v>
@@ -62225,7 +62294,7 @@
         <v>1356</v>
       </c>
       <c r="M1956" t="s">
-        <v>4517</v>
+        <v>4519</v>
       </c>
     </row>
     <row r="1957" spans="1:13" x14ac:dyDescent="0.3">
@@ -62233,7 +62302,7 @@
         <v>1963</v>
       </c>
       <c r="B1957" t="s">
-        <v>3961</v>
+        <v>3965</v>
       </c>
       <c r="C1957" t="s">
         <v>3878</v>
@@ -62248,7 +62317,7 @@
         <v>1356</v>
       </c>
       <c r="M1957" t="s">
-        <v>3962</v>
+        <v>4520</v>
       </c>
     </row>
     <row r="1958" spans="1:13" x14ac:dyDescent="0.3">
@@ -62256,7 +62325,7 @@
         <v>1964</v>
       </c>
       <c r="B1958" t="s">
-        <v>3963</v>
+        <v>3966</v>
       </c>
       <c r="C1958" t="s">
         <v>3878</v>
@@ -62271,7 +62340,7 @@
         <v>1356</v>
       </c>
       <c r="M1958" t="s">
-        <v>4518</v>
+        <v>4521</v>
       </c>
     </row>
     <row r="1959" spans="1:13" x14ac:dyDescent="0.3">
@@ -62279,7 +62348,7 @@
         <v>1965</v>
       </c>
       <c r="B1959" t="s">
-        <v>3964</v>
+        <v>3967</v>
       </c>
       <c r="C1959" t="s">
         <v>3878</v>
@@ -62294,7 +62363,7 @@
         <v>1356</v>
       </c>
       <c r="M1959" t="s">
-        <v>4519</v>
+        <v>4522</v>
       </c>
     </row>
     <row r="1960" spans="1:13" x14ac:dyDescent="0.3">
@@ -62302,7 +62371,7 @@
         <v>1966</v>
       </c>
       <c r="B1960" t="s">
-        <v>3965</v>
+        <v>3968</v>
       </c>
       <c r="C1960" t="s">
         <v>3878</v>
@@ -62317,7 +62386,7 @@
         <v>1356</v>
       </c>
       <c r="M1960" t="s">
-        <v>4520</v>
+        <v>4523</v>
       </c>
     </row>
     <row r="1961" spans="1:13" x14ac:dyDescent="0.3">
@@ -62325,7 +62394,7 @@
         <v>1967</v>
       </c>
       <c r="B1961" t="s">
-        <v>3966</v>
+        <v>3969</v>
       </c>
       <c r="C1961" t="s">
         <v>3878</v>
@@ -62340,7 +62409,7 @@
         <v>1356</v>
       </c>
       <c r="M1961" t="s">
-        <v>4521</v>
+        <v>3970</v>
       </c>
     </row>
     <row r="1962" spans="1:13" x14ac:dyDescent="0.3">
@@ -62348,7 +62417,7 @@
         <v>1968</v>
       </c>
       <c r="B1962" t="s">
-        <v>3967</v>
+        <v>3971</v>
       </c>
       <c r="C1962" t="s">
         <v>3878</v>
@@ -62363,7 +62432,7 @@
         <v>1356</v>
       </c>
       <c r="M1962" t="s">
-        <v>4522</v>
+        <v>4524</v>
       </c>
     </row>
     <row r="1963" spans="1:13" x14ac:dyDescent="0.3">
@@ -62371,7 +62440,7 @@
         <v>1969</v>
       </c>
       <c r="B1963" t="s">
-        <v>3968</v>
+        <v>3972</v>
       </c>
       <c r="C1963" t="s">
         <v>3878</v>
@@ -62386,7 +62455,7 @@
         <v>1356</v>
       </c>
       <c r="M1963" t="s">
-        <v>4523</v>
+        <v>4525</v>
       </c>
     </row>
     <row r="1964" spans="1:13" x14ac:dyDescent="0.3">
@@ -62394,7 +62463,7 @@
         <v>1970</v>
       </c>
       <c r="B1964" t="s">
-        <v>3969</v>
+        <v>3973</v>
       </c>
       <c r="C1964" t="s">
         <v>3878</v>
@@ -62409,7 +62478,7 @@
         <v>1356</v>
       </c>
       <c r="M1964" t="s">
-        <v>3970</v>
+        <v>3974</v>
       </c>
     </row>
     <row r="1965" spans="1:13" x14ac:dyDescent="0.3">
@@ -62417,7 +62486,7 @@
         <v>1971</v>
       </c>
       <c r="B1965" t="s">
-        <v>3971</v>
+        <v>3975</v>
       </c>
       <c r="C1965" t="s">
         <v>3878</v>
@@ -62432,7 +62501,7 @@
         <v>1356</v>
       </c>
       <c r="M1965" t="s">
-        <v>4524</v>
+        <v>3976</v>
       </c>
     </row>
     <row r="1966" spans="1:13" x14ac:dyDescent="0.3">
@@ -62440,7 +62509,7 @@
         <v>1972</v>
       </c>
       <c r="B1966" t="s">
-        <v>3972</v>
+        <v>3977</v>
       </c>
       <c r="C1966" t="s">
         <v>3878</v>
@@ -62455,7 +62524,7 @@
         <v>1356</v>
       </c>
       <c r="M1966" t="s">
-        <v>4525</v>
+        <v>4526</v>
       </c>
     </row>
     <row r="1967" spans="1:13" x14ac:dyDescent="0.3">
@@ -62463,7 +62532,7 @@
         <v>1973</v>
       </c>
       <c r="B1967" t="s">
-        <v>3973</v>
+        <v>3978</v>
       </c>
       <c r="C1967" t="s">
         <v>3878</v>
@@ -62478,7 +62547,7 @@
         <v>1356</v>
       </c>
       <c r="M1967" t="s">
-        <v>3974</v>
+        <v>3979</v>
       </c>
     </row>
     <row r="1968" spans="1:13" x14ac:dyDescent="0.3">
@@ -62486,7 +62555,7 @@
         <v>1974</v>
       </c>
       <c r="B1968" t="s">
-        <v>3975</v>
+        <v>3980</v>
       </c>
       <c r="C1968" t="s">
         <v>3878</v>
@@ -62501,7 +62570,7 @@
         <v>1356</v>
       </c>
       <c r="M1968" t="s">
-        <v>3976</v>
+        <v>4527</v>
       </c>
     </row>
     <row r="1969" spans="1:13" x14ac:dyDescent="0.3">
@@ -62509,7 +62578,7 @@
         <v>1975</v>
       </c>
       <c r="B1969" t="s">
-        <v>3977</v>
+        <v>3981</v>
       </c>
       <c r="C1969" t="s">
         <v>3878</v>
@@ -62524,7 +62593,7 @@
         <v>1356</v>
       </c>
       <c r="M1969" t="s">
-        <v>4526</v>
+        <v>4528</v>
       </c>
     </row>
     <row r="1970" spans="1:13" x14ac:dyDescent="0.3">
@@ -62532,7 +62601,7 @@
         <v>1976</v>
       </c>
       <c r="B1970" t="s">
-        <v>3978</v>
+        <v>3982</v>
       </c>
       <c r="C1970" t="s">
         <v>3878</v>
@@ -62547,7 +62616,7 @@
         <v>1356</v>
       </c>
       <c r="M1970" t="s">
-        <v>3979</v>
+        <v>4529</v>
       </c>
     </row>
     <row r="1971" spans="1:13" x14ac:dyDescent="0.3">
@@ -62555,7 +62624,7 @@
         <v>1977</v>
       </c>
       <c r="B1971" t="s">
-        <v>3980</v>
+        <v>3983</v>
       </c>
       <c r="C1971" t="s">
         <v>3878</v>
@@ -62570,7 +62639,7 @@
         <v>1356</v>
       </c>
       <c r="M1971" t="s">
-        <v>4527</v>
+        <v>4530</v>
       </c>
     </row>
     <row r="1972" spans="1:13" x14ac:dyDescent="0.3">
@@ -62578,7 +62647,7 @@
         <v>1978</v>
       </c>
       <c r="B1972" t="s">
-        <v>3981</v>
+        <v>3984</v>
       </c>
       <c r="C1972" t="s">
         <v>3878</v>
@@ -62593,7 +62662,7 @@
         <v>1356</v>
       </c>
       <c r="M1972" t="s">
-        <v>4528</v>
+        <v>4531</v>
       </c>
     </row>
     <row r="1973" spans="1:13" x14ac:dyDescent="0.3">
@@ -62601,7 +62670,7 @@
         <v>1979</v>
       </c>
       <c r="B1973" t="s">
-        <v>3982</v>
+        <v>3985</v>
       </c>
       <c r="C1973" t="s">
         <v>3878</v>
@@ -62616,7 +62685,7 @@
         <v>1356</v>
       </c>
       <c r="M1973" t="s">
-        <v>4529</v>
+        <v>3986</v>
       </c>
     </row>
     <row r="1974" spans="1:13" x14ac:dyDescent="0.3">
@@ -62624,7 +62693,7 @@
         <v>1980</v>
       </c>
       <c r="B1974" t="s">
-        <v>3983</v>
+        <v>3987</v>
       </c>
       <c r="C1974" t="s">
         <v>3878</v>
@@ -62639,7 +62708,7 @@
         <v>1356</v>
       </c>
       <c r="M1974" t="s">
-        <v>4530</v>
+        <v>4532</v>
       </c>
     </row>
     <row r="1975" spans="1:13" x14ac:dyDescent="0.3">
@@ -62647,7 +62716,7 @@
         <v>1981</v>
       </c>
       <c r="B1975" t="s">
-        <v>3984</v>
+        <v>3988</v>
       </c>
       <c r="C1975" t="s">
         <v>3878</v>
@@ -62662,7 +62731,7 @@
         <v>1356</v>
       </c>
       <c r="M1975" t="s">
-        <v>4531</v>
+        <v>3989</v>
       </c>
     </row>
     <row r="1976" spans="1:13" x14ac:dyDescent="0.3">
@@ -62670,7 +62739,7 @@
         <v>1982</v>
       </c>
       <c r="B1976" t="s">
-        <v>3985</v>
+        <v>3990</v>
       </c>
       <c r="C1976" t="s">
         <v>3878</v>
@@ -62685,7 +62754,7 @@
         <v>1356</v>
       </c>
       <c r="M1976" t="s">
-        <v>3986</v>
+        <v>4533</v>
       </c>
     </row>
     <row r="1977" spans="1:13" x14ac:dyDescent="0.3">
@@ -62693,7 +62762,7 @@
         <v>1983</v>
       </c>
       <c r="B1977" t="s">
-        <v>3987</v>
+        <v>3991</v>
       </c>
       <c r="C1977" t="s">
         <v>3878</v>
@@ -62708,7 +62777,7 @@
         <v>1356</v>
       </c>
       <c r="M1977" t="s">
-        <v>4532</v>
+        <v>3992</v>
       </c>
     </row>
     <row r="1978" spans="1:13" x14ac:dyDescent="0.3">
@@ -62716,7 +62785,7 @@
         <v>1984</v>
       </c>
       <c r="B1978" t="s">
-        <v>3988</v>
+        <v>3993</v>
       </c>
       <c r="C1978" t="s">
         <v>3878</v>
@@ -62731,7 +62800,7 @@
         <v>1356</v>
       </c>
       <c r="M1978" t="s">
-        <v>3989</v>
+        <v>3994</v>
       </c>
     </row>
     <row r="1979" spans="1:13" x14ac:dyDescent="0.3">
@@ -62739,7 +62808,7 @@
         <v>1985</v>
       </c>
       <c r="B1979" t="s">
-        <v>3990</v>
+        <v>3995</v>
       </c>
       <c r="C1979" t="s">
         <v>3878</v>
@@ -62754,7 +62823,7 @@
         <v>1356</v>
       </c>
       <c r="M1979" t="s">
-        <v>4533</v>
+        <v>4534</v>
       </c>
     </row>
     <row r="1980" spans="1:13" x14ac:dyDescent="0.3">
@@ -62762,7 +62831,7 @@
         <v>1986</v>
       </c>
       <c r="B1980" t="s">
-        <v>3991</v>
+        <v>3996</v>
       </c>
       <c r="C1980" t="s">
         <v>3878</v>
@@ -62777,7 +62846,7 @@
         <v>1356</v>
       </c>
       <c r="M1980" t="s">
-        <v>3992</v>
+        <v>4535</v>
       </c>
     </row>
     <row r="1981" spans="1:13" x14ac:dyDescent="0.3">
@@ -62785,7 +62854,7 @@
         <v>1987</v>
       </c>
       <c r="B1981" t="s">
-        <v>3993</v>
+        <v>3997</v>
       </c>
       <c r="C1981" t="s">
         <v>3878</v>
@@ -62800,7 +62869,7 @@
         <v>1356</v>
       </c>
       <c r="M1981" t="s">
-        <v>3994</v>
+        <v>3998</v>
       </c>
     </row>
     <row r="1982" spans="1:13" x14ac:dyDescent="0.3">
@@ -62808,7 +62877,7 @@
         <v>1988</v>
       </c>
       <c r="B1982" t="s">
-        <v>3995</v>
+        <v>3999</v>
       </c>
       <c r="C1982" t="s">
         <v>3878</v>
@@ -62823,7 +62892,7 @@
         <v>1356</v>
       </c>
       <c r="M1982" t="s">
-        <v>4534</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="1983" spans="1:13" x14ac:dyDescent="0.3">
@@ -62831,7 +62900,7 @@
         <v>1989</v>
       </c>
       <c r="B1983" t="s">
-        <v>3996</v>
+        <v>4001</v>
       </c>
       <c r="C1983" t="s">
         <v>3878</v>
@@ -62846,7 +62915,7 @@
         <v>1356</v>
       </c>
       <c r="M1983" t="s">
-        <v>4535</v>
+        <v>4536</v>
       </c>
     </row>
     <row r="1984" spans="1:13" x14ac:dyDescent="0.3">
@@ -62854,7 +62923,7 @@
         <v>1990</v>
       </c>
       <c r="B1984" t="s">
-        <v>3997</v>
+        <v>4002</v>
       </c>
       <c r="C1984" t="s">
         <v>3878</v>
@@ -62869,7 +62938,7 @@
         <v>1356</v>
       </c>
       <c r="M1984" t="s">
-        <v>3998</v>
+        <v>4003</v>
       </c>
     </row>
     <row r="1985" spans="1:13" x14ac:dyDescent="0.3">
@@ -62877,7 +62946,7 @@
         <v>1991</v>
       </c>
       <c r="B1985" t="s">
-        <v>3999</v>
+        <v>4004</v>
       </c>
       <c r="C1985" t="s">
         <v>3878</v>
@@ -62892,7 +62961,7 @@
         <v>1356</v>
       </c>
       <c r="M1985" t="s">
-        <v>4000</v>
+        <v>4537</v>
       </c>
     </row>
     <row r="1986" spans="1:13" x14ac:dyDescent="0.3">
@@ -62900,7 +62969,7 @@
         <v>1992</v>
       </c>
       <c r="B1986" t="s">
-        <v>4001</v>
+        <v>4005</v>
       </c>
       <c r="C1986" t="s">
         <v>3878</v>
@@ -62915,7 +62984,7 @@
         <v>1356</v>
       </c>
       <c r="M1986" t="s">
-        <v>4536</v>
+        <v>4538</v>
       </c>
     </row>
     <row r="1987" spans="1:13" x14ac:dyDescent="0.3">
@@ -62923,7 +62992,7 @@
         <v>1993</v>
       </c>
       <c r="B1987" t="s">
-        <v>4002</v>
+        <v>4006</v>
       </c>
       <c r="C1987" t="s">
         <v>3878</v>
@@ -62938,7 +63007,7 @@
         <v>1356</v>
       </c>
       <c r="M1987" t="s">
-        <v>4003</v>
+        <v>4539</v>
       </c>
     </row>
     <row r="1988" spans="1:13" x14ac:dyDescent="0.3">
@@ -62946,7 +63015,7 @@
         <v>1994</v>
       </c>
       <c r="B1988" t="s">
-        <v>4004</v>
+        <v>4007</v>
       </c>
       <c r="C1988" t="s">
         <v>3878</v>
@@ -62961,7 +63030,7 @@
         <v>1356</v>
       </c>
       <c r="M1988" t="s">
-        <v>4537</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="1989" spans="1:13" x14ac:dyDescent="0.3">
@@ -62969,7 +63038,7 @@
         <v>1995</v>
       </c>
       <c r="B1989" t="s">
-        <v>4005</v>
+        <v>4008</v>
       </c>
       <c r="C1989" t="s">
         <v>3878</v>
@@ -62984,7 +63053,7 @@
         <v>1356</v>
       </c>
       <c r="M1989" t="s">
-        <v>4538</v>
+        <v>4541</v>
       </c>
     </row>
     <row r="1990" spans="1:13" x14ac:dyDescent="0.3">
@@ -62992,7 +63061,7 @@
         <v>1996</v>
       </c>
       <c r="B1990" t="s">
-        <v>4006</v>
+        <v>4009</v>
       </c>
       <c r="C1990" t="s">
         <v>3878</v>
@@ -63007,7 +63076,7 @@
         <v>1356</v>
       </c>
       <c r="M1990" t="s">
-        <v>4539</v>
+        <v>4542</v>
       </c>
     </row>
     <row r="1991" spans="1:13" x14ac:dyDescent="0.3">
@@ -63015,7 +63084,7 @@
         <v>1997</v>
       </c>
       <c r="B1991" t="s">
-        <v>4007</v>
+        <v>4010</v>
       </c>
       <c r="C1991" t="s">
         <v>3878</v>
@@ -63030,7 +63099,7 @@
         <v>1356</v>
       </c>
       <c r="M1991" t="s">
-        <v>4540</v>
+        <v>4011</v>
       </c>
     </row>
     <row r="1992" spans="1:13" x14ac:dyDescent="0.3">
@@ -63038,7 +63107,7 @@
         <v>1998</v>
       </c>
       <c r="B1992" t="s">
-        <v>4008</v>
+        <v>4012</v>
       </c>
       <c r="C1992" t="s">
         <v>3878</v>
@@ -63053,7 +63122,7 @@
         <v>1356</v>
       </c>
       <c r="M1992" t="s">
-        <v>4541</v>
+        <v>4543</v>
       </c>
     </row>
     <row r="1993" spans="1:13" x14ac:dyDescent="0.3">
@@ -63061,7 +63130,7 @@
         <v>1999</v>
       </c>
       <c r="B1993" t="s">
-        <v>4009</v>
+        <v>4013</v>
       </c>
       <c r="C1993" t="s">
         <v>3878</v>
@@ -63076,7 +63145,7 @@
         <v>1356</v>
       </c>
       <c r="M1993" t="s">
-        <v>4542</v>
+        <v>4544</v>
       </c>
     </row>
     <row r="1994" spans="1:13" x14ac:dyDescent="0.3">
@@ -63084,7 +63153,7 @@
         <v>2000</v>
       </c>
       <c r="B1994" t="s">
-        <v>4010</v>
+        <v>4014</v>
       </c>
       <c r="C1994" t="s">
         <v>3878</v>
@@ -63099,7 +63168,7 @@
         <v>1356</v>
       </c>
       <c r="M1994" t="s">
-        <v>4011</v>
+        <v>4015</v>
       </c>
     </row>
     <row r="1995" spans="1:13" x14ac:dyDescent="0.3">
@@ -63107,7 +63176,7 @@
         <v>2001</v>
       </c>
       <c r="B1995" t="s">
-        <v>4012</v>
+        <v>4016</v>
       </c>
       <c r="C1995" t="s">
         <v>3878</v>
@@ -63122,7 +63191,7 @@
         <v>1356</v>
       </c>
       <c r="M1995" t="s">
-        <v>4543</v>
+        <v>4545</v>
       </c>
     </row>
     <row r="1996" spans="1:13" x14ac:dyDescent="0.3">
@@ -63130,7 +63199,7 @@
         <v>2002</v>
       </c>
       <c r="B1996" t="s">
-        <v>4013</v>
+        <v>4017</v>
       </c>
       <c r="C1996" t="s">
         <v>3878</v>
@@ -63145,7 +63214,7 @@
         <v>1356</v>
       </c>
       <c r="M1996" t="s">
-        <v>4544</v>
+        <v>4018</v>
       </c>
     </row>
     <row r="1997" spans="1:13" x14ac:dyDescent="0.3">
@@ -63153,7 +63222,7 @@
         <v>2003</v>
       </c>
       <c r="B1997" t="s">
-        <v>4014</v>
+        <v>4019</v>
       </c>
       <c r="C1997" t="s">
         <v>3878</v>
@@ -63168,7 +63237,7 @@
         <v>1356</v>
       </c>
       <c r="M1997" t="s">
-        <v>4015</v>
+        <v>4020</v>
       </c>
     </row>
     <row r="1998" spans="1:13" x14ac:dyDescent="0.3">
@@ -63176,7 +63245,7 @@
         <v>2004</v>
       </c>
       <c r="B1998" t="s">
-        <v>4016</v>
+        <v>4021</v>
       </c>
       <c r="C1998" t="s">
         <v>3878</v>
@@ -63191,7 +63260,7 @@
         <v>1356</v>
       </c>
       <c r="M1998" t="s">
-        <v>4545</v>
+        <v>4546</v>
       </c>
     </row>
     <row r="1999" spans="1:13" x14ac:dyDescent="0.3">
@@ -63199,7 +63268,7 @@
         <v>2005</v>
       </c>
       <c r="B1999" t="s">
-        <v>4017</v>
+        <v>4022</v>
       </c>
       <c r="C1999" t="s">
         <v>3878</v>
@@ -63214,7 +63283,7 @@
         <v>1356</v>
       </c>
       <c r="M1999" t="s">
-        <v>4018</v>
+        <v>4023</v>
       </c>
     </row>
     <row r="2000" spans="1:13" x14ac:dyDescent="0.3">
@@ -63222,7 +63291,7 @@
         <v>2006</v>
       </c>
       <c r="B2000" t="s">
-        <v>4019</v>
+        <v>4024</v>
       </c>
       <c r="C2000" t="s">
         <v>3878</v>
@@ -63237,7 +63306,7 @@
         <v>1356</v>
       </c>
       <c r="M2000" t="s">
-        <v>4020</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="2001" spans="1:13" x14ac:dyDescent="0.3">
@@ -63245,7 +63314,7 @@
         <v>2007</v>
       </c>
       <c r="B2001" t="s">
-        <v>4021</v>
+        <v>4025</v>
       </c>
       <c r="C2001" t="s">
         <v>3878</v>
@@ -63260,7 +63329,7 @@
         <v>1356</v>
       </c>
       <c r="M2001" t="s">
-        <v>4546</v>
+        <v>4548</v>
       </c>
     </row>
     <row r="2002" spans="1:13" x14ac:dyDescent="0.3">
@@ -63268,7 +63337,7 @@
         <v>2008</v>
       </c>
       <c r="B2002" t="s">
-        <v>4022</v>
+        <v>4026</v>
       </c>
       <c r="C2002" t="s">
         <v>3878</v>
@@ -63283,7 +63352,7 @@
         <v>1356</v>
       </c>
       <c r="M2002" t="s">
-        <v>4023</v>
+        <v>4549</v>
       </c>
     </row>
     <row r="2003" spans="1:13" x14ac:dyDescent="0.3">
@@ -63291,7 +63360,7 @@
         <v>2009</v>
       </c>
       <c r="B2003" t="s">
-        <v>4024</v>
+        <v>4027</v>
       </c>
       <c r="C2003" t="s">
         <v>3878</v>
@@ -63306,7 +63375,7 @@
         <v>1356</v>
       </c>
       <c r="M2003" t="s">
-        <v>4547</v>
+        <v>4550</v>
       </c>
     </row>
     <row r="2004" spans="1:13" x14ac:dyDescent="0.3">
@@ -63314,7 +63383,7 @@
         <v>2010</v>
       </c>
       <c r="B2004" t="s">
-        <v>4025</v>
+        <v>4028</v>
       </c>
       <c r="C2004" t="s">
         <v>3878</v>
@@ -63329,7 +63398,7 @@
         <v>1356</v>
       </c>
       <c r="M2004" t="s">
-        <v>4548</v>
+        <v>4551</v>
       </c>
     </row>
     <row r="2005" spans="1:13" x14ac:dyDescent="0.3">
@@ -63337,7 +63406,7 @@
         <v>2011</v>
       </c>
       <c r="B2005" t="s">
-        <v>4026</v>
+        <v>4029</v>
       </c>
       <c r="C2005" t="s">
         <v>3878</v>
@@ -63352,7 +63421,7 @@
         <v>1356</v>
       </c>
       <c r="M2005" t="s">
-        <v>4549</v>
+        <v>4030</v>
       </c>
     </row>
     <row r="2006" spans="1:13" x14ac:dyDescent="0.3">
@@ -63360,7 +63429,7 @@
         <v>2012</v>
       </c>
       <c r="B2006" t="s">
-        <v>4027</v>
+        <v>4031</v>
       </c>
       <c r="C2006" t="s">
         <v>3878</v>
@@ -63375,7 +63444,7 @@
         <v>1356</v>
       </c>
       <c r="M2006" t="s">
-        <v>4550</v>
+        <v>4552</v>
       </c>
     </row>
     <row r="2007" spans="1:13" x14ac:dyDescent="0.3">
@@ -63383,7 +63452,7 @@
         <v>2013</v>
       </c>
       <c r="B2007" t="s">
-        <v>4028</v>
+        <v>4032</v>
       </c>
       <c r="C2007" t="s">
         <v>3878</v>
@@ -63398,7 +63467,7 @@
         <v>1356</v>
       </c>
       <c r="M2007" t="s">
-        <v>4551</v>
+        <v>4553</v>
       </c>
     </row>
     <row r="2008" spans="1:13" x14ac:dyDescent="0.3">
@@ -63406,7 +63475,7 @@
         <v>2014</v>
       </c>
       <c r="B2008" t="s">
-        <v>4029</v>
+        <v>4033</v>
       </c>
       <c r="C2008" t="s">
         <v>3878</v>
@@ -63421,7 +63490,7 @@
         <v>1356</v>
       </c>
       <c r="M2008" t="s">
-        <v>4030</v>
+        <v>4034</v>
       </c>
     </row>
     <row r="2009" spans="1:13" x14ac:dyDescent="0.3">
@@ -63429,7 +63498,7 @@
         <v>2015</v>
       </c>
       <c r="B2009" t="s">
-        <v>4031</v>
+        <v>4035</v>
       </c>
       <c r="C2009" t="s">
         <v>3878</v>
@@ -63444,7 +63513,7 @@
         <v>1356</v>
       </c>
       <c r="M2009" t="s">
-        <v>4552</v>
+        <v>4036</v>
       </c>
     </row>
     <row r="2010" spans="1:13" x14ac:dyDescent="0.3">
@@ -63452,7 +63521,7 @@
         <v>2016</v>
       </c>
       <c r="B2010" t="s">
-        <v>4032</v>
+        <v>4037</v>
       </c>
       <c r="C2010" t="s">
         <v>3878</v>
@@ -63467,7 +63536,7 @@
         <v>1356</v>
       </c>
       <c r="M2010" t="s">
-        <v>4553</v>
+        <v>4038</v>
       </c>
     </row>
     <row r="2011" spans="1:13" x14ac:dyDescent="0.3">
@@ -63475,7 +63544,7 @@
         <v>2017</v>
       </c>
       <c r="B2011" t="s">
-        <v>4033</v>
+        <v>4039</v>
       </c>
       <c r="C2011" t="s">
         <v>3878</v>
@@ -63490,7 +63559,7 @@
         <v>1356</v>
       </c>
       <c r="M2011" t="s">
-        <v>4034</v>
+        <v>4040</v>
       </c>
     </row>
     <row r="2012" spans="1:13" x14ac:dyDescent="0.3">
@@ -63498,7 +63567,7 @@
         <v>2018</v>
       </c>
       <c r="B2012" t="s">
-        <v>4035</v>
+        <v>4041</v>
       </c>
       <c r="C2012" t="s">
         <v>3878</v>
@@ -63513,7 +63582,7 @@
         <v>1356</v>
       </c>
       <c r="M2012" t="s">
-        <v>4036</v>
+        <v>4554</v>
       </c>
     </row>
     <row r="2013" spans="1:13" x14ac:dyDescent="0.3">
@@ -63521,7 +63590,7 @@
         <v>2019</v>
       </c>
       <c r="B2013" t="s">
-        <v>4037</v>
+        <v>4042</v>
       </c>
       <c r="C2013" t="s">
         <v>3878</v>
@@ -63536,7 +63605,7 @@
         <v>1356</v>
       </c>
       <c r="M2013" t="s">
-        <v>4038</v>
+        <v>4043</v>
       </c>
     </row>
     <row r="2014" spans="1:13" x14ac:dyDescent="0.3">
@@ -63544,7 +63613,7 @@
         <v>2020</v>
       </c>
       <c r="B2014" t="s">
-        <v>4039</v>
+        <v>4044</v>
       </c>
       <c r="C2014" t="s">
         <v>3878</v>
@@ -63559,7 +63628,7 @@
         <v>1356</v>
       </c>
       <c r="M2014" t="s">
-        <v>4040</v>
+        <v>4045</v>
       </c>
     </row>
     <row r="2015" spans="1:13" x14ac:dyDescent="0.3">
@@ -63567,7 +63636,7 @@
         <v>2021</v>
       </c>
       <c r="B2015" t="s">
-        <v>4041</v>
+        <v>4046</v>
       </c>
       <c r="C2015" t="s">
         <v>3878</v>
@@ -63582,7 +63651,7 @@
         <v>1356</v>
       </c>
       <c r="M2015" t="s">
-        <v>4554</v>
+        <v>4555</v>
       </c>
     </row>
     <row r="2016" spans="1:13" x14ac:dyDescent="0.3">
@@ -63590,7 +63659,7 @@
         <v>2022</v>
       </c>
       <c r="B2016" t="s">
-        <v>4042</v>
+        <v>4047</v>
       </c>
       <c r="C2016" t="s">
         <v>3878</v>
@@ -63605,7 +63674,7 @@
         <v>1356</v>
       </c>
       <c r="M2016" t="s">
-        <v>4043</v>
+        <v>4048</v>
       </c>
     </row>
     <row r="2017" spans="1:13" x14ac:dyDescent="0.3">
@@ -63613,7 +63682,7 @@
         <v>2023</v>
       </c>
       <c r="B2017" t="s">
-        <v>4044</v>
+        <v>4049</v>
       </c>
       <c r="C2017" t="s">
         <v>3878</v>
@@ -63628,7 +63697,7 @@
         <v>1356</v>
       </c>
       <c r="M2017" t="s">
-        <v>4045</v>
+        <v>4556</v>
       </c>
     </row>
     <row r="2018" spans="1:13" x14ac:dyDescent="0.3">
@@ -63636,7 +63705,7 @@
         <v>2024</v>
       </c>
       <c r="B2018" t="s">
-        <v>4046</v>
+        <v>4050</v>
       </c>
       <c r="C2018" t="s">
         <v>3878</v>
@@ -63651,7 +63720,7 @@
         <v>1356</v>
       </c>
       <c r="M2018" t="s">
-        <v>4555</v>
+        <v>4051</v>
       </c>
     </row>
     <row r="2019" spans="1:13" x14ac:dyDescent="0.3">
@@ -63659,7 +63728,7 @@
         <v>2025</v>
       </c>
       <c r="B2019" t="s">
-        <v>4047</v>
+        <v>4052</v>
       </c>
       <c r="C2019" t="s">
         <v>3878</v>
@@ -63674,7 +63743,7 @@
         <v>1356</v>
       </c>
       <c r="M2019" t="s">
-        <v>4048</v>
+        <v>4053</v>
       </c>
     </row>
     <row r="2020" spans="1:13" x14ac:dyDescent="0.3">
@@ -63682,7 +63751,7 @@
         <v>2026</v>
       </c>
       <c r="B2020" t="s">
-        <v>4049</v>
+        <v>4054</v>
       </c>
       <c r="C2020" t="s">
         <v>3878</v>
@@ -63697,7 +63766,7 @@
         <v>1356</v>
       </c>
       <c r="M2020" t="s">
-        <v>4556</v>
+        <v>4055</v>
       </c>
     </row>
     <row r="2021" spans="1:13" x14ac:dyDescent="0.3">
@@ -63705,7 +63774,7 @@
         <v>2027</v>
       </c>
       <c r="B2021" t="s">
-        <v>4050</v>
+        <v>4056</v>
       </c>
       <c r="C2021" t="s">
         <v>3878</v>
@@ -63720,7 +63789,7 @@
         <v>1356</v>
       </c>
       <c r="M2021" t="s">
-        <v>4051</v>
+        <v>4557</v>
       </c>
     </row>
     <row r="2022" spans="1:13" x14ac:dyDescent="0.3">
@@ -63728,7 +63797,7 @@
         <v>2028</v>
       </c>
       <c r="B2022" t="s">
-        <v>4052</v>
+        <v>4057</v>
       </c>
       <c r="C2022" t="s">
         <v>3878</v>
@@ -63743,7 +63812,7 @@
         <v>1356</v>
       </c>
       <c r="M2022" t="s">
-        <v>4053</v>
+        <v>4558</v>
       </c>
     </row>
     <row r="2023" spans="1:13" x14ac:dyDescent="0.3">
@@ -63751,7 +63820,7 @@
         <v>2029</v>
       </c>
       <c r="B2023" t="s">
-        <v>4054</v>
+        <v>4058</v>
       </c>
       <c r="C2023" t="s">
         <v>3878</v>
@@ -63766,7 +63835,7 @@
         <v>1356</v>
       </c>
       <c r="M2023" t="s">
-        <v>4055</v>
+        <v>4559</v>
       </c>
     </row>
     <row r="2024" spans="1:13" x14ac:dyDescent="0.3">
@@ -63774,7 +63843,7 @@
         <v>2030</v>
       </c>
       <c r="B2024" t="s">
-        <v>4056</v>
+        <v>4059</v>
       </c>
       <c r="C2024" t="s">
         <v>3878</v>
@@ -63789,7 +63858,7 @@
         <v>1356</v>
       </c>
       <c r="M2024" t="s">
-        <v>4557</v>
+        <v>4560</v>
       </c>
     </row>
     <row r="2025" spans="1:13" x14ac:dyDescent="0.3">
@@ -63797,7 +63866,7 @@
         <v>2031</v>
       </c>
       <c r="B2025" t="s">
-        <v>4057</v>
+        <v>4060</v>
       </c>
       <c r="C2025" t="s">
         <v>3878</v>
@@ -63812,7 +63881,7 @@
         <v>1356</v>
       </c>
       <c r="M2025" t="s">
-        <v>4558</v>
+        <v>4561</v>
       </c>
     </row>
     <row r="2026" spans="1:13" x14ac:dyDescent="0.3">
@@ -63820,7 +63889,7 @@
         <v>2032</v>
       </c>
       <c r="B2026" t="s">
-        <v>4058</v>
+        <v>4061</v>
       </c>
       <c r="C2026" t="s">
         <v>3878</v>
@@ -63835,7 +63904,7 @@
         <v>1356</v>
       </c>
       <c r="M2026" t="s">
-        <v>4559</v>
+        <v>4062</v>
       </c>
     </row>
     <row r="2027" spans="1:13" x14ac:dyDescent="0.3">
@@ -63843,7 +63912,7 @@
         <v>2033</v>
       </c>
       <c r="B2027" t="s">
-        <v>4059</v>
+        <v>4063</v>
       </c>
       <c r="C2027" t="s">
         <v>3878</v>
@@ -63858,7 +63927,7 @@
         <v>1356</v>
       </c>
       <c r="M2027" t="s">
-        <v>4560</v>
+        <v>4562</v>
       </c>
     </row>
     <row r="2028" spans="1:13" x14ac:dyDescent="0.3">
@@ -63866,7 +63935,7 @@
         <v>2034</v>
       </c>
       <c r="B2028" t="s">
-        <v>4060</v>
+        <v>4064</v>
       </c>
       <c r="C2028" t="s">
         <v>3878</v>
@@ -63881,80 +63950,11 @@
         <v>1356</v>
       </c>
       <c r="M2028" t="s">
-        <v>4561</v>
-      </c>
-    </row>
-    <row r="2029" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2029">
-        <v>2035</v>
-      </c>
-      <c r="B2029" t="s">
-        <v>4061</v>
-      </c>
-      <c r="C2029" t="s">
-        <v>3878</v>
-      </c>
-      <c r="D2029">
-        <v>68000</v>
-      </c>
-      <c r="E2029" t="s">
-        <v>154</v>
-      </c>
-      <c r="H2029" t="s">
-        <v>1356</v>
-      </c>
-      <c r="M2029" t="s">
-        <v>4062</v>
-      </c>
-    </row>
-    <row r="2030" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2030">
-        <v>2036</v>
-      </c>
-      <c r="B2030" t="s">
-        <v>4063</v>
-      </c>
-      <c r="C2030" t="s">
-        <v>3878</v>
-      </c>
-      <c r="D2030">
-        <v>68000</v>
-      </c>
-      <c r="E2030" t="s">
-        <v>154</v>
-      </c>
-      <c r="H2030" t="s">
-        <v>1356</v>
-      </c>
-      <c r="M2030" t="s">
-        <v>4562</v>
-      </c>
-    </row>
-    <row r="2031" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2031">
-        <v>2037</v>
-      </c>
-      <c r="B2031" t="s">
-        <v>4064</v>
-      </c>
-      <c r="C2031" t="s">
-        <v>3878</v>
-      </c>
-      <c r="D2031">
-        <v>68000</v>
-      </c>
-      <c r="E2031" t="s">
-        <v>154</v>
-      </c>
-      <c r="H2031" t="s">
-        <v>1356</v>
-      </c>
-      <c r="M2031" t="s">
         <v>4065</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M2031"/>
+  <autoFilter ref="A1:M2028"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
036 : added working vulgus driver
</commit_message>
<xml_diff>
--- a/0.36/compatibility.xlsx
+++ b/0.36/compatibility.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
     <sheet name="Playable" sheetId="4" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12399" uniqueCount="4566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12402" uniqueCount="4566">
   <si>
     <t>romname</t>
   </si>
@@ -14077,10 +14077,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P55"/>
+  <dimension ref="A1:P58"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="M55" sqref="M55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M62" sqref="M62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15347,6 +15347,84 @@
         <v>4565</v>
       </c>
     </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>56</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1574</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1575</v>
+      </c>
+      <c r="D56" t="s">
+        <v>14</v>
+      </c>
+      <c r="E56" t="s">
+        <v>154</v>
+      </c>
+      <c r="H56" t="s">
+        <v>172</v>
+      </c>
+      <c r="M56" t="s">
+        <v>1576</v>
+      </c>
+      <c r="O56" t="s">
+        <v>4563</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>57</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1577</v>
+      </c>
+      <c r="C57" t="s">
+        <v>1575</v>
+      </c>
+      <c r="D57" t="s">
+        <v>14</v>
+      </c>
+      <c r="E57" t="s">
+        <v>154</v>
+      </c>
+      <c r="H57" t="s">
+        <v>172</v>
+      </c>
+      <c r="M57" t="s">
+        <v>1578</v>
+      </c>
+      <c r="O57" t="s">
+        <v>4563</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>58</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1579</v>
+      </c>
+      <c r="C58" t="s">
+        <v>1575</v>
+      </c>
+      <c r="D58" t="s">
+        <v>14</v>
+      </c>
+      <c r="E58" t="s">
+        <v>154</v>
+      </c>
+      <c r="H58" t="s">
+        <v>172</v>
+      </c>
+      <c r="M58" t="s">
+        <v>1580</v>
+      </c>
+      <c r="O58" t="s">
+        <v>4563</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15356,8 +15434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1994"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="M129" sqref="M129"/>
+    <sheetView topLeftCell="A735" workbookViewId="0">
+      <selection activeCell="A750" sqref="A750:XFD752"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33429,75 +33507,6 @@
         <v>4225</v>
       </c>
     </row>
-    <row r="750" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A750">
-        <v>768</v>
-      </c>
-      <c r="B750" t="s">
-        <v>1574</v>
-      </c>
-      <c r="C750" t="s">
-        <v>1575</v>
-      </c>
-      <c r="D750" t="s">
-        <v>14</v>
-      </c>
-      <c r="E750" t="s">
-        <v>154</v>
-      </c>
-      <c r="H750" t="s">
-        <v>172</v>
-      </c>
-      <c r="M750" t="s">
-        <v>1576</v>
-      </c>
-    </row>
-    <row r="751" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A751">
-        <v>769</v>
-      </c>
-      <c r="B751" t="s">
-        <v>1577</v>
-      </c>
-      <c r="C751" t="s">
-        <v>1575</v>
-      </c>
-      <c r="D751" t="s">
-        <v>14</v>
-      </c>
-      <c r="E751" t="s">
-        <v>154</v>
-      </c>
-      <c r="H751" t="s">
-        <v>172</v>
-      </c>
-      <c r="M751" t="s">
-        <v>1578</v>
-      </c>
-    </row>
-    <row r="752" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A752">
-        <v>770</v>
-      </c>
-      <c r="B752" t="s">
-        <v>1579</v>
-      </c>
-      <c r="C752" t="s">
-        <v>1575</v>
-      </c>
-      <c r="D752" t="s">
-        <v>14</v>
-      </c>
-      <c r="E752" t="s">
-        <v>154</v>
-      </c>
-      <c r="H752" t="s">
-        <v>172</v>
-      </c>
-      <c r="M752" t="s">
-        <v>1580</v>
-      </c>
-    </row>
     <row r="753" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A753">
         <v>771</v>

</xml_diff>

<commit_message>
036 : Added marineb driver
</commit_message>
<xml_diff>
--- a/0.36/compatibility.xlsx
+++ b/0.36/compatibility.xlsx
@@ -16,8 +16,8 @@
     <sheet name="ALL" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ALL!$A$1:$M$1989</definedName>
-    <definedName name="LIST" localSheetId="1">ALL!$B$1:$M$1989</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ALL!$A$1:$M$1981</definedName>
+    <definedName name="LIST" localSheetId="1">ALL!$B$1:$M$1981</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12402" uniqueCount="4566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12410" uniqueCount="4567">
   <si>
     <t>romname</t>
   </si>
@@ -13754,6 +13754,9 @@
   </si>
   <si>
     <t>segacrpt machine</t>
+  </si>
+  <si>
+    <t>uses espial machine,vidhrdw</t>
   </si>
 </sst>
 </file>
@@ -14077,10 +14080,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P60"/>
+  <dimension ref="A1:P68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="O68" sqref="O68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15472,6 +15475,190 @@
         <v>3737</v>
       </c>
     </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>61</v>
+      </c>
+      <c r="B61" t="s">
+        <v>3702</v>
+      </c>
+      <c r="C61" t="s">
+        <v>3703</v>
+      </c>
+      <c r="D61" t="s">
+        <v>14</v>
+      </c>
+      <c r="H61" t="s">
+        <v>71</v>
+      </c>
+      <c r="M61" t="s">
+        <v>3704</v>
+      </c>
+      <c r="O61" t="s">
+        <v>4566</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>62</v>
+      </c>
+      <c r="B62" t="s">
+        <v>3705</v>
+      </c>
+      <c r="C62" t="s">
+        <v>3703</v>
+      </c>
+      <c r="D62" t="s">
+        <v>14</v>
+      </c>
+      <c r="H62" t="s">
+        <v>71</v>
+      </c>
+      <c r="M62" t="s">
+        <v>3706</v>
+      </c>
+      <c r="O62" t="s">
+        <v>4566</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>63</v>
+      </c>
+      <c r="B63" t="s">
+        <v>3707</v>
+      </c>
+      <c r="C63" t="s">
+        <v>3703</v>
+      </c>
+      <c r="D63" t="s">
+        <v>14</v>
+      </c>
+      <c r="H63" t="s">
+        <v>71</v>
+      </c>
+      <c r="M63" t="s">
+        <v>3708</v>
+      </c>
+      <c r="O63" t="s">
+        <v>4566</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>64</v>
+      </c>
+      <c r="B64" t="s">
+        <v>3709</v>
+      </c>
+      <c r="C64" t="s">
+        <v>3703</v>
+      </c>
+      <c r="D64" t="s">
+        <v>14</v>
+      </c>
+      <c r="H64" t="s">
+        <v>71</v>
+      </c>
+      <c r="M64" t="s">
+        <v>3710</v>
+      </c>
+      <c r="O64" t="s">
+        <v>4566</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>65</v>
+      </c>
+      <c r="B65" t="s">
+        <v>3711</v>
+      </c>
+      <c r="C65" t="s">
+        <v>3703</v>
+      </c>
+      <c r="D65" t="s">
+        <v>14</v>
+      </c>
+      <c r="H65" t="s">
+        <v>71</v>
+      </c>
+      <c r="M65" t="s">
+        <v>3712</v>
+      </c>
+      <c r="O65" t="s">
+        <v>4566</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>66</v>
+      </c>
+      <c r="B66" t="s">
+        <v>3713</v>
+      </c>
+      <c r="C66" t="s">
+        <v>3703</v>
+      </c>
+      <c r="D66" t="s">
+        <v>14</v>
+      </c>
+      <c r="H66" t="s">
+        <v>71</v>
+      </c>
+      <c r="M66" t="s">
+        <v>3714</v>
+      </c>
+      <c r="O66" t="s">
+        <v>4566</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>67</v>
+      </c>
+      <c r="B67" t="s">
+        <v>3715</v>
+      </c>
+      <c r="C67" t="s">
+        <v>3703</v>
+      </c>
+      <c r="D67" t="s">
+        <v>14</v>
+      </c>
+      <c r="H67" t="s">
+        <v>71</v>
+      </c>
+      <c r="M67" t="s">
+        <v>3716</v>
+      </c>
+      <c r="O67" t="s">
+        <v>4566</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>68</v>
+      </c>
+      <c r="B68" t="s">
+        <v>3717</v>
+      </c>
+      <c r="C68" t="s">
+        <v>3703</v>
+      </c>
+      <c r="D68" t="s">
+        <v>14</v>
+      </c>
+      <c r="H68" t="s">
+        <v>172</v>
+      </c>
+      <c r="M68" t="s">
+        <v>3718</v>
+      </c>
+      <c r="O68" t="s">
+        <v>4566</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15479,10 +15666,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1989"/>
+  <dimension ref="A1:M1981"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q1810" sqref="Q1810"/>
+    <sheetView topLeftCell="A1956" workbookViewId="0">
+      <selection activeCell="A1797" sqref="A1797:XFD1804"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -59596,13 +59783,13 @@
     </row>
     <row r="1797" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1797">
-        <v>1826</v>
+        <v>1834</v>
       </c>
       <c r="B1797" t="s">
-        <v>3702</v>
+        <v>3719</v>
       </c>
       <c r="C1797" t="s">
-        <v>3703</v>
+        <v>3720</v>
       </c>
       <c r="D1797" t="s">
         <v>14</v>
@@ -59611,18 +59798,18 @@
         <v>71</v>
       </c>
       <c r="M1797" t="s">
-        <v>3704</v>
+        <v>3721</v>
       </c>
     </row>
     <row r="1798" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1798">
-        <v>1827</v>
+        <v>1835</v>
       </c>
       <c r="B1798" t="s">
-        <v>3705</v>
+        <v>3722</v>
       </c>
       <c r="C1798" t="s">
-        <v>3703</v>
+        <v>3720</v>
       </c>
       <c r="D1798" t="s">
         <v>14</v>
@@ -59631,270 +59818,285 @@
         <v>71</v>
       </c>
       <c r="M1798" t="s">
-        <v>3706</v>
+        <v>3723</v>
       </c>
     </row>
     <row r="1799" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1799">
-        <v>1828</v>
+        <v>1836</v>
       </c>
       <c r="B1799" t="s">
-        <v>3707</v>
+        <v>3724</v>
       </c>
       <c r="C1799" t="s">
-        <v>3703</v>
+        <v>3725</v>
       </c>
       <c r="D1799" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1799" t="s">
         <v>14</v>
       </c>
       <c r="H1799" t="s">
         <v>71</v>
       </c>
       <c r="M1799" t="s">
-        <v>3708</v>
+        <v>3726</v>
       </c>
     </row>
     <row r="1800" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1800">
-        <v>1829</v>
+        <v>1837</v>
       </c>
       <c r="B1800" t="s">
-        <v>3709</v>
+        <v>3727</v>
       </c>
       <c r="C1800" t="s">
-        <v>3703</v>
+        <v>3725</v>
       </c>
       <c r="D1800" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1800" t="s">
         <v>14</v>
       </c>
       <c r="H1800" t="s">
         <v>71</v>
       </c>
       <c r="M1800" t="s">
-        <v>3710</v>
+        <v>3728</v>
       </c>
     </row>
     <row r="1801" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1801">
-        <v>1830</v>
+        <v>1838</v>
       </c>
       <c r="B1801" t="s">
-        <v>3711</v>
+        <v>3729</v>
       </c>
       <c r="C1801" t="s">
-        <v>3703</v>
+        <v>3725</v>
       </c>
       <c r="D1801" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1801" t="s">
         <v>14</v>
       </c>
       <c r="H1801" t="s">
         <v>71</v>
       </c>
       <c r="M1801" t="s">
-        <v>3712</v>
+        <v>3730</v>
       </c>
     </row>
     <row r="1802" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1802">
-        <v>1831</v>
+        <v>1839</v>
       </c>
       <c r="B1802" t="s">
-        <v>3713</v>
+        <v>3731</v>
       </c>
       <c r="C1802" t="s">
-        <v>3703</v>
+        <v>3725</v>
       </c>
       <c r="D1802" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1802" t="s">
         <v>14</v>
       </c>
       <c r="H1802" t="s">
         <v>71</v>
       </c>
       <c r="M1802" t="s">
-        <v>3714</v>
+        <v>3732</v>
       </c>
     </row>
     <row r="1803" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1803">
-        <v>1832</v>
+        <v>1842</v>
       </c>
       <c r="B1803" t="s">
-        <v>3715</v>
+        <v>3738</v>
       </c>
       <c r="C1803" t="s">
-        <v>3703</v>
+        <v>3739</v>
       </c>
       <c r="D1803" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1803" t="s">
         <v>14</v>
       </c>
       <c r="H1803" t="s">
         <v>71</v>
       </c>
       <c r="M1803" t="s">
-        <v>3716</v>
+        <v>3740</v>
       </c>
     </row>
     <row r="1804" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1804">
-        <v>1833</v>
+        <v>1843</v>
       </c>
       <c r="B1804" t="s">
-        <v>3717</v>
+        <v>3741</v>
       </c>
       <c r="C1804" t="s">
-        <v>3703</v>
+        <v>3739</v>
       </c>
       <c r="D1804" t="s">
         <v>14</v>
       </c>
+      <c r="E1804" t="s">
+        <v>14</v>
+      </c>
       <c r="H1804" t="s">
-        <v>172</v>
+        <v>71</v>
       </c>
       <c r="M1804" t="s">
-        <v>3718</v>
+        <v>3742</v>
       </c>
     </row>
     <row r="1805" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1805">
-        <v>1834</v>
+        <v>1844</v>
       </c>
       <c r="B1805" t="s">
-        <v>3719</v>
+        <v>3743</v>
       </c>
       <c r="C1805" t="s">
-        <v>3720</v>
-      </c>
-      <c r="D1805" t="s">
+        <v>3744</v>
+      </c>
+      <c r="D1805">
+        <v>68000</v>
+      </c>
+      <c r="E1805" t="s">
         <v>14</v>
       </c>
       <c r="H1805" t="s">
-        <v>71</v>
+        <v>349</v>
       </c>
       <c r="M1805" t="s">
-        <v>3721</v>
+        <v>3745</v>
       </c>
     </row>
     <row r="1806" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1806">
-        <v>1835</v>
+        <v>1845</v>
       </c>
       <c r="B1806" t="s">
-        <v>3722</v>
+        <v>3746</v>
       </c>
       <c r="C1806" t="s">
-        <v>3720</v>
-      </c>
-      <c r="D1806" t="s">
-        <v>14</v>
+        <v>3747</v>
+      </c>
+      <c r="D1806">
+        <v>68000</v>
       </c>
       <c r="H1806" t="s">
-        <v>71</v>
+        <v>172</v>
+      </c>
+      <c r="I1806" t="s">
+        <v>1495</v>
       </c>
       <c r="M1806" t="s">
-        <v>3723</v>
+        <v>3748</v>
       </c>
     </row>
     <row r="1807" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1807">
-        <v>1836</v>
+        <v>1846</v>
       </c>
       <c r="B1807" t="s">
-        <v>3724</v>
+        <v>3749</v>
       </c>
       <c r="C1807" t="s">
-        <v>3725</v>
-      </c>
-      <c r="D1807" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1807" t="s">
-        <v>14</v>
+        <v>3747</v>
+      </c>
+      <c r="D1807">
+        <v>68000</v>
       </c>
       <c r="H1807" t="s">
-        <v>71</v>
+        <v>172</v>
+      </c>
+      <c r="I1807" t="s">
+        <v>1495</v>
       </c>
       <c r="M1807" t="s">
-        <v>3726</v>
+        <v>3750</v>
       </c>
     </row>
     <row r="1808" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1808">
-        <v>1837</v>
+        <v>1847</v>
       </c>
       <c r="B1808" t="s">
-        <v>3727</v>
+        <v>3751</v>
       </c>
       <c r="C1808" t="s">
-        <v>3725</v>
-      </c>
-      <c r="D1808" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1808" t="s">
-        <v>14</v>
+        <v>3747</v>
+      </c>
+      <c r="D1808">
+        <v>68000</v>
       </c>
       <c r="H1808" t="s">
-        <v>71</v>
+        <v>2378</v>
       </c>
       <c r="M1808" t="s">
-        <v>3728</v>
+        <v>3752</v>
       </c>
     </row>
     <row r="1809" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1809">
-        <v>1838</v>
+        <v>1848</v>
       </c>
       <c r="B1809" t="s">
-        <v>3729</v>
+        <v>3753</v>
       </c>
       <c r="C1809" t="s">
-        <v>3725</v>
-      </c>
-      <c r="D1809" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1809" t="s">
-        <v>14</v>
+        <v>3747</v>
+      </c>
+      <c r="D1809">
+        <v>68000</v>
       </c>
       <c r="H1809" t="s">
-        <v>71</v>
+        <v>2378</v>
       </c>
       <c r="M1809" t="s">
-        <v>3730</v>
+        <v>4492</v>
       </c>
     </row>
     <row r="1810" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1810">
-        <v>1839</v>
+        <v>1849</v>
       </c>
       <c r="B1810" t="s">
-        <v>3731</v>
+        <v>3754</v>
       </c>
       <c r="C1810" t="s">
-        <v>3725</v>
-      </c>
-      <c r="D1810" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1810" t="s">
-        <v>14</v>
+        <v>3755</v>
+      </c>
+      <c r="D1810">
+        <v>68000</v>
       </c>
       <c r="H1810" t="s">
-        <v>71</v>
+        <v>1495</v>
       </c>
       <c r="M1810" t="s">
-        <v>3732</v>
+        <v>3756</v>
       </c>
     </row>
     <row r="1811" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1811">
-        <v>1842</v>
+        <v>1850</v>
       </c>
       <c r="B1811" t="s">
-        <v>3738</v>
+        <v>3757</v>
       </c>
       <c r="C1811" t="s">
-        <v>3739</v>
+        <v>3758</v>
       </c>
       <c r="D1811" t="s">
         <v>14</v>
@@ -59902,676 +60104,730 @@
       <c r="E1811" t="s">
         <v>14</v>
       </c>
+      <c r="F1811" t="s">
+        <v>14</v>
+      </c>
       <c r="H1811" t="s">
-        <v>71</v>
+        <v>336</v>
+      </c>
+      <c r="I1811" t="s">
+        <v>1495</v>
       </c>
       <c r="M1811" t="s">
-        <v>3740</v>
+        <v>3759</v>
       </c>
     </row>
     <row r="1812" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1812">
-        <v>1843</v>
+        <v>1851</v>
       </c>
       <c r="B1812" t="s">
-        <v>3741</v>
+        <v>3760</v>
       </c>
       <c r="C1812" t="s">
-        <v>3739</v>
+        <v>3761</v>
       </c>
       <c r="D1812" t="s">
         <v>14</v>
       </c>
       <c r="E1812" t="s">
-        <v>14</v>
+        <v>728</v>
       </c>
       <c r="H1812" t="s">
-        <v>71</v>
+        <v>166</v>
       </c>
       <c r="M1812" t="s">
-        <v>3742</v>
+        <v>4493</v>
       </c>
     </row>
     <row r="1813" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1813">
-        <v>1844</v>
+        <v>1852</v>
       </c>
       <c r="B1813" t="s">
-        <v>3743</v>
+        <v>3762</v>
       </c>
       <c r="C1813" t="s">
-        <v>3744</v>
-      </c>
-      <c r="D1813">
-        <v>68000</v>
+        <v>3761</v>
+      </c>
+      <c r="D1813" t="s">
+        <v>14</v>
       </c>
       <c r="E1813" t="s">
-        <v>14</v>
+        <v>728</v>
       </c>
       <c r="H1813" t="s">
-        <v>349</v>
+        <v>166</v>
       </c>
       <c r="M1813" t="s">
-        <v>3745</v>
+        <v>3763</v>
       </c>
     </row>
     <row r="1814" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1814">
-        <v>1845</v>
+        <v>1853</v>
       </c>
       <c r="B1814" t="s">
-        <v>3746</v>
+        <v>3764</v>
       </c>
       <c r="C1814" t="s">
-        <v>3747</v>
-      </c>
-      <c r="D1814">
-        <v>68000</v>
+        <v>3761</v>
+      </c>
+      <c r="D1814" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1814" t="s">
+        <v>728</v>
       </c>
       <c r="H1814" t="s">
-        <v>172</v>
-      </c>
-      <c r="I1814" t="s">
-        <v>1495</v>
+        <v>166</v>
       </c>
       <c r="M1814" t="s">
-        <v>3748</v>
+        <v>3765</v>
       </c>
     </row>
     <row r="1815" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1815">
-        <v>1846</v>
+        <v>1854</v>
       </c>
       <c r="B1815" t="s">
-        <v>3749</v>
+        <v>3766</v>
       </c>
       <c r="C1815" t="s">
-        <v>3747</v>
-      </c>
-      <c r="D1815">
-        <v>68000</v>
+        <v>3761</v>
+      </c>
+      <c r="D1815" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1815" t="s">
+        <v>728</v>
       </c>
       <c r="H1815" t="s">
-        <v>172</v>
-      </c>
-      <c r="I1815" t="s">
-        <v>1495</v>
+        <v>166</v>
       </c>
       <c r="M1815" t="s">
-        <v>3750</v>
+        <v>3767</v>
       </c>
     </row>
     <row r="1816" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1816">
-        <v>1847</v>
+        <v>1855</v>
       </c>
       <c r="B1816" t="s">
-        <v>3751</v>
+        <v>3768</v>
       </c>
       <c r="C1816" t="s">
-        <v>3747</v>
-      </c>
-      <c r="D1816">
-        <v>68000</v>
+        <v>3761</v>
+      </c>
+      <c r="D1816" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1816" t="s">
+        <v>728</v>
       </c>
       <c r="H1816" t="s">
-        <v>2378</v>
+        <v>166</v>
       </c>
       <c r="M1816" t="s">
-        <v>3752</v>
+        <v>3769</v>
       </c>
     </row>
     <row r="1817" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1817">
-        <v>1848</v>
+        <v>1856</v>
       </c>
       <c r="B1817" t="s">
-        <v>3753</v>
+        <v>3777</v>
       </c>
       <c r="C1817" t="s">
-        <v>3747</v>
-      </c>
-      <c r="D1817">
-        <v>68000</v>
+        <v>3778</v>
+      </c>
+      <c r="D1817" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1817" t="s">
+        <v>154</v>
       </c>
       <c r="H1817" t="s">
-        <v>2378</v>
+        <v>172</v>
       </c>
       <c r="M1817" t="s">
-        <v>4492</v>
+        <v>3779</v>
       </c>
     </row>
     <row r="1818" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1818">
-        <v>1849</v>
+        <v>1857</v>
       </c>
       <c r="B1818" t="s">
-        <v>3754</v>
+        <v>3780</v>
       </c>
       <c r="C1818" t="s">
-        <v>3755</v>
-      </c>
-      <c r="D1818">
-        <v>68000</v>
+        <v>3781</v>
+      </c>
+      <c r="D1818" t="s">
+        <v>14</v>
       </c>
       <c r="H1818" t="s">
-        <v>1495</v>
+        <v>172</v>
       </c>
       <c r="M1818" t="s">
-        <v>3756</v>
+        <v>3782</v>
       </c>
     </row>
     <row r="1819" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1819">
-        <v>1850</v>
+        <v>1858</v>
       </c>
       <c r="B1819" t="s">
-        <v>3757</v>
+        <v>3783</v>
       </c>
       <c r="C1819" t="s">
-        <v>3758</v>
+        <v>3781</v>
       </c>
       <c r="D1819" t="s">
         <v>14</v>
       </c>
-      <c r="E1819" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1819" t="s">
-        <v>14</v>
-      </c>
       <c r="H1819" t="s">
-        <v>336</v>
-      </c>
-      <c r="I1819" t="s">
-        <v>1495</v>
+        <v>172</v>
       </c>
       <c r="M1819" t="s">
-        <v>3759</v>
+        <v>3784</v>
       </c>
     </row>
     <row r="1820" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1820">
-        <v>1851</v>
+        <v>1859</v>
       </c>
       <c r="B1820" t="s">
-        <v>3760</v>
+        <v>3785</v>
       </c>
       <c r="C1820" t="s">
-        <v>3761</v>
+        <v>3786</v>
       </c>
       <c r="D1820" t="s">
         <v>14</v>
       </c>
-      <c r="E1820" t="s">
-        <v>728</v>
-      </c>
       <c r="H1820" t="s">
-        <v>166</v>
+        <v>336</v>
       </c>
       <c r="M1820" t="s">
-        <v>4493</v>
+        <v>3787</v>
       </c>
     </row>
     <row r="1821" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1821">
-        <v>1852</v>
+        <v>1860</v>
       </c>
       <c r="B1821" t="s">
-        <v>3762</v>
+        <v>3788</v>
       </c>
       <c r="C1821" t="s">
-        <v>3761</v>
+        <v>3786</v>
       </c>
       <c r="D1821" t="s">
         <v>14</v>
       </c>
-      <c r="E1821" t="s">
-        <v>728</v>
-      </c>
       <c r="H1821" t="s">
-        <v>166</v>
+        <v>336</v>
       </c>
       <c r="M1821" t="s">
-        <v>3763</v>
+        <v>3789</v>
       </c>
     </row>
     <row r="1822" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1822">
-        <v>1853</v>
+        <v>1861</v>
       </c>
       <c r="B1822" t="s">
-        <v>3764</v>
+        <v>3790</v>
       </c>
       <c r="C1822" t="s">
-        <v>3761</v>
+        <v>3786</v>
       </c>
       <c r="D1822" t="s">
         <v>14</v>
       </c>
-      <c r="E1822" t="s">
-        <v>728</v>
-      </c>
       <c r="H1822" t="s">
-        <v>166</v>
+        <v>336</v>
       </c>
       <c r="M1822" t="s">
-        <v>3765</v>
+        <v>3791</v>
       </c>
     </row>
     <row r="1823" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1823">
-        <v>1854</v>
+        <v>1862</v>
       </c>
       <c r="B1823" t="s">
-        <v>3766</v>
+        <v>3792</v>
       </c>
       <c r="C1823" t="s">
-        <v>3761</v>
+        <v>3786</v>
       </c>
       <c r="D1823" t="s">
         <v>14</v>
       </c>
-      <c r="E1823" t="s">
-        <v>728</v>
-      </c>
       <c r="H1823" t="s">
-        <v>166</v>
+        <v>336</v>
       </c>
       <c r="M1823" t="s">
-        <v>3767</v>
+        <v>3793</v>
       </c>
     </row>
     <row r="1824" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1824">
-        <v>1855</v>
+        <v>1863</v>
       </c>
       <c r="B1824" t="s">
-        <v>3768</v>
+        <v>3794</v>
       </c>
       <c r="C1824" t="s">
-        <v>3761</v>
+        <v>3795</v>
       </c>
       <c r="D1824" t="s">
-        <v>14</v>
+        <v>405</v>
       </c>
       <c r="E1824" t="s">
-        <v>728</v>
+        <v>1187</v>
       </c>
       <c r="H1824" t="s">
-        <v>166</v>
+        <v>71</v>
       </c>
       <c r="M1824" t="s">
-        <v>3769</v>
+        <v>3796</v>
       </c>
     </row>
     <row r="1825" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1825">
-        <v>1856</v>
+        <v>1864</v>
       </c>
       <c r="B1825" t="s">
-        <v>3777</v>
+        <v>3797</v>
       </c>
       <c r="C1825" t="s">
-        <v>3778</v>
+        <v>3795</v>
       </c>
       <c r="D1825" t="s">
-        <v>14</v>
+        <v>405</v>
       </c>
       <c r="E1825" t="s">
-        <v>154</v>
+        <v>1187</v>
       </c>
       <c r="H1825" t="s">
-        <v>172</v>
+        <v>71</v>
       </c>
       <c r="M1825" t="s">
-        <v>3779</v>
+        <v>3798</v>
       </c>
     </row>
     <row r="1826" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1826">
-        <v>1857</v>
+        <v>1865</v>
       </c>
       <c r="B1826" t="s">
-        <v>3780</v>
+        <v>3799</v>
       </c>
       <c r="C1826" t="s">
-        <v>3781</v>
+        <v>3800</v>
       </c>
       <c r="D1826" t="s">
         <v>14</v>
       </c>
       <c r="H1826" t="s">
-        <v>172</v>
+        <v>71</v>
       </c>
       <c r="M1826" t="s">
-        <v>3782</v>
+        <v>3801</v>
       </c>
     </row>
     <row r="1827" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1827">
-        <v>1858</v>
+        <v>1866</v>
       </c>
       <c r="B1827" t="s">
-        <v>3783</v>
+        <v>3802</v>
       </c>
       <c r="C1827" t="s">
-        <v>3781</v>
+        <v>3803</v>
       </c>
       <c r="D1827" t="s">
-        <v>14</v>
+        <v>405</v>
+      </c>
+      <c r="E1827" t="s">
+        <v>1187</v>
+      </c>
+      <c r="F1827" t="s">
+        <v>3804</v>
       </c>
       <c r="H1827" t="s">
-        <v>172</v>
+        <v>71</v>
       </c>
       <c r="M1827" t="s">
-        <v>3784</v>
+        <v>3805</v>
       </c>
     </row>
     <row r="1828" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1828">
-        <v>1859</v>
+        <v>1867</v>
       </c>
       <c r="B1828" t="s">
-        <v>3785</v>
+        <v>3806</v>
       </c>
       <c r="C1828" t="s">
-        <v>3786</v>
+        <v>3807</v>
       </c>
       <c r="D1828" t="s">
-        <v>14</v>
+        <v>473</v>
       </c>
       <c r="H1828" t="s">
-        <v>336</v>
+        <v>2939</v>
       </c>
       <c r="M1828" t="s">
-        <v>3787</v>
+        <v>3808</v>
       </c>
     </row>
     <row r="1829" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1829">
-        <v>1860</v>
+        <v>1868</v>
       </c>
       <c r="B1829" t="s">
-        <v>3788</v>
+        <v>3809</v>
       </c>
       <c r="C1829" t="s">
-        <v>3786</v>
+        <v>3810</v>
       </c>
       <c r="D1829" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1829" t="s">
-        <v>336</v>
+        <v>473</v>
       </c>
       <c r="M1829" t="s">
-        <v>3789</v>
+        <v>3811</v>
       </c>
     </row>
     <row r="1830" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1830">
-        <v>1861</v>
+        <v>1869</v>
       </c>
       <c r="B1830" t="s">
-        <v>3790</v>
+        <v>3812</v>
       </c>
       <c r="C1830" t="s">
-        <v>3786</v>
+        <v>3810</v>
       </c>
       <c r="D1830" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1830" t="s">
-        <v>336</v>
+        <v>473</v>
       </c>
       <c r="M1830" t="s">
-        <v>3791</v>
+        <v>3813</v>
       </c>
     </row>
     <row r="1831" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1831">
-        <v>1862</v>
+        <v>1870</v>
       </c>
       <c r="B1831" t="s">
-        <v>3792</v>
+        <v>3814</v>
       </c>
       <c r="C1831" t="s">
-        <v>3786</v>
-      </c>
-      <c r="D1831" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1831" t="s">
-        <v>336</v>
+        <v>3815</v>
+      </c>
+      <c r="D1831">
+        <v>8080</v>
       </c>
       <c r="M1831" t="s">
-        <v>3793</v>
+        <v>3816</v>
       </c>
     </row>
     <row r="1832" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1832">
-        <v>1863</v>
+        <v>1871</v>
       </c>
       <c r="B1832" t="s">
-        <v>3794</v>
+        <v>3817</v>
       </c>
       <c r="C1832" t="s">
-        <v>3795</v>
+        <v>3818</v>
       </c>
       <c r="D1832" t="s">
-        <v>405</v>
+        <v>3439</v>
       </c>
       <c r="E1832" t="s">
+        <v>3439</v>
+      </c>
+      <c r="F1832" t="s">
         <v>1187</v>
       </c>
+      <c r="G1832" t="s">
+        <v>1187</v>
+      </c>
       <c r="H1832" t="s">
-        <v>71</v>
+        <v>333</v>
+      </c>
+      <c r="I1832" t="s">
+        <v>551</v>
       </c>
       <c r="M1832" t="s">
-        <v>3796</v>
+        <v>3819</v>
       </c>
     </row>
     <row r="1833" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1833">
-        <v>1864</v>
+        <v>1872</v>
       </c>
       <c r="B1833" t="s">
-        <v>3797</v>
+        <v>3820</v>
       </c>
       <c r="C1833" t="s">
-        <v>3795</v>
+        <v>3821</v>
       </c>
       <c r="D1833" t="s">
-        <v>405</v>
-      </c>
-      <c r="E1833" t="s">
-        <v>1187</v>
+        <v>14</v>
       </c>
       <c r="H1833" t="s">
-        <v>71</v>
+        <v>172</v>
       </c>
       <c r="M1833" t="s">
-        <v>3798</v>
+        <v>3822</v>
       </c>
     </row>
     <row r="1834" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1834">
-        <v>1865</v>
+        <v>1873</v>
       </c>
       <c r="B1834" t="s">
-        <v>3799</v>
+        <v>3823</v>
       </c>
       <c r="C1834" t="s">
-        <v>3800</v>
+        <v>3824</v>
       </c>
       <c r="D1834" t="s">
         <v>14</v>
+      </c>
+      <c r="E1834" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1834" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1834" t="s">
+        <v>154</v>
       </c>
       <c r="H1834" t="s">
         <v>71</v>
       </c>
+      <c r="I1834" t="s">
+        <v>166</v>
+      </c>
       <c r="M1834" t="s">
-        <v>3801</v>
+        <v>3825</v>
       </c>
     </row>
     <row r="1835" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1835">
-        <v>1866</v>
+        <v>1874</v>
       </c>
       <c r="B1835" t="s">
-        <v>3802</v>
+        <v>3826</v>
       </c>
       <c r="C1835" t="s">
-        <v>3803</v>
+        <v>3824</v>
       </c>
       <c r="D1835" t="s">
-        <v>405</v>
+        <v>14</v>
       </c>
       <c r="E1835" t="s">
-        <v>1187</v>
+        <v>14</v>
       </c>
       <c r="F1835" t="s">
-        <v>3804</v>
+        <v>14</v>
+      </c>
+      <c r="G1835" t="s">
+        <v>154</v>
       </c>
       <c r="H1835" t="s">
         <v>71</v>
       </c>
+      <c r="I1835" t="s">
+        <v>166</v>
+      </c>
       <c r="M1835" t="s">
-        <v>3805</v>
+        <v>3827</v>
       </c>
     </row>
     <row r="1836" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1836">
-        <v>1867</v>
+        <v>1875</v>
       </c>
       <c r="B1836" t="s">
-        <v>3806</v>
+        <v>3828</v>
       </c>
       <c r="C1836" t="s">
-        <v>3807</v>
+        <v>3824</v>
       </c>
       <c r="D1836" t="s">
-        <v>473</v>
+        <v>14</v>
+      </c>
+      <c r="E1836" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1836" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1836" t="s">
+        <v>154</v>
       </c>
       <c r="H1836" t="s">
-        <v>2939</v>
+        <v>71</v>
+      </c>
+      <c r="I1836" t="s">
+        <v>166</v>
       </c>
       <c r="M1836" t="s">
-        <v>3808</v>
+        <v>3829</v>
       </c>
     </row>
     <row r="1837" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1837">
-        <v>1868</v>
+        <v>1876</v>
       </c>
       <c r="B1837" t="s">
-        <v>3809</v>
+        <v>3830</v>
       </c>
       <c r="C1837" t="s">
-        <v>3810</v>
+        <v>3824</v>
       </c>
       <c r="D1837" t="s">
-        <v>473</v>
+        <v>14</v>
+      </c>
+      <c r="E1837" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1837" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1837" t="s">
+        <v>154</v>
+      </c>
+      <c r="H1837" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1837" t="s">
+        <v>166</v>
       </c>
       <c r="M1837" t="s">
-        <v>3811</v>
+        <v>3831</v>
       </c>
     </row>
     <row r="1838" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1838">
-        <v>1869</v>
+        <v>1877</v>
       </c>
       <c r="B1838" t="s">
-        <v>3812</v>
+        <v>3832</v>
       </c>
       <c r="C1838" t="s">
-        <v>3810</v>
-      </c>
-      <c r="D1838" t="s">
-        <v>473</v>
+        <v>3833</v>
+      </c>
+      <c r="D1838">
+        <v>68000</v>
+      </c>
+      <c r="E1838" t="s">
+        <v>154</v>
+      </c>
+      <c r="H1838" t="s">
+        <v>1495</v>
       </c>
       <c r="M1838" t="s">
-        <v>3813</v>
+        <v>3834</v>
       </c>
     </row>
     <row r="1839" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1839">
-        <v>1870</v>
+        <v>1878</v>
       </c>
       <c r="B1839" t="s">
-        <v>3814</v>
+        <v>3835</v>
       </c>
       <c r="C1839" t="s">
-        <v>3815</v>
-      </c>
-      <c r="D1839">
-        <v>8080</v>
+        <v>3836</v>
+      </c>
+      <c r="D1839" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1839" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1839" t="s">
+        <v>1239</v>
+      </c>
+      <c r="I1839" t="s">
+        <v>333</v>
       </c>
       <c r="M1839" t="s">
-        <v>3816</v>
+        <v>3837</v>
       </c>
     </row>
     <row r="1840" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1840">
-        <v>1871</v>
+        <v>1879</v>
       </c>
       <c r="B1840" t="s">
-        <v>3817</v>
+        <v>3838</v>
       </c>
       <c r="C1840" t="s">
-        <v>3818</v>
+        <v>3836</v>
       </c>
       <c r="D1840" t="s">
-        <v>3439</v>
+        <v>14</v>
       </c>
       <c r="E1840" t="s">
-        <v>3439</v>
-      </c>
-      <c r="F1840" t="s">
-        <v>1187</v>
-      </c>
-      <c r="G1840" t="s">
-        <v>1187</v>
+        <v>14</v>
       </c>
       <c r="H1840" t="s">
+        <v>1239</v>
+      </c>
+      <c r="I1840" t="s">
         <v>333</v>
       </c>
-      <c r="I1840" t="s">
-        <v>551</v>
-      </c>
       <c r="M1840" t="s">
-        <v>3819</v>
+        <v>4494</v>
       </c>
     </row>
     <row r="1841" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1841">
-        <v>1872</v>
+        <v>1880</v>
       </c>
       <c r="B1841" t="s">
-        <v>3820</v>
+        <v>3839</v>
       </c>
       <c r="C1841" t="s">
-        <v>3821</v>
+        <v>3836</v>
       </c>
       <c r="D1841" t="s">
         <v>14</v>
       </c>
+      <c r="E1841" t="s">
+        <v>14</v>
+      </c>
       <c r="H1841" t="s">
-        <v>172</v>
+        <v>71</v>
+      </c>
+      <c r="I1841" t="s">
+        <v>166</v>
       </c>
       <c r="M1841" t="s">
-        <v>3822</v>
+        <v>4495</v>
       </c>
     </row>
     <row r="1842" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1842">
-        <v>1873</v>
+        <v>1881</v>
       </c>
       <c r="B1842" t="s">
-        <v>3823</v>
+        <v>3840</v>
       </c>
       <c r="C1842" t="s">
-        <v>3824</v>
+        <v>3836</v>
       </c>
       <c r="D1842" t="s">
         <v>14</v>
@@ -60579,31 +60835,25 @@
       <c r="E1842" t="s">
         <v>14</v>
       </c>
-      <c r="F1842" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1842" t="s">
-        <v>154</v>
-      </c>
       <c r="H1842" t="s">
-        <v>71</v>
+        <v>1239</v>
       </c>
       <c r="I1842" t="s">
-        <v>166</v>
+        <v>333</v>
       </c>
       <c r="M1842" t="s">
-        <v>3825</v>
+        <v>3841</v>
       </c>
     </row>
     <row r="1843" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1843">
-        <v>1874</v>
+        <v>1882</v>
       </c>
       <c r="B1843" t="s">
-        <v>3826</v>
+        <v>3842</v>
       </c>
       <c r="C1843" t="s">
-        <v>3824</v>
+        <v>3843</v>
       </c>
       <c r="D1843" t="s">
         <v>14</v>
@@ -60611,417 +60861,369 @@
       <c r="E1843" t="s">
         <v>14</v>
       </c>
-      <c r="F1843" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1843" t="s">
-        <v>154</v>
-      </c>
       <c r="H1843" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1843" t="s">
-        <v>166</v>
+        <v>349</v>
       </c>
       <c r="M1843" t="s">
-        <v>3827</v>
+        <v>3844</v>
       </c>
     </row>
     <row r="1844" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1844">
-        <v>1875</v>
+        <v>1883</v>
       </c>
       <c r="B1844" t="s">
-        <v>3828</v>
+        <v>3845</v>
       </c>
       <c r="C1844" t="s">
-        <v>3824</v>
+        <v>3846</v>
       </c>
       <c r="D1844" t="s">
         <v>14</v>
       </c>
       <c r="E1844" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1844" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1844" t="s">
         <v>154</v>
       </c>
       <c r="H1844" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1844" t="s">
-        <v>166</v>
+        <v>349</v>
       </c>
       <c r="M1844" t="s">
-        <v>3829</v>
+        <v>3847</v>
       </c>
     </row>
     <row r="1845" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1845">
-        <v>1876</v>
+        <v>1884</v>
       </c>
       <c r="B1845" t="s">
-        <v>3830</v>
+        <v>3848</v>
       </c>
       <c r="C1845" t="s">
-        <v>3824</v>
+        <v>3849</v>
       </c>
       <c r="D1845" t="s">
         <v>14</v>
       </c>
-      <c r="E1845" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1845" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1845" t="s">
-        <v>154</v>
-      </c>
       <c r="H1845" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1845" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="M1845" t="s">
-        <v>3831</v>
+        <v>3850</v>
       </c>
     </row>
     <row r="1846" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1846">
-        <v>1877</v>
+        <v>1885</v>
       </c>
       <c r="B1846" t="s">
-        <v>3832</v>
+        <v>3851</v>
       </c>
       <c r="C1846" t="s">
-        <v>3833</v>
+        <v>3852</v>
       </c>
       <c r="D1846">
-        <v>68000</v>
-      </c>
-      <c r="E1846" t="s">
-        <v>154</v>
+        <v>8080</v>
       </c>
       <c r="H1846" t="s">
-        <v>1495</v>
+        <v>406</v>
       </c>
       <c r="M1846" t="s">
-        <v>3834</v>
+        <v>3853</v>
       </c>
     </row>
     <row r="1847" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1847">
-        <v>1878</v>
+        <v>1886</v>
       </c>
       <c r="B1847" t="s">
-        <v>3835</v>
+        <v>3854</v>
       </c>
       <c r="C1847" t="s">
-        <v>3836</v>
+        <v>3855</v>
       </c>
       <c r="D1847" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1847" t="s">
-        <v>14</v>
+        <v>1108</v>
       </c>
       <c r="H1847" t="s">
-        <v>1239</v>
-      </c>
-      <c r="I1847" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="M1847" t="s">
-        <v>3837</v>
+        <v>3856</v>
       </c>
     </row>
     <row r="1848" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1848">
-        <v>1879</v>
+        <v>1887</v>
       </c>
       <c r="B1848" t="s">
-        <v>3838</v>
+        <v>3857</v>
       </c>
       <c r="C1848" t="s">
-        <v>3836</v>
+        <v>3858</v>
       </c>
       <c r="D1848" t="s">
         <v>14</v>
       </c>
       <c r="E1848" t="s">
-        <v>14</v>
+        <v>154</v>
       </c>
       <c r="H1848" t="s">
-        <v>1239</v>
-      </c>
-      <c r="I1848" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="M1848" t="s">
-        <v>4494</v>
+        <v>3859</v>
       </c>
     </row>
     <row r="1849" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1849">
-        <v>1880</v>
+        <v>1888</v>
       </c>
       <c r="B1849" t="s">
-        <v>3839</v>
+        <v>3860</v>
       </c>
       <c r="C1849" t="s">
-        <v>3836</v>
+        <v>3858</v>
       </c>
       <c r="D1849" t="s">
         <v>14</v>
       </c>
       <c r="E1849" t="s">
-        <v>14</v>
+        <v>154</v>
       </c>
       <c r="H1849" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1849" t="s">
-        <v>166</v>
+        <v>336</v>
       </c>
       <c r="M1849" t="s">
-        <v>4495</v>
+        <v>3861</v>
       </c>
     </row>
     <row r="1850" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1850">
-        <v>1881</v>
+        <v>1889</v>
       </c>
       <c r="B1850" t="s">
-        <v>3840</v>
+        <v>3862</v>
       </c>
       <c r="C1850" t="s">
-        <v>3836</v>
+        <v>3863</v>
       </c>
       <c r="D1850" t="s">
-        <v>14</v>
+        <v>3864</v>
       </c>
       <c r="E1850" t="s">
-        <v>14</v>
+        <v>728</v>
       </c>
       <c r="H1850" t="s">
-        <v>1239</v>
-      </c>
-      <c r="I1850" t="s">
-        <v>333</v>
+        <v>2073</v>
       </c>
       <c r="M1850" t="s">
-        <v>3841</v>
+        <v>3865</v>
       </c>
     </row>
     <row r="1851" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1851">
-        <v>1882</v>
+        <v>1890</v>
       </c>
       <c r="B1851" t="s">
-        <v>3842</v>
+        <v>3866</v>
       </c>
       <c r="C1851" t="s">
-        <v>3843</v>
-      </c>
-      <c r="D1851" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1851" t="s">
-        <v>14</v>
+        <v>3867</v>
+      </c>
+      <c r="D1851">
+        <v>68000</v>
       </c>
       <c r="H1851" t="s">
-        <v>349</v>
+        <v>2378</v>
       </c>
       <c r="M1851" t="s">
-        <v>3844</v>
+        <v>3868</v>
       </c>
     </row>
     <row r="1852" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1852">
-        <v>1883</v>
+        <v>1891</v>
       </c>
       <c r="B1852" t="s">
-        <v>3845</v>
+        <v>3869</v>
       </c>
       <c r="C1852" t="s">
-        <v>3846</v>
-      </c>
-      <c r="D1852" t="s">
-        <v>14</v>
+        <v>3870</v>
+      </c>
+      <c r="D1852">
+        <v>68000</v>
       </c>
       <c r="E1852" t="s">
         <v>154</v>
       </c>
       <c r="H1852" t="s">
-        <v>349</v>
+        <v>1239</v>
       </c>
       <c r="M1852" t="s">
-        <v>3847</v>
+        <v>3871</v>
       </c>
     </row>
     <row r="1853" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1853">
-        <v>1884</v>
+        <v>1892</v>
       </c>
       <c r="B1853" t="s">
-        <v>3848</v>
+        <v>3872</v>
       </c>
       <c r="C1853" t="s">
-        <v>3849</v>
+        <v>3873</v>
       </c>
       <c r="D1853" t="s">
-        <v>14</v>
+        <v>405</v>
       </c>
       <c r="H1853" t="s">
-        <v>172</v>
+        <v>71</v>
       </c>
       <c r="M1853" t="s">
-        <v>3850</v>
+        <v>3874</v>
       </c>
     </row>
     <row r="1854" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1854">
-        <v>1885</v>
+        <v>1893</v>
       </c>
       <c r="B1854" t="s">
-        <v>3851</v>
+        <v>3875</v>
       </c>
       <c r="C1854" t="s">
-        <v>3852</v>
-      </c>
-      <c r="D1854">
-        <v>8080</v>
-      </c>
-      <c r="H1854" t="s">
-        <v>406</v>
+        <v>3876</v>
+      </c>
+      <c r="D1854" t="s">
+        <v>14</v>
       </c>
       <c r="M1854" t="s">
-        <v>3853</v>
+        <v>4496</v>
       </c>
     </row>
     <row r="1855" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1855">
-        <v>1886</v>
+        <v>1894</v>
       </c>
       <c r="B1855" t="s">
-        <v>3854</v>
+        <v>3877</v>
       </c>
       <c r="C1855" t="s">
-        <v>3855</v>
-      </c>
-      <c r="D1855" t="s">
-        <v>1108</v>
+        <v>3878</v>
+      </c>
+      <c r="D1855">
+        <v>68000</v>
+      </c>
+      <c r="E1855" t="s">
+        <v>154</v>
       </c>
       <c r="H1855" t="s">
-        <v>336</v>
+        <v>1356</v>
       </c>
       <c r="M1855" t="s">
-        <v>3856</v>
+        <v>3879</v>
       </c>
     </row>
     <row r="1856" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1856">
-        <v>1887</v>
+        <v>1895</v>
       </c>
       <c r="B1856" t="s">
-        <v>3857</v>
+        <v>3880</v>
       </c>
       <c r="C1856" t="s">
-        <v>3858</v>
-      </c>
-      <c r="D1856" t="s">
-        <v>14</v>
+        <v>3878</v>
+      </c>
+      <c r="D1856">
+        <v>68000</v>
       </c>
       <c r="E1856" t="s">
         <v>154</v>
       </c>
       <c r="H1856" t="s">
-        <v>336</v>
+        <v>1356</v>
       </c>
       <c r="M1856" t="s">
-        <v>3859</v>
+        <v>4497</v>
       </c>
     </row>
     <row r="1857" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1857">
-        <v>1888</v>
+        <v>1896</v>
       </c>
       <c r="B1857" t="s">
-        <v>3860</v>
+        <v>3881</v>
       </c>
       <c r="C1857" t="s">
-        <v>3858</v>
-      </c>
-      <c r="D1857" t="s">
-        <v>14</v>
+        <v>3878</v>
+      </c>
+      <c r="D1857">
+        <v>68000</v>
       </c>
       <c r="E1857" t="s">
         <v>154</v>
       </c>
       <c r="H1857" t="s">
-        <v>336</v>
+        <v>1356</v>
       </c>
       <c r="M1857" t="s">
-        <v>3861</v>
+        <v>3882</v>
       </c>
     </row>
     <row r="1858" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1858">
-        <v>1889</v>
+        <v>1897</v>
       </c>
       <c r="B1858" t="s">
-        <v>3862</v>
+        <v>3883</v>
       </c>
       <c r="C1858" t="s">
-        <v>3863</v>
-      </c>
-      <c r="D1858" t="s">
-        <v>3864</v>
+        <v>3878</v>
+      </c>
+      <c r="D1858">
+        <v>68000</v>
       </c>
       <c r="E1858" t="s">
-        <v>728</v>
+        <v>154</v>
       </c>
       <c r="H1858" t="s">
-        <v>2073</v>
+        <v>1356</v>
       </c>
       <c r="M1858" t="s">
-        <v>3865</v>
+        <v>3884</v>
       </c>
     </row>
     <row r="1859" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1859">
-        <v>1890</v>
+        <v>1898</v>
       </c>
       <c r="B1859" t="s">
-        <v>3866</v>
+        <v>3885</v>
       </c>
       <c r="C1859" t="s">
-        <v>3867</v>
+        <v>3878</v>
       </c>
       <c r="D1859">
         <v>68000</v>
       </c>
+      <c r="E1859" t="s">
+        <v>154</v>
+      </c>
       <c r="H1859" t="s">
-        <v>2378</v>
+        <v>1356</v>
       </c>
       <c r="M1859" t="s">
-        <v>3868</v>
+        <v>3886</v>
       </c>
     </row>
     <row r="1860" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1860">
-        <v>1891</v>
+        <v>1899</v>
       </c>
       <c r="B1860" t="s">
-        <v>3869</v>
+        <v>3887</v>
       </c>
       <c r="C1860" t="s">
-        <v>3870</v>
+        <v>3878</v>
       </c>
       <c r="D1860">
         <v>68000</v>
@@ -61030,55 +61232,64 @@
         <v>154</v>
       </c>
       <c r="H1860" t="s">
-        <v>1239</v>
+        <v>1356</v>
       </c>
       <c r="M1860" t="s">
-        <v>3871</v>
+        <v>3888</v>
       </c>
     </row>
     <row r="1861" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1861">
-        <v>1892</v>
+        <v>1900</v>
       </c>
       <c r="B1861" t="s">
-        <v>3872</v>
+        <v>3889</v>
       </c>
       <c r="C1861" t="s">
-        <v>3873</v>
-      </c>
-      <c r="D1861" t="s">
-        <v>405</v>
+        <v>3878</v>
+      </c>
+      <c r="D1861">
+        <v>68000</v>
+      </c>
+      <c r="E1861" t="s">
+        <v>154</v>
       </c>
       <c r="H1861" t="s">
-        <v>71</v>
+        <v>1356</v>
       </c>
       <c r="M1861" t="s">
-        <v>3874</v>
+        <v>3890</v>
       </c>
     </row>
     <row r="1862" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1862">
-        <v>1893</v>
+        <v>1901</v>
       </c>
       <c r="B1862" t="s">
-        <v>3875</v>
+        <v>3891</v>
       </c>
       <c r="C1862" t="s">
-        <v>3876</v>
-      </c>
-      <c r="D1862" t="s">
-        <v>14</v>
+        <v>3878</v>
+      </c>
+      <c r="D1862">
+        <v>68000</v>
+      </c>
+      <c r="E1862" t="s">
+        <v>154</v>
+      </c>
+      <c r="H1862" t="s">
+        <v>1356</v>
       </c>
       <c r="M1862" t="s">
-        <v>4496</v>
+        <v>4498</v>
       </c>
     </row>
     <row r="1863" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1863">
-        <v>1894</v>
+        <v>1902</v>
       </c>
       <c r="B1863" t="s">
-        <v>3877</v>
+        <v>3892</v>
       </c>
       <c r="C1863" t="s">
         <v>3878</v>
@@ -61093,15 +61304,15 @@
         <v>1356</v>
       </c>
       <c r="M1863" t="s">
-        <v>3879</v>
+        <v>3893</v>
       </c>
     </row>
     <row r="1864" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1864">
-        <v>1895</v>
+        <v>1903</v>
       </c>
       <c r="B1864" t="s">
-        <v>3880</v>
+        <v>3894</v>
       </c>
       <c r="C1864" t="s">
         <v>3878</v>
@@ -61116,15 +61327,15 @@
         <v>1356</v>
       </c>
       <c r="M1864" t="s">
-        <v>4497</v>
+        <v>3895</v>
       </c>
     </row>
     <row r="1865" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1865">
-        <v>1896</v>
+        <v>1904</v>
       </c>
       <c r="B1865" t="s">
-        <v>3881</v>
+        <v>3896</v>
       </c>
       <c r="C1865" t="s">
         <v>3878</v>
@@ -61139,15 +61350,15 @@
         <v>1356</v>
       </c>
       <c r="M1865" t="s">
-        <v>3882</v>
+        <v>3897</v>
       </c>
     </row>
     <row r="1866" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1866">
-        <v>1897</v>
+        <v>1905</v>
       </c>
       <c r="B1866" t="s">
-        <v>3883</v>
+        <v>3898</v>
       </c>
       <c r="C1866" t="s">
         <v>3878</v>
@@ -61162,15 +61373,15 @@
         <v>1356</v>
       </c>
       <c r="M1866" t="s">
-        <v>3884</v>
+        <v>3899</v>
       </c>
     </row>
     <row r="1867" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1867">
-        <v>1898</v>
+        <v>1906</v>
       </c>
       <c r="B1867" t="s">
-        <v>3885</v>
+        <v>3900</v>
       </c>
       <c r="C1867" t="s">
         <v>3878</v>
@@ -61185,15 +61396,15 @@
         <v>1356</v>
       </c>
       <c r="M1867" t="s">
-        <v>3886</v>
+        <v>3901</v>
       </c>
     </row>
     <row r="1868" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1868">
-        <v>1899</v>
+        <v>1907</v>
       </c>
       <c r="B1868" t="s">
-        <v>3887</v>
+        <v>3902</v>
       </c>
       <c r="C1868" t="s">
         <v>3878</v>
@@ -61208,15 +61419,15 @@
         <v>1356</v>
       </c>
       <c r="M1868" t="s">
-        <v>3888</v>
+        <v>4499</v>
       </c>
     </row>
     <row r="1869" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1869">
-        <v>1900</v>
+        <v>1908</v>
       </c>
       <c r="B1869" t="s">
-        <v>3889</v>
+        <v>3903</v>
       </c>
       <c r="C1869" t="s">
         <v>3878</v>
@@ -61231,15 +61442,15 @@
         <v>1356</v>
       </c>
       <c r="M1869" t="s">
-        <v>3890</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="1870" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1870">
-        <v>1901</v>
+        <v>1909</v>
       </c>
       <c r="B1870" t="s">
-        <v>3891</v>
+        <v>3904</v>
       </c>
       <c r="C1870" t="s">
         <v>3878</v>
@@ -61254,15 +61465,15 @@
         <v>1356</v>
       </c>
       <c r="M1870" t="s">
-        <v>4498</v>
+        <v>3905</v>
       </c>
     </row>
     <row r="1871" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1871">
-        <v>1902</v>
+        <v>1910</v>
       </c>
       <c r="B1871" t="s">
-        <v>3892</v>
+        <v>3906</v>
       </c>
       <c r="C1871" t="s">
         <v>3878</v>
@@ -61277,15 +61488,15 @@
         <v>1356</v>
       </c>
       <c r="M1871" t="s">
-        <v>3893</v>
+        <v>3907</v>
       </c>
     </row>
     <row r="1872" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1872">
-        <v>1903</v>
+        <v>1911</v>
       </c>
       <c r="B1872" t="s">
-        <v>3894</v>
+        <v>3908</v>
       </c>
       <c r="C1872" t="s">
         <v>3878</v>
@@ -61300,15 +61511,15 @@
         <v>1356</v>
       </c>
       <c r="M1872" t="s">
-        <v>3895</v>
+        <v>3909</v>
       </c>
     </row>
     <row r="1873" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1873">
-        <v>1904</v>
+        <v>1912</v>
       </c>
       <c r="B1873" t="s">
-        <v>3896</v>
+        <v>3910</v>
       </c>
       <c r="C1873" t="s">
         <v>3878</v>
@@ -61323,15 +61534,15 @@
         <v>1356</v>
       </c>
       <c r="M1873" t="s">
-        <v>3897</v>
+        <v>3911</v>
       </c>
     </row>
     <row r="1874" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1874">
-        <v>1905</v>
+        <v>1913</v>
       </c>
       <c r="B1874" t="s">
-        <v>3898</v>
+        <v>3912</v>
       </c>
       <c r="C1874" t="s">
         <v>3878</v>
@@ -61346,15 +61557,15 @@
         <v>1356</v>
       </c>
       <c r="M1874" t="s">
-        <v>3899</v>
+        <v>3913</v>
       </c>
     </row>
     <row r="1875" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1875">
-        <v>1906</v>
+        <v>1914</v>
       </c>
       <c r="B1875" t="s">
-        <v>3900</v>
+        <v>3914</v>
       </c>
       <c r="C1875" t="s">
         <v>3878</v>
@@ -61369,15 +61580,15 @@
         <v>1356</v>
       </c>
       <c r="M1875" t="s">
-        <v>3901</v>
+        <v>3915</v>
       </c>
     </row>
     <row r="1876" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1876">
-        <v>1907</v>
+        <v>1915</v>
       </c>
       <c r="B1876" t="s">
-        <v>3902</v>
+        <v>3916</v>
       </c>
       <c r="C1876" t="s">
         <v>3878</v>
@@ -61392,15 +61603,15 @@
         <v>1356</v>
       </c>
       <c r="M1876" t="s">
-        <v>4499</v>
+        <v>4501</v>
       </c>
     </row>
     <row r="1877" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1877">
-        <v>1908</v>
+        <v>1916</v>
       </c>
       <c r="B1877" t="s">
-        <v>3903</v>
+        <v>3917</v>
       </c>
       <c r="C1877" t="s">
         <v>3878</v>
@@ -61415,15 +61626,15 @@
         <v>1356</v>
       </c>
       <c r="M1877" t="s">
-        <v>4500</v>
+        <v>3918</v>
       </c>
     </row>
     <row r="1878" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1878">
-        <v>1909</v>
+        <v>1917</v>
       </c>
       <c r="B1878" t="s">
-        <v>3904</v>
+        <v>3919</v>
       </c>
       <c r="C1878" t="s">
         <v>3878</v>
@@ -61438,15 +61649,15 @@
         <v>1356</v>
       </c>
       <c r="M1878" t="s">
-        <v>3905</v>
+        <v>3920</v>
       </c>
     </row>
     <row r="1879" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1879">
-        <v>1910</v>
+        <v>1918</v>
       </c>
       <c r="B1879" t="s">
-        <v>3906</v>
+        <v>3921</v>
       </c>
       <c r="C1879" t="s">
         <v>3878</v>
@@ -61461,15 +61672,15 @@
         <v>1356</v>
       </c>
       <c r="M1879" t="s">
-        <v>3907</v>
+        <v>3922</v>
       </c>
     </row>
     <row r="1880" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1880">
-        <v>1911</v>
+        <v>1919</v>
       </c>
       <c r="B1880" t="s">
-        <v>3908</v>
+        <v>3923</v>
       </c>
       <c r="C1880" t="s">
         <v>3878</v>
@@ -61484,15 +61695,15 @@
         <v>1356</v>
       </c>
       <c r="M1880" t="s">
-        <v>3909</v>
+        <v>4502</v>
       </c>
     </row>
     <row r="1881" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1881">
-        <v>1912</v>
+        <v>1920</v>
       </c>
       <c r="B1881" t="s">
-        <v>3910</v>
+        <v>3924</v>
       </c>
       <c r="C1881" t="s">
         <v>3878</v>
@@ -61507,15 +61718,15 @@
         <v>1356</v>
       </c>
       <c r="M1881" t="s">
-        <v>3911</v>
+        <v>4503</v>
       </c>
     </row>
     <row r="1882" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1882">
-        <v>1913</v>
+        <v>1921</v>
       </c>
       <c r="B1882" t="s">
-        <v>3912</v>
+        <v>3925</v>
       </c>
       <c r="C1882" t="s">
         <v>3878</v>
@@ -61530,15 +61741,15 @@
         <v>1356</v>
       </c>
       <c r="M1882" t="s">
-        <v>3913</v>
+        <v>4504</v>
       </c>
     </row>
     <row r="1883" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1883">
-        <v>1914</v>
+        <v>1922</v>
       </c>
       <c r="B1883" t="s">
-        <v>3914</v>
+        <v>3926</v>
       </c>
       <c r="C1883" t="s">
         <v>3878</v>
@@ -61553,15 +61764,15 @@
         <v>1356</v>
       </c>
       <c r="M1883" t="s">
-        <v>3915</v>
+        <v>3927</v>
       </c>
     </row>
     <row r="1884" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1884">
-        <v>1915</v>
+        <v>1923</v>
       </c>
       <c r="B1884" t="s">
-        <v>3916</v>
+        <v>3928</v>
       </c>
       <c r="C1884" t="s">
         <v>3878</v>
@@ -61576,15 +61787,15 @@
         <v>1356</v>
       </c>
       <c r="M1884" t="s">
-        <v>4501</v>
+        <v>3929</v>
       </c>
     </row>
     <row r="1885" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1885">
-        <v>1916</v>
+        <v>1924</v>
       </c>
       <c r="B1885" t="s">
-        <v>3917</v>
+        <v>3930</v>
       </c>
       <c r="C1885" t="s">
         <v>3878</v>
@@ -61599,15 +61810,15 @@
         <v>1356</v>
       </c>
       <c r="M1885" t="s">
-        <v>3918</v>
+        <v>4505</v>
       </c>
     </row>
     <row r="1886" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1886">
-        <v>1917</v>
+        <v>1925</v>
       </c>
       <c r="B1886" t="s">
-        <v>3919</v>
+        <v>3931</v>
       </c>
       <c r="C1886" t="s">
         <v>3878</v>
@@ -61622,15 +61833,15 @@
         <v>1356</v>
       </c>
       <c r="M1886" t="s">
-        <v>3920</v>
+        <v>3932</v>
       </c>
     </row>
     <row r="1887" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1887">
-        <v>1918</v>
+        <v>1926</v>
       </c>
       <c r="B1887" t="s">
-        <v>3921</v>
+        <v>3933</v>
       </c>
       <c r="C1887" t="s">
         <v>3878</v>
@@ -61645,15 +61856,15 @@
         <v>1356</v>
       </c>
       <c r="M1887" t="s">
-        <v>3922</v>
+        <v>4506</v>
       </c>
     </row>
     <row r="1888" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1888">
-        <v>1919</v>
+        <v>1927</v>
       </c>
       <c r="B1888" t="s">
-        <v>3923</v>
+        <v>3934</v>
       </c>
       <c r="C1888" t="s">
         <v>3878</v>
@@ -61668,15 +61879,15 @@
         <v>1356</v>
       </c>
       <c r="M1888" t="s">
-        <v>4502</v>
+        <v>3935</v>
       </c>
     </row>
     <row r="1889" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1889">
-        <v>1920</v>
+        <v>1928</v>
       </c>
       <c r="B1889" t="s">
-        <v>3924</v>
+        <v>3936</v>
       </c>
       <c r="C1889" t="s">
         <v>3878</v>
@@ -61691,15 +61902,15 @@
         <v>1356</v>
       </c>
       <c r="M1889" t="s">
-        <v>4503</v>
+        <v>3937</v>
       </c>
     </row>
     <row r="1890" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1890">
-        <v>1921</v>
+        <v>1929</v>
       </c>
       <c r="B1890" t="s">
-        <v>3925</v>
+        <v>3938</v>
       </c>
       <c r="C1890" t="s">
         <v>3878</v>
@@ -61714,15 +61925,15 @@
         <v>1356</v>
       </c>
       <c r="M1890" t="s">
-        <v>4504</v>
+        <v>4507</v>
       </c>
     </row>
     <row r="1891" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1891">
-        <v>1922</v>
+        <v>1930</v>
       </c>
       <c r="B1891" t="s">
-        <v>3926</v>
+        <v>3939</v>
       </c>
       <c r="C1891" t="s">
         <v>3878</v>
@@ -61737,15 +61948,15 @@
         <v>1356</v>
       </c>
       <c r="M1891" t="s">
-        <v>3927</v>
+        <v>4508</v>
       </c>
     </row>
     <row r="1892" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1892">
-        <v>1923</v>
+        <v>1931</v>
       </c>
       <c r="B1892" t="s">
-        <v>3928</v>
+        <v>3940</v>
       </c>
       <c r="C1892" t="s">
         <v>3878</v>
@@ -61760,15 +61971,15 @@
         <v>1356</v>
       </c>
       <c r="M1892" t="s">
-        <v>3929</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="1893" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1893">
-        <v>1924</v>
+        <v>1932</v>
       </c>
       <c r="B1893" t="s">
-        <v>3930</v>
+        <v>3942</v>
       </c>
       <c r="C1893" t="s">
         <v>3878</v>
@@ -61783,15 +61994,15 @@
         <v>1356</v>
       </c>
       <c r="M1893" t="s">
-        <v>4505</v>
+        <v>4509</v>
       </c>
     </row>
     <row r="1894" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1894">
-        <v>1925</v>
+        <v>1933</v>
       </c>
       <c r="B1894" t="s">
-        <v>3931</v>
+        <v>3943</v>
       </c>
       <c r="C1894" t="s">
         <v>3878</v>
@@ -61806,15 +62017,15 @@
         <v>1356</v>
       </c>
       <c r="M1894" t="s">
-        <v>3932</v>
+        <v>4510</v>
       </c>
     </row>
     <row r="1895" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1895">
-        <v>1926</v>
+        <v>1934</v>
       </c>
       <c r="B1895" t="s">
-        <v>3933</v>
+        <v>3944</v>
       </c>
       <c r="C1895" t="s">
         <v>3878</v>
@@ -61829,15 +62040,15 @@
         <v>1356</v>
       </c>
       <c r="M1895" t="s">
-        <v>4506</v>
+        <v>4511</v>
       </c>
     </row>
     <row r="1896" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1896">
-        <v>1927</v>
+        <v>1935</v>
       </c>
       <c r="B1896" t="s">
-        <v>3934</v>
+        <v>3945</v>
       </c>
       <c r="C1896" t="s">
         <v>3878</v>
@@ -61852,15 +62063,15 @@
         <v>1356</v>
       </c>
       <c r="M1896" t="s">
-        <v>3935</v>
+        <v>4512</v>
       </c>
     </row>
     <row r="1897" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1897">
-        <v>1928</v>
+        <v>1936</v>
       </c>
       <c r="B1897" t="s">
-        <v>3936</v>
+        <v>3946</v>
       </c>
       <c r="C1897" t="s">
         <v>3878</v>
@@ -61875,15 +62086,15 @@
         <v>1356</v>
       </c>
       <c r="M1897" t="s">
-        <v>3937</v>
+        <v>4513</v>
       </c>
     </row>
     <row r="1898" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1898">
-        <v>1929</v>
+        <v>1937</v>
       </c>
       <c r="B1898" t="s">
-        <v>3938</v>
+        <v>3947</v>
       </c>
       <c r="C1898" t="s">
         <v>3878</v>
@@ -61898,15 +62109,15 @@
         <v>1356</v>
       </c>
       <c r="M1898" t="s">
-        <v>4507</v>
+        <v>4514</v>
       </c>
     </row>
     <row r="1899" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1899">
-        <v>1930</v>
+        <v>1938</v>
       </c>
       <c r="B1899" t="s">
-        <v>3939</v>
+        <v>3948</v>
       </c>
       <c r="C1899" t="s">
         <v>3878</v>
@@ -61921,15 +62132,15 @@
         <v>1356</v>
       </c>
       <c r="M1899" t="s">
-        <v>4508</v>
+        <v>4515</v>
       </c>
     </row>
     <row r="1900" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1900">
-        <v>1931</v>
+        <v>1939</v>
       </c>
       <c r="B1900" t="s">
-        <v>3940</v>
+        <v>3949</v>
       </c>
       <c r="C1900" t="s">
         <v>3878</v>
@@ -61944,15 +62155,15 @@
         <v>1356</v>
       </c>
       <c r="M1900" t="s">
-        <v>3941</v>
+        <v>3950</v>
       </c>
     </row>
     <row r="1901" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1901">
-        <v>1932</v>
+        <v>1940</v>
       </c>
       <c r="B1901" t="s">
-        <v>3942</v>
+        <v>3951</v>
       </c>
       <c r="C1901" t="s">
         <v>3878</v>
@@ -61967,15 +62178,15 @@
         <v>1356</v>
       </c>
       <c r="M1901" t="s">
-        <v>4509</v>
+        <v>3952</v>
       </c>
     </row>
     <row r="1902" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1902">
-        <v>1933</v>
+        <v>1941</v>
       </c>
       <c r="B1902" t="s">
-        <v>3943</v>
+        <v>3953</v>
       </c>
       <c r="C1902" t="s">
         <v>3878</v>
@@ -61990,15 +62201,15 @@
         <v>1356</v>
       </c>
       <c r="M1902" t="s">
-        <v>4510</v>
+        <v>3954</v>
       </c>
     </row>
     <row r="1903" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1903">
-        <v>1934</v>
+        <v>1942</v>
       </c>
       <c r="B1903" t="s">
-        <v>3944</v>
+        <v>3955</v>
       </c>
       <c r="C1903" t="s">
         <v>3878</v>
@@ -62013,15 +62224,15 @@
         <v>1356</v>
       </c>
       <c r="M1903" t="s">
-        <v>4511</v>
+        <v>4516</v>
       </c>
     </row>
     <row r="1904" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1904">
-        <v>1935</v>
+        <v>1943</v>
       </c>
       <c r="B1904" t="s">
-        <v>3945</v>
+        <v>3956</v>
       </c>
       <c r="C1904" t="s">
         <v>3878</v>
@@ -62036,15 +62247,15 @@
         <v>1356</v>
       </c>
       <c r="M1904" t="s">
-        <v>4512</v>
+        <v>3957</v>
       </c>
     </row>
     <row r="1905" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1905">
-        <v>1936</v>
+        <v>1944</v>
       </c>
       <c r="B1905" t="s">
-        <v>3946</v>
+        <v>3958</v>
       </c>
       <c r="C1905" t="s">
         <v>3878</v>
@@ -62059,15 +62270,15 @@
         <v>1356</v>
       </c>
       <c r="M1905" t="s">
-        <v>4513</v>
+        <v>3959</v>
       </c>
     </row>
     <row r="1906" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1906">
-        <v>1937</v>
+        <v>1945</v>
       </c>
       <c r="B1906" t="s">
-        <v>3947</v>
+        <v>3960</v>
       </c>
       <c r="C1906" t="s">
         <v>3878</v>
@@ -62082,15 +62293,15 @@
         <v>1356</v>
       </c>
       <c r="M1906" t="s">
-        <v>4514</v>
+        <v>4517</v>
       </c>
     </row>
     <row r="1907" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1907">
-        <v>1938</v>
+        <v>1946</v>
       </c>
       <c r="B1907" t="s">
-        <v>3948</v>
+        <v>3961</v>
       </c>
       <c r="C1907" t="s">
         <v>3878</v>
@@ -62105,15 +62316,15 @@
         <v>1356</v>
       </c>
       <c r="M1907" t="s">
-        <v>4515</v>
+        <v>3962</v>
       </c>
     </row>
     <row r="1908" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1908">
-        <v>1939</v>
+        <v>1947</v>
       </c>
       <c r="B1908" t="s">
-        <v>3949</v>
+        <v>3963</v>
       </c>
       <c r="C1908" t="s">
         <v>3878</v>
@@ -62128,15 +62339,15 @@
         <v>1356</v>
       </c>
       <c r="M1908" t="s">
-        <v>3950</v>
+        <v>4518</v>
       </c>
     </row>
     <row r="1909" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1909">
-        <v>1940</v>
+        <v>1948</v>
       </c>
       <c r="B1909" t="s">
-        <v>3951</v>
+        <v>3964</v>
       </c>
       <c r="C1909" t="s">
         <v>3878</v>
@@ -62151,15 +62362,15 @@
         <v>1356</v>
       </c>
       <c r="M1909" t="s">
-        <v>3952</v>
+        <v>4519</v>
       </c>
     </row>
     <row r="1910" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1910">
-        <v>1941</v>
+        <v>1949</v>
       </c>
       <c r="B1910" t="s">
-        <v>3953</v>
+        <v>3965</v>
       </c>
       <c r="C1910" t="s">
         <v>3878</v>
@@ -62174,15 +62385,15 @@
         <v>1356</v>
       </c>
       <c r="M1910" t="s">
-        <v>3954</v>
+        <v>4520</v>
       </c>
     </row>
     <row r="1911" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1911">
-        <v>1942</v>
+        <v>1950</v>
       </c>
       <c r="B1911" t="s">
-        <v>3955</v>
+        <v>3966</v>
       </c>
       <c r="C1911" t="s">
         <v>3878</v>
@@ -62197,15 +62408,15 @@
         <v>1356</v>
       </c>
       <c r="M1911" t="s">
-        <v>4516</v>
+        <v>4521</v>
       </c>
     </row>
     <row r="1912" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1912">
-        <v>1943</v>
+        <v>1951</v>
       </c>
       <c r="B1912" t="s">
-        <v>3956</v>
+        <v>3967</v>
       </c>
       <c r="C1912" t="s">
         <v>3878</v>
@@ -62220,15 +62431,15 @@
         <v>1356</v>
       </c>
       <c r="M1912" t="s">
-        <v>3957</v>
+        <v>4522</v>
       </c>
     </row>
     <row r="1913" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1913">
-        <v>1944</v>
+        <v>1952</v>
       </c>
       <c r="B1913" t="s">
-        <v>3958</v>
+        <v>3968</v>
       </c>
       <c r="C1913" t="s">
         <v>3878</v>
@@ -62243,15 +62454,15 @@
         <v>1356</v>
       </c>
       <c r="M1913" t="s">
-        <v>3959</v>
+        <v>4523</v>
       </c>
     </row>
     <row r="1914" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1914">
-        <v>1945</v>
+        <v>1953</v>
       </c>
       <c r="B1914" t="s">
-        <v>3960</v>
+        <v>3969</v>
       </c>
       <c r="C1914" t="s">
         <v>3878</v>
@@ -62266,15 +62477,15 @@
         <v>1356</v>
       </c>
       <c r="M1914" t="s">
-        <v>4517</v>
+        <v>3970</v>
       </c>
     </row>
     <row r="1915" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1915">
-        <v>1946</v>
+        <v>1954</v>
       </c>
       <c r="B1915" t="s">
-        <v>3961</v>
+        <v>3971</v>
       </c>
       <c r="C1915" t="s">
         <v>3878</v>
@@ -62289,15 +62500,15 @@
         <v>1356</v>
       </c>
       <c r="M1915" t="s">
-        <v>3962</v>
+        <v>4524</v>
       </c>
     </row>
     <row r="1916" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1916">
-        <v>1947</v>
+        <v>1955</v>
       </c>
       <c r="B1916" t="s">
-        <v>3963</v>
+        <v>3972</v>
       </c>
       <c r="C1916" t="s">
         <v>3878</v>
@@ -62312,15 +62523,15 @@
         <v>1356</v>
       </c>
       <c r="M1916" t="s">
-        <v>4518</v>
+        <v>4525</v>
       </c>
     </row>
     <row r="1917" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1917">
-        <v>1948</v>
+        <v>1956</v>
       </c>
       <c r="B1917" t="s">
-        <v>3964</v>
+        <v>3973</v>
       </c>
       <c r="C1917" t="s">
         <v>3878</v>
@@ -62335,15 +62546,15 @@
         <v>1356</v>
       </c>
       <c r="M1917" t="s">
-        <v>4519</v>
+        <v>3974</v>
       </c>
     </row>
     <row r="1918" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1918">
-        <v>1949</v>
+        <v>1957</v>
       </c>
       <c r="B1918" t="s">
-        <v>3965</v>
+        <v>3975</v>
       </c>
       <c r="C1918" t="s">
         <v>3878</v>
@@ -62358,15 +62569,15 @@
         <v>1356</v>
       </c>
       <c r="M1918" t="s">
-        <v>4520</v>
+        <v>3976</v>
       </c>
     </row>
     <row r="1919" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1919">
-        <v>1950</v>
+        <v>1958</v>
       </c>
       <c r="B1919" t="s">
-        <v>3966</v>
+        <v>3977</v>
       </c>
       <c r="C1919" t="s">
         <v>3878</v>
@@ -62381,15 +62592,15 @@
         <v>1356</v>
       </c>
       <c r="M1919" t="s">
-        <v>4521</v>
+        <v>4526</v>
       </c>
     </row>
     <row r="1920" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1920">
-        <v>1951</v>
+        <v>1959</v>
       </c>
       <c r="B1920" t="s">
-        <v>3967</v>
+        <v>3978</v>
       </c>
       <c r="C1920" t="s">
         <v>3878</v>
@@ -62404,15 +62615,15 @@
         <v>1356</v>
       </c>
       <c r="M1920" t="s">
-        <v>4522</v>
+        <v>3979</v>
       </c>
     </row>
     <row r="1921" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1921">
-        <v>1952</v>
+        <v>1960</v>
       </c>
       <c r="B1921" t="s">
-        <v>3968</v>
+        <v>3980</v>
       </c>
       <c r="C1921" t="s">
         <v>3878</v>
@@ -62427,15 +62638,15 @@
         <v>1356</v>
       </c>
       <c r="M1921" t="s">
-        <v>4523</v>
+        <v>4527</v>
       </c>
     </row>
     <row r="1922" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1922">
-        <v>1953</v>
+        <v>1961</v>
       </c>
       <c r="B1922" t="s">
-        <v>3969</v>
+        <v>3981</v>
       </c>
       <c r="C1922" t="s">
         <v>3878</v>
@@ -62450,15 +62661,15 @@
         <v>1356</v>
       </c>
       <c r="M1922" t="s">
-        <v>3970</v>
+        <v>4528</v>
       </c>
     </row>
     <row r="1923" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1923">
-        <v>1954</v>
+        <v>1962</v>
       </c>
       <c r="B1923" t="s">
-        <v>3971</v>
+        <v>3982</v>
       </c>
       <c r="C1923" t="s">
         <v>3878</v>
@@ -62473,15 +62684,15 @@
         <v>1356</v>
       </c>
       <c r="M1923" t="s">
-        <v>4524</v>
+        <v>4529</v>
       </c>
     </row>
     <row r="1924" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1924">
-        <v>1955</v>
+        <v>1963</v>
       </c>
       <c r="B1924" t="s">
-        <v>3972</v>
+        <v>3983</v>
       </c>
       <c r="C1924" t="s">
         <v>3878</v>
@@ -62496,15 +62707,15 @@
         <v>1356</v>
       </c>
       <c r="M1924" t="s">
-        <v>4525</v>
+        <v>4530</v>
       </c>
     </row>
     <row r="1925" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1925">
-        <v>1956</v>
+        <v>1964</v>
       </c>
       <c r="B1925" t="s">
-        <v>3973</v>
+        <v>3984</v>
       </c>
       <c r="C1925" t="s">
         <v>3878</v>
@@ -62519,15 +62730,15 @@
         <v>1356</v>
       </c>
       <c r="M1925" t="s">
-        <v>3974</v>
+        <v>4531</v>
       </c>
     </row>
     <row r="1926" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1926">
-        <v>1957</v>
+        <v>1965</v>
       </c>
       <c r="B1926" t="s">
-        <v>3975</v>
+        <v>3985</v>
       </c>
       <c r="C1926" t="s">
         <v>3878</v>
@@ -62542,15 +62753,15 @@
         <v>1356</v>
       </c>
       <c r="M1926" t="s">
-        <v>3976</v>
+        <v>3986</v>
       </c>
     </row>
     <row r="1927" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1927">
-        <v>1958</v>
+        <v>1966</v>
       </c>
       <c r="B1927" t="s">
-        <v>3977</v>
+        <v>3987</v>
       </c>
       <c r="C1927" t="s">
         <v>3878</v>
@@ -62565,15 +62776,15 @@
         <v>1356</v>
       </c>
       <c r="M1927" t="s">
-        <v>4526</v>
+        <v>4532</v>
       </c>
     </row>
     <row r="1928" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1928">
-        <v>1959</v>
+        <v>1967</v>
       </c>
       <c r="B1928" t="s">
-        <v>3978</v>
+        <v>3988</v>
       </c>
       <c r="C1928" t="s">
         <v>3878</v>
@@ -62588,15 +62799,15 @@
         <v>1356</v>
       </c>
       <c r="M1928" t="s">
-        <v>3979</v>
+        <v>3989</v>
       </c>
     </row>
     <row r="1929" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1929">
-        <v>1960</v>
+        <v>1968</v>
       </c>
       <c r="B1929" t="s">
-        <v>3980</v>
+        <v>3990</v>
       </c>
       <c r="C1929" t="s">
         <v>3878</v>
@@ -62611,15 +62822,15 @@
         <v>1356</v>
       </c>
       <c r="M1929" t="s">
-        <v>4527</v>
+        <v>4533</v>
       </c>
     </row>
     <row r="1930" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1930">
-        <v>1961</v>
+        <v>1969</v>
       </c>
       <c r="B1930" t="s">
-        <v>3981</v>
+        <v>3991</v>
       </c>
       <c r="C1930" t="s">
         <v>3878</v>
@@ -62634,15 +62845,15 @@
         <v>1356</v>
       </c>
       <c r="M1930" t="s">
-        <v>4528</v>
+        <v>3992</v>
       </c>
     </row>
     <row r="1931" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1931">
-        <v>1962</v>
+        <v>1970</v>
       </c>
       <c r="B1931" t="s">
-        <v>3982</v>
+        <v>3993</v>
       </c>
       <c r="C1931" t="s">
         <v>3878</v>
@@ -62657,15 +62868,15 @@
         <v>1356</v>
       </c>
       <c r="M1931" t="s">
-        <v>4529</v>
+        <v>3994</v>
       </c>
     </row>
     <row r="1932" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1932">
-        <v>1963</v>
+        <v>1971</v>
       </c>
       <c r="B1932" t="s">
-        <v>3983</v>
+        <v>3995</v>
       </c>
       <c r="C1932" t="s">
         <v>3878</v>
@@ -62680,15 +62891,15 @@
         <v>1356</v>
       </c>
       <c r="M1932" t="s">
-        <v>4530</v>
+        <v>4534</v>
       </c>
     </row>
     <row r="1933" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1933">
-        <v>1964</v>
+        <v>1972</v>
       </c>
       <c r="B1933" t="s">
-        <v>3984</v>
+        <v>3996</v>
       </c>
       <c r="C1933" t="s">
         <v>3878</v>
@@ -62703,15 +62914,15 @@
         <v>1356</v>
       </c>
       <c r="M1933" t="s">
-        <v>4531</v>
+        <v>4535</v>
       </c>
     </row>
     <row r="1934" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1934">
-        <v>1965</v>
+        <v>1973</v>
       </c>
       <c r="B1934" t="s">
-        <v>3985</v>
+        <v>3997</v>
       </c>
       <c r="C1934" t="s">
         <v>3878</v>
@@ -62726,15 +62937,15 @@
         <v>1356</v>
       </c>
       <c r="M1934" t="s">
-        <v>3986</v>
+        <v>3998</v>
       </c>
     </row>
     <row r="1935" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1935">
-        <v>1966</v>
+        <v>1974</v>
       </c>
       <c r="B1935" t="s">
-        <v>3987</v>
+        <v>3999</v>
       </c>
       <c r="C1935" t="s">
         <v>3878</v>
@@ -62749,15 +62960,15 @@
         <v>1356</v>
       </c>
       <c r="M1935" t="s">
-        <v>4532</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="1936" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1936">
-        <v>1967</v>
+        <v>1975</v>
       </c>
       <c r="B1936" t="s">
-        <v>3988</v>
+        <v>4001</v>
       </c>
       <c r="C1936" t="s">
         <v>3878</v>
@@ -62772,15 +62983,15 @@
         <v>1356</v>
       </c>
       <c r="M1936" t="s">
-        <v>3989</v>
+        <v>4536</v>
       </c>
     </row>
     <row r="1937" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1937">
-        <v>1968</v>
+        <v>1976</v>
       </c>
       <c r="B1937" t="s">
-        <v>3990</v>
+        <v>4002</v>
       </c>
       <c r="C1937" t="s">
         <v>3878</v>
@@ -62795,15 +63006,15 @@
         <v>1356</v>
       </c>
       <c r="M1937" t="s">
-        <v>4533</v>
+        <v>4003</v>
       </c>
     </row>
     <row r="1938" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1938">
-        <v>1969</v>
+        <v>1977</v>
       </c>
       <c r="B1938" t="s">
-        <v>3991</v>
+        <v>4004</v>
       </c>
       <c r="C1938" t="s">
         <v>3878</v>
@@ -62818,15 +63029,15 @@
         <v>1356</v>
       </c>
       <c r="M1938" t="s">
-        <v>3992</v>
+        <v>4537</v>
       </c>
     </row>
     <row r="1939" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1939">
-        <v>1970</v>
+        <v>1978</v>
       </c>
       <c r="B1939" t="s">
-        <v>3993</v>
+        <v>4005</v>
       </c>
       <c r="C1939" t="s">
         <v>3878</v>
@@ -62841,15 +63052,15 @@
         <v>1356</v>
       </c>
       <c r="M1939" t="s">
-        <v>3994</v>
+        <v>4538</v>
       </c>
     </row>
     <row r="1940" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1940">
-        <v>1971</v>
+        <v>1979</v>
       </c>
       <c r="B1940" t="s">
-        <v>3995</v>
+        <v>4006</v>
       </c>
       <c r="C1940" t="s">
         <v>3878</v>
@@ -62864,15 +63075,15 @@
         <v>1356</v>
       </c>
       <c r="M1940" t="s">
-        <v>4534</v>
+        <v>4539</v>
       </c>
     </row>
     <row r="1941" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1941">
-        <v>1972</v>
+        <v>1980</v>
       </c>
       <c r="B1941" t="s">
-        <v>3996</v>
+        <v>4007</v>
       </c>
       <c r="C1941" t="s">
         <v>3878</v>
@@ -62887,15 +63098,15 @@
         <v>1356</v>
       </c>
       <c r="M1941" t="s">
-        <v>4535</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="1942" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1942">
-        <v>1973</v>
+        <v>1981</v>
       </c>
       <c r="B1942" t="s">
-        <v>3997</v>
+        <v>4008</v>
       </c>
       <c r="C1942" t="s">
         <v>3878</v>
@@ -62910,15 +63121,15 @@
         <v>1356</v>
       </c>
       <c r="M1942" t="s">
-        <v>3998</v>
+        <v>4541</v>
       </c>
     </row>
     <row r="1943" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1943">
-        <v>1974</v>
+        <v>1982</v>
       </c>
       <c r="B1943" t="s">
-        <v>3999</v>
+        <v>4009</v>
       </c>
       <c r="C1943" t="s">
         <v>3878</v>
@@ -62933,15 +63144,15 @@
         <v>1356</v>
       </c>
       <c r="M1943" t="s">
-        <v>4000</v>
+        <v>4542</v>
       </c>
     </row>
     <row r="1944" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1944">
-        <v>1975</v>
+        <v>1983</v>
       </c>
       <c r="B1944" t="s">
-        <v>4001</v>
+        <v>4010</v>
       </c>
       <c r="C1944" t="s">
         <v>3878</v>
@@ -62956,15 +63167,15 @@
         <v>1356</v>
       </c>
       <c r="M1944" t="s">
-        <v>4536</v>
+        <v>4011</v>
       </c>
     </row>
     <row r="1945" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1945">
-        <v>1976</v>
+        <v>1984</v>
       </c>
       <c r="B1945" t="s">
-        <v>4002</v>
+        <v>4012</v>
       </c>
       <c r="C1945" t="s">
         <v>3878</v>
@@ -62979,15 +63190,15 @@
         <v>1356</v>
       </c>
       <c r="M1945" t="s">
-        <v>4003</v>
+        <v>4543</v>
       </c>
     </row>
     <row r="1946" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1946">
-        <v>1977</v>
+        <v>1985</v>
       </c>
       <c r="B1946" t="s">
-        <v>4004</v>
+        <v>4013</v>
       </c>
       <c r="C1946" t="s">
         <v>3878</v>
@@ -63002,15 +63213,15 @@
         <v>1356</v>
       </c>
       <c r="M1946" t="s">
-        <v>4537</v>
+        <v>4544</v>
       </c>
     </row>
     <row r="1947" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1947">
-        <v>1978</v>
+        <v>1986</v>
       </c>
       <c r="B1947" t="s">
-        <v>4005</v>
+        <v>4014</v>
       </c>
       <c r="C1947" t="s">
         <v>3878</v>
@@ -63025,15 +63236,15 @@
         <v>1356</v>
       </c>
       <c r="M1947" t="s">
-        <v>4538</v>
+        <v>4015</v>
       </c>
     </row>
     <row r="1948" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1948">
-        <v>1979</v>
+        <v>1987</v>
       </c>
       <c r="B1948" t="s">
-        <v>4006</v>
+        <v>4016</v>
       </c>
       <c r="C1948" t="s">
         <v>3878</v>
@@ -63048,15 +63259,15 @@
         <v>1356</v>
       </c>
       <c r="M1948" t="s">
-        <v>4539</v>
+        <v>4545</v>
       </c>
     </row>
     <row r="1949" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1949">
-        <v>1980</v>
+        <v>1988</v>
       </c>
       <c r="B1949" t="s">
-        <v>4007</v>
+        <v>4017</v>
       </c>
       <c r="C1949" t="s">
         <v>3878</v>
@@ -63071,15 +63282,15 @@
         <v>1356</v>
       </c>
       <c r="M1949" t="s">
-        <v>4540</v>
+        <v>4018</v>
       </c>
     </row>
     <row r="1950" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1950">
-        <v>1981</v>
+        <v>1989</v>
       </c>
       <c r="B1950" t="s">
-        <v>4008</v>
+        <v>4019</v>
       </c>
       <c r="C1950" t="s">
         <v>3878</v>
@@ -63094,15 +63305,15 @@
         <v>1356</v>
       </c>
       <c r="M1950" t="s">
-        <v>4541</v>
+        <v>4020</v>
       </c>
     </row>
     <row r="1951" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1951">
-        <v>1982</v>
+        <v>1990</v>
       </c>
       <c r="B1951" t="s">
-        <v>4009</v>
+        <v>4021</v>
       </c>
       <c r="C1951" t="s">
         <v>3878</v>
@@ -63117,15 +63328,15 @@
         <v>1356</v>
       </c>
       <c r="M1951" t="s">
-        <v>4542</v>
+        <v>4546</v>
       </c>
     </row>
     <row r="1952" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1952">
-        <v>1983</v>
+        <v>1991</v>
       </c>
       <c r="B1952" t="s">
-        <v>4010</v>
+        <v>4022</v>
       </c>
       <c r="C1952" t="s">
         <v>3878</v>
@@ -63140,15 +63351,15 @@
         <v>1356</v>
       </c>
       <c r="M1952" t="s">
-        <v>4011</v>
+        <v>4023</v>
       </c>
     </row>
     <row r="1953" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1953">
-        <v>1984</v>
+        <v>1992</v>
       </c>
       <c r="B1953" t="s">
-        <v>4012</v>
+        <v>4024</v>
       </c>
       <c r="C1953" t="s">
         <v>3878</v>
@@ -63163,15 +63374,15 @@
         <v>1356</v>
       </c>
       <c r="M1953" t="s">
-        <v>4543</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="1954" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1954">
-        <v>1985</v>
+        <v>1993</v>
       </c>
       <c r="B1954" t="s">
-        <v>4013</v>
+        <v>4025</v>
       </c>
       <c r="C1954" t="s">
         <v>3878</v>
@@ -63186,15 +63397,15 @@
         <v>1356</v>
       </c>
       <c r="M1954" t="s">
-        <v>4544</v>
+        <v>4548</v>
       </c>
     </row>
     <row r="1955" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1955">
-        <v>1986</v>
+        <v>1994</v>
       </c>
       <c r="B1955" t="s">
-        <v>4014</v>
+        <v>4026</v>
       </c>
       <c r="C1955" t="s">
         <v>3878</v>
@@ -63209,15 +63420,15 @@
         <v>1356</v>
       </c>
       <c r="M1955" t="s">
-        <v>4015</v>
+        <v>4549</v>
       </c>
     </row>
     <row r="1956" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1956">
-        <v>1987</v>
+        <v>1995</v>
       </c>
       <c r="B1956" t="s">
-        <v>4016</v>
+        <v>4027</v>
       </c>
       <c r="C1956" t="s">
         <v>3878</v>
@@ -63232,15 +63443,15 @@
         <v>1356</v>
       </c>
       <c r="M1956" t="s">
-        <v>4545</v>
+        <v>4550</v>
       </c>
     </row>
     <row r="1957" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1957">
-        <v>1988</v>
+        <v>1996</v>
       </c>
       <c r="B1957" t="s">
-        <v>4017</v>
+        <v>4028</v>
       </c>
       <c r="C1957" t="s">
         <v>3878</v>
@@ -63255,15 +63466,15 @@
         <v>1356</v>
       </c>
       <c r="M1957" t="s">
-        <v>4018</v>
+        <v>4551</v>
       </c>
     </row>
     <row r="1958" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1958">
-        <v>1989</v>
+        <v>1997</v>
       </c>
       <c r="B1958" t="s">
-        <v>4019</v>
+        <v>4029</v>
       </c>
       <c r="C1958" t="s">
         <v>3878</v>
@@ -63278,15 +63489,15 @@
         <v>1356</v>
       </c>
       <c r="M1958" t="s">
-        <v>4020</v>
+        <v>4030</v>
       </c>
     </row>
     <row r="1959" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1959">
-        <v>1990</v>
+        <v>1998</v>
       </c>
       <c r="B1959" t="s">
-        <v>4021</v>
+        <v>4031</v>
       </c>
       <c r="C1959" t="s">
         <v>3878</v>
@@ -63301,15 +63512,15 @@
         <v>1356</v>
       </c>
       <c r="M1959" t="s">
-        <v>4546</v>
+        <v>4552</v>
       </c>
     </row>
     <row r="1960" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1960">
-        <v>1991</v>
+        <v>1999</v>
       </c>
       <c r="B1960" t="s">
-        <v>4022</v>
+        <v>4032</v>
       </c>
       <c r="C1960" t="s">
         <v>3878</v>
@@ -63324,15 +63535,15 @@
         <v>1356</v>
       </c>
       <c r="M1960" t="s">
-        <v>4023</v>
+        <v>4553</v>
       </c>
     </row>
     <row r="1961" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1961">
-        <v>1992</v>
+        <v>2000</v>
       </c>
       <c r="B1961" t="s">
-        <v>4024</v>
+        <v>4033</v>
       </c>
       <c r="C1961" t="s">
         <v>3878</v>
@@ -63347,15 +63558,15 @@
         <v>1356</v>
       </c>
       <c r="M1961" t="s">
-        <v>4547</v>
+        <v>4034</v>
       </c>
     </row>
     <row r="1962" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1962">
-        <v>1993</v>
+        <v>2001</v>
       </c>
       <c r="B1962" t="s">
-        <v>4025</v>
+        <v>4035</v>
       </c>
       <c r="C1962" t="s">
         <v>3878</v>
@@ -63370,15 +63581,15 @@
         <v>1356</v>
       </c>
       <c r="M1962" t="s">
-        <v>4548</v>
+        <v>4036</v>
       </c>
     </row>
     <row r="1963" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1963">
-        <v>1994</v>
+        <v>2002</v>
       </c>
       <c r="B1963" t="s">
-        <v>4026</v>
+        <v>4037</v>
       </c>
       <c r="C1963" t="s">
         <v>3878</v>
@@ -63393,15 +63604,15 @@
         <v>1356</v>
       </c>
       <c r="M1963" t="s">
-        <v>4549</v>
+        <v>4038</v>
       </c>
     </row>
     <row r="1964" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1964">
-        <v>1995</v>
+        <v>2003</v>
       </c>
       <c r="B1964" t="s">
-        <v>4027</v>
+        <v>4039</v>
       </c>
       <c r="C1964" t="s">
         <v>3878</v>
@@ -63416,15 +63627,15 @@
         <v>1356</v>
       </c>
       <c r="M1964" t="s">
-        <v>4550</v>
+        <v>4040</v>
       </c>
     </row>
     <row r="1965" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1965">
-        <v>1996</v>
+        <v>2004</v>
       </c>
       <c r="B1965" t="s">
-        <v>4028</v>
+        <v>4041</v>
       </c>
       <c r="C1965" t="s">
         <v>3878</v>
@@ -63439,15 +63650,15 @@
         <v>1356</v>
       </c>
       <c r="M1965" t="s">
-        <v>4551</v>
+        <v>4554</v>
       </c>
     </row>
     <row r="1966" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1966">
-        <v>1997</v>
+        <v>2005</v>
       </c>
       <c r="B1966" t="s">
-        <v>4029</v>
+        <v>4042</v>
       </c>
       <c r="C1966" t="s">
         <v>3878</v>
@@ -63462,15 +63673,15 @@
         <v>1356</v>
       </c>
       <c r="M1966" t="s">
-        <v>4030</v>
+        <v>4043</v>
       </c>
     </row>
     <row r="1967" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1967">
-        <v>1998</v>
+        <v>2006</v>
       </c>
       <c r="B1967" t="s">
-        <v>4031</v>
+        <v>4044</v>
       </c>
       <c r="C1967" t="s">
         <v>3878</v>
@@ -63485,15 +63696,15 @@
         <v>1356</v>
       </c>
       <c r="M1967" t="s">
-        <v>4552</v>
+        <v>4045</v>
       </c>
     </row>
     <row r="1968" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1968">
-        <v>1999</v>
+        <v>2007</v>
       </c>
       <c r="B1968" t="s">
-        <v>4032</v>
+        <v>4046</v>
       </c>
       <c r="C1968" t="s">
         <v>3878</v>
@@ -63508,15 +63719,15 @@
         <v>1356</v>
       </c>
       <c r="M1968" t="s">
-        <v>4553</v>
+        <v>4555</v>
       </c>
     </row>
     <row r="1969" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1969">
-        <v>2000</v>
+        <v>2008</v>
       </c>
       <c r="B1969" t="s">
-        <v>4033</v>
+        <v>4047</v>
       </c>
       <c r="C1969" t="s">
         <v>3878</v>
@@ -63531,15 +63742,15 @@
         <v>1356</v>
       </c>
       <c r="M1969" t="s">
-        <v>4034</v>
+        <v>4048</v>
       </c>
     </row>
     <row r="1970" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1970">
-        <v>2001</v>
+        <v>2009</v>
       </c>
       <c r="B1970" t="s">
-        <v>4035</v>
+        <v>4049</v>
       </c>
       <c r="C1970" t="s">
         <v>3878</v>
@@ -63554,15 +63765,15 @@
         <v>1356</v>
       </c>
       <c r="M1970" t="s">
-        <v>4036</v>
+        <v>4556</v>
       </c>
     </row>
     <row r="1971" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1971">
-        <v>2002</v>
+        <v>2010</v>
       </c>
       <c r="B1971" t="s">
-        <v>4037</v>
+        <v>4050</v>
       </c>
       <c r="C1971" t="s">
         <v>3878</v>
@@ -63577,15 +63788,15 @@
         <v>1356</v>
       </c>
       <c r="M1971" t="s">
-        <v>4038</v>
+        <v>4051</v>
       </c>
     </row>
     <row r="1972" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1972">
-        <v>2003</v>
+        <v>2011</v>
       </c>
       <c r="B1972" t="s">
-        <v>4039</v>
+        <v>4052</v>
       </c>
       <c r="C1972" t="s">
         <v>3878</v>
@@ -63600,15 +63811,15 @@
         <v>1356</v>
       </c>
       <c r="M1972" t="s">
-        <v>4040</v>
+        <v>4053</v>
       </c>
     </row>
     <row r="1973" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1973">
-        <v>2004</v>
+        <v>2012</v>
       </c>
       <c r="B1973" t="s">
-        <v>4041</v>
+        <v>4054</v>
       </c>
       <c r="C1973" t="s">
         <v>3878</v>
@@ -63623,15 +63834,15 @@
         <v>1356</v>
       </c>
       <c r="M1973" t="s">
-        <v>4554</v>
+        <v>4055</v>
       </c>
     </row>
     <row r="1974" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1974">
-        <v>2005</v>
+        <v>2013</v>
       </c>
       <c r="B1974" t="s">
-        <v>4042</v>
+        <v>4056</v>
       </c>
       <c r="C1974" t="s">
         <v>3878</v>
@@ -63646,15 +63857,15 @@
         <v>1356</v>
       </c>
       <c r="M1974" t="s">
-        <v>4043</v>
+        <v>4557</v>
       </c>
     </row>
     <row r="1975" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1975">
-        <v>2006</v>
+        <v>2014</v>
       </c>
       <c r="B1975" t="s">
-        <v>4044</v>
+        <v>4057</v>
       </c>
       <c r="C1975" t="s">
         <v>3878</v>
@@ -63669,15 +63880,15 @@
         <v>1356</v>
       </c>
       <c r="M1975" t="s">
-        <v>4045</v>
+        <v>4558</v>
       </c>
     </row>
     <row r="1976" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1976">
-        <v>2007</v>
+        <v>2015</v>
       </c>
       <c r="B1976" t="s">
-        <v>4046</v>
+        <v>4058</v>
       </c>
       <c r="C1976" t="s">
         <v>3878</v>
@@ -63692,15 +63903,15 @@
         <v>1356</v>
       </c>
       <c r="M1976" t="s">
-        <v>4555</v>
+        <v>4559</v>
       </c>
     </row>
     <row r="1977" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1977">
-        <v>2008</v>
+        <v>2016</v>
       </c>
       <c r="B1977" t="s">
-        <v>4047</v>
+        <v>4059</v>
       </c>
       <c r="C1977" t="s">
         <v>3878</v>
@@ -63715,15 +63926,15 @@
         <v>1356</v>
       </c>
       <c r="M1977" t="s">
-        <v>4048</v>
+        <v>4560</v>
       </c>
     </row>
     <row r="1978" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1978">
-        <v>2009</v>
+        <v>2017</v>
       </c>
       <c r="B1978" t="s">
-        <v>4049</v>
+        <v>4060</v>
       </c>
       <c r="C1978" t="s">
         <v>3878</v>
@@ -63738,15 +63949,15 @@
         <v>1356</v>
       </c>
       <c r="M1978" t="s">
-        <v>4556</v>
+        <v>4561</v>
       </c>
     </row>
     <row r="1979" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1979">
-        <v>2010</v>
+        <v>2018</v>
       </c>
       <c r="B1979" t="s">
-        <v>4050</v>
+        <v>4061</v>
       </c>
       <c r="C1979" t="s">
         <v>3878</v>
@@ -63761,15 +63972,15 @@
         <v>1356</v>
       </c>
       <c r="M1979" t="s">
-        <v>4051</v>
+        <v>4062</v>
       </c>
     </row>
     <row r="1980" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1980">
-        <v>2011</v>
+        <v>2019</v>
       </c>
       <c r="B1980" t="s">
-        <v>4052</v>
+        <v>4063</v>
       </c>
       <c r="C1980" t="s">
         <v>3878</v>
@@ -63784,15 +63995,15 @@
         <v>1356</v>
       </c>
       <c r="M1980" t="s">
-        <v>4053</v>
+        <v>4562</v>
       </c>
     </row>
     <row r="1981" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1981">
-        <v>2012</v>
+        <v>2020</v>
       </c>
       <c r="B1981" t="s">
-        <v>4054</v>
+        <v>4064</v>
       </c>
       <c r="C1981" t="s">
         <v>3878</v>
@@ -63807,195 +64018,11 @@
         <v>1356</v>
       </c>
       <c r="M1981" t="s">
-        <v>4055</v>
-      </c>
-    </row>
-    <row r="1982" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1982">
-        <v>2013</v>
-      </c>
-      <c r="B1982" t="s">
-        <v>4056</v>
-      </c>
-      <c r="C1982" t="s">
-        <v>3878</v>
-      </c>
-      <c r="D1982">
-        <v>68000</v>
-      </c>
-      <c r="E1982" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1982" t="s">
-        <v>1356</v>
-      </c>
-      <c r="M1982" t="s">
-        <v>4557</v>
-      </c>
-    </row>
-    <row r="1983" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1983">
-        <v>2014</v>
-      </c>
-      <c r="B1983" t="s">
-        <v>4057</v>
-      </c>
-      <c r="C1983" t="s">
-        <v>3878</v>
-      </c>
-      <c r="D1983">
-        <v>68000</v>
-      </c>
-      <c r="E1983" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1983" t="s">
-        <v>1356</v>
-      </c>
-      <c r="M1983" t="s">
-        <v>4558</v>
-      </c>
-    </row>
-    <row r="1984" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1984">
-        <v>2015</v>
-      </c>
-      <c r="B1984" t="s">
-        <v>4058</v>
-      </c>
-      <c r="C1984" t="s">
-        <v>3878</v>
-      </c>
-      <c r="D1984">
-        <v>68000</v>
-      </c>
-      <c r="E1984" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1984" t="s">
-        <v>1356</v>
-      </c>
-      <c r="M1984" t="s">
-        <v>4559</v>
-      </c>
-    </row>
-    <row r="1985" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1985">
-        <v>2016</v>
-      </c>
-      <c r="B1985" t="s">
-        <v>4059</v>
-      </c>
-      <c r="C1985" t="s">
-        <v>3878</v>
-      </c>
-      <c r="D1985">
-        <v>68000</v>
-      </c>
-      <c r="E1985" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1985" t="s">
-        <v>1356</v>
-      </c>
-      <c r="M1985" t="s">
-        <v>4560</v>
-      </c>
-    </row>
-    <row r="1986" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1986">
-        <v>2017</v>
-      </c>
-      <c r="B1986" t="s">
-        <v>4060</v>
-      </c>
-      <c r="C1986" t="s">
-        <v>3878</v>
-      </c>
-      <c r="D1986">
-        <v>68000</v>
-      </c>
-      <c r="E1986" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1986" t="s">
-        <v>1356</v>
-      </c>
-      <c r="M1986" t="s">
-        <v>4561</v>
-      </c>
-    </row>
-    <row r="1987" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1987">
-        <v>2018</v>
-      </c>
-      <c r="B1987" t="s">
-        <v>4061</v>
-      </c>
-      <c r="C1987" t="s">
-        <v>3878</v>
-      </c>
-      <c r="D1987">
-        <v>68000</v>
-      </c>
-      <c r="E1987" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1987" t="s">
-        <v>1356</v>
-      </c>
-      <c r="M1987" t="s">
-        <v>4062</v>
-      </c>
-    </row>
-    <row r="1988" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1988">
-        <v>2019</v>
-      </c>
-      <c r="B1988" t="s">
-        <v>4063</v>
-      </c>
-      <c r="C1988" t="s">
-        <v>3878</v>
-      </c>
-      <c r="D1988">
-        <v>68000</v>
-      </c>
-      <c r="E1988" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1988" t="s">
-        <v>1356</v>
-      </c>
-      <c r="M1988" t="s">
-        <v>4562</v>
-      </c>
-    </row>
-    <row r="1989" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1989">
-        <v>2020</v>
-      </c>
-      <c r="B1989" t="s">
-        <v>4064</v>
-      </c>
-      <c r="C1989" t="s">
-        <v>3878</v>
-      </c>
-      <c r="D1989">
-        <v>68000</v>
-      </c>
-      <c r="E1989" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1989" t="s">
-        <v>1356</v>
-      </c>
-      <c r="M1989" t="s">
         <v>4065</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M1989"/>
+  <autoFilter ref="A1:M1981"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
036 : added working kyugo driver
</commit_message>
<xml_diff>
--- a/0.36/compatibility.xlsx
+++ b/0.36/compatibility.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
     <sheet name="Playable" sheetId="4" r:id="rId1"/>
@@ -14086,10 +14086,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P77"/>
+  <dimension ref="A1:P87"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="O74" sqref="O74"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15869,6 +15869,236 @@
         <v>4567</v>
       </c>
     </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>78</v>
+      </c>
+      <c r="B78" t="s">
+        <v>1506</v>
+      </c>
+      <c r="C78" t="s">
+        <v>1507</v>
+      </c>
+      <c r="D78" t="s">
+        <v>14</v>
+      </c>
+      <c r="E78" t="s">
+        <v>14</v>
+      </c>
+      <c r="H78" t="s">
+        <v>172</v>
+      </c>
+      <c r="M78" t="s">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>79</v>
+      </c>
+      <c r="B79" t="s">
+        <v>1509</v>
+      </c>
+      <c r="C79" t="s">
+        <v>1507</v>
+      </c>
+      <c r="D79" t="s">
+        <v>14</v>
+      </c>
+      <c r="E79" t="s">
+        <v>14</v>
+      </c>
+      <c r="H79" t="s">
+        <v>172</v>
+      </c>
+      <c r="M79" t="s">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>80</v>
+      </c>
+      <c r="B80" t="s">
+        <v>1511</v>
+      </c>
+      <c r="C80" t="s">
+        <v>1507</v>
+      </c>
+      <c r="D80" t="s">
+        <v>14</v>
+      </c>
+      <c r="E80" t="s">
+        <v>14</v>
+      </c>
+      <c r="H80" t="s">
+        <v>172</v>
+      </c>
+      <c r="M80" t="s">
+        <v>1512</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>81</v>
+      </c>
+      <c r="B81" t="s">
+        <v>1513</v>
+      </c>
+      <c r="C81" t="s">
+        <v>1507</v>
+      </c>
+      <c r="D81" t="s">
+        <v>14</v>
+      </c>
+      <c r="E81" t="s">
+        <v>14</v>
+      </c>
+      <c r="H81" t="s">
+        <v>172</v>
+      </c>
+      <c r="M81" t="s">
+        <v>1514</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>82</v>
+      </c>
+      <c r="B82" t="s">
+        <v>1515</v>
+      </c>
+      <c r="C82" t="s">
+        <v>1507</v>
+      </c>
+      <c r="D82" t="s">
+        <v>14</v>
+      </c>
+      <c r="E82" t="s">
+        <v>14</v>
+      </c>
+      <c r="H82" t="s">
+        <v>172</v>
+      </c>
+      <c r="M82" t="s">
+        <v>4219</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>83</v>
+      </c>
+      <c r="B83" t="s">
+        <v>1516</v>
+      </c>
+      <c r="C83" t="s">
+        <v>1507</v>
+      </c>
+      <c r="D83" t="s">
+        <v>14</v>
+      </c>
+      <c r="E83" t="s">
+        <v>14</v>
+      </c>
+      <c r="H83" t="s">
+        <v>172</v>
+      </c>
+      <c r="M83" t="s">
+        <v>1517</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>84</v>
+      </c>
+      <c r="B84" t="s">
+        <v>1518</v>
+      </c>
+      <c r="C84" t="s">
+        <v>1507</v>
+      </c>
+      <c r="D84" t="s">
+        <v>14</v>
+      </c>
+      <c r="E84" t="s">
+        <v>14</v>
+      </c>
+      <c r="H84" t="s">
+        <v>172</v>
+      </c>
+      <c r="M84" t="s">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>85</v>
+      </c>
+      <c r="B85" t="s">
+        <v>1520</v>
+      </c>
+      <c r="C85" t="s">
+        <v>1507</v>
+      </c>
+      <c r="D85" t="s">
+        <v>14</v>
+      </c>
+      <c r="E85" t="s">
+        <v>14</v>
+      </c>
+      <c r="H85" t="s">
+        <v>172</v>
+      </c>
+      <c r="M85" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>86</v>
+      </c>
+      <c r="B86" t="s">
+        <v>1522</v>
+      </c>
+      <c r="C86" t="s">
+        <v>1507</v>
+      </c>
+      <c r="D86" t="s">
+        <v>14</v>
+      </c>
+      <c r="E86" t="s">
+        <v>14</v>
+      </c>
+      <c r="H86" t="s">
+        <v>172</v>
+      </c>
+      <c r="M86" t="s">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>87</v>
+      </c>
+      <c r="B87" t="s">
+        <v>1524</v>
+      </c>
+      <c r="C87" t="s">
+        <v>1507</v>
+      </c>
+      <c r="D87" t="s">
+        <v>14</v>
+      </c>
+      <c r="E87" t="s">
+        <v>14</v>
+      </c>
+      <c r="H87" t="s">
+        <v>172</v>
+      </c>
+      <c r="M87" t="s">
+        <v>1525</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15878,8 +16108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1972"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A490" workbookViewId="0">
-      <selection activeCell="H490" sqref="H490"/>
+    <sheetView topLeftCell="A706" workbookViewId="0">
+      <selection activeCell="A714" sqref="A714:XFD723"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33102,236 +33332,6 @@
         <v>4218</v>
       </c>
     </row>
-    <row r="714" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A714">
-        <v>732</v>
-      </c>
-      <c r="B714" t="s">
-        <v>1506</v>
-      </c>
-      <c r="C714" t="s">
-        <v>1507</v>
-      </c>
-      <c r="D714" t="s">
-        <v>14</v>
-      </c>
-      <c r="E714" t="s">
-        <v>14</v>
-      </c>
-      <c r="H714" t="s">
-        <v>172</v>
-      </c>
-      <c r="M714" t="s">
-        <v>1508</v>
-      </c>
-    </row>
-    <row r="715" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A715">
-        <v>733</v>
-      </c>
-      <c r="B715" t="s">
-        <v>1509</v>
-      </c>
-      <c r="C715" t="s">
-        <v>1507</v>
-      </c>
-      <c r="D715" t="s">
-        <v>14</v>
-      </c>
-      <c r="E715" t="s">
-        <v>14</v>
-      </c>
-      <c r="H715" t="s">
-        <v>172</v>
-      </c>
-      <c r="M715" t="s">
-        <v>1510</v>
-      </c>
-    </row>
-    <row r="716" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A716">
-        <v>734</v>
-      </c>
-      <c r="B716" t="s">
-        <v>1511</v>
-      </c>
-      <c r="C716" t="s">
-        <v>1507</v>
-      </c>
-      <c r="D716" t="s">
-        <v>14</v>
-      </c>
-      <c r="E716" t="s">
-        <v>14</v>
-      </c>
-      <c r="H716" t="s">
-        <v>172</v>
-      </c>
-      <c r="M716" t="s">
-        <v>1512</v>
-      </c>
-    </row>
-    <row r="717" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A717">
-        <v>735</v>
-      </c>
-      <c r="B717" t="s">
-        <v>1513</v>
-      </c>
-      <c r="C717" t="s">
-        <v>1507</v>
-      </c>
-      <c r="D717" t="s">
-        <v>14</v>
-      </c>
-      <c r="E717" t="s">
-        <v>14</v>
-      </c>
-      <c r="H717" t="s">
-        <v>172</v>
-      </c>
-      <c r="M717" t="s">
-        <v>1514</v>
-      </c>
-    </row>
-    <row r="718" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A718">
-        <v>736</v>
-      </c>
-      <c r="B718" t="s">
-        <v>1515</v>
-      </c>
-      <c r="C718" t="s">
-        <v>1507</v>
-      </c>
-      <c r="D718" t="s">
-        <v>14</v>
-      </c>
-      <c r="E718" t="s">
-        <v>14</v>
-      </c>
-      <c r="H718" t="s">
-        <v>172</v>
-      </c>
-      <c r="M718" t="s">
-        <v>4219</v>
-      </c>
-    </row>
-    <row r="719" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A719">
-        <v>737</v>
-      </c>
-      <c r="B719" t="s">
-        <v>1516</v>
-      </c>
-      <c r="C719" t="s">
-        <v>1507</v>
-      </c>
-      <c r="D719" t="s">
-        <v>14</v>
-      </c>
-      <c r="E719" t="s">
-        <v>14</v>
-      </c>
-      <c r="H719" t="s">
-        <v>172</v>
-      </c>
-      <c r="M719" t="s">
-        <v>1517</v>
-      </c>
-    </row>
-    <row r="720" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A720">
-        <v>738</v>
-      </c>
-      <c r="B720" t="s">
-        <v>1518</v>
-      </c>
-      <c r="C720" t="s">
-        <v>1507</v>
-      </c>
-      <c r="D720" t="s">
-        <v>14</v>
-      </c>
-      <c r="E720" t="s">
-        <v>14</v>
-      </c>
-      <c r="H720" t="s">
-        <v>172</v>
-      </c>
-      <c r="M720" t="s">
-        <v>1519</v>
-      </c>
-    </row>
-    <row r="721" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A721">
-        <v>739</v>
-      </c>
-      <c r="B721" t="s">
-        <v>1520</v>
-      </c>
-      <c r="C721" t="s">
-        <v>1507</v>
-      </c>
-      <c r="D721" t="s">
-        <v>14</v>
-      </c>
-      <c r="E721" t="s">
-        <v>14</v>
-      </c>
-      <c r="H721" t="s">
-        <v>172</v>
-      </c>
-      <c r="M721" t="s">
-        <v>1521</v>
-      </c>
-    </row>
-    <row r="722" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A722">
-        <v>740</v>
-      </c>
-      <c r="B722" t="s">
-        <v>1522</v>
-      </c>
-      <c r="C722" t="s">
-        <v>1507</v>
-      </c>
-      <c r="D722" t="s">
-        <v>14</v>
-      </c>
-      <c r="E722" t="s">
-        <v>14</v>
-      </c>
-      <c r="H722" t="s">
-        <v>172</v>
-      </c>
-      <c r="M722" t="s">
-        <v>1523</v>
-      </c>
-    </row>
-    <row r="723" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A723">
-        <v>741</v>
-      </c>
-      <c r="B723" t="s">
-        <v>1524</v>
-      </c>
-      <c r="C723" t="s">
-        <v>1507</v>
-      </c>
-      <c r="D723" t="s">
-        <v>14</v>
-      </c>
-      <c r="E723" t="s">
-        <v>14</v>
-      </c>
-      <c r="H723" t="s">
-        <v>172</v>
-      </c>
-      <c r="M723" t="s">
-        <v>1525</v>
-      </c>
-    </row>
     <row r="724" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A724">
         <v>742</v>

</xml_diff>

<commit_message>
036 : zodiack driver
</commit_message>
<xml_diff>
--- a/0.36/compatibility.xlsx
+++ b/0.36/compatibility.xlsx
@@ -17,8 +17,8 @@
     <sheet name="GAME_NOT_WORKING FLAG" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ALL!$A$1:$M$1855</definedName>
-    <definedName name="LIST" localSheetId="1">ALL!$B$1:$M$1855</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ALL!$A$1:$M$1851</definedName>
+    <definedName name="LIST" localSheetId="1">ALL!$B$1:$M$1851</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -14087,10 +14087,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P193"/>
+  <dimension ref="A1:P197"/>
   <sheetViews>
-    <sheetView topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="F195" sqref="F195"/>
+    <sheetView topLeftCell="A182" workbookViewId="0">
+      <selection activeCell="A190" sqref="A190:A197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18415,6 +18415,98 @@
         <v>3486</v>
       </c>
     </row>
+    <row r="194" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A194">
+        <v>194</v>
+      </c>
+      <c r="B194" t="s">
+        <v>3724</v>
+      </c>
+      <c r="C194" t="s">
+        <v>3725</v>
+      </c>
+      <c r="D194" t="s">
+        <v>14</v>
+      </c>
+      <c r="E194" t="s">
+        <v>14</v>
+      </c>
+      <c r="H194" t="s">
+        <v>71</v>
+      </c>
+      <c r="M194" t="s">
+        <v>3726</v>
+      </c>
+    </row>
+    <row r="195" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A195">
+        <v>195</v>
+      </c>
+      <c r="B195" t="s">
+        <v>3727</v>
+      </c>
+      <c r="C195" t="s">
+        <v>3725</v>
+      </c>
+      <c r="D195" t="s">
+        <v>14</v>
+      </c>
+      <c r="E195" t="s">
+        <v>14</v>
+      </c>
+      <c r="H195" t="s">
+        <v>71</v>
+      </c>
+      <c r="M195" t="s">
+        <v>3728</v>
+      </c>
+    </row>
+    <row r="196" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A196">
+        <v>196</v>
+      </c>
+      <c r="B196" t="s">
+        <v>3729</v>
+      </c>
+      <c r="C196" t="s">
+        <v>3725</v>
+      </c>
+      <c r="D196" t="s">
+        <v>14</v>
+      </c>
+      <c r="E196" t="s">
+        <v>14</v>
+      </c>
+      <c r="H196" t="s">
+        <v>71</v>
+      </c>
+      <c r="M196" t="s">
+        <v>3730</v>
+      </c>
+    </row>
+    <row r="197" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A197">
+        <v>197</v>
+      </c>
+      <c r="B197" t="s">
+        <v>3731</v>
+      </c>
+      <c r="C197" t="s">
+        <v>3725</v>
+      </c>
+      <c r="D197" t="s">
+        <v>14</v>
+      </c>
+      <c r="E197" t="s">
+        <v>14</v>
+      </c>
+      <c r="H197" t="s">
+        <v>71</v>
+      </c>
+      <c r="M197" t="s">
+        <v>3732</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18422,10 +18514,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1855"/>
+  <dimension ref="A1:M1851"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1836" workbookViewId="0">
-      <selection activeCell="O1587" sqref="O1587"/>
+    <sheetView tabSelected="1" topLeftCell="A1659" workbookViewId="0">
+      <selection activeCell="I1669" sqref="I1669"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -59842,13 +59934,13 @@
     </row>
     <row r="1674" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1674">
-        <v>1836</v>
+        <v>1842</v>
       </c>
       <c r="B1674" t="s">
-        <v>3724</v>
+        <v>3738</v>
       </c>
       <c r="C1674" t="s">
-        <v>3725</v>
+        <v>3739</v>
       </c>
       <c r="D1674" t="s">
         <v>14</v>
@@ -59860,18 +59952,18 @@
         <v>71</v>
       </c>
       <c r="M1674" t="s">
-        <v>3726</v>
+        <v>3740</v>
       </c>
     </row>
     <row r="1675" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1675">
-        <v>1837</v>
+        <v>1843</v>
       </c>
       <c r="B1675" t="s">
-        <v>3727</v>
+        <v>3741</v>
       </c>
       <c r="C1675" t="s">
-        <v>3725</v>
+        <v>3739</v>
       </c>
       <c r="D1675" t="s">
         <v>14</v>
@@ -59883,265 +59975,265 @@
         <v>71</v>
       </c>
       <c r="M1675" t="s">
-        <v>3728</v>
+        <v>3742</v>
       </c>
     </row>
     <row r="1676" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1676">
-        <v>1838</v>
+        <v>1844</v>
       </c>
       <c r="B1676" t="s">
-        <v>3729</v>
+        <v>3743</v>
       </c>
       <c r="C1676" t="s">
-        <v>3725</v>
-      </c>
-      <c r="D1676" t="s">
-        <v>14</v>
+        <v>3744</v>
+      </c>
+      <c r="D1676">
+        <v>68000</v>
       </c>
       <c r="E1676" t="s">
         <v>14</v>
       </c>
       <c r="H1676" t="s">
-        <v>71</v>
+        <v>349</v>
       </c>
       <c r="M1676" t="s">
-        <v>3730</v>
+        <v>3745</v>
       </c>
     </row>
     <row r="1677" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1677">
-        <v>1839</v>
+        <v>1845</v>
       </c>
       <c r="B1677" t="s">
-        <v>3731</v>
+        <v>3746</v>
       </c>
       <c r="C1677" t="s">
-        <v>3725</v>
-      </c>
-      <c r="D1677" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1677" t="s">
-        <v>14</v>
+        <v>3747</v>
+      </c>
+      <c r="D1677">
+        <v>68000</v>
       </c>
       <c r="H1677" t="s">
-        <v>71</v>
+        <v>172</v>
+      </c>
+      <c r="I1677" t="s">
+        <v>1495</v>
       </c>
       <c r="M1677" t="s">
-        <v>3732</v>
+        <v>3748</v>
       </c>
     </row>
     <row r="1678" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1678">
-        <v>1842</v>
+        <v>1846</v>
       </c>
       <c r="B1678" t="s">
-        <v>3738</v>
+        <v>3749</v>
       </c>
       <c r="C1678" t="s">
-        <v>3739</v>
-      </c>
-      <c r="D1678" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1678" t="s">
-        <v>14</v>
+        <v>3747</v>
+      </c>
+      <c r="D1678">
+        <v>68000</v>
       </c>
       <c r="H1678" t="s">
-        <v>71</v>
+        <v>172</v>
+      </c>
+      <c r="I1678" t="s">
+        <v>1495</v>
       </c>
       <c r="M1678" t="s">
-        <v>3740</v>
+        <v>3750</v>
       </c>
     </row>
     <row r="1679" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1679">
-        <v>1843</v>
+        <v>1847</v>
       </c>
       <c r="B1679" t="s">
-        <v>3741</v>
+        <v>3751</v>
       </c>
       <c r="C1679" t="s">
-        <v>3739</v>
-      </c>
-      <c r="D1679" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1679" t="s">
-        <v>14</v>
+        <v>3747</v>
+      </c>
+      <c r="D1679">
+        <v>68000</v>
       </c>
       <c r="H1679" t="s">
-        <v>71</v>
+        <v>2378</v>
       </c>
       <c r="M1679" t="s">
-        <v>3742</v>
+        <v>3752</v>
       </c>
     </row>
     <row r="1680" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1680">
-        <v>1844</v>
+        <v>1848</v>
       </c>
       <c r="B1680" t="s">
-        <v>3743</v>
+        <v>3753</v>
       </c>
       <c r="C1680" t="s">
-        <v>3744</v>
+        <v>3747</v>
       </c>
       <c r="D1680">
         <v>68000</v>
       </c>
-      <c r="E1680" t="s">
-        <v>14</v>
-      </c>
       <c r="H1680" t="s">
-        <v>349</v>
+        <v>2378</v>
       </c>
       <c r="M1680" t="s">
-        <v>3745</v>
+        <v>4492</v>
       </c>
     </row>
     <row r="1681" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1681">
-        <v>1845</v>
+        <v>1849</v>
       </c>
       <c r="B1681" t="s">
-        <v>3746</v>
+        <v>3754</v>
       </c>
       <c r="C1681" t="s">
-        <v>3747</v>
+        <v>3755</v>
       </c>
       <c r="D1681">
         <v>68000</v>
       </c>
       <c r="H1681" t="s">
-        <v>172</v>
-      </c>
-      <c r="I1681" t="s">
         <v>1495</v>
       </c>
       <c r="M1681" t="s">
-        <v>3748</v>
+        <v>3756</v>
       </c>
     </row>
     <row r="1682" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1682">
-        <v>1846</v>
+        <v>1850</v>
       </c>
       <c r="B1682" t="s">
-        <v>3749</v>
+        <v>3757</v>
       </c>
       <c r="C1682" t="s">
-        <v>3747</v>
-      </c>
-      <c r="D1682">
-        <v>68000</v>
+        <v>3758</v>
+      </c>
+      <c r="D1682" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1682" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1682" t="s">
+        <v>14</v>
       </c>
       <c r="H1682" t="s">
-        <v>172</v>
+        <v>336</v>
       </c>
       <c r="I1682" t="s">
         <v>1495</v>
       </c>
       <c r="M1682" t="s">
-        <v>3750</v>
+        <v>3759</v>
       </c>
     </row>
     <row r="1683" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1683">
-        <v>1847</v>
+        <v>1851</v>
       </c>
       <c r="B1683" t="s">
-        <v>3751</v>
+        <v>3760</v>
       </c>
       <c r="C1683" t="s">
-        <v>3747</v>
-      </c>
-      <c r="D1683">
-        <v>68000</v>
+        <v>3761</v>
+      </c>
+      <c r="D1683" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1683" t="s">
+        <v>728</v>
       </c>
       <c r="H1683" t="s">
-        <v>2378</v>
+        <v>166</v>
       </c>
       <c r="M1683" t="s">
-        <v>3752</v>
+        <v>4493</v>
       </c>
     </row>
     <row r="1684" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1684">
-        <v>1848</v>
+        <v>1852</v>
       </c>
       <c r="B1684" t="s">
-        <v>3753</v>
+        <v>3762</v>
       </c>
       <c r="C1684" t="s">
-        <v>3747</v>
-      </c>
-      <c r="D1684">
-        <v>68000</v>
+        <v>3761</v>
+      </c>
+      <c r="D1684" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1684" t="s">
+        <v>728</v>
       </c>
       <c r="H1684" t="s">
-        <v>2378</v>
+        <v>166</v>
       </c>
       <c r="M1684" t="s">
-        <v>4492</v>
+        <v>3763</v>
       </c>
     </row>
     <row r="1685" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1685">
-        <v>1849</v>
+        <v>1853</v>
       </c>
       <c r="B1685" t="s">
-        <v>3754</v>
+        <v>3764</v>
       </c>
       <c r="C1685" t="s">
-        <v>3755</v>
-      </c>
-      <c r="D1685">
-        <v>68000</v>
+        <v>3761</v>
+      </c>
+      <c r="D1685" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1685" t="s">
+        <v>728</v>
       </c>
       <c r="H1685" t="s">
-        <v>1495</v>
+        <v>166</v>
       </c>
       <c r="M1685" t="s">
-        <v>3756</v>
+        <v>3765</v>
       </c>
     </row>
     <row r="1686" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1686">
-        <v>1850</v>
+        <v>1854</v>
       </c>
       <c r="B1686" t="s">
-        <v>3757</v>
+        <v>3766</v>
       </c>
       <c r="C1686" t="s">
-        <v>3758</v>
+        <v>3761</v>
       </c>
       <c r="D1686" t="s">
         <v>14</v>
       </c>
       <c r="E1686" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1686" t="s">
-        <v>14</v>
+        <v>728</v>
       </c>
       <c r="H1686" t="s">
-        <v>336</v>
-      </c>
-      <c r="I1686" t="s">
-        <v>1495</v>
+        <v>166</v>
       </c>
       <c r="M1686" t="s">
-        <v>3759</v>
+        <v>3767</v>
       </c>
     </row>
     <row r="1687" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1687">
-        <v>1851</v>
+        <v>1855</v>
       </c>
       <c r="B1687" t="s">
-        <v>3760</v>
+        <v>3768</v>
       </c>
       <c r="C1687" t="s">
         <v>3761</v>
@@ -60156,480 +60248,507 @@
         <v>166</v>
       </c>
       <c r="M1687" t="s">
-        <v>4493</v>
+        <v>3769</v>
       </c>
     </row>
     <row r="1688" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1688">
-        <v>1852</v>
+        <v>1856</v>
       </c>
       <c r="B1688" t="s">
-        <v>3762</v>
+        <v>3777</v>
       </c>
       <c r="C1688" t="s">
-        <v>3761</v>
+        <v>3778</v>
       </c>
       <c r="D1688" t="s">
         <v>14</v>
       </c>
       <c r="E1688" t="s">
-        <v>728</v>
+        <v>154</v>
       </c>
       <c r="H1688" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="M1688" t="s">
-        <v>3763</v>
+        <v>3779</v>
       </c>
     </row>
     <row r="1689" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1689">
-        <v>1853</v>
+        <v>1857</v>
       </c>
       <c r="B1689" t="s">
-        <v>3764</v>
+        <v>3780</v>
       </c>
       <c r="C1689" t="s">
-        <v>3761</v>
+        <v>3781</v>
       </c>
       <c r="D1689" t="s">
         <v>14</v>
       </c>
-      <c r="E1689" t="s">
-        <v>728</v>
-      </c>
       <c r="H1689" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="M1689" t="s">
-        <v>3765</v>
+        <v>3782</v>
       </c>
     </row>
     <row r="1690" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1690">
-        <v>1854</v>
+        <v>1858</v>
       </c>
       <c r="B1690" t="s">
-        <v>3766</v>
+        <v>3783</v>
       </c>
       <c r="C1690" t="s">
-        <v>3761</v>
+        <v>3781</v>
       </c>
       <c r="D1690" t="s">
         <v>14</v>
       </c>
-      <c r="E1690" t="s">
-        <v>728</v>
-      </c>
       <c r="H1690" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="M1690" t="s">
-        <v>3767</v>
+        <v>3784</v>
       </c>
     </row>
     <row r="1691" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1691">
-        <v>1855</v>
+        <v>1859</v>
       </c>
       <c r="B1691" t="s">
-        <v>3768</v>
+        <v>3785</v>
       </c>
       <c r="C1691" t="s">
-        <v>3761</v>
+        <v>3786</v>
       </c>
       <c r="D1691" t="s">
         <v>14</v>
       </c>
-      <c r="E1691" t="s">
-        <v>728</v>
-      </c>
       <c r="H1691" t="s">
-        <v>166</v>
+        <v>336</v>
       </c>
       <c r="M1691" t="s">
-        <v>3769</v>
+        <v>3787</v>
       </c>
     </row>
     <row r="1692" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1692">
-        <v>1856</v>
+        <v>1860</v>
       </c>
       <c r="B1692" t="s">
-        <v>3777</v>
+        <v>3788</v>
       </c>
       <c r="C1692" t="s">
-        <v>3778</v>
+        <v>3786</v>
       </c>
       <c r="D1692" t="s">
         <v>14</v>
       </c>
-      <c r="E1692" t="s">
-        <v>154</v>
-      </c>
       <c r="H1692" t="s">
-        <v>172</v>
+        <v>336</v>
       </c>
       <c r="M1692" t="s">
-        <v>3779</v>
+        <v>3789</v>
       </c>
     </row>
     <row r="1693" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1693">
-        <v>1857</v>
+        <v>1861</v>
       </c>
       <c r="B1693" t="s">
-        <v>3780</v>
+        <v>3790</v>
       </c>
       <c r="C1693" t="s">
-        <v>3781</v>
+        <v>3786</v>
       </c>
       <c r="D1693" t="s">
         <v>14</v>
       </c>
       <c r="H1693" t="s">
-        <v>172</v>
+        <v>336</v>
       </c>
       <c r="M1693" t="s">
-        <v>3782</v>
+        <v>3791</v>
       </c>
     </row>
     <row r="1694" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1694">
-        <v>1858</v>
+        <v>1862</v>
       </c>
       <c r="B1694" t="s">
-        <v>3783</v>
+        <v>3792</v>
       </c>
       <c r="C1694" t="s">
-        <v>3781</v>
+        <v>3786</v>
       </c>
       <c r="D1694" t="s">
         <v>14</v>
       </c>
       <c r="H1694" t="s">
-        <v>172</v>
+        <v>336</v>
       </c>
       <c r="M1694" t="s">
-        <v>3784</v>
+        <v>3793</v>
       </c>
     </row>
     <row r="1695" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1695">
-        <v>1859</v>
+        <v>1863</v>
       </c>
       <c r="B1695" t="s">
-        <v>3785</v>
+        <v>3794</v>
       </c>
       <c r="C1695" t="s">
-        <v>3786</v>
+        <v>3795</v>
       </c>
       <c r="D1695" t="s">
-        <v>14</v>
+        <v>405</v>
+      </c>
+      <c r="E1695" t="s">
+        <v>1187</v>
       </c>
       <c r="H1695" t="s">
-        <v>336</v>
+        <v>71</v>
       </c>
       <c r="M1695" t="s">
-        <v>3787</v>
+        <v>3796</v>
       </c>
     </row>
     <row r="1696" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1696">
-        <v>1860</v>
+        <v>1864</v>
       </c>
       <c r="B1696" t="s">
-        <v>3788</v>
+        <v>3797</v>
       </c>
       <c r="C1696" t="s">
-        <v>3786</v>
+        <v>3795</v>
       </c>
       <c r="D1696" t="s">
-        <v>14</v>
+        <v>405</v>
+      </c>
+      <c r="E1696" t="s">
+        <v>1187</v>
       </c>
       <c r="H1696" t="s">
-        <v>336</v>
+        <v>71</v>
       </c>
       <c r="M1696" t="s">
-        <v>3789</v>
+        <v>3798</v>
       </c>
     </row>
     <row r="1697" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1697">
-        <v>1861</v>
+        <v>1866</v>
       </c>
       <c r="B1697" t="s">
-        <v>3790</v>
+        <v>3802</v>
       </c>
       <c r="C1697" t="s">
-        <v>3786</v>
+        <v>3803</v>
       </c>
       <c r="D1697" t="s">
-        <v>14</v>
+        <v>405</v>
+      </c>
+      <c r="E1697" t="s">
+        <v>1187</v>
+      </c>
+      <c r="F1697" t="s">
+        <v>3804</v>
       </c>
       <c r="H1697" t="s">
-        <v>336</v>
+        <v>71</v>
       </c>
       <c r="M1697" t="s">
-        <v>3791</v>
+        <v>3805</v>
       </c>
     </row>
     <row r="1698" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1698">
-        <v>1862</v>
+        <v>1867</v>
       </c>
       <c r="B1698" t="s">
-        <v>3792</v>
+        <v>3806</v>
       </c>
       <c r="C1698" t="s">
-        <v>3786</v>
+        <v>3807</v>
       </c>
       <c r="D1698" t="s">
-        <v>14</v>
+        <v>473</v>
       </c>
       <c r="H1698" t="s">
-        <v>336</v>
+        <v>2939</v>
       </c>
       <c r="M1698" t="s">
-        <v>3793</v>
+        <v>3808</v>
       </c>
     </row>
     <row r="1699" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1699">
-        <v>1863</v>
+        <v>1868</v>
       </c>
       <c r="B1699" t="s">
-        <v>3794</v>
+        <v>3809</v>
       </c>
       <c r="C1699" t="s">
-        <v>3795</v>
+        <v>3810</v>
       </c>
       <c r="D1699" t="s">
-        <v>405</v>
-      </c>
-      <c r="E1699" t="s">
-        <v>1187</v>
-      </c>
-      <c r="H1699" t="s">
-        <v>71</v>
+        <v>473</v>
       </c>
       <c r="M1699" t="s">
-        <v>3796</v>
+        <v>3811</v>
       </c>
     </row>
     <row r="1700" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1700">
-        <v>1864</v>
+        <v>1869</v>
       </c>
       <c r="B1700" t="s">
-        <v>3797</v>
+        <v>3812</v>
       </c>
       <c r="C1700" t="s">
-        <v>3795</v>
+        <v>3810</v>
       </c>
       <c r="D1700" t="s">
-        <v>405</v>
-      </c>
-      <c r="E1700" t="s">
-        <v>1187</v>
-      </c>
-      <c r="H1700" t="s">
-        <v>71</v>
+        <v>473</v>
       </c>
       <c r="M1700" t="s">
-        <v>3798</v>
+        <v>3813</v>
       </c>
     </row>
     <row r="1701" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1701">
-        <v>1866</v>
+        <v>1870</v>
       </c>
       <c r="B1701" t="s">
-        <v>3802</v>
+        <v>3814</v>
       </c>
       <c r="C1701" t="s">
-        <v>3803</v>
-      </c>
-      <c r="D1701" t="s">
-        <v>405</v>
-      </c>
-      <c r="E1701" t="s">
-        <v>1187</v>
-      </c>
-      <c r="F1701" t="s">
-        <v>3804</v>
-      </c>
-      <c r="H1701" t="s">
-        <v>71</v>
+        <v>3815</v>
+      </c>
+      <c r="D1701">
+        <v>8080</v>
       </c>
       <c r="M1701" t="s">
-        <v>3805</v>
+        <v>3816</v>
       </c>
     </row>
     <row r="1702" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1702">
-        <v>1867</v>
+        <v>1871</v>
       </c>
       <c r="B1702" t="s">
-        <v>3806</v>
+        <v>3817</v>
       </c>
       <c r="C1702" t="s">
-        <v>3807</v>
+        <v>3818</v>
       </c>
       <c r="D1702" t="s">
-        <v>473</v>
+        <v>3439</v>
+      </c>
+      <c r="E1702" t="s">
+        <v>3439</v>
+      </c>
+      <c r="F1702" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G1702" t="s">
+        <v>1187</v>
       </c>
       <c r="H1702" t="s">
-        <v>2939</v>
+        <v>333</v>
+      </c>
+      <c r="I1702" t="s">
+        <v>551</v>
       </c>
       <c r="M1702" t="s">
-        <v>3808</v>
+        <v>3819</v>
       </c>
     </row>
     <row r="1703" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1703">
-        <v>1868</v>
+        <v>1872</v>
       </c>
       <c r="B1703" t="s">
-        <v>3809</v>
+        <v>3820</v>
       </c>
       <c r="C1703" t="s">
-        <v>3810</v>
+        <v>3821</v>
       </c>
       <c r="D1703" t="s">
-        <v>473</v>
+        <v>14</v>
+      </c>
+      <c r="H1703" t="s">
+        <v>172</v>
       </c>
       <c r="M1703" t="s">
-        <v>3811</v>
+        <v>3822</v>
       </c>
     </row>
     <row r="1704" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1704">
-        <v>1869</v>
+        <v>1873</v>
       </c>
       <c r="B1704" t="s">
-        <v>3812</v>
+        <v>3823</v>
       </c>
       <c r="C1704" t="s">
-        <v>3810</v>
+        <v>3824</v>
       </c>
       <c r="D1704" t="s">
-        <v>473</v>
+        <v>14</v>
+      </c>
+      <c r="E1704" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1704" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1704" t="s">
+        <v>154</v>
+      </c>
+      <c r="H1704" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1704" t="s">
+        <v>166</v>
       </c>
       <c r="M1704" t="s">
-        <v>3813</v>
+        <v>3825</v>
       </c>
     </row>
     <row r="1705" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1705">
-        <v>1870</v>
+        <v>1874</v>
       </c>
       <c r="B1705" t="s">
-        <v>3814</v>
+        <v>3826</v>
       </c>
       <c r="C1705" t="s">
-        <v>3815</v>
-      </c>
-      <c r="D1705">
-        <v>8080</v>
+        <v>3824</v>
+      </c>
+      <c r="D1705" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1705" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1705" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1705" t="s">
+        <v>154</v>
+      </c>
+      <c r="H1705" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1705" t="s">
+        <v>166</v>
       </c>
       <c r="M1705" t="s">
-        <v>3816</v>
+        <v>3827</v>
       </c>
     </row>
     <row r="1706" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1706">
-        <v>1871</v>
+        <v>1875</v>
       </c>
       <c r="B1706" t="s">
-        <v>3817</v>
+        <v>3828</v>
       </c>
       <c r="C1706" t="s">
-        <v>3818</v>
+        <v>3824</v>
       </c>
       <c r="D1706" t="s">
-        <v>3439</v>
+        <v>14</v>
       </c>
       <c r="E1706" t="s">
-        <v>3439</v>
+        <v>14</v>
       </c>
       <c r="F1706" t="s">
-        <v>1187</v>
+        <v>14</v>
       </c>
       <c r="G1706" t="s">
-        <v>1187</v>
+        <v>154</v>
       </c>
       <c r="H1706" t="s">
-        <v>333</v>
+        <v>71</v>
       </c>
       <c r="I1706" t="s">
-        <v>551</v>
+        <v>166</v>
       </c>
       <c r="M1706" t="s">
-        <v>3819</v>
+        <v>3829</v>
       </c>
     </row>
     <row r="1707" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1707">
-        <v>1872</v>
+        <v>1876</v>
       </c>
       <c r="B1707" t="s">
-        <v>3820</v>
+        <v>3830</v>
       </c>
       <c r="C1707" t="s">
-        <v>3821</v>
+        <v>3824</v>
       </c>
       <c r="D1707" t="s">
         <v>14</v>
       </c>
+      <c r="E1707" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1707" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1707" t="s">
+        <v>154</v>
+      </c>
       <c r="H1707" t="s">
-        <v>172</v>
+        <v>71</v>
+      </c>
+      <c r="I1707" t="s">
+        <v>166</v>
       </c>
       <c r="M1707" t="s">
-        <v>3822</v>
+        <v>3831</v>
       </c>
     </row>
     <row r="1708" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1708">
-        <v>1873</v>
+        <v>1877</v>
       </c>
       <c r="B1708" t="s">
-        <v>3823</v>
+        <v>3832</v>
       </c>
       <c r="C1708" t="s">
-        <v>3824</v>
-      </c>
-      <c r="D1708" t="s">
-        <v>14</v>
+        <v>3833</v>
+      </c>
+      <c r="D1708">
+        <v>68000</v>
       </c>
       <c r="E1708" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1708" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1708" t="s">
         <v>154</v>
       </c>
       <c r="H1708" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1708" t="s">
-        <v>166</v>
+        <v>1495</v>
       </c>
       <c r="M1708" t="s">
-        <v>3825</v>
+        <v>3834</v>
       </c>
     </row>
     <row r="1709" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1709">
-        <v>1874</v>
+        <v>1878</v>
       </c>
       <c r="B1709" t="s">
-        <v>3826</v>
+        <v>3835</v>
       </c>
       <c r="C1709" t="s">
-        <v>3824</v>
+        <v>3836</v>
       </c>
       <c r="D1709" t="s">
         <v>14</v>
@@ -60637,31 +60756,25 @@
       <c r="E1709" t="s">
         <v>14</v>
       </c>
-      <c r="F1709" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1709" t="s">
-        <v>154</v>
-      </c>
       <c r="H1709" t="s">
-        <v>71</v>
+        <v>1239</v>
       </c>
       <c r="I1709" t="s">
-        <v>166</v>
+        <v>333</v>
       </c>
       <c r="M1709" t="s">
-        <v>3827</v>
+        <v>3837</v>
       </c>
     </row>
     <row r="1710" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1710">
-        <v>1875</v>
+        <v>1879</v>
       </c>
       <c r="B1710" t="s">
-        <v>3828</v>
+        <v>3838</v>
       </c>
       <c r="C1710" t="s">
-        <v>3824</v>
+        <v>3836</v>
       </c>
       <c r="D1710" t="s">
         <v>14</v>
@@ -60669,43 +60782,31 @@
       <c r="E1710" t="s">
         <v>14</v>
       </c>
-      <c r="F1710" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1710" t="s">
-        <v>154</v>
-      </c>
       <c r="H1710" t="s">
-        <v>71</v>
+        <v>1239</v>
       </c>
       <c r="I1710" t="s">
-        <v>166</v>
+        <v>333</v>
       </c>
       <c r="M1710" t="s">
-        <v>3829</v>
+        <v>4494</v>
       </c>
     </row>
     <row r="1711" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1711">
-        <v>1876</v>
+        <v>1880</v>
       </c>
       <c r="B1711" t="s">
-        <v>3830</v>
+        <v>3839</v>
       </c>
       <c r="C1711" t="s">
-        <v>3824</v>
+        <v>3836</v>
       </c>
       <c r="D1711" t="s">
         <v>14</v>
       </c>
       <c r="E1711" t="s">
         <v>14</v>
-      </c>
-      <c r="F1711" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1711" t="s">
-        <v>154</v>
       </c>
       <c r="H1711" t="s">
         <v>71</v>
@@ -60714,41 +60815,44 @@
         <v>166</v>
       </c>
       <c r="M1711" t="s">
-        <v>3831</v>
+        <v>4495</v>
       </c>
     </row>
     <row r="1712" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1712">
-        <v>1877</v>
+        <v>1881</v>
       </c>
       <c r="B1712" t="s">
-        <v>3832</v>
+        <v>3840</v>
       </c>
       <c r="C1712" t="s">
-        <v>3833</v>
-      </c>
-      <c r="D1712">
-        <v>68000</v>
+        <v>3836</v>
+      </c>
+      <c r="D1712" t="s">
+        <v>14</v>
       </c>
       <c r="E1712" t="s">
-        <v>154</v>
+        <v>14</v>
       </c>
       <c r="H1712" t="s">
-        <v>1495</v>
+        <v>1239</v>
+      </c>
+      <c r="I1712" t="s">
+        <v>333</v>
       </c>
       <c r="M1712" t="s">
-        <v>3834</v>
+        <v>3841</v>
       </c>
     </row>
     <row r="1713" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1713">
-        <v>1878</v>
+        <v>1882</v>
       </c>
       <c r="B1713" t="s">
-        <v>3835</v>
+        <v>3842</v>
       </c>
       <c r="C1713" t="s">
-        <v>3836</v>
+        <v>3843</v>
       </c>
       <c r="D1713" t="s">
         <v>14</v>
@@ -60757,125 +60861,104 @@
         <v>14</v>
       </c>
       <c r="H1713" t="s">
-        <v>1239</v>
-      </c>
-      <c r="I1713" t="s">
-        <v>333</v>
+        <v>349</v>
       </c>
       <c r="M1713" t="s">
-        <v>3837</v>
+        <v>3844</v>
       </c>
     </row>
     <row r="1714" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1714">
-        <v>1879</v>
+        <v>1883</v>
       </c>
       <c r="B1714" t="s">
-        <v>3838</v>
+        <v>3845</v>
       </c>
       <c r="C1714" t="s">
-        <v>3836</v>
+        <v>3846</v>
       </c>
       <c r="D1714" t="s">
         <v>14</v>
       </c>
       <c r="E1714" t="s">
-        <v>14</v>
+        <v>154</v>
       </c>
       <c r="H1714" t="s">
-        <v>1239</v>
-      </c>
-      <c r="I1714" t="s">
-        <v>333</v>
+        <v>349</v>
       </c>
       <c r="M1714" t="s">
-        <v>4494</v>
+        <v>3847</v>
       </c>
     </row>
     <row r="1715" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1715">
-        <v>1880</v>
+        <v>1884</v>
       </c>
       <c r="B1715" t="s">
-        <v>3839</v>
+        <v>3848</v>
       </c>
       <c r="C1715" t="s">
-        <v>3836</v>
+        <v>3849</v>
       </c>
       <c r="D1715" t="s">
         <v>14</v>
       </c>
-      <c r="E1715" t="s">
-        <v>14</v>
-      </c>
       <c r="H1715" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1715" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="M1715" t="s">
-        <v>4495</v>
+        <v>3850</v>
       </c>
     </row>
     <row r="1716" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1716">
-        <v>1881</v>
+        <v>1885</v>
       </c>
       <c r="B1716" t="s">
-        <v>3840</v>
+        <v>3851</v>
       </c>
       <c r="C1716" t="s">
-        <v>3836</v>
-      </c>
-      <c r="D1716" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1716" t="s">
-        <v>14</v>
+        <v>3852</v>
+      </c>
+      <c r="D1716">
+        <v>8080</v>
       </c>
       <c r="H1716" t="s">
-        <v>1239</v>
-      </c>
-      <c r="I1716" t="s">
-        <v>333</v>
+        <v>406</v>
       </c>
       <c r="M1716" t="s">
-        <v>3841</v>
+        <v>3853</v>
       </c>
     </row>
     <row r="1717" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1717">
-        <v>1882</v>
+        <v>1886</v>
       </c>
       <c r="B1717" t="s">
-        <v>3842</v>
+        <v>3854</v>
       </c>
       <c r="C1717" t="s">
-        <v>3843</v>
+        <v>3855</v>
       </c>
       <c r="D1717" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1717" t="s">
-        <v>14</v>
+        <v>1108</v>
       </c>
       <c r="H1717" t="s">
-        <v>349</v>
+        <v>336</v>
       </c>
       <c r="M1717" t="s">
-        <v>3844</v>
+        <v>3856</v>
       </c>
     </row>
     <row r="1718" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1718">
-        <v>1883</v>
+        <v>1887</v>
       </c>
       <c r="B1718" t="s">
-        <v>3845</v>
+        <v>3857</v>
       </c>
       <c r="C1718" t="s">
-        <v>3846</v>
+        <v>3858</v>
       </c>
       <c r="D1718" t="s">
         <v>14</v>
@@ -60884,170 +60967,170 @@
         <v>154</v>
       </c>
       <c r="H1718" t="s">
-        <v>349</v>
+        <v>336</v>
       </c>
       <c r="M1718" t="s">
-        <v>3847</v>
+        <v>3859</v>
       </c>
     </row>
     <row r="1719" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1719">
-        <v>1884</v>
+        <v>1888</v>
       </c>
       <c r="B1719" t="s">
-        <v>3848</v>
+        <v>3860</v>
       </c>
       <c r="C1719" t="s">
-        <v>3849</v>
+        <v>3858</v>
       </c>
       <c r="D1719" t="s">
         <v>14</v>
       </c>
+      <c r="E1719" t="s">
+        <v>154</v>
+      </c>
       <c r="H1719" t="s">
-        <v>172</v>
+        <v>336</v>
       </c>
       <c r="M1719" t="s">
-        <v>3850</v>
+        <v>3861</v>
       </c>
     </row>
     <row r="1720" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1720">
-        <v>1885</v>
+        <v>1889</v>
       </c>
       <c r="B1720" t="s">
-        <v>3851</v>
+        <v>3862</v>
       </c>
       <c r="C1720" t="s">
-        <v>3852</v>
-      </c>
-      <c r="D1720">
-        <v>8080</v>
+        <v>3863</v>
+      </c>
+      <c r="D1720" t="s">
+        <v>3864</v>
+      </c>
+      <c r="E1720" t="s">
+        <v>728</v>
       </c>
       <c r="H1720" t="s">
-        <v>406</v>
+        <v>2073</v>
       </c>
       <c r="M1720" t="s">
-        <v>3853</v>
+        <v>3865</v>
       </c>
     </row>
     <row r="1721" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1721">
-        <v>1886</v>
+        <v>1890</v>
       </c>
       <c r="B1721" t="s">
-        <v>3854</v>
+        <v>3866</v>
       </c>
       <c r="C1721" t="s">
-        <v>3855</v>
-      </c>
-      <c r="D1721" t="s">
-        <v>1108</v>
+        <v>3867</v>
+      </c>
+      <c r="D1721">
+        <v>68000</v>
       </c>
       <c r="H1721" t="s">
-        <v>336</v>
+        <v>2378</v>
       </c>
       <c r="M1721" t="s">
-        <v>3856</v>
+        <v>3868</v>
       </c>
     </row>
     <row r="1722" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1722">
-        <v>1887</v>
+        <v>1891</v>
       </c>
       <c r="B1722" t="s">
-        <v>3857</v>
+        <v>3869</v>
       </c>
       <c r="C1722" t="s">
-        <v>3858</v>
-      </c>
-      <c r="D1722" t="s">
-        <v>14</v>
+        <v>3870</v>
+      </c>
+      <c r="D1722">
+        <v>68000</v>
       </c>
       <c r="E1722" t="s">
         <v>154</v>
       </c>
       <c r="H1722" t="s">
-        <v>336</v>
+        <v>1239</v>
       </c>
       <c r="M1722" t="s">
-        <v>3859</v>
+        <v>3871</v>
       </c>
     </row>
     <row r="1723" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1723">
-        <v>1888</v>
+        <v>1892</v>
       </c>
       <c r="B1723" t="s">
-        <v>3860</v>
+        <v>3872</v>
       </c>
       <c r="C1723" t="s">
-        <v>3858</v>
+        <v>3873</v>
       </c>
       <c r="D1723" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1723" t="s">
-        <v>154</v>
+        <v>405</v>
       </c>
       <c r="H1723" t="s">
-        <v>336</v>
+        <v>71</v>
       </c>
       <c r="M1723" t="s">
-        <v>3861</v>
+        <v>3874</v>
       </c>
     </row>
     <row r="1724" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1724">
-        <v>1889</v>
+        <v>1893</v>
       </c>
       <c r="B1724" t="s">
-        <v>3862</v>
+        <v>3875</v>
       </c>
       <c r="C1724" t="s">
-        <v>3863</v>
+        <v>3876</v>
       </c>
       <c r="D1724" t="s">
-        <v>3864</v>
-      </c>
-      <c r="E1724" t="s">
-        <v>728</v>
-      </c>
-      <c r="H1724" t="s">
-        <v>2073</v>
+        <v>14</v>
       </c>
       <c r="M1724" t="s">
-        <v>3865</v>
+        <v>4496</v>
       </c>
     </row>
     <row r="1725" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1725">
-        <v>1890</v>
+        <v>1894</v>
       </c>
       <c r="B1725" t="s">
-        <v>3866</v>
+        <v>3877</v>
       </c>
       <c r="C1725" t="s">
-        <v>3867</v>
+        <v>3878</v>
       </c>
       <c r="D1725">
         <v>68000</v>
       </c>
+      <c r="E1725" t="s">
+        <v>154</v>
+      </c>
       <c r="H1725" t="s">
-        <v>2378</v>
+        <v>1356</v>
       </c>
       <c r="M1725" t="s">
-        <v>3868</v>
+        <v>3879</v>
       </c>
     </row>
     <row r="1726" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1726">
-        <v>1891</v>
+        <v>1895</v>
       </c>
       <c r="B1726" t="s">
-        <v>3869</v>
+        <v>3880</v>
       </c>
       <c r="C1726" t="s">
-        <v>3870</v>
+        <v>3878</v>
       </c>
       <c r="D1726">
         <v>68000</v>
@@ -61056,55 +61139,64 @@
         <v>154</v>
       </c>
       <c r="H1726" t="s">
-        <v>1239</v>
+        <v>1356</v>
       </c>
       <c r="M1726" t="s">
-        <v>3871</v>
+        <v>4497</v>
       </c>
     </row>
     <row r="1727" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1727">
-        <v>1892</v>
+        <v>1896</v>
       </c>
       <c r="B1727" t="s">
-        <v>3872</v>
+        <v>3881</v>
       </c>
       <c r="C1727" t="s">
-        <v>3873</v>
-      </c>
-      <c r="D1727" t="s">
-        <v>405</v>
+        <v>3878</v>
+      </c>
+      <c r="D1727">
+        <v>68000</v>
+      </c>
+      <c r="E1727" t="s">
+        <v>154</v>
       </c>
       <c r="H1727" t="s">
-        <v>71</v>
+        <v>1356</v>
       </c>
       <c r="M1727" t="s">
-        <v>3874</v>
+        <v>3882</v>
       </c>
     </row>
     <row r="1728" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1728">
-        <v>1893</v>
+        <v>1897</v>
       </c>
       <c r="B1728" t="s">
-        <v>3875</v>
+        <v>3883</v>
       </c>
       <c r="C1728" t="s">
-        <v>3876</v>
-      </c>
-      <c r="D1728" t="s">
-        <v>14</v>
+        <v>3878</v>
+      </c>
+      <c r="D1728">
+        <v>68000</v>
+      </c>
+      <c r="E1728" t="s">
+        <v>154</v>
+      </c>
+      <c r="H1728" t="s">
+        <v>1356</v>
       </c>
       <c r="M1728" t="s">
-        <v>4496</v>
+        <v>3884</v>
       </c>
     </row>
     <row r="1729" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1729">
-        <v>1894</v>
+        <v>1898</v>
       </c>
       <c r="B1729" t="s">
-        <v>3877</v>
+        <v>3885</v>
       </c>
       <c r="C1729" t="s">
         <v>3878</v>
@@ -61119,15 +61211,15 @@
         <v>1356</v>
       </c>
       <c r="M1729" t="s">
-        <v>3879</v>
+        <v>3886</v>
       </c>
     </row>
     <row r="1730" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1730">
-        <v>1895</v>
+        <v>1899</v>
       </c>
       <c r="B1730" t="s">
-        <v>3880</v>
+        <v>3887</v>
       </c>
       <c r="C1730" t="s">
         <v>3878</v>
@@ -61142,15 +61234,15 @@
         <v>1356</v>
       </c>
       <c r="M1730" t="s">
-        <v>4497</v>
+        <v>3888</v>
       </c>
     </row>
     <row r="1731" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1731">
-        <v>1896</v>
+        <v>1900</v>
       </c>
       <c r="B1731" t="s">
-        <v>3881</v>
+        <v>3889</v>
       </c>
       <c r="C1731" t="s">
         <v>3878</v>
@@ -61165,15 +61257,15 @@
         <v>1356</v>
       </c>
       <c r="M1731" t="s">
-        <v>3882</v>
+        <v>3890</v>
       </c>
     </row>
     <row r="1732" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1732">
-        <v>1897</v>
+        <v>1901</v>
       </c>
       <c r="B1732" t="s">
-        <v>3883</v>
+        <v>3891</v>
       </c>
       <c r="C1732" t="s">
         <v>3878</v>
@@ -61188,15 +61280,15 @@
         <v>1356</v>
       </c>
       <c r="M1732" t="s">
-        <v>3884</v>
+        <v>4498</v>
       </c>
     </row>
     <row r="1733" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1733">
-        <v>1898</v>
+        <v>1902</v>
       </c>
       <c r="B1733" t="s">
-        <v>3885</v>
+        <v>3892</v>
       </c>
       <c r="C1733" t="s">
         <v>3878</v>
@@ -61211,15 +61303,15 @@
         <v>1356</v>
       </c>
       <c r="M1733" t="s">
-        <v>3886</v>
+        <v>3893</v>
       </c>
     </row>
     <row r="1734" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1734">
-        <v>1899</v>
+        <v>1903</v>
       </c>
       <c r="B1734" t="s">
-        <v>3887</v>
+        <v>3894</v>
       </c>
       <c r="C1734" t="s">
         <v>3878</v>
@@ -61234,15 +61326,15 @@
         <v>1356</v>
       </c>
       <c r="M1734" t="s">
-        <v>3888</v>
+        <v>3895</v>
       </c>
     </row>
     <row r="1735" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1735">
-        <v>1900</v>
+        <v>1904</v>
       </c>
       <c r="B1735" t="s">
-        <v>3889</v>
+        <v>3896</v>
       </c>
       <c r="C1735" t="s">
         <v>3878</v>
@@ -61257,15 +61349,15 @@
         <v>1356</v>
       </c>
       <c r="M1735" t="s">
-        <v>3890</v>
+        <v>3897</v>
       </c>
     </row>
     <row r="1736" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1736">
-        <v>1901</v>
+        <v>1905</v>
       </c>
       <c r="B1736" t="s">
-        <v>3891</v>
+        <v>3898</v>
       </c>
       <c r="C1736" t="s">
         <v>3878</v>
@@ -61280,15 +61372,15 @@
         <v>1356</v>
       </c>
       <c r="M1736" t="s">
-        <v>4498</v>
+        <v>3899</v>
       </c>
     </row>
     <row r="1737" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1737">
-        <v>1902</v>
+        <v>1906</v>
       </c>
       <c r="B1737" t="s">
-        <v>3892</v>
+        <v>3900</v>
       </c>
       <c r="C1737" t="s">
         <v>3878</v>
@@ -61303,15 +61395,15 @@
         <v>1356</v>
       </c>
       <c r="M1737" t="s">
-        <v>3893</v>
+        <v>3901</v>
       </c>
     </row>
     <row r="1738" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1738">
-        <v>1903</v>
+        <v>1907</v>
       </c>
       <c r="B1738" t="s">
-        <v>3894</v>
+        <v>3902</v>
       </c>
       <c r="C1738" t="s">
         <v>3878</v>
@@ -61326,15 +61418,15 @@
         <v>1356</v>
       </c>
       <c r="M1738" t="s">
-        <v>3895</v>
+        <v>4499</v>
       </c>
     </row>
     <row r="1739" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1739">
-        <v>1904</v>
+        <v>1908</v>
       </c>
       <c r="B1739" t="s">
-        <v>3896</v>
+        <v>3903</v>
       </c>
       <c r="C1739" t="s">
         <v>3878</v>
@@ -61349,15 +61441,15 @@
         <v>1356</v>
       </c>
       <c r="M1739" t="s">
-        <v>3897</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="1740" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1740">
-        <v>1905</v>
+        <v>1909</v>
       </c>
       <c r="B1740" t="s">
-        <v>3898</v>
+        <v>3904</v>
       </c>
       <c r="C1740" t="s">
         <v>3878</v>
@@ -61372,15 +61464,15 @@
         <v>1356</v>
       </c>
       <c r="M1740" t="s">
-        <v>3899</v>
+        <v>3905</v>
       </c>
     </row>
     <row r="1741" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1741">
-        <v>1906</v>
+        <v>1910</v>
       </c>
       <c r="B1741" t="s">
-        <v>3900</v>
+        <v>3906</v>
       </c>
       <c r="C1741" t="s">
         <v>3878</v>
@@ -61395,15 +61487,15 @@
         <v>1356</v>
       </c>
       <c r="M1741" t="s">
-        <v>3901</v>
+        <v>3907</v>
       </c>
     </row>
     <row r="1742" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1742">
-        <v>1907</v>
+        <v>1911</v>
       </c>
       <c r="B1742" t="s">
-        <v>3902</v>
+        <v>3908</v>
       </c>
       <c r="C1742" t="s">
         <v>3878</v>
@@ -61418,15 +61510,15 @@
         <v>1356</v>
       </c>
       <c r="M1742" t="s">
-        <v>4499</v>
+        <v>3909</v>
       </c>
     </row>
     <row r="1743" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1743">
-        <v>1908</v>
+        <v>1912</v>
       </c>
       <c r="B1743" t="s">
-        <v>3903</v>
+        <v>3910</v>
       </c>
       <c r="C1743" t="s">
         <v>3878</v>
@@ -61441,15 +61533,15 @@
         <v>1356</v>
       </c>
       <c r="M1743" t="s">
-        <v>4500</v>
+        <v>3911</v>
       </c>
     </row>
     <row r="1744" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1744">
-        <v>1909</v>
+        <v>1913</v>
       </c>
       <c r="B1744" t="s">
-        <v>3904</v>
+        <v>3912</v>
       </c>
       <c r="C1744" t="s">
         <v>3878</v>
@@ -61464,15 +61556,15 @@
         <v>1356</v>
       </c>
       <c r="M1744" t="s">
-        <v>3905</v>
+        <v>3913</v>
       </c>
     </row>
     <row r="1745" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1745">
-        <v>1910</v>
+        <v>1914</v>
       </c>
       <c r="B1745" t="s">
-        <v>3906</v>
+        <v>3914</v>
       </c>
       <c r="C1745" t="s">
         <v>3878</v>
@@ -61487,15 +61579,15 @@
         <v>1356</v>
       </c>
       <c r="M1745" t="s">
-        <v>3907</v>
+        <v>3915</v>
       </c>
     </row>
     <row r="1746" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1746">
-        <v>1911</v>
+        <v>1915</v>
       </c>
       <c r="B1746" t="s">
-        <v>3908</v>
+        <v>3916</v>
       </c>
       <c r="C1746" t="s">
         <v>3878</v>
@@ -61510,15 +61602,15 @@
         <v>1356</v>
       </c>
       <c r="M1746" t="s">
-        <v>3909</v>
+        <v>4501</v>
       </c>
     </row>
     <row r="1747" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1747">
-        <v>1912</v>
+        <v>1916</v>
       </c>
       <c r="B1747" t="s">
-        <v>3910</v>
+        <v>3917</v>
       </c>
       <c r="C1747" t="s">
         <v>3878</v>
@@ -61533,15 +61625,15 @@
         <v>1356</v>
       </c>
       <c r="M1747" t="s">
-        <v>3911</v>
+        <v>3918</v>
       </c>
     </row>
     <row r="1748" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1748">
-        <v>1913</v>
+        <v>1917</v>
       </c>
       <c r="B1748" t="s">
-        <v>3912</v>
+        <v>3919</v>
       </c>
       <c r="C1748" t="s">
         <v>3878</v>
@@ -61556,15 +61648,15 @@
         <v>1356</v>
       </c>
       <c r="M1748" t="s">
-        <v>3913</v>
+        <v>3920</v>
       </c>
     </row>
     <row r="1749" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1749">
-        <v>1914</v>
+        <v>1918</v>
       </c>
       <c r="B1749" t="s">
-        <v>3914</v>
+        <v>3921</v>
       </c>
       <c r="C1749" t="s">
         <v>3878</v>
@@ -61579,15 +61671,15 @@
         <v>1356</v>
       </c>
       <c r="M1749" t="s">
-        <v>3915</v>
+        <v>3922</v>
       </c>
     </row>
     <row r="1750" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1750">
-        <v>1915</v>
+        <v>1919</v>
       </c>
       <c r="B1750" t="s">
-        <v>3916</v>
+        <v>3923</v>
       </c>
       <c r="C1750" t="s">
         <v>3878</v>
@@ -61602,15 +61694,15 @@
         <v>1356</v>
       </c>
       <c r="M1750" t="s">
-        <v>4501</v>
+        <v>4502</v>
       </c>
     </row>
     <row r="1751" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1751">
-        <v>1916</v>
+        <v>1920</v>
       </c>
       <c r="B1751" t="s">
-        <v>3917</v>
+        <v>3924</v>
       </c>
       <c r="C1751" t="s">
         <v>3878</v>
@@ -61625,15 +61717,15 @@
         <v>1356</v>
       </c>
       <c r="M1751" t="s">
-        <v>3918</v>
+        <v>4503</v>
       </c>
     </row>
     <row r="1752" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1752">
-        <v>1917</v>
+        <v>1921</v>
       </c>
       <c r="B1752" t="s">
-        <v>3919</v>
+        <v>3925</v>
       </c>
       <c r="C1752" t="s">
         <v>3878</v>
@@ -61648,15 +61740,15 @@
         <v>1356</v>
       </c>
       <c r="M1752" t="s">
-        <v>3920</v>
+        <v>4504</v>
       </c>
     </row>
     <row r="1753" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1753">
-        <v>1918</v>
+        <v>1922</v>
       </c>
       <c r="B1753" t="s">
-        <v>3921</v>
+        <v>3926</v>
       </c>
       <c r="C1753" t="s">
         <v>3878</v>
@@ -61671,15 +61763,15 @@
         <v>1356</v>
       </c>
       <c r="M1753" t="s">
-        <v>3922</v>
+        <v>3927</v>
       </c>
     </row>
     <row r="1754" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1754">
-        <v>1919</v>
+        <v>1923</v>
       </c>
       <c r="B1754" t="s">
-        <v>3923</v>
+        <v>3928</v>
       </c>
       <c r="C1754" t="s">
         <v>3878</v>
@@ -61694,15 +61786,15 @@
         <v>1356</v>
       </c>
       <c r="M1754" t="s">
-        <v>4502</v>
+        <v>3929</v>
       </c>
     </row>
     <row r="1755" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1755">
-        <v>1920</v>
+        <v>1924</v>
       </c>
       <c r="B1755" t="s">
-        <v>3924</v>
+        <v>3930</v>
       </c>
       <c r="C1755" t="s">
         <v>3878</v>
@@ -61717,15 +61809,15 @@
         <v>1356</v>
       </c>
       <c r="M1755" t="s">
-        <v>4503</v>
+        <v>4505</v>
       </c>
     </row>
     <row r="1756" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1756">
-        <v>1921</v>
+        <v>1925</v>
       </c>
       <c r="B1756" t="s">
-        <v>3925</v>
+        <v>3931</v>
       </c>
       <c r="C1756" t="s">
         <v>3878</v>
@@ -61740,15 +61832,15 @@
         <v>1356</v>
       </c>
       <c r="M1756" t="s">
-        <v>4504</v>
+        <v>3932</v>
       </c>
     </row>
     <row r="1757" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1757">
-        <v>1922</v>
+        <v>1926</v>
       </c>
       <c r="B1757" t="s">
-        <v>3926</v>
+        <v>3933</v>
       </c>
       <c r="C1757" t="s">
         <v>3878</v>
@@ -61763,15 +61855,15 @@
         <v>1356</v>
       </c>
       <c r="M1757" t="s">
-        <v>3927</v>
+        <v>4506</v>
       </c>
     </row>
     <row r="1758" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1758">
-        <v>1923</v>
+        <v>1927</v>
       </c>
       <c r="B1758" t="s">
-        <v>3928</v>
+        <v>3934</v>
       </c>
       <c r="C1758" t="s">
         <v>3878</v>
@@ -61786,15 +61878,15 @@
         <v>1356</v>
       </c>
       <c r="M1758" t="s">
-        <v>3929</v>
+        <v>3935</v>
       </c>
     </row>
     <row r="1759" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1759">
-        <v>1924</v>
+        <v>1928</v>
       </c>
       <c r="B1759" t="s">
-        <v>3930</v>
+        <v>3936</v>
       </c>
       <c r="C1759" t="s">
         <v>3878</v>
@@ -61809,15 +61901,15 @@
         <v>1356</v>
       </c>
       <c r="M1759" t="s">
-        <v>4505</v>
+        <v>3937</v>
       </c>
     </row>
     <row r="1760" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1760">
-        <v>1925</v>
+        <v>1929</v>
       </c>
       <c r="B1760" t="s">
-        <v>3931</v>
+        <v>3938</v>
       </c>
       <c r="C1760" t="s">
         <v>3878</v>
@@ -61832,15 +61924,15 @@
         <v>1356</v>
       </c>
       <c r="M1760" t="s">
-        <v>3932</v>
+        <v>4507</v>
       </c>
     </row>
     <row r="1761" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1761">
-        <v>1926</v>
+        <v>1930</v>
       </c>
       <c r="B1761" t="s">
-        <v>3933</v>
+        <v>3939</v>
       </c>
       <c r="C1761" t="s">
         <v>3878</v>
@@ -61855,15 +61947,15 @@
         <v>1356</v>
       </c>
       <c r="M1761" t="s">
-        <v>4506</v>
+        <v>4508</v>
       </c>
     </row>
     <row r="1762" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1762">
-        <v>1927</v>
+        <v>1931</v>
       </c>
       <c r="B1762" t="s">
-        <v>3934</v>
+        <v>3940</v>
       </c>
       <c r="C1762" t="s">
         <v>3878</v>
@@ -61878,15 +61970,15 @@
         <v>1356</v>
       </c>
       <c r="M1762" t="s">
-        <v>3935</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="1763" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1763">
-        <v>1928</v>
+        <v>1932</v>
       </c>
       <c r="B1763" t="s">
-        <v>3936</v>
+        <v>3942</v>
       </c>
       <c r="C1763" t="s">
         <v>3878</v>
@@ -61901,15 +61993,15 @@
         <v>1356</v>
       </c>
       <c r="M1763" t="s">
-        <v>3937</v>
+        <v>4509</v>
       </c>
     </row>
     <row r="1764" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1764">
-        <v>1929</v>
+        <v>1933</v>
       </c>
       <c r="B1764" t="s">
-        <v>3938</v>
+        <v>3943</v>
       </c>
       <c r="C1764" t="s">
         <v>3878</v>
@@ -61924,15 +62016,15 @@
         <v>1356</v>
       </c>
       <c r="M1764" t="s">
-        <v>4507</v>
+        <v>4510</v>
       </c>
     </row>
     <row r="1765" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1765">
-        <v>1930</v>
+        <v>1934</v>
       </c>
       <c r="B1765" t="s">
-        <v>3939</v>
+        <v>3944</v>
       </c>
       <c r="C1765" t="s">
         <v>3878</v>
@@ -61947,15 +62039,15 @@
         <v>1356</v>
       </c>
       <c r="M1765" t="s">
-        <v>4508</v>
+        <v>4511</v>
       </c>
     </row>
     <row r="1766" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1766">
-        <v>1931</v>
+        <v>1935</v>
       </c>
       <c r="B1766" t="s">
-        <v>3940</v>
+        <v>3945</v>
       </c>
       <c r="C1766" t="s">
         <v>3878</v>
@@ -61970,15 +62062,15 @@
         <v>1356</v>
       </c>
       <c r="M1766" t="s">
-        <v>3941</v>
+        <v>4512</v>
       </c>
     </row>
     <row r="1767" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1767">
-        <v>1932</v>
+        <v>1936</v>
       </c>
       <c r="B1767" t="s">
-        <v>3942</v>
+        <v>3946</v>
       </c>
       <c r="C1767" t="s">
         <v>3878</v>
@@ -61993,15 +62085,15 @@
         <v>1356</v>
       </c>
       <c r="M1767" t="s">
-        <v>4509</v>
+        <v>4513</v>
       </c>
     </row>
     <row r="1768" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1768">
-        <v>1933</v>
+        <v>1937</v>
       </c>
       <c r="B1768" t="s">
-        <v>3943</v>
+        <v>3947</v>
       </c>
       <c r="C1768" t="s">
         <v>3878</v>
@@ -62016,15 +62108,15 @@
         <v>1356</v>
       </c>
       <c r="M1768" t="s">
-        <v>4510</v>
+        <v>4514</v>
       </c>
     </row>
     <row r="1769" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1769">
-        <v>1934</v>
+        <v>1938</v>
       </c>
       <c r="B1769" t="s">
-        <v>3944</v>
+        <v>3948</v>
       </c>
       <c r="C1769" t="s">
         <v>3878</v>
@@ -62039,15 +62131,15 @@
         <v>1356</v>
       </c>
       <c r="M1769" t="s">
-        <v>4511</v>
+        <v>4515</v>
       </c>
     </row>
     <row r="1770" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1770">
-        <v>1935</v>
+        <v>1939</v>
       </c>
       <c r="B1770" t="s">
-        <v>3945</v>
+        <v>3949</v>
       </c>
       <c r="C1770" t="s">
         <v>3878</v>
@@ -62062,15 +62154,15 @@
         <v>1356</v>
       </c>
       <c r="M1770" t="s">
-        <v>4512</v>
+        <v>3950</v>
       </c>
     </row>
     <row r="1771" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1771">
-        <v>1936</v>
+        <v>1940</v>
       </c>
       <c r="B1771" t="s">
-        <v>3946</v>
+        <v>3951</v>
       </c>
       <c r="C1771" t="s">
         <v>3878</v>
@@ -62085,15 +62177,15 @@
         <v>1356</v>
       </c>
       <c r="M1771" t="s">
-        <v>4513</v>
+        <v>3952</v>
       </c>
     </row>
     <row r="1772" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1772">
-        <v>1937</v>
+        <v>1941</v>
       </c>
       <c r="B1772" t="s">
-        <v>3947</v>
+        <v>3953</v>
       </c>
       <c r="C1772" t="s">
         <v>3878</v>
@@ -62108,15 +62200,15 @@
         <v>1356</v>
       </c>
       <c r="M1772" t="s">
-        <v>4514</v>
+        <v>3954</v>
       </c>
     </row>
     <row r="1773" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1773">
-        <v>1938</v>
+        <v>1942</v>
       </c>
       <c r="B1773" t="s">
-        <v>3948</v>
+        <v>3955</v>
       </c>
       <c r="C1773" t="s">
         <v>3878</v>
@@ -62131,15 +62223,15 @@
         <v>1356</v>
       </c>
       <c r="M1773" t="s">
-        <v>4515</v>
+        <v>4516</v>
       </c>
     </row>
     <row r="1774" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1774">
-        <v>1939</v>
+        <v>1943</v>
       </c>
       <c r="B1774" t="s">
-        <v>3949</v>
+        <v>3956</v>
       </c>
       <c r="C1774" t="s">
         <v>3878</v>
@@ -62154,15 +62246,15 @@
         <v>1356</v>
       </c>
       <c r="M1774" t="s">
-        <v>3950</v>
+        <v>3957</v>
       </c>
     </row>
     <row r="1775" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1775">
-        <v>1940</v>
+        <v>1944</v>
       </c>
       <c r="B1775" t="s">
-        <v>3951</v>
+        <v>3958</v>
       </c>
       <c r="C1775" t="s">
         <v>3878</v>
@@ -62177,15 +62269,15 @@
         <v>1356</v>
       </c>
       <c r="M1775" t="s">
-        <v>3952</v>
+        <v>3959</v>
       </c>
     </row>
     <row r="1776" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1776">
-        <v>1941</v>
+        <v>1945</v>
       </c>
       <c r="B1776" t="s">
-        <v>3953</v>
+        <v>3960</v>
       </c>
       <c r="C1776" t="s">
         <v>3878</v>
@@ -62200,15 +62292,15 @@
         <v>1356</v>
       </c>
       <c r="M1776" t="s">
-        <v>3954</v>
+        <v>4517</v>
       </c>
     </row>
     <row r="1777" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1777">
-        <v>1942</v>
+        <v>1946</v>
       </c>
       <c r="B1777" t="s">
-        <v>3955</v>
+        <v>3961</v>
       </c>
       <c r="C1777" t="s">
         <v>3878</v>
@@ -62223,15 +62315,15 @@
         <v>1356</v>
       </c>
       <c r="M1777" t="s">
-        <v>4516</v>
+        <v>3962</v>
       </c>
     </row>
     <row r="1778" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1778">
-        <v>1943</v>
+        <v>1947</v>
       </c>
       <c r="B1778" t="s">
-        <v>3956</v>
+        <v>3963</v>
       </c>
       <c r="C1778" t="s">
         <v>3878</v>
@@ -62246,15 +62338,15 @@
         <v>1356</v>
       </c>
       <c r="M1778" t="s">
-        <v>3957</v>
+        <v>4518</v>
       </c>
     </row>
     <row r="1779" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1779">
-        <v>1944</v>
+        <v>1948</v>
       </c>
       <c r="B1779" t="s">
-        <v>3958</v>
+        <v>3964</v>
       </c>
       <c r="C1779" t="s">
         <v>3878</v>
@@ -62269,15 +62361,15 @@
         <v>1356</v>
       </c>
       <c r="M1779" t="s">
-        <v>3959</v>
+        <v>4519</v>
       </c>
     </row>
     <row r="1780" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1780">
-        <v>1945</v>
+        <v>1949</v>
       </c>
       <c r="B1780" t="s">
-        <v>3960</v>
+        <v>3965</v>
       </c>
       <c r="C1780" t="s">
         <v>3878</v>
@@ -62292,15 +62384,15 @@
         <v>1356</v>
       </c>
       <c r="M1780" t="s">
-        <v>4517</v>
+        <v>4520</v>
       </c>
     </row>
     <row r="1781" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1781">
-        <v>1946</v>
+        <v>1950</v>
       </c>
       <c r="B1781" t="s">
-        <v>3961</v>
+        <v>3966</v>
       </c>
       <c r="C1781" t="s">
         <v>3878</v>
@@ -62315,15 +62407,15 @@
         <v>1356</v>
       </c>
       <c r="M1781" t="s">
-        <v>3962</v>
+        <v>4521</v>
       </c>
     </row>
     <row r="1782" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1782">
-        <v>1947</v>
+        <v>1951</v>
       </c>
       <c r="B1782" t="s">
-        <v>3963</v>
+        <v>3967</v>
       </c>
       <c r="C1782" t="s">
         <v>3878</v>
@@ -62338,15 +62430,15 @@
         <v>1356</v>
       </c>
       <c r="M1782" t="s">
-        <v>4518</v>
+        <v>4522</v>
       </c>
     </row>
     <row r="1783" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1783">
-        <v>1948</v>
+        <v>1952</v>
       </c>
       <c r="B1783" t="s">
-        <v>3964</v>
+        <v>3968</v>
       </c>
       <c r="C1783" t="s">
         <v>3878</v>
@@ -62361,15 +62453,15 @@
         <v>1356</v>
       </c>
       <c r="M1783" t="s">
-        <v>4519</v>
+        <v>4523</v>
       </c>
     </row>
     <row r="1784" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1784">
-        <v>1949</v>
+        <v>1953</v>
       </c>
       <c r="B1784" t="s">
-        <v>3965</v>
+        <v>3969</v>
       </c>
       <c r="C1784" t="s">
         <v>3878</v>
@@ -62384,15 +62476,15 @@
         <v>1356</v>
       </c>
       <c r="M1784" t="s">
-        <v>4520</v>
+        <v>3970</v>
       </c>
     </row>
     <row r="1785" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1785">
-        <v>1950</v>
+        <v>1954</v>
       </c>
       <c r="B1785" t="s">
-        <v>3966</v>
+        <v>3971</v>
       </c>
       <c r="C1785" t="s">
         <v>3878</v>
@@ -62407,15 +62499,15 @@
         <v>1356</v>
       </c>
       <c r="M1785" t="s">
-        <v>4521</v>
+        <v>4524</v>
       </c>
     </row>
     <row r="1786" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1786">
-        <v>1951</v>
+        <v>1955</v>
       </c>
       <c r="B1786" t="s">
-        <v>3967</v>
+        <v>3972</v>
       </c>
       <c r="C1786" t="s">
         <v>3878</v>
@@ -62430,15 +62522,15 @@
         <v>1356</v>
       </c>
       <c r="M1786" t="s">
-        <v>4522</v>
+        <v>4525</v>
       </c>
     </row>
     <row r="1787" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1787">
-        <v>1952</v>
+        <v>1956</v>
       </c>
       <c r="B1787" t="s">
-        <v>3968</v>
+        <v>3973</v>
       </c>
       <c r="C1787" t="s">
         <v>3878</v>
@@ -62453,15 +62545,15 @@
         <v>1356</v>
       </c>
       <c r="M1787" t="s">
-        <v>4523</v>
+        <v>3974</v>
       </c>
     </row>
     <row r="1788" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1788">
-        <v>1953</v>
+        <v>1957</v>
       </c>
       <c r="B1788" t="s">
-        <v>3969</v>
+        <v>3975</v>
       </c>
       <c r="C1788" t="s">
         <v>3878</v>
@@ -62476,15 +62568,15 @@
         <v>1356</v>
       </c>
       <c r="M1788" t="s">
-        <v>3970</v>
+        <v>3976</v>
       </c>
     </row>
     <row r="1789" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1789">
-        <v>1954</v>
+        <v>1958</v>
       </c>
       <c r="B1789" t="s">
-        <v>3971</v>
+        <v>3977</v>
       </c>
       <c r="C1789" t="s">
         <v>3878</v>
@@ -62499,15 +62591,15 @@
         <v>1356</v>
       </c>
       <c r="M1789" t="s">
-        <v>4524</v>
+        <v>4526</v>
       </c>
     </row>
     <row r="1790" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1790">
-        <v>1955</v>
+        <v>1959</v>
       </c>
       <c r="B1790" t="s">
-        <v>3972</v>
+        <v>3978</v>
       </c>
       <c r="C1790" t="s">
         <v>3878</v>
@@ -62522,15 +62614,15 @@
         <v>1356</v>
       </c>
       <c r="M1790" t="s">
-        <v>4525</v>
+        <v>3979</v>
       </c>
     </row>
     <row r="1791" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1791">
-        <v>1956</v>
+        <v>1960</v>
       </c>
       <c r="B1791" t="s">
-        <v>3973</v>
+        <v>3980</v>
       </c>
       <c r="C1791" t="s">
         <v>3878</v>
@@ -62545,15 +62637,15 @@
         <v>1356</v>
       </c>
       <c r="M1791" t="s">
-        <v>3974</v>
+        <v>4527</v>
       </c>
     </row>
     <row r="1792" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1792">
-        <v>1957</v>
+        <v>1961</v>
       </c>
       <c r="B1792" t="s">
-        <v>3975</v>
+        <v>3981</v>
       </c>
       <c r="C1792" t="s">
         <v>3878</v>
@@ -62568,15 +62660,15 @@
         <v>1356</v>
       </c>
       <c r="M1792" t="s">
-        <v>3976</v>
+        <v>4528</v>
       </c>
     </row>
     <row r="1793" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1793">
-        <v>1958</v>
+        <v>1962</v>
       </c>
       <c r="B1793" t="s">
-        <v>3977</v>
+        <v>3982</v>
       </c>
       <c r="C1793" t="s">
         <v>3878</v>
@@ -62591,15 +62683,15 @@
         <v>1356</v>
       </c>
       <c r="M1793" t="s">
-        <v>4526</v>
+        <v>4529</v>
       </c>
     </row>
     <row r="1794" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1794">
-        <v>1959</v>
+        <v>1963</v>
       </c>
       <c r="B1794" t="s">
-        <v>3978</v>
+        <v>3983</v>
       </c>
       <c r="C1794" t="s">
         <v>3878</v>
@@ -62614,15 +62706,15 @@
         <v>1356</v>
       </c>
       <c r="M1794" t="s">
-        <v>3979</v>
+        <v>4530</v>
       </c>
     </row>
     <row r="1795" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1795">
-        <v>1960</v>
+        <v>1964</v>
       </c>
       <c r="B1795" t="s">
-        <v>3980</v>
+        <v>3984</v>
       </c>
       <c r="C1795" t="s">
         <v>3878</v>
@@ -62637,15 +62729,15 @@
         <v>1356</v>
       </c>
       <c r="M1795" t="s">
-        <v>4527</v>
+        <v>4531</v>
       </c>
     </row>
     <row r="1796" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1796">
-        <v>1961</v>
+        <v>1965</v>
       </c>
       <c r="B1796" t="s">
-        <v>3981</v>
+        <v>3985</v>
       </c>
       <c r="C1796" t="s">
         <v>3878</v>
@@ -62660,15 +62752,15 @@
         <v>1356</v>
       </c>
       <c r="M1796" t="s">
-        <v>4528</v>
+        <v>3986</v>
       </c>
     </row>
     <row r="1797" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1797">
-        <v>1962</v>
+        <v>1966</v>
       </c>
       <c r="B1797" t="s">
-        <v>3982</v>
+        <v>3987</v>
       </c>
       <c r="C1797" t="s">
         <v>3878</v>
@@ -62683,15 +62775,15 @@
         <v>1356</v>
       </c>
       <c r="M1797" t="s">
-        <v>4529</v>
+        <v>4532</v>
       </c>
     </row>
     <row r="1798" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1798">
-        <v>1963</v>
+        <v>1967</v>
       </c>
       <c r="B1798" t="s">
-        <v>3983</v>
+        <v>3988</v>
       </c>
       <c r="C1798" t="s">
         <v>3878</v>
@@ -62706,15 +62798,15 @@
         <v>1356</v>
       </c>
       <c r="M1798" t="s">
-        <v>4530</v>
+        <v>3989</v>
       </c>
     </row>
     <row r="1799" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1799">
-        <v>1964</v>
+        <v>1968</v>
       </c>
       <c r="B1799" t="s">
-        <v>3984</v>
+        <v>3990</v>
       </c>
       <c r="C1799" t="s">
         <v>3878</v>
@@ -62729,15 +62821,15 @@
         <v>1356</v>
       </c>
       <c r="M1799" t="s">
-        <v>4531</v>
+        <v>4533</v>
       </c>
     </row>
     <row r="1800" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1800">
-        <v>1965</v>
+        <v>1969</v>
       </c>
       <c r="B1800" t="s">
-        <v>3985</v>
+        <v>3991</v>
       </c>
       <c r="C1800" t="s">
         <v>3878</v>
@@ -62752,15 +62844,15 @@
         <v>1356</v>
       </c>
       <c r="M1800" t="s">
-        <v>3986</v>
+        <v>3992</v>
       </c>
     </row>
     <row r="1801" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1801">
-        <v>1966</v>
+        <v>1970</v>
       </c>
       <c r="B1801" t="s">
-        <v>3987</v>
+        <v>3993</v>
       </c>
       <c r="C1801" t="s">
         <v>3878</v>
@@ -62775,15 +62867,15 @@
         <v>1356</v>
       </c>
       <c r="M1801" t="s">
-        <v>4532</v>
+        <v>3994</v>
       </c>
     </row>
     <row r="1802" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1802">
-        <v>1967</v>
+        <v>1971</v>
       </c>
       <c r="B1802" t="s">
-        <v>3988</v>
+        <v>3995</v>
       </c>
       <c r="C1802" t="s">
         <v>3878</v>
@@ -62798,15 +62890,15 @@
         <v>1356</v>
       </c>
       <c r="M1802" t="s">
-        <v>3989</v>
+        <v>4534</v>
       </c>
     </row>
     <row r="1803" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1803">
-        <v>1968</v>
+        <v>1972</v>
       </c>
       <c r="B1803" t="s">
-        <v>3990</v>
+        <v>3996</v>
       </c>
       <c r="C1803" t="s">
         <v>3878</v>
@@ -62821,15 +62913,15 @@
         <v>1356</v>
       </c>
       <c r="M1803" t="s">
-        <v>4533</v>
+        <v>4535</v>
       </c>
     </row>
     <row r="1804" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1804">
-        <v>1969</v>
+        <v>1973</v>
       </c>
       <c r="B1804" t="s">
-        <v>3991</v>
+        <v>3997</v>
       </c>
       <c r="C1804" t="s">
         <v>3878</v>
@@ -62844,15 +62936,15 @@
         <v>1356</v>
       </c>
       <c r="M1804" t="s">
-        <v>3992</v>
+        <v>3998</v>
       </c>
     </row>
     <row r="1805" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1805">
-        <v>1970</v>
+        <v>1974</v>
       </c>
       <c r="B1805" t="s">
-        <v>3993</v>
+        <v>3999</v>
       </c>
       <c r="C1805" t="s">
         <v>3878</v>
@@ -62867,15 +62959,15 @@
         <v>1356</v>
       </c>
       <c r="M1805" t="s">
-        <v>3994</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="1806" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1806">
-        <v>1971</v>
+        <v>1975</v>
       </c>
       <c r="B1806" t="s">
-        <v>3995</v>
+        <v>4001</v>
       </c>
       <c r="C1806" t="s">
         <v>3878</v>
@@ -62890,15 +62982,15 @@
         <v>1356</v>
       </c>
       <c r="M1806" t="s">
-        <v>4534</v>
+        <v>4536</v>
       </c>
     </row>
     <row r="1807" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1807">
-        <v>1972</v>
+        <v>1976</v>
       </c>
       <c r="B1807" t="s">
-        <v>3996</v>
+        <v>4002</v>
       </c>
       <c r="C1807" t="s">
         <v>3878</v>
@@ -62913,15 +63005,15 @@
         <v>1356</v>
       </c>
       <c r="M1807" t="s">
-        <v>4535</v>
+        <v>4003</v>
       </c>
     </row>
     <row r="1808" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1808">
-        <v>1973</v>
+        <v>1977</v>
       </c>
       <c r="B1808" t="s">
-        <v>3997</v>
+        <v>4004</v>
       </c>
       <c r="C1808" t="s">
         <v>3878</v>
@@ -62936,15 +63028,15 @@
         <v>1356</v>
       </c>
       <c r="M1808" t="s">
-        <v>3998</v>
+        <v>4537</v>
       </c>
     </row>
     <row r="1809" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1809">
-        <v>1974</v>
+        <v>1978</v>
       </c>
       <c r="B1809" t="s">
-        <v>3999</v>
+        <v>4005</v>
       </c>
       <c r="C1809" t="s">
         <v>3878</v>
@@ -62959,15 +63051,15 @@
         <v>1356</v>
       </c>
       <c r="M1809" t="s">
-        <v>4000</v>
+        <v>4538</v>
       </c>
     </row>
     <row r="1810" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1810">
-        <v>1975</v>
+        <v>1979</v>
       </c>
       <c r="B1810" t="s">
-        <v>4001</v>
+        <v>4006</v>
       </c>
       <c r="C1810" t="s">
         <v>3878</v>
@@ -62982,15 +63074,15 @@
         <v>1356</v>
       </c>
       <c r="M1810" t="s">
-        <v>4536</v>
+        <v>4539</v>
       </c>
     </row>
     <row r="1811" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1811">
-        <v>1976</v>
+        <v>1980</v>
       </c>
       <c r="B1811" t="s">
-        <v>4002</v>
+        <v>4007</v>
       </c>
       <c r="C1811" t="s">
         <v>3878</v>
@@ -63005,15 +63097,15 @@
         <v>1356</v>
       </c>
       <c r="M1811" t="s">
-        <v>4003</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="1812" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1812">
-        <v>1977</v>
+        <v>1981</v>
       </c>
       <c r="B1812" t="s">
-        <v>4004</v>
+        <v>4008</v>
       </c>
       <c r="C1812" t="s">
         <v>3878</v>
@@ -63028,15 +63120,15 @@
         <v>1356</v>
       </c>
       <c r="M1812" t="s">
-        <v>4537</v>
+        <v>4541</v>
       </c>
     </row>
     <row r="1813" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1813">
-        <v>1978</v>
+        <v>1982</v>
       </c>
       <c r="B1813" t="s">
-        <v>4005</v>
+        <v>4009</v>
       </c>
       <c r="C1813" t="s">
         <v>3878</v>
@@ -63051,15 +63143,15 @@
         <v>1356</v>
       </c>
       <c r="M1813" t="s">
-        <v>4538</v>
+        <v>4542</v>
       </c>
     </row>
     <row r="1814" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1814">
-        <v>1979</v>
+        <v>1983</v>
       </c>
       <c r="B1814" t="s">
-        <v>4006</v>
+        <v>4010</v>
       </c>
       <c r="C1814" t="s">
         <v>3878</v>
@@ -63074,15 +63166,15 @@
         <v>1356</v>
       </c>
       <c r="M1814" t="s">
-        <v>4539</v>
+        <v>4011</v>
       </c>
     </row>
     <row r="1815" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1815">
-        <v>1980</v>
+        <v>1984</v>
       </c>
       <c r="B1815" t="s">
-        <v>4007</v>
+        <v>4012</v>
       </c>
       <c r="C1815" t="s">
         <v>3878</v>
@@ -63097,15 +63189,15 @@
         <v>1356</v>
       </c>
       <c r="M1815" t="s">
-        <v>4540</v>
+        <v>4543</v>
       </c>
     </row>
     <row r="1816" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1816">
-        <v>1981</v>
+        <v>1985</v>
       </c>
       <c r="B1816" t="s">
-        <v>4008</v>
+        <v>4013</v>
       </c>
       <c r="C1816" t="s">
         <v>3878</v>
@@ -63120,15 +63212,15 @@
         <v>1356</v>
       </c>
       <c r="M1816" t="s">
-        <v>4541</v>
+        <v>4544</v>
       </c>
     </row>
     <row r="1817" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1817">
-        <v>1982</v>
+        <v>1986</v>
       </c>
       <c r="B1817" t="s">
-        <v>4009</v>
+        <v>4014</v>
       </c>
       <c r="C1817" t="s">
         <v>3878</v>
@@ -63143,15 +63235,15 @@
         <v>1356</v>
       </c>
       <c r="M1817" t="s">
-        <v>4542</v>
+        <v>4015</v>
       </c>
     </row>
     <row r="1818" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1818">
-        <v>1983</v>
+        <v>1987</v>
       </c>
       <c r="B1818" t="s">
-        <v>4010</v>
+        <v>4016</v>
       </c>
       <c r="C1818" t="s">
         <v>3878</v>
@@ -63166,15 +63258,15 @@
         <v>1356</v>
       </c>
       <c r="M1818" t="s">
-        <v>4011</v>
+        <v>4545</v>
       </c>
     </row>
     <row r="1819" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1819">
-        <v>1984</v>
+        <v>1988</v>
       </c>
       <c r="B1819" t="s">
-        <v>4012</v>
+        <v>4017</v>
       </c>
       <c r="C1819" t="s">
         <v>3878</v>
@@ -63189,15 +63281,15 @@
         <v>1356</v>
       </c>
       <c r="M1819" t="s">
-        <v>4543</v>
+        <v>4018</v>
       </c>
     </row>
     <row r="1820" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1820">
-        <v>1985</v>
+        <v>1989</v>
       </c>
       <c r="B1820" t="s">
-        <v>4013</v>
+        <v>4019</v>
       </c>
       <c r="C1820" t="s">
         <v>3878</v>
@@ -63212,15 +63304,15 @@
         <v>1356</v>
       </c>
       <c r="M1820" t="s">
-        <v>4544</v>
+        <v>4020</v>
       </c>
     </row>
     <row r="1821" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1821">
-        <v>1986</v>
+        <v>1990</v>
       </c>
       <c r="B1821" t="s">
-        <v>4014</v>
+        <v>4021</v>
       </c>
       <c r="C1821" t="s">
         <v>3878</v>
@@ -63235,15 +63327,15 @@
         <v>1356</v>
       </c>
       <c r="M1821" t="s">
-        <v>4015</v>
+        <v>4546</v>
       </c>
     </row>
     <row r="1822" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1822">
-        <v>1987</v>
+        <v>1991</v>
       </c>
       <c r="B1822" t="s">
-        <v>4016</v>
+        <v>4022</v>
       </c>
       <c r="C1822" t="s">
         <v>3878</v>
@@ -63258,15 +63350,15 @@
         <v>1356</v>
       </c>
       <c r="M1822" t="s">
-        <v>4545</v>
+        <v>4023</v>
       </c>
     </row>
     <row r="1823" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1823">
-        <v>1988</v>
+        <v>1992</v>
       </c>
       <c r="B1823" t="s">
-        <v>4017</v>
+        <v>4024</v>
       </c>
       <c r="C1823" t="s">
         <v>3878</v>
@@ -63281,15 +63373,15 @@
         <v>1356</v>
       </c>
       <c r="M1823" t="s">
-        <v>4018</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="1824" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1824">
-        <v>1989</v>
+        <v>1993</v>
       </c>
       <c r="B1824" t="s">
-        <v>4019</v>
+        <v>4025</v>
       </c>
       <c r="C1824" t="s">
         <v>3878</v>
@@ -63304,15 +63396,15 @@
         <v>1356</v>
       </c>
       <c r="M1824" t="s">
-        <v>4020</v>
+        <v>4548</v>
       </c>
     </row>
     <row r="1825" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1825">
-        <v>1990</v>
+        <v>1994</v>
       </c>
       <c r="B1825" t="s">
-        <v>4021</v>
+        <v>4026</v>
       </c>
       <c r="C1825" t="s">
         <v>3878</v>
@@ -63327,15 +63419,15 @@
         <v>1356</v>
       </c>
       <c r="M1825" t="s">
-        <v>4546</v>
+        <v>4549</v>
       </c>
     </row>
     <row r="1826" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1826">
-        <v>1991</v>
+        <v>1995</v>
       </c>
       <c r="B1826" t="s">
-        <v>4022</v>
+        <v>4027</v>
       </c>
       <c r="C1826" t="s">
         <v>3878</v>
@@ -63350,15 +63442,15 @@
         <v>1356</v>
       </c>
       <c r="M1826" t="s">
-        <v>4023</v>
+        <v>4550</v>
       </c>
     </row>
     <row r="1827" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1827">
-        <v>1992</v>
+        <v>1996</v>
       </c>
       <c r="B1827" t="s">
-        <v>4024</v>
+        <v>4028</v>
       </c>
       <c r="C1827" t="s">
         <v>3878</v>
@@ -63373,15 +63465,15 @@
         <v>1356</v>
       </c>
       <c r="M1827" t="s">
-        <v>4547</v>
+        <v>4551</v>
       </c>
     </row>
     <row r="1828" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1828">
-        <v>1993</v>
+        <v>1997</v>
       </c>
       <c r="B1828" t="s">
-        <v>4025</v>
+        <v>4029</v>
       </c>
       <c r="C1828" t="s">
         <v>3878</v>
@@ -63396,15 +63488,15 @@
         <v>1356</v>
       </c>
       <c r="M1828" t="s">
-        <v>4548</v>
+        <v>4030</v>
       </c>
     </row>
     <row r="1829" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1829">
-        <v>1994</v>
+        <v>1998</v>
       </c>
       <c r="B1829" t="s">
-        <v>4026</v>
+        <v>4031</v>
       </c>
       <c r="C1829" t="s">
         <v>3878</v>
@@ -63419,15 +63511,15 @@
         <v>1356</v>
       </c>
       <c r="M1829" t="s">
-        <v>4549</v>
+        <v>4552</v>
       </c>
     </row>
     <row r="1830" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1830">
-        <v>1995</v>
+        <v>1999</v>
       </c>
       <c r="B1830" t="s">
-        <v>4027</v>
+        <v>4032</v>
       </c>
       <c r="C1830" t="s">
         <v>3878</v>
@@ -63442,15 +63534,15 @@
         <v>1356</v>
       </c>
       <c r="M1830" t="s">
-        <v>4550</v>
+        <v>4553</v>
       </c>
     </row>
     <row r="1831" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1831">
-        <v>1996</v>
+        <v>2000</v>
       </c>
       <c r="B1831" t="s">
-        <v>4028</v>
+        <v>4033</v>
       </c>
       <c r="C1831" t="s">
         <v>3878</v>
@@ -63465,15 +63557,15 @@
         <v>1356</v>
       </c>
       <c r="M1831" t="s">
-        <v>4551</v>
+        <v>4034</v>
       </c>
     </row>
     <row r="1832" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1832">
-        <v>1997</v>
+        <v>2001</v>
       </c>
       <c r="B1832" t="s">
-        <v>4029</v>
+        <v>4035</v>
       </c>
       <c r="C1832" t="s">
         <v>3878</v>
@@ -63488,15 +63580,15 @@
         <v>1356</v>
       </c>
       <c r="M1832" t="s">
-        <v>4030</v>
+        <v>4036</v>
       </c>
     </row>
     <row r="1833" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1833">
-        <v>1998</v>
+        <v>2002</v>
       </c>
       <c r="B1833" t="s">
-        <v>4031</v>
+        <v>4037</v>
       </c>
       <c r="C1833" t="s">
         <v>3878</v>
@@ -63511,15 +63603,15 @@
         <v>1356</v>
       </c>
       <c r="M1833" t="s">
-        <v>4552</v>
+        <v>4038</v>
       </c>
     </row>
     <row r="1834" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1834">
-        <v>1999</v>
+        <v>2003</v>
       </c>
       <c r="B1834" t="s">
-        <v>4032</v>
+        <v>4039</v>
       </c>
       <c r="C1834" t="s">
         <v>3878</v>
@@ -63534,15 +63626,15 @@
         <v>1356</v>
       </c>
       <c r="M1834" t="s">
-        <v>4553</v>
+        <v>4040</v>
       </c>
     </row>
     <row r="1835" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1835">
-        <v>2000</v>
+        <v>2004</v>
       </c>
       <c r="B1835" t="s">
-        <v>4033</v>
+        <v>4041</v>
       </c>
       <c r="C1835" t="s">
         <v>3878</v>
@@ -63557,15 +63649,15 @@
         <v>1356</v>
       </c>
       <c r="M1835" t="s">
-        <v>4034</v>
+        <v>4554</v>
       </c>
     </row>
     <row r="1836" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1836">
-        <v>2001</v>
+        <v>2005</v>
       </c>
       <c r="B1836" t="s">
-        <v>4035</v>
+        <v>4042</v>
       </c>
       <c r="C1836" t="s">
         <v>3878</v>
@@ -63580,15 +63672,15 @@
         <v>1356</v>
       </c>
       <c r="M1836" t="s">
-        <v>4036</v>
+        <v>4043</v>
       </c>
     </row>
     <row r="1837" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1837">
-        <v>2002</v>
+        <v>2006</v>
       </c>
       <c r="B1837" t="s">
-        <v>4037</v>
+        <v>4044</v>
       </c>
       <c r="C1837" t="s">
         <v>3878</v>
@@ -63603,15 +63695,15 @@
         <v>1356</v>
       </c>
       <c r="M1837" t="s">
-        <v>4038</v>
+        <v>4045</v>
       </c>
     </row>
     <row r="1838" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1838">
-        <v>2003</v>
+        <v>2007</v>
       </c>
       <c r="B1838" t="s">
-        <v>4039</v>
+        <v>4046</v>
       </c>
       <c r="C1838" t="s">
         <v>3878</v>
@@ -63626,15 +63718,15 @@
         <v>1356</v>
       </c>
       <c r="M1838" t="s">
-        <v>4040</v>
+        <v>4555</v>
       </c>
     </row>
     <row r="1839" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1839">
-        <v>2004</v>
+        <v>2008</v>
       </c>
       <c r="B1839" t="s">
-        <v>4041</v>
+        <v>4047</v>
       </c>
       <c r="C1839" t="s">
         <v>3878</v>
@@ -63649,15 +63741,15 @@
         <v>1356</v>
       </c>
       <c r="M1839" t="s">
-        <v>4554</v>
+        <v>4048</v>
       </c>
     </row>
     <row r="1840" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1840">
-        <v>2005</v>
+        <v>2009</v>
       </c>
       <c r="B1840" t="s">
-        <v>4042</v>
+        <v>4049</v>
       </c>
       <c r="C1840" t="s">
         <v>3878</v>
@@ -63672,15 +63764,15 @@
         <v>1356</v>
       </c>
       <c r="M1840" t="s">
-        <v>4043</v>
+        <v>4556</v>
       </c>
     </row>
     <row r="1841" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1841">
-        <v>2006</v>
+        <v>2010</v>
       </c>
       <c r="B1841" t="s">
-        <v>4044</v>
+        <v>4050</v>
       </c>
       <c r="C1841" t="s">
         <v>3878</v>
@@ -63695,15 +63787,15 @@
         <v>1356</v>
       </c>
       <c r="M1841" t="s">
-        <v>4045</v>
+        <v>4051</v>
       </c>
     </row>
     <row r="1842" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1842">
-        <v>2007</v>
+        <v>2011</v>
       </c>
       <c r="B1842" t="s">
-        <v>4046</v>
+        <v>4052</v>
       </c>
       <c r="C1842" t="s">
         <v>3878</v>
@@ -63718,15 +63810,15 @@
         <v>1356</v>
       </c>
       <c r="M1842" t="s">
-        <v>4555</v>
+        <v>4053</v>
       </c>
     </row>
     <row r="1843" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1843">
-        <v>2008</v>
+        <v>2012</v>
       </c>
       <c r="B1843" t="s">
-        <v>4047</v>
+        <v>4054</v>
       </c>
       <c r="C1843" t="s">
         <v>3878</v>
@@ -63741,15 +63833,15 @@
         <v>1356</v>
       </c>
       <c r="M1843" t="s">
-        <v>4048</v>
+        <v>4055</v>
       </c>
     </row>
     <row r="1844" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1844">
-        <v>2009</v>
+        <v>2013</v>
       </c>
       <c r="B1844" t="s">
-        <v>4049</v>
+        <v>4056</v>
       </c>
       <c r="C1844" t="s">
         <v>3878</v>
@@ -63764,15 +63856,15 @@
         <v>1356</v>
       </c>
       <c r="M1844" t="s">
-        <v>4556</v>
+        <v>4557</v>
       </c>
     </row>
     <row r="1845" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1845">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="B1845" t="s">
-        <v>4050</v>
+        <v>4057</v>
       </c>
       <c r="C1845" t="s">
         <v>3878</v>
@@ -63787,15 +63879,15 @@
         <v>1356</v>
       </c>
       <c r="M1845" t="s">
-        <v>4051</v>
+        <v>4558</v>
       </c>
     </row>
     <row r="1846" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1846">
-        <v>2011</v>
+        <v>2015</v>
       </c>
       <c r="B1846" t="s">
-        <v>4052</v>
+        <v>4058</v>
       </c>
       <c r="C1846" t="s">
         <v>3878</v>
@@ -63810,15 +63902,15 @@
         <v>1356</v>
       </c>
       <c r="M1846" t="s">
-        <v>4053</v>
+        <v>4559</v>
       </c>
     </row>
     <row r="1847" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1847">
-        <v>2012</v>
+        <v>2016</v>
       </c>
       <c r="B1847" t="s">
-        <v>4054</v>
+        <v>4059</v>
       </c>
       <c r="C1847" t="s">
         <v>3878</v>
@@ -63833,15 +63925,15 @@
         <v>1356</v>
       </c>
       <c r="M1847" t="s">
-        <v>4055</v>
+        <v>4560</v>
       </c>
     </row>
     <row r="1848" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1848">
-        <v>2013</v>
+        <v>2017</v>
       </c>
       <c r="B1848" t="s">
-        <v>4056</v>
+        <v>4060</v>
       </c>
       <c r="C1848" t="s">
         <v>3878</v>
@@ -63856,15 +63948,15 @@
         <v>1356</v>
       </c>
       <c r="M1848" t="s">
-        <v>4557</v>
+        <v>4561</v>
       </c>
     </row>
     <row r="1849" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1849">
-        <v>2014</v>
+        <v>2018</v>
       </c>
       <c r="B1849" t="s">
-        <v>4057</v>
+        <v>4061</v>
       </c>
       <c r="C1849" t="s">
         <v>3878</v>
@@ -63879,15 +63971,15 @@
         <v>1356</v>
       </c>
       <c r="M1849" t="s">
-        <v>4558</v>
+        <v>4062</v>
       </c>
     </row>
     <row r="1850" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1850">
-        <v>2015</v>
+        <v>2019</v>
       </c>
       <c r="B1850" t="s">
-        <v>4058</v>
+        <v>4063</v>
       </c>
       <c r="C1850" t="s">
         <v>3878</v>
@@ -63902,15 +63994,15 @@
         <v>1356</v>
       </c>
       <c r="M1850" t="s">
-        <v>4559</v>
+        <v>4562</v>
       </c>
     </row>
     <row r="1851" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1851">
-        <v>2016</v>
+        <v>2020</v>
       </c>
       <c r="B1851" t="s">
-        <v>4059</v>
+        <v>4064</v>
       </c>
       <c r="C1851" t="s">
         <v>3878</v>
@@ -63925,103 +64017,11 @@
         <v>1356</v>
       </c>
       <c r="M1851" t="s">
-        <v>4560</v>
-      </c>
-    </row>
-    <row r="1852" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1852">
-        <v>2017</v>
-      </c>
-      <c r="B1852" t="s">
-        <v>4060</v>
-      </c>
-      <c r="C1852" t="s">
-        <v>3878</v>
-      </c>
-      <c r="D1852">
-        <v>68000</v>
-      </c>
-      <c r="E1852" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1852" t="s">
-        <v>1356</v>
-      </c>
-      <c r="M1852" t="s">
-        <v>4561</v>
-      </c>
-    </row>
-    <row r="1853" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1853">
-        <v>2018</v>
-      </c>
-      <c r="B1853" t="s">
-        <v>4061</v>
-      </c>
-      <c r="C1853" t="s">
-        <v>3878</v>
-      </c>
-      <c r="D1853">
-        <v>68000</v>
-      </c>
-      <c r="E1853" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1853" t="s">
-        <v>1356</v>
-      </c>
-      <c r="M1853" t="s">
-        <v>4062</v>
-      </c>
-    </row>
-    <row r="1854" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1854">
-        <v>2019</v>
-      </c>
-      <c r="B1854" t="s">
-        <v>4063</v>
-      </c>
-      <c r="C1854" t="s">
-        <v>3878</v>
-      </c>
-      <c r="D1854">
-        <v>68000</v>
-      </c>
-      <c r="E1854" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1854" t="s">
-        <v>1356</v>
-      </c>
-      <c r="M1854" t="s">
-        <v>4562</v>
-      </c>
-    </row>
-    <row r="1855" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1855">
-        <v>2020</v>
-      </c>
-      <c r="B1855" t="s">
-        <v>4064</v>
-      </c>
-      <c r="C1855" t="s">
-        <v>3878</v>
-      </c>
-      <c r="D1855">
-        <v>68000</v>
-      </c>
-      <c r="E1855" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1855" t="s">
-        <v>1356</v>
-      </c>
-      <c r="M1855" t="s">
         <v>4065</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M1855"/>
+  <autoFilter ref="A1:M1851"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
036 : added ambush driver
</commit_message>
<xml_diff>
--- a/0.36/compatibility.xlsx
+++ b/0.36/compatibility.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Playable (untested)" sheetId="4" r:id="rId1"/>
@@ -17,8 +17,8 @@
     <sheet name="GAME_NOT_WORKING FLAG" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ALL!$A$1:$M$1752</definedName>
-    <definedName name="LIST" localSheetId="1">ALL!$B$1:$M$1752</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ALL!$A$1:$M$1751</definedName>
+    <definedName name="LIST" localSheetId="1">ALL!$B$1:$M$1751</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -14078,10 +14078,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P293"/>
+  <dimension ref="A1:P294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A275" workbookViewId="0">
-      <selection activeCell="A295" sqref="A295"/>
+    <sheetView topLeftCell="A275" workbookViewId="0">
+      <selection activeCell="A291" sqref="A291:A294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20685,6 +20685,26 @@
         <v>2065</v>
       </c>
     </row>
+    <row r="294" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A294">
+        <v>294</v>
+      </c>
+      <c r="B294" t="s">
+        <v>3845</v>
+      </c>
+      <c r="C294" t="s">
+        <v>3846</v>
+      </c>
+      <c r="D294" t="s">
+        <v>14</v>
+      </c>
+      <c r="H294" t="s">
+        <v>172</v>
+      </c>
+      <c r="M294" t="s">
+        <v>3847</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -20693,10 +20713,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1752"/>
+  <dimension ref="A1:M1751"/>
   <sheetViews>
-    <sheetView topLeftCell="A810" workbookViewId="0">
-      <selection activeCell="G829" sqref="G829"/>
+    <sheetView tabSelected="1" topLeftCell="A1601" workbookViewId="0">
+      <selection activeCell="A1616" sqref="A1616:XFD1616"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -60806,70 +60826,73 @@
     </row>
     <row r="1616" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1616">
-        <v>1644</v>
+        <v>1645</v>
       </c>
       <c r="B1616" t="s">
-        <v>3845</v>
+        <v>3848</v>
       </c>
       <c r="C1616" t="s">
-        <v>3846</v>
-      </c>
-      <c r="D1616" t="s">
-        <v>14</v>
+        <v>3849</v>
+      </c>
+      <c r="D1616">
+        <v>8080</v>
       </c>
       <c r="H1616" t="s">
-        <v>172</v>
+        <v>406</v>
       </c>
       <c r="M1616" t="s">
-        <v>3847</v>
+        <v>3850</v>
       </c>
     </row>
     <row r="1617" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1617">
-        <v>1645</v>
+        <v>1646</v>
       </c>
       <c r="B1617" t="s">
-        <v>3848</v>
+        <v>3851</v>
       </c>
       <c r="C1617" t="s">
-        <v>3849</v>
-      </c>
-      <c r="D1617">
-        <v>8080</v>
+        <v>3852</v>
+      </c>
+      <c r="D1617" t="s">
+        <v>1105</v>
       </c>
       <c r="H1617" t="s">
-        <v>406</v>
+        <v>336</v>
       </c>
       <c r="M1617" t="s">
-        <v>3850</v>
+        <v>3853</v>
       </c>
     </row>
     <row r="1618" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1618">
-        <v>1646</v>
+        <v>1647</v>
       </c>
       <c r="B1618" t="s">
-        <v>3851</v>
+        <v>3854</v>
       </c>
       <c r="C1618" t="s">
-        <v>3852</v>
+        <v>3855</v>
       </c>
       <c r="D1618" t="s">
-        <v>1105</v>
+        <v>14</v>
+      </c>
+      <c r="E1618" t="s">
+        <v>154</v>
       </c>
       <c r="H1618" t="s">
         <v>336</v>
       </c>
       <c r="M1618" t="s">
-        <v>3853</v>
+        <v>3856</v>
       </c>
     </row>
     <row r="1619" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1619">
-        <v>1647</v>
+        <v>1648</v>
       </c>
       <c r="B1619" t="s">
-        <v>3854</v>
+        <v>3857</v>
       </c>
       <c r="C1619" t="s">
         <v>3855</v>
@@ -60884,141 +60907,141 @@
         <v>336</v>
       </c>
       <c r="M1619" t="s">
-        <v>3856</v>
+        <v>3858</v>
       </c>
     </row>
     <row r="1620" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1620">
-        <v>1648</v>
+        <v>1649</v>
       </c>
       <c r="B1620" t="s">
-        <v>3857</v>
+        <v>3859</v>
       </c>
       <c r="C1620" t="s">
-        <v>3855</v>
+        <v>3860</v>
       </c>
       <c r="D1620" t="s">
-        <v>14</v>
+        <v>3861</v>
       </c>
       <c r="E1620" t="s">
-        <v>154</v>
+        <v>725</v>
       </c>
       <c r="H1620" t="s">
-        <v>336</v>
+        <v>2070</v>
       </c>
       <c r="M1620" t="s">
-        <v>3858</v>
+        <v>3862</v>
       </c>
     </row>
     <row r="1621" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1621">
-        <v>1649</v>
+        <v>1650</v>
       </c>
       <c r="B1621" t="s">
-        <v>3859</v>
+        <v>3863</v>
       </c>
       <c r="C1621" t="s">
-        <v>3860</v>
-      </c>
-      <c r="D1621" t="s">
-        <v>3861</v>
-      </c>
-      <c r="E1621" t="s">
-        <v>725</v>
+        <v>3864</v>
+      </c>
+      <c r="D1621">
+        <v>68000</v>
       </c>
       <c r="H1621" t="s">
-        <v>2070</v>
+        <v>2375</v>
       </c>
       <c r="M1621" t="s">
-        <v>3862</v>
+        <v>3865</v>
       </c>
     </row>
     <row r="1622" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1622">
-        <v>1650</v>
+        <v>1651</v>
       </c>
       <c r="B1622" t="s">
-        <v>3863</v>
+        <v>3866</v>
       </c>
       <c r="C1622" t="s">
-        <v>3864</v>
+        <v>3867</v>
       </c>
       <c r="D1622">
         <v>68000</v>
       </c>
+      <c r="E1622" t="s">
+        <v>154</v>
+      </c>
       <c r="H1622" t="s">
-        <v>2375</v>
+        <v>1236</v>
       </c>
       <c r="M1622" t="s">
-        <v>3865</v>
+        <v>3868</v>
       </c>
     </row>
     <row r="1623" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1623">
-        <v>1651</v>
+        <v>1652</v>
       </c>
       <c r="B1623" t="s">
-        <v>3866</v>
+        <v>3869</v>
       </c>
       <c r="C1623" t="s">
-        <v>3867</v>
-      </c>
-      <c r="D1623">
-        <v>68000</v>
-      </c>
-      <c r="E1623" t="s">
-        <v>154</v>
+        <v>3870</v>
+      </c>
+      <c r="D1623" t="s">
+        <v>405</v>
       </c>
       <c r="H1623" t="s">
-        <v>1236</v>
+        <v>71</v>
       </c>
       <c r="M1623" t="s">
-        <v>3868</v>
+        <v>3871</v>
       </c>
     </row>
     <row r="1624" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1624">
-        <v>1652</v>
+        <v>1653</v>
       </c>
       <c r="B1624" t="s">
-        <v>3869</v>
+        <v>3872</v>
       </c>
       <c r="C1624" t="s">
-        <v>3870</v>
+        <v>3873</v>
       </c>
       <c r="D1624" t="s">
-        <v>405</v>
-      </c>
-      <c r="H1624" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="M1624" t="s">
-        <v>3871</v>
+        <v>4493</v>
       </c>
     </row>
     <row r="1625" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1625">
-        <v>1653</v>
+        <v>1654</v>
       </c>
       <c r="B1625" t="s">
-        <v>3872</v>
+        <v>3874</v>
       </c>
       <c r="C1625" t="s">
-        <v>3873</v>
-      </c>
-      <c r="D1625" t="s">
-        <v>14</v>
+        <v>3875</v>
+      </c>
+      <c r="D1625">
+        <v>68000</v>
+      </c>
+      <c r="E1625" t="s">
+        <v>154</v>
+      </c>
+      <c r="H1625" t="s">
+        <v>1353</v>
       </c>
       <c r="M1625" t="s">
-        <v>4493</v>
+        <v>3876</v>
       </c>
     </row>
     <row r="1626" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1626">
-        <v>1654</v>
+        <v>1655</v>
       </c>
       <c r="B1626" t="s">
-        <v>3874</v>
+        <v>3877</v>
       </c>
       <c r="C1626" t="s">
         <v>3875</v>
@@ -61033,15 +61056,15 @@
         <v>1353</v>
       </c>
       <c r="M1626" t="s">
-        <v>3876</v>
+        <v>4494</v>
       </c>
     </row>
     <row r="1627" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1627">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="B1627" t="s">
-        <v>3877</v>
+        <v>3878</v>
       </c>
       <c r="C1627" t="s">
         <v>3875</v>
@@ -61056,15 +61079,15 @@
         <v>1353</v>
       </c>
       <c r="M1627" t="s">
-        <v>4494</v>
+        <v>3879</v>
       </c>
     </row>
     <row r="1628" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1628">
-        <v>1656</v>
+        <v>1657</v>
       </c>
       <c r="B1628" t="s">
-        <v>3878</v>
+        <v>3880</v>
       </c>
       <c r="C1628" t="s">
         <v>3875</v>
@@ -61079,15 +61102,15 @@
         <v>1353</v>
       </c>
       <c r="M1628" t="s">
-        <v>3879</v>
+        <v>3881</v>
       </c>
     </row>
     <row r="1629" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1629">
-        <v>1657</v>
+        <v>1658</v>
       </c>
       <c r="B1629" t="s">
-        <v>3880</v>
+        <v>3882</v>
       </c>
       <c r="C1629" t="s">
         <v>3875</v>
@@ -61102,15 +61125,15 @@
         <v>1353</v>
       </c>
       <c r="M1629" t="s">
-        <v>3881</v>
+        <v>3883</v>
       </c>
     </row>
     <row r="1630" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1630">
-        <v>1658</v>
+        <v>1659</v>
       </c>
       <c r="B1630" t="s">
-        <v>3882</v>
+        <v>3884</v>
       </c>
       <c r="C1630" t="s">
         <v>3875</v>
@@ -61125,15 +61148,15 @@
         <v>1353</v>
       </c>
       <c r="M1630" t="s">
-        <v>3883</v>
+        <v>3885</v>
       </c>
     </row>
     <row r="1631" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1631">
-        <v>1659</v>
+        <v>1660</v>
       </c>
       <c r="B1631" t="s">
-        <v>3884</v>
+        <v>3886</v>
       </c>
       <c r="C1631" t="s">
         <v>3875</v>
@@ -61148,15 +61171,15 @@
         <v>1353</v>
       </c>
       <c r="M1631" t="s">
-        <v>3885</v>
+        <v>3887</v>
       </c>
     </row>
     <row r="1632" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1632">
-        <v>1660</v>
+        <v>1661</v>
       </c>
       <c r="B1632" t="s">
-        <v>3886</v>
+        <v>3888</v>
       </c>
       <c r="C1632" t="s">
         <v>3875</v>
@@ -61171,15 +61194,15 @@
         <v>1353</v>
       </c>
       <c r="M1632" t="s">
-        <v>3887</v>
+        <v>4495</v>
       </c>
     </row>
     <row r="1633" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1633">
-        <v>1661</v>
+        <v>1662</v>
       </c>
       <c r="B1633" t="s">
-        <v>3888</v>
+        <v>3889</v>
       </c>
       <c r="C1633" t="s">
         <v>3875</v>
@@ -61194,15 +61217,15 @@
         <v>1353</v>
       </c>
       <c r="M1633" t="s">
-        <v>4495</v>
+        <v>3890</v>
       </c>
     </row>
     <row r="1634" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1634">
-        <v>1662</v>
+        <v>1663</v>
       </c>
       <c r="B1634" t="s">
-        <v>3889</v>
+        <v>3891</v>
       </c>
       <c r="C1634" t="s">
         <v>3875</v>
@@ -61217,15 +61240,15 @@
         <v>1353</v>
       </c>
       <c r="M1634" t="s">
-        <v>3890</v>
+        <v>3892</v>
       </c>
     </row>
     <row r="1635" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1635">
-        <v>1663</v>
+        <v>1664</v>
       </c>
       <c r="B1635" t="s">
-        <v>3891</v>
+        <v>3893</v>
       </c>
       <c r="C1635" t="s">
         <v>3875</v>
@@ -61240,15 +61263,15 @@
         <v>1353</v>
       </c>
       <c r="M1635" t="s">
-        <v>3892</v>
+        <v>3894</v>
       </c>
     </row>
     <row r="1636" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1636">
-        <v>1664</v>
+        <v>1665</v>
       </c>
       <c r="B1636" t="s">
-        <v>3893</v>
+        <v>3895</v>
       </c>
       <c r="C1636" t="s">
         <v>3875</v>
@@ -61263,15 +61286,15 @@
         <v>1353</v>
       </c>
       <c r="M1636" t="s">
-        <v>3894</v>
+        <v>3896</v>
       </c>
     </row>
     <row r="1637" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1637">
-        <v>1665</v>
+        <v>1666</v>
       </c>
       <c r="B1637" t="s">
-        <v>3895</v>
+        <v>3897</v>
       </c>
       <c r="C1637" t="s">
         <v>3875</v>
@@ -61286,15 +61309,15 @@
         <v>1353</v>
       </c>
       <c r="M1637" t="s">
-        <v>3896</v>
+        <v>3898</v>
       </c>
     </row>
     <row r="1638" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1638">
-        <v>1666</v>
+        <v>1667</v>
       </c>
       <c r="B1638" t="s">
-        <v>3897</v>
+        <v>3899</v>
       </c>
       <c r="C1638" t="s">
         <v>3875</v>
@@ -61309,15 +61332,15 @@
         <v>1353</v>
       </c>
       <c r="M1638" t="s">
-        <v>3898</v>
+        <v>4496</v>
       </c>
     </row>
     <row r="1639" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1639">
-        <v>1667</v>
+        <v>1668</v>
       </c>
       <c r="B1639" t="s">
-        <v>3899</v>
+        <v>3900</v>
       </c>
       <c r="C1639" t="s">
         <v>3875</v>
@@ -61332,15 +61355,15 @@
         <v>1353</v>
       </c>
       <c r="M1639" t="s">
-        <v>4496</v>
+        <v>4497</v>
       </c>
     </row>
     <row r="1640" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1640">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="B1640" t="s">
-        <v>3900</v>
+        <v>3901</v>
       </c>
       <c r="C1640" t="s">
         <v>3875</v>
@@ -61355,15 +61378,15 @@
         <v>1353</v>
       </c>
       <c r="M1640" t="s">
-        <v>4497</v>
+        <v>3902</v>
       </c>
     </row>
     <row r="1641" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1641">
-        <v>1669</v>
+        <v>1670</v>
       </c>
       <c r="B1641" t="s">
-        <v>3901</v>
+        <v>3903</v>
       </c>
       <c r="C1641" t="s">
         <v>3875</v>
@@ -61378,15 +61401,15 @@
         <v>1353</v>
       </c>
       <c r="M1641" t="s">
-        <v>3902</v>
+        <v>3904</v>
       </c>
     </row>
     <row r="1642" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1642">
-        <v>1670</v>
+        <v>1671</v>
       </c>
       <c r="B1642" t="s">
-        <v>3903</v>
+        <v>3905</v>
       </c>
       <c r="C1642" t="s">
         <v>3875</v>
@@ -61401,15 +61424,15 @@
         <v>1353</v>
       </c>
       <c r="M1642" t="s">
-        <v>3904</v>
+        <v>3906</v>
       </c>
     </row>
     <row r="1643" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1643">
-        <v>1671</v>
+        <v>1672</v>
       </c>
       <c r="B1643" t="s">
-        <v>3905</v>
+        <v>3907</v>
       </c>
       <c r="C1643" t="s">
         <v>3875</v>
@@ -61424,15 +61447,15 @@
         <v>1353</v>
       </c>
       <c r="M1643" t="s">
-        <v>3906</v>
+        <v>3908</v>
       </c>
     </row>
     <row r="1644" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1644">
-        <v>1672</v>
+        <v>1673</v>
       </c>
       <c r="B1644" t="s">
-        <v>3907</v>
+        <v>3909</v>
       </c>
       <c r="C1644" t="s">
         <v>3875</v>
@@ -61447,15 +61470,15 @@
         <v>1353</v>
       </c>
       <c r="M1644" t="s">
-        <v>3908</v>
+        <v>3910</v>
       </c>
     </row>
     <row r="1645" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1645">
-        <v>1673</v>
+        <v>1674</v>
       </c>
       <c r="B1645" t="s">
-        <v>3909</v>
+        <v>3911</v>
       </c>
       <c r="C1645" t="s">
         <v>3875</v>
@@ -61470,15 +61493,15 @@
         <v>1353</v>
       </c>
       <c r="M1645" t="s">
-        <v>3910</v>
+        <v>3912</v>
       </c>
     </row>
     <row r="1646" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1646">
-        <v>1674</v>
+        <v>1675</v>
       </c>
       <c r="B1646" t="s">
-        <v>3911</v>
+        <v>3913</v>
       </c>
       <c r="C1646" t="s">
         <v>3875</v>
@@ -61493,15 +61516,15 @@
         <v>1353</v>
       </c>
       <c r="M1646" t="s">
-        <v>3912</v>
+        <v>4498</v>
       </c>
     </row>
     <row r="1647" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1647">
-        <v>1675</v>
+        <v>1676</v>
       </c>
       <c r="B1647" t="s">
-        <v>3913</v>
+        <v>3914</v>
       </c>
       <c r="C1647" t="s">
         <v>3875</v>
@@ -61516,15 +61539,15 @@
         <v>1353</v>
       </c>
       <c r="M1647" t="s">
-        <v>4498</v>
+        <v>3915</v>
       </c>
     </row>
     <row r="1648" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1648">
-        <v>1676</v>
+        <v>1677</v>
       </c>
       <c r="B1648" t="s">
-        <v>3914</v>
+        <v>3916</v>
       </c>
       <c r="C1648" t="s">
         <v>3875</v>
@@ -61539,15 +61562,15 @@
         <v>1353</v>
       </c>
       <c r="M1648" t="s">
-        <v>3915</v>
+        <v>3917</v>
       </c>
     </row>
     <row r="1649" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1649">
-        <v>1677</v>
+        <v>1678</v>
       </c>
       <c r="B1649" t="s">
-        <v>3916</v>
+        <v>3918</v>
       </c>
       <c r="C1649" t="s">
         <v>3875</v>
@@ -61562,15 +61585,15 @@
         <v>1353</v>
       </c>
       <c r="M1649" t="s">
-        <v>3917</v>
+        <v>3919</v>
       </c>
     </row>
     <row r="1650" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1650">
-        <v>1678</v>
+        <v>1679</v>
       </c>
       <c r="B1650" t="s">
-        <v>3918</v>
+        <v>3920</v>
       </c>
       <c r="C1650" t="s">
         <v>3875</v>
@@ -61585,15 +61608,15 @@
         <v>1353</v>
       </c>
       <c r="M1650" t="s">
-        <v>3919</v>
+        <v>4499</v>
       </c>
     </row>
     <row r="1651" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1651">
-        <v>1679</v>
+        <v>1680</v>
       </c>
       <c r="B1651" t="s">
-        <v>3920</v>
+        <v>3921</v>
       </c>
       <c r="C1651" t="s">
         <v>3875</v>
@@ -61608,15 +61631,15 @@
         <v>1353</v>
       </c>
       <c r="M1651" t="s">
-        <v>4499</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="1652" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1652">
-        <v>1680</v>
+        <v>1681</v>
       </c>
       <c r="B1652" t="s">
-        <v>3921</v>
+        <v>3922</v>
       </c>
       <c r="C1652" t="s">
         <v>3875</v>
@@ -61631,15 +61654,15 @@
         <v>1353</v>
       </c>
       <c r="M1652" t="s">
-        <v>4500</v>
+        <v>4501</v>
       </c>
     </row>
     <row r="1653" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1653">
-        <v>1681</v>
+        <v>1682</v>
       </c>
       <c r="B1653" t="s">
-        <v>3922</v>
+        <v>3923</v>
       </c>
       <c r="C1653" t="s">
         <v>3875</v>
@@ -61654,15 +61677,15 @@
         <v>1353</v>
       </c>
       <c r="M1653" t="s">
-        <v>4501</v>
+        <v>3924</v>
       </c>
     </row>
     <row r="1654" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1654">
-        <v>1682</v>
+        <v>1683</v>
       </c>
       <c r="B1654" t="s">
-        <v>3923</v>
+        <v>3925</v>
       </c>
       <c r="C1654" t="s">
         <v>3875</v>
@@ -61677,15 +61700,15 @@
         <v>1353</v>
       </c>
       <c r="M1654" t="s">
-        <v>3924</v>
+        <v>3926</v>
       </c>
     </row>
     <row r="1655" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1655">
-        <v>1683</v>
+        <v>1684</v>
       </c>
       <c r="B1655" t="s">
-        <v>3925</v>
+        <v>3927</v>
       </c>
       <c r="C1655" t="s">
         <v>3875</v>
@@ -61700,15 +61723,15 @@
         <v>1353</v>
       </c>
       <c r="M1655" t="s">
-        <v>3926</v>
+        <v>4502</v>
       </c>
     </row>
     <row r="1656" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1656">
-        <v>1684</v>
+        <v>1685</v>
       </c>
       <c r="B1656" t="s">
-        <v>3927</v>
+        <v>3928</v>
       </c>
       <c r="C1656" t="s">
         <v>3875</v>
@@ -61723,15 +61746,15 @@
         <v>1353</v>
       </c>
       <c r="M1656" t="s">
-        <v>4502</v>
+        <v>3929</v>
       </c>
     </row>
     <row r="1657" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1657">
-        <v>1685</v>
+        <v>1686</v>
       </c>
       <c r="B1657" t="s">
-        <v>3928</v>
+        <v>3930</v>
       </c>
       <c r="C1657" t="s">
         <v>3875</v>
@@ -61746,15 +61769,15 @@
         <v>1353</v>
       </c>
       <c r="M1657" t="s">
-        <v>3929</v>
+        <v>4503</v>
       </c>
     </row>
     <row r="1658" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1658">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="B1658" t="s">
-        <v>3930</v>
+        <v>3931</v>
       </c>
       <c r="C1658" t="s">
         <v>3875</v>
@@ -61769,15 +61792,15 @@
         <v>1353</v>
       </c>
       <c r="M1658" t="s">
-        <v>4503</v>
+        <v>3932</v>
       </c>
     </row>
     <row r="1659" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1659">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="B1659" t="s">
-        <v>3931</v>
+        <v>3933</v>
       </c>
       <c r="C1659" t="s">
         <v>3875</v>
@@ -61792,15 +61815,15 @@
         <v>1353</v>
       </c>
       <c r="M1659" t="s">
-        <v>3932</v>
+        <v>3934</v>
       </c>
     </row>
     <row r="1660" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1660">
-        <v>1688</v>
+        <v>1689</v>
       </c>
       <c r="B1660" t="s">
-        <v>3933</v>
+        <v>3935</v>
       </c>
       <c r="C1660" t="s">
         <v>3875</v>
@@ -61815,15 +61838,15 @@
         <v>1353</v>
       </c>
       <c r="M1660" t="s">
-        <v>3934</v>
+        <v>4504</v>
       </c>
     </row>
     <row r="1661" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1661">
-        <v>1689</v>
+        <v>1690</v>
       </c>
       <c r="B1661" t="s">
-        <v>3935</v>
+        <v>3936</v>
       </c>
       <c r="C1661" t="s">
         <v>3875</v>
@@ -61838,15 +61861,15 @@
         <v>1353</v>
       </c>
       <c r="M1661" t="s">
-        <v>4504</v>
+        <v>4505</v>
       </c>
     </row>
     <row r="1662" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1662">
-        <v>1690</v>
+        <v>1691</v>
       </c>
       <c r="B1662" t="s">
-        <v>3936</v>
+        <v>3937</v>
       </c>
       <c r="C1662" t="s">
         <v>3875</v>
@@ -61861,15 +61884,15 @@
         <v>1353</v>
       </c>
       <c r="M1662" t="s">
-        <v>4505</v>
+        <v>3938</v>
       </c>
     </row>
     <row r="1663" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1663">
-        <v>1691</v>
+        <v>1692</v>
       </c>
       <c r="B1663" t="s">
-        <v>3937</v>
+        <v>3939</v>
       </c>
       <c r="C1663" t="s">
         <v>3875</v>
@@ -61884,15 +61907,15 @@
         <v>1353</v>
       </c>
       <c r="M1663" t="s">
-        <v>3938</v>
+        <v>4506</v>
       </c>
     </row>
     <row r="1664" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1664">
-        <v>1692</v>
+        <v>1693</v>
       </c>
       <c r="B1664" t="s">
-        <v>3939</v>
+        <v>3940</v>
       </c>
       <c r="C1664" t="s">
         <v>3875</v>
@@ -61907,15 +61930,15 @@
         <v>1353</v>
       </c>
       <c r="M1664" t="s">
-        <v>4506</v>
+        <v>4507</v>
       </c>
     </row>
     <row r="1665" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1665">
-        <v>1693</v>
+        <v>1694</v>
       </c>
       <c r="B1665" t="s">
-        <v>3940</v>
+        <v>3941</v>
       </c>
       <c r="C1665" t="s">
         <v>3875</v>
@@ -61930,15 +61953,15 @@
         <v>1353</v>
       </c>
       <c r="M1665" t="s">
-        <v>4507</v>
+        <v>4508</v>
       </c>
     </row>
     <row r="1666" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1666">
-        <v>1694</v>
+        <v>1695</v>
       </c>
       <c r="B1666" t="s">
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C1666" t="s">
         <v>3875</v>
@@ -61953,15 +61976,15 @@
         <v>1353</v>
       </c>
       <c r="M1666" t="s">
-        <v>4508</v>
+        <v>4509</v>
       </c>
     </row>
     <row r="1667" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1667">
-        <v>1695</v>
+        <v>1696</v>
       </c>
       <c r="B1667" t="s">
-        <v>3942</v>
+        <v>3943</v>
       </c>
       <c r="C1667" t="s">
         <v>3875</v>
@@ -61976,15 +61999,15 @@
         <v>1353</v>
       </c>
       <c r="M1667" t="s">
-        <v>4509</v>
+        <v>4510</v>
       </c>
     </row>
     <row r="1668" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1668">
-        <v>1696</v>
+        <v>1697</v>
       </c>
       <c r="B1668" t="s">
-        <v>3943</v>
+        <v>3944</v>
       </c>
       <c r="C1668" t="s">
         <v>3875</v>
@@ -61999,15 +62022,15 @@
         <v>1353</v>
       </c>
       <c r="M1668" t="s">
-        <v>4510</v>
+        <v>4511</v>
       </c>
     </row>
     <row r="1669" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1669">
-        <v>1697</v>
+        <v>1698</v>
       </c>
       <c r="B1669" t="s">
-        <v>3944</v>
+        <v>3945</v>
       </c>
       <c r="C1669" t="s">
         <v>3875</v>
@@ -62022,15 +62045,15 @@
         <v>1353</v>
       </c>
       <c r="M1669" t="s">
-        <v>4511</v>
+        <v>4512</v>
       </c>
     </row>
     <row r="1670" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1670">
-        <v>1698</v>
+        <v>1699</v>
       </c>
       <c r="B1670" t="s">
-        <v>3945</v>
+        <v>3946</v>
       </c>
       <c r="C1670" t="s">
         <v>3875</v>
@@ -62045,15 +62068,15 @@
         <v>1353</v>
       </c>
       <c r="M1670" t="s">
-        <v>4512</v>
+        <v>3947</v>
       </c>
     </row>
     <row r="1671" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1671">
-        <v>1699</v>
+        <v>1700</v>
       </c>
       <c r="B1671" t="s">
-        <v>3946</v>
+        <v>3948</v>
       </c>
       <c r="C1671" t="s">
         <v>3875</v>
@@ -62068,15 +62091,15 @@
         <v>1353</v>
       </c>
       <c r="M1671" t="s">
-        <v>3947</v>
+        <v>3949</v>
       </c>
     </row>
     <row r="1672" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1672">
-        <v>1700</v>
+        <v>1701</v>
       </c>
       <c r="B1672" t="s">
-        <v>3948</v>
+        <v>3950</v>
       </c>
       <c r="C1672" t="s">
         <v>3875</v>
@@ -62091,15 +62114,15 @@
         <v>1353</v>
       </c>
       <c r="M1672" t="s">
-        <v>3949</v>
+        <v>3951</v>
       </c>
     </row>
     <row r="1673" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1673">
-        <v>1701</v>
+        <v>1702</v>
       </c>
       <c r="B1673" t="s">
-        <v>3950</v>
+        <v>3952</v>
       </c>
       <c r="C1673" t="s">
         <v>3875</v>
@@ -62114,15 +62137,15 @@
         <v>1353</v>
       </c>
       <c r="M1673" t="s">
-        <v>3951</v>
+        <v>4513</v>
       </c>
     </row>
     <row r="1674" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1674">
-        <v>1702</v>
+        <v>1703</v>
       </c>
       <c r="B1674" t="s">
-        <v>3952</v>
+        <v>3953</v>
       </c>
       <c r="C1674" t="s">
         <v>3875</v>
@@ -62137,15 +62160,15 @@
         <v>1353</v>
       </c>
       <c r="M1674" t="s">
-        <v>4513</v>
+        <v>3954</v>
       </c>
     </row>
     <row r="1675" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1675">
-        <v>1703</v>
+        <v>1704</v>
       </c>
       <c r="B1675" t="s">
-        <v>3953</v>
+        <v>3955</v>
       </c>
       <c r="C1675" t="s">
         <v>3875</v>
@@ -62160,15 +62183,15 @@
         <v>1353</v>
       </c>
       <c r="M1675" t="s">
-        <v>3954</v>
+        <v>3956</v>
       </c>
     </row>
     <row r="1676" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1676">
-        <v>1704</v>
+        <v>1705</v>
       </c>
       <c r="B1676" t="s">
-        <v>3955</v>
+        <v>3957</v>
       </c>
       <c r="C1676" t="s">
         <v>3875</v>
@@ -62183,15 +62206,15 @@
         <v>1353</v>
       </c>
       <c r="M1676" t="s">
-        <v>3956</v>
+        <v>4514</v>
       </c>
     </row>
     <row r="1677" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1677">
-        <v>1705</v>
+        <v>1706</v>
       </c>
       <c r="B1677" t="s">
-        <v>3957</v>
+        <v>3958</v>
       </c>
       <c r="C1677" t="s">
         <v>3875</v>
@@ -62206,15 +62229,15 @@
         <v>1353</v>
       </c>
       <c r="M1677" t="s">
-        <v>4514</v>
+        <v>3959</v>
       </c>
     </row>
     <row r="1678" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1678">
-        <v>1706</v>
+        <v>1707</v>
       </c>
       <c r="B1678" t="s">
-        <v>3958</v>
+        <v>3960</v>
       </c>
       <c r="C1678" t="s">
         <v>3875</v>
@@ -62229,15 +62252,15 @@
         <v>1353</v>
       </c>
       <c r="M1678" t="s">
-        <v>3959</v>
+        <v>4515</v>
       </c>
     </row>
     <row r="1679" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1679">
-        <v>1707</v>
+        <v>1708</v>
       </c>
       <c r="B1679" t="s">
-        <v>3960</v>
+        <v>3961</v>
       </c>
       <c r="C1679" t="s">
         <v>3875</v>
@@ -62252,15 +62275,15 @@
         <v>1353</v>
       </c>
       <c r="M1679" t="s">
-        <v>4515</v>
+        <v>4516</v>
       </c>
     </row>
     <row r="1680" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1680">
-        <v>1708</v>
+        <v>1709</v>
       </c>
       <c r="B1680" t="s">
-        <v>3961</v>
+        <v>3962</v>
       </c>
       <c r="C1680" t="s">
         <v>3875</v>
@@ -62275,15 +62298,15 @@
         <v>1353</v>
       </c>
       <c r="M1680" t="s">
-        <v>4516</v>
+        <v>4517</v>
       </c>
     </row>
     <row r="1681" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1681">
-        <v>1709</v>
+        <v>1710</v>
       </c>
       <c r="B1681" t="s">
-        <v>3962</v>
+        <v>3963</v>
       </c>
       <c r="C1681" t="s">
         <v>3875</v>
@@ -62298,15 +62321,15 @@
         <v>1353</v>
       </c>
       <c r="M1681" t="s">
-        <v>4517</v>
+        <v>4518</v>
       </c>
     </row>
     <row r="1682" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1682">
-        <v>1710</v>
+        <v>1711</v>
       </c>
       <c r="B1682" t="s">
-        <v>3963</v>
+        <v>3964</v>
       </c>
       <c r="C1682" t="s">
         <v>3875</v>
@@ -62321,15 +62344,15 @@
         <v>1353</v>
       </c>
       <c r="M1682" t="s">
-        <v>4518</v>
+        <v>4519</v>
       </c>
     </row>
     <row r="1683" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1683">
-        <v>1711</v>
+        <v>1712</v>
       </c>
       <c r="B1683" t="s">
-        <v>3964</v>
+        <v>3965</v>
       </c>
       <c r="C1683" t="s">
         <v>3875</v>
@@ -62344,15 +62367,15 @@
         <v>1353</v>
       </c>
       <c r="M1683" t="s">
-        <v>4519</v>
+        <v>4520</v>
       </c>
     </row>
     <row r="1684" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1684">
-        <v>1712</v>
+        <v>1713</v>
       </c>
       <c r="B1684" t="s">
-        <v>3965</v>
+        <v>3966</v>
       </c>
       <c r="C1684" t="s">
         <v>3875</v>
@@ -62367,15 +62390,15 @@
         <v>1353</v>
       </c>
       <c r="M1684" t="s">
-        <v>4520</v>
+        <v>3967</v>
       </c>
     </row>
     <row r="1685" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1685">
-        <v>1713</v>
+        <v>1714</v>
       </c>
       <c r="B1685" t="s">
-        <v>3966</v>
+        <v>3968</v>
       </c>
       <c r="C1685" t="s">
         <v>3875</v>
@@ -62390,15 +62413,15 @@
         <v>1353</v>
       </c>
       <c r="M1685" t="s">
-        <v>3967</v>
+        <v>4521</v>
       </c>
     </row>
     <row r="1686" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1686">
-        <v>1714</v>
+        <v>1715</v>
       </c>
       <c r="B1686" t="s">
-        <v>3968</v>
+        <v>3969</v>
       </c>
       <c r="C1686" t="s">
         <v>3875</v>
@@ -62413,15 +62436,15 @@
         <v>1353</v>
       </c>
       <c r="M1686" t="s">
-        <v>4521</v>
+        <v>4522</v>
       </c>
     </row>
     <row r="1687" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1687">
-        <v>1715</v>
+        <v>1716</v>
       </c>
       <c r="B1687" t="s">
-        <v>3969</v>
+        <v>3970</v>
       </c>
       <c r="C1687" t="s">
         <v>3875</v>
@@ -62436,15 +62459,15 @@
         <v>1353</v>
       </c>
       <c r="M1687" t="s">
-        <v>4522</v>
+        <v>3971</v>
       </c>
     </row>
     <row r="1688" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1688">
-        <v>1716</v>
+        <v>1717</v>
       </c>
       <c r="B1688" t="s">
-        <v>3970</v>
+        <v>3972</v>
       </c>
       <c r="C1688" t="s">
         <v>3875</v>
@@ -62459,15 +62482,15 @@
         <v>1353</v>
       </c>
       <c r="M1688" t="s">
-        <v>3971</v>
+        <v>3973</v>
       </c>
     </row>
     <row r="1689" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1689">
-        <v>1717</v>
+        <v>1718</v>
       </c>
       <c r="B1689" t="s">
-        <v>3972</v>
+        <v>3974</v>
       </c>
       <c r="C1689" t="s">
         <v>3875</v>
@@ -62482,15 +62505,15 @@
         <v>1353</v>
       </c>
       <c r="M1689" t="s">
-        <v>3973</v>
+        <v>4523</v>
       </c>
     </row>
     <row r="1690" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1690">
-        <v>1718</v>
+        <v>1719</v>
       </c>
       <c r="B1690" t="s">
-        <v>3974</v>
+        <v>3975</v>
       </c>
       <c r="C1690" t="s">
         <v>3875</v>
@@ -62505,15 +62528,15 @@
         <v>1353</v>
       </c>
       <c r="M1690" t="s">
-        <v>4523</v>
+        <v>3976</v>
       </c>
     </row>
     <row r="1691" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1691">
-        <v>1719</v>
+        <v>1720</v>
       </c>
       <c r="B1691" t="s">
-        <v>3975</v>
+        <v>3977</v>
       </c>
       <c r="C1691" t="s">
         <v>3875</v>
@@ -62528,15 +62551,15 @@
         <v>1353</v>
       </c>
       <c r="M1691" t="s">
-        <v>3976</v>
+        <v>4524</v>
       </c>
     </row>
     <row r="1692" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1692">
-        <v>1720</v>
+        <v>1721</v>
       </c>
       <c r="B1692" t="s">
-        <v>3977</v>
+        <v>3978</v>
       </c>
       <c r="C1692" t="s">
         <v>3875</v>
@@ -62551,15 +62574,15 @@
         <v>1353</v>
       </c>
       <c r="M1692" t="s">
-        <v>4524</v>
+        <v>4525</v>
       </c>
     </row>
     <row r="1693" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1693">
-        <v>1721</v>
+        <v>1722</v>
       </c>
       <c r="B1693" t="s">
-        <v>3978</v>
+        <v>3979</v>
       </c>
       <c r="C1693" t="s">
         <v>3875</v>
@@ -62574,15 +62597,15 @@
         <v>1353</v>
       </c>
       <c r="M1693" t="s">
-        <v>4525</v>
+        <v>4526</v>
       </c>
     </row>
     <row r="1694" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1694">
-        <v>1722</v>
+        <v>1723</v>
       </c>
       <c r="B1694" t="s">
-        <v>3979</v>
+        <v>3980</v>
       </c>
       <c r="C1694" t="s">
         <v>3875</v>
@@ -62597,15 +62620,15 @@
         <v>1353</v>
       </c>
       <c r="M1694" t="s">
-        <v>4526</v>
+        <v>4527</v>
       </c>
     </row>
     <row r="1695" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1695">
-        <v>1723</v>
+        <v>1724</v>
       </c>
       <c r="B1695" t="s">
-        <v>3980</v>
+        <v>3981</v>
       </c>
       <c r="C1695" t="s">
         <v>3875</v>
@@ -62620,15 +62643,15 @@
         <v>1353</v>
       </c>
       <c r="M1695" t="s">
-        <v>4527</v>
+        <v>4528</v>
       </c>
     </row>
     <row r="1696" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1696">
-        <v>1724</v>
+        <v>1725</v>
       </c>
       <c r="B1696" t="s">
-        <v>3981</v>
+        <v>3982</v>
       </c>
       <c r="C1696" t="s">
         <v>3875</v>
@@ -62643,15 +62666,15 @@
         <v>1353</v>
       </c>
       <c r="M1696" t="s">
-        <v>4528</v>
+        <v>3983</v>
       </c>
     </row>
     <row r="1697" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1697">
-        <v>1725</v>
+        <v>1726</v>
       </c>
       <c r="B1697" t="s">
-        <v>3982</v>
+        <v>3984</v>
       </c>
       <c r="C1697" t="s">
         <v>3875</v>
@@ -62666,15 +62689,15 @@
         <v>1353</v>
       </c>
       <c r="M1697" t="s">
-        <v>3983</v>
+        <v>4529</v>
       </c>
     </row>
     <row r="1698" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1698">
-        <v>1726</v>
+        <v>1727</v>
       </c>
       <c r="B1698" t="s">
-        <v>3984</v>
+        <v>3985</v>
       </c>
       <c r="C1698" t="s">
         <v>3875</v>
@@ -62689,15 +62712,15 @@
         <v>1353</v>
       </c>
       <c r="M1698" t="s">
-        <v>4529</v>
+        <v>3986</v>
       </c>
     </row>
     <row r="1699" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1699">
-        <v>1727</v>
+        <v>1728</v>
       </c>
       <c r="B1699" t="s">
-        <v>3985</v>
+        <v>3987</v>
       </c>
       <c r="C1699" t="s">
         <v>3875</v>
@@ -62712,15 +62735,15 @@
         <v>1353</v>
       </c>
       <c r="M1699" t="s">
-        <v>3986</v>
+        <v>4530</v>
       </c>
     </row>
     <row r="1700" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1700">
-        <v>1728</v>
+        <v>1729</v>
       </c>
       <c r="B1700" t="s">
-        <v>3987</v>
+        <v>3988</v>
       </c>
       <c r="C1700" t="s">
         <v>3875</v>
@@ -62735,15 +62758,15 @@
         <v>1353</v>
       </c>
       <c r="M1700" t="s">
-        <v>4530</v>
+        <v>3989</v>
       </c>
     </row>
     <row r="1701" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1701">
-        <v>1729</v>
+        <v>1730</v>
       </c>
       <c r="B1701" t="s">
-        <v>3988</v>
+        <v>3990</v>
       </c>
       <c r="C1701" t="s">
         <v>3875</v>
@@ -62758,15 +62781,15 @@
         <v>1353</v>
       </c>
       <c r="M1701" t="s">
-        <v>3989</v>
+        <v>3991</v>
       </c>
     </row>
     <row r="1702" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1702">
-        <v>1730</v>
+        <v>1731</v>
       </c>
       <c r="B1702" t="s">
-        <v>3990</v>
+        <v>3992</v>
       </c>
       <c r="C1702" t="s">
         <v>3875</v>
@@ -62781,15 +62804,15 @@
         <v>1353</v>
       </c>
       <c r="M1702" t="s">
-        <v>3991</v>
+        <v>4531</v>
       </c>
     </row>
     <row r="1703" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1703">
-        <v>1731</v>
+        <v>1732</v>
       </c>
       <c r="B1703" t="s">
-        <v>3992</v>
+        <v>3993</v>
       </c>
       <c r="C1703" t="s">
         <v>3875</v>
@@ -62804,15 +62827,15 @@
         <v>1353</v>
       </c>
       <c r="M1703" t="s">
-        <v>4531</v>
+        <v>4532</v>
       </c>
     </row>
     <row r="1704" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1704">
-        <v>1732</v>
+        <v>1733</v>
       </c>
       <c r="B1704" t="s">
-        <v>3993</v>
+        <v>3994</v>
       </c>
       <c r="C1704" t="s">
         <v>3875</v>
@@ -62827,15 +62850,15 @@
         <v>1353</v>
       </c>
       <c r="M1704" t="s">
-        <v>4532</v>
+        <v>3995</v>
       </c>
     </row>
     <row r="1705" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1705">
-        <v>1733</v>
+        <v>1734</v>
       </c>
       <c r="B1705" t="s">
-        <v>3994</v>
+        <v>3996</v>
       </c>
       <c r="C1705" t="s">
         <v>3875</v>
@@ -62850,15 +62873,15 @@
         <v>1353</v>
       </c>
       <c r="M1705" t="s">
-        <v>3995</v>
+        <v>3997</v>
       </c>
     </row>
     <row r="1706" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1706">
-        <v>1734</v>
+        <v>1735</v>
       </c>
       <c r="B1706" t="s">
-        <v>3996</v>
+        <v>3998</v>
       </c>
       <c r="C1706" t="s">
         <v>3875</v>
@@ -62873,15 +62896,15 @@
         <v>1353</v>
       </c>
       <c r="M1706" t="s">
-        <v>3997</v>
+        <v>4533</v>
       </c>
     </row>
     <row r="1707" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1707">
-        <v>1735</v>
+        <v>1736</v>
       </c>
       <c r="B1707" t="s">
-        <v>3998</v>
+        <v>3999</v>
       </c>
       <c r="C1707" t="s">
         <v>3875</v>
@@ -62896,15 +62919,15 @@
         <v>1353</v>
       </c>
       <c r="M1707" t="s">
-        <v>4533</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="1708" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1708">
-        <v>1736</v>
+        <v>1737</v>
       </c>
       <c r="B1708" t="s">
-        <v>3999</v>
+        <v>4001</v>
       </c>
       <c r="C1708" t="s">
         <v>3875</v>
@@ -62919,15 +62942,15 @@
         <v>1353</v>
       </c>
       <c r="M1708" t="s">
-        <v>4000</v>
+        <v>4534</v>
       </c>
     </row>
     <row r="1709" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1709">
-        <v>1737</v>
+        <v>1738</v>
       </c>
       <c r="B1709" t="s">
-        <v>4001</v>
+        <v>4002</v>
       </c>
       <c r="C1709" t="s">
         <v>3875</v>
@@ -62942,15 +62965,15 @@
         <v>1353</v>
       </c>
       <c r="M1709" t="s">
-        <v>4534</v>
+        <v>4535</v>
       </c>
     </row>
     <row r="1710" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1710">
-        <v>1738</v>
+        <v>1739</v>
       </c>
       <c r="B1710" t="s">
-        <v>4002</v>
+        <v>4003</v>
       </c>
       <c r="C1710" t="s">
         <v>3875</v>
@@ -62965,15 +62988,15 @@
         <v>1353</v>
       </c>
       <c r="M1710" t="s">
-        <v>4535</v>
+        <v>4536</v>
       </c>
     </row>
     <row r="1711" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1711">
-        <v>1739</v>
+        <v>1740</v>
       </c>
       <c r="B1711" t="s">
-        <v>4003</v>
+        <v>4004</v>
       </c>
       <c r="C1711" t="s">
         <v>3875</v>
@@ -62988,15 +63011,15 @@
         <v>1353</v>
       </c>
       <c r="M1711" t="s">
-        <v>4536</v>
+        <v>4537</v>
       </c>
     </row>
     <row r="1712" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1712">
-        <v>1740</v>
+        <v>1741</v>
       </c>
       <c r="B1712" t="s">
-        <v>4004</v>
+        <v>4005</v>
       </c>
       <c r="C1712" t="s">
         <v>3875</v>
@@ -63011,15 +63034,15 @@
         <v>1353</v>
       </c>
       <c r="M1712" t="s">
-        <v>4537</v>
+        <v>4538</v>
       </c>
     </row>
     <row r="1713" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1713">
-        <v>1741</v>
+        <v>1742</v>
       </c>
       <c r="B1713" t="s">
-        <v>4005</v>
+        <v>4006</v>
       </c>
       <c r="C1713" t="s">
         <v>3875</v>
@@ -63034,15 +63057,15 @@
         <v>1353</v>
       </c>
       <c r="M1713" t="s">
-        <v>4538</v>
+        <v>4539</v>
       </c>
     </row>
     <row r="1714" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1714">
-        <v>1742</v>
+        <v>1743</v>
       </c>
       <c r="B1714" t="s">
-        <v>4006</v>
+        <v>4007</v>
       </c>
       <c r="C1714" t="s">
         <v>3875</v>
@@ -63057,15 +63080,15 @@
         <v>1353</v>
       </c>
       <c r="M1714" t="s">
-        <v>4539</v>
+        <v>4008</v>
       </c>
     </row>
     <row r="1715" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1715">
-        <v>1743</v>
+        <v>1744</v>
       </c>
       <c r="B1715" t="s">
-        <v>4007</v>
+        <v>4009</v>
       </c>
       <c r="C1715" t="s">
         <v>3875</v>
@@ -63080,15 +63103,15 @@
         <v>1353</v>
       </c>
       <c r="M1715" t="s">
-        <v>4008</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="1716" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1716">
-        <v>1744</v>
+        <v>1745</v>
       </c>
       <c r="B1716" t="s">
-        <v>4009</v>
+        <v>4010</v>
       </c>
       <c r="C1716" t="s">
         <v>3875</v>
@@ -63103,15 +63126,15 @@
         <v>1353</v>
       </c>
       <c r="M1716" t="s">
-        <v>4540</v>
+        <v>4541</v>
       </c>
     </row>
     <row r="1717" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1717">
-        <v>1745</v>
+        <v>1746</v>
       </c>
       <c r="B1717" t="s">
-        <v>4010</v>
+        <v>4011</v>
       </c>
       <c r="C1717" t="s">
         <v>3875</v>
@@ -63126,15 +63149,15 @@
         <v>1353</v>
       </c>
       <c r="M1717" t="s">
-        <v>4541</v>
+        <v>4012</v>
       </c>
     </row>
     <row r="1718" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1718">
-        <v>1746</v>
+        <v>1747</v>
       </c>
       <c r="B1718" t="s">
-        <v>4011</v>
+        <v>4013</v>
       </c>
       <c r="C1718" t="s">
         <v>3875</v>
@@ -63149,15 +63172,15 @@
         <v>1353</v>
       </c>
       <c r="M1718" t="s">
-        <v>4012</v>
+        <v>4542</v>
       </c>
     </row>
     <row r="1719" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1719">
-        <v>1747</v>
+        <v>1748</v>
       </c>
       <c r="B1719" t="s">
-        <v>4013</v>
+        <v>4014</v>
       </c>
       <c r="C1719" t="s">
         <v>3875</v>
@@ -63172,15 +63195,15 @@
         <v>1353</v>
       </c>
       <c r="M1719" t="s">
-        <v>4542</v>
+        <v>4015</v>
       </c>
     </row>
     <row r="1720" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1720">
-        <v>1748</v>
+        <v>1749</v>
       </c>
       <c r="B1720" t="s">
-        <v>4014</v>
+        <v>4016</v>
       </c>
       <c r="C1720" t="s">
         <v>3875</v>
@@ -63195,15 +63218,15 @@
         <v>1353</v>
       </c>
       <c r="M1720" t="s">
-        <v>4015</v>
+        <v>4017</v>
       </c>
     </row>
     <row r="1721" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1721">
-        <v>1749</v>
+        <v>1750</v>
       </c>
       <c r="B1721" t="s">
-        <v>4016</v>
+        <v>4018</v>
       </c>
       <c r="C1721" t="s">
         <v>3875</v>
@@ -63218,15 +63241,15 @@
         <v>1353</v>
       </c>
       <c r="M1721" t="s">
-        <v>4017</v>
+        <v>4543</v>
       </c>
     </row>
     <row r="1722" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1722">
-        <v>1750</v>
+        <v>1751</v>
       </c>
       <c r="B1722" t="s">
-        <v>4018</v>
+        <v>4019</v>
       </c>
       <c r="C1722" t="s">
         <v>3875</v>
@@ -63241,15 +63264,15 @@
         <v>1353</v>
       </c>
       <c r="M1722" t="s">
-        <v>4543</v>
+        <v>4020</v>
       </c>
     </row>
     <row r="1723" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1723">
-        <v>1751</v>
+        <v>1752</v>
       </c>
       <c r="B1723" t="s">
-        <v>4019</v>
+        <v>4021</v>
       </c>
       <c r="C1723" t="s">
         <v>3875</v>
@@ -63264,15 +63287,15 @@
         <v>1353</v>
       </c>
       <c r="M1723" t="s">
-        <v>4020</v>
+        <v>4544</v>
       </c>
     </row>
     <row r="1724" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1724">
-        <v>1752</v>
+        <v>1753</v>
       </c>
       <c r="B1724" t="s">
-        <v>4021</v>
+        <v>4022</v>
       </c>
       <c r="C1724" t="s">
         <v>3875</v>
@@ -63287,15 +63310,15 @@
         <v>1353</v>
       </c>
       <c r="M1724" t="s">
-        <v>4544</v>
+        <v>4545</v>
       </c>
     </row>
     <row r="1725" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1725">
-        <v>1753</v>
+        <v>1754</v>
       </c>
       <c r="B1725" t="s">
-        <v>4022</v>
+        <v>4023</v>
       </c>
       <c r="C1725" t="s">
         <v>3875</v>
@@ -63310,15 +63333,15 @@
         <v>1353</v>
       </c>
       <c r="M1725" t="s">
-        <v>4545</v>
+        <v>4546</v>
       </c>
     </row>
     <row r="1726" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1726">
-        <v>1754</v>
+        <v>1755</v>
       </c>
       <c r="B1726" t="s">
-        <v>4023</v>
+        <v>4024</v>
       </c>
       <c r="C1726" t="s">
         <v>3875</v>
@@ -63333,15 +63356,15 @@
         <v>1353</v>
       </c>
       <c r="M1726" t="s">
-        <v>4546</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="1727" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1727">
-        <v>1755</v>
+        <v>1756</v>
       </c>
       <c r="B1727" t="s">
-        <v>4024</v>
+        <v>4025</v>
       </c>
       <c r="C1727" t="s">
         <v>3875</v>
@@ -63356,15 +63379,15 @@
         <v>1353</v>
       </c>
       <c r="M1727" t="s">
-        <v>4547</v>
+        <v>4548</v>
       </c>
     </row>
     <row r="1728" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1728">
-        <v>1756</v>
+        <v>1757</v>
       </c>
       <c r="B1728" t="s">
-        <v>4025</v>
+        <v>4026</v>
       </c>
       <c r="C1728" t="s">
         <v>3875</v>
@@ -63379,15 +63402,15 @@
         <v>1353</v>
       </c>
       <c r="M1728" t="s">
-        <v>4548</v>
+        <v>4027</v>
       </c>
     </row>
     <row r="1729" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1729">
-        <v>1757</v>
+        <v>1758</v>
       </c>
       <c r="B1729" t="s">
-        <v>4026</v>
+        <v>4028</v>
       </c>
       <c r="C1729" t="s">
         <v>3875</v>
@@ -63402,15 +63425,15 @@
         <v>1353</v>
       </c>
       <c r="M1729" t="s">
-        <v>4027</v>
+        <v>4549</v>
       </c>
     </row>
     <row r="1730" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1730">
-        <v>1758</v>
+        <v>1759</v>
       </c>
       <c r="B1730" t="s">
-        <v>4028</v>
+        <v>4029</v>
       </c>
       <c r="C1730" t="s">
         <v>3875</v>
@@ -63425,15 +63448,15 @@
         <v>1353</v>
       </c>
       <c r="M1730" t="s">
-        <v>4549</v>
+        <v>4550</v>
       </c>
     </row>
     <row r="1731" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1731">
-        <v>1759</v>
+        <v>1760</v>
       </c>
       <c r="B1731" t="s">
-        <v>4029</v>
+        <v>4030</v>
       </c>
       <c r="C1731" t="s">
         <v>3875</v>
@@ -63448,15 +63471,15 @@
         <v>1353</v>
       </c>
       <c r="M1731" t="s">
-        <v>4550</v>
+        <v>4031</v>
       </c>
     </row>
     <row r="1732" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1732">
-        <v>1760</v>
+        <v>1761</v>
       </c>
       <c r="B1732" t="s">
-        <v>4030</v>
+        <v>4032</v>
       </c>
       <c r="C1732" t="s">
         <v>3875</v>
@@ -63471,15 +63494,15 @@
         <v>1353</v>
       </c>
       <c r="M1732" t="s">
-        <v>4031</v>
+        <v>4033</v>
       </c>
     </row>
     <row r="1733" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1733">
-        <v>1761</v>
+        <v>1762</v>
       </c>
       <c r="B1733" t="s">
-        <v>4032</v>
+        <v>4034</v>
       </c>
       <c r="C1733" t="s">
         <v>3875</v>
@@ -63494,15 +63517,15 @@
         <v>1353</v>
       </c>
       <c r="M1733" t="s">
-        <v>4033</v>
+        <v>4035</v>
       </c>
     </row>
     <row r="1734" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1734">
-        <v>1762</v>
+        <v>1763</v>
       </c>
       <c r="B1734" t="s">
-        <v>4034</v>
+        <v>4036</v>
       </c>
       <c r="C1734" t="s">
         <v>3875</v>
@@ -63517,15 +63540,15 @@
         <v>1353</v>
       </c>
       <c r="M1734" t="s">
-        <v>4035</v>
+        <v>4037</v>
       </c>
     </row>
     <row r="1735" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1735">
-        <v>1763</v>
+        <v>1764</v>
       </c>
       <c r="B1735" t="s">
-        <v>4036</v>
+        <v>4038</v>
       </c>
       <c r="C1735" t="s">
         <v>3875</v>
@@ -63540,15 +63563,15 @@
         <v>1353</v>
       </c>
       <c r="M1735" t="s">
-        <v>4037</v>
+        <v>4551</v>
       </c>
     </row>
     <row r="1736" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1736">
-        <v>1764</v>
+        <v>1765</v>
       </c>
       <c r="B1736" t="s">
-        <v>4038</v>
+        <v>4039</v>
       </c>
       <c r="C1736" t="s">
         <v>3875</v>
@@ -63563,15 +63586,15 @@
         <v>1353</v>
       </c>
       <c r="M1736" t="s">
-        <v>4551</v>
+        <v>4040</v>
       </c>
     </row>
     <row r="1737" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1737">
-        <v>1765</v>
+        <v>1766</v>
       </c>
       <c r="B1737" t="s">
-        <v>4039</v>
+        <v>4041</v>
       </c>
       <c r="C1737" t="s">
         <v>3875</v>
@@ -63586,15 +63609,15 @@
         <v>1353</v>
       </c>
       <c r="M1737" t="s">
-        <v>4040</v>
+        <v>4042</v>
       </c>
     </row>
     <row r="1738" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1738">
-        <v>1766</v>
+        <v>1767</v>
       </c>
       <c r="B1738" t="s">
-        <v>4041</v>
+        <v>4043</v>
       </c>
       <c r="C1738" t="s">
         <v>3875</v>
@@ -63609,15 +63632,15 @@
         <v>1353</v>
       </c>
       <c r="M1738" t="s">
-        <v>4042</v>
+        <v>4552</v>
       </c>
     </row>
     <row r="1739" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1739">
-        <v>1767</v>
+        <v>1768</v>
       </c>
       <c r="B1739" t="s">
-        <v>4043</v>
+        <v>4044</v>
       </c>
       <c r="C1739" t="s">
         <v>3875</v>
@@ -63632,15 +63655,15 @@
         <v>1353</v>
       </c>
       <c r="M1739" t="s">
-        <v>4552</v>
+        <v>4045</v>
       </c>
     </row>
     <row r="1740" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1740">
-        <v>1768</v>
+        <v>1769</v>
       </c>
       <c r="B1740" t="s">
-        <v>4044</v>
+        <v>4046</v>
       </c>
       <c r="C1740" t="s">
         <v>3875</v>
@@ -63655,15 +63678,15 @@
         <v>1353</v>
       </c>
       <c r="M1740" t="s">
-        <v>4045</v>
+        <v>4553</v>
       </c>
     </row>
     <row r="1741" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1741">
-        <v>1769</v>
+        <v>1770</v>
       </c>
       <c r="B1741" t="s">
-        <v>4046</v>
+        <v>4047</v>
       </c>
       <c r="C1741" t="s">
         <v>3875</v>
@@ -63678,15 +63701,15 @@
         <v>1353</v>
       </c>
       <c r="M1741" t="s">
-        <v>4553</v>
+        <v>4048</v>
       </c>
     </row>
     <row r="1742" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1742">
-        <v>1770</v>
+        <v>1771</v>
       </c>
       <c r="B1742" t="s">
-        <v>4047</v>
+        <v>4049</v>
       </c>
       <c r="C1742" t="s">
         <v>3875</v>
@@ -63701,15 +63724,15 @@
         <v>1353</v>
       </c>
       <c r="M1742" t="s">
-        <v>4048</v>
+        <v>4050</v>
       </c>
     </row>
     <row r="1743" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1743">
-        <v>1771</v>
+        <v>1772</v>
       </c>
       <c r="B1743" t="s">
-        <v>4049</v>
+        <v>4051</v>
       </c>
       <c r="C1743" t="s">
         <v>3875</v>
@@ -63724,15 +63747,15 @@
         <v>1353</v>
       </c>
       <c r="M1743" t="s">
-        <v>4050</v>
+        <v>4052</v>
       </c>
     </row>
     <row r="1744" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1744">
-        <v>1772</v>
+        <v>1773</v>
       </c>
       <c r="B1744" t="s">
-        <v>4051</v>
+        <v>4053</v>
       </c>
       <c r="C1744" t="s">
         <v>3875</v>
@@ -63747,15 +63770,15 @@
         <v>1353</v>
       </c>
       <c r="M1744" t="s">
-        <v>4052</v>
+        <v>4554</v>
       </c>
     </row>
     <row r="1745" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1745">
-        <v>1773</v>
+        <v>1774</v>
       </c>
       <c r="B1745" t="s">
-        <v>4053</v>
+        <v>4054</v>
       </c>
       <c r="C1745" t="s">
         <v>3875</v>
@@ -63770,15 +63793,15 @@
         <v>1353</v>
       </c>
       <c r="M1745" t="s">
-        <v>4554</v>
+        <v>4555</v>
       </c>
     </row>
     <row r="1746" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1746">
-        <v>1774</v>
+        <v>1775</v>
       </c>
       <c r="B1746" t="s">
-        <v>4054</v>
+        <v>4055</v>
       </c>
       <c r="C1746" t="s">
         <v>3875</v>
@@ -63793,15 +63816,15 @@
         <v>1353</v>
       </c>
       <c r="M1746" t="s">
-        <v>4555</v>
+        <v>4556</v>
       </c>
     </row>
     <row r="1747" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1747">
-        <v>1775</v>
+        <v>1776</v>
       </c>
       <c r="B1747" t="s">
-        <v>4055</v>
+        <v>4056</v>
       </c>
       <c r="C1747" t="s">
         <v>3875</v>
@@ -63816,15 +63839,15 @@
         <v>1353</v>
       </c>
       <c r="M1747" t="s">
-        <v>4556</v>
+        <v>4557</v>
       </c>
     </row>
     <row r="1748" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1748">
-        <v>1776</v>
+        <v>1777</v>
       </c>
       <c r="B1748" t="s">
-        <v>4056</v>
+        <v>4057</v>
       </c>
       <c r="C1748" t="s">
         <v>3875</v>
@@ -63839,15 +63862,15 @@
         <v>1353</v>
       </c>
       <c r="M1748" t="s">
-        <v>4557</v>
+        <v>4558</v>
       </c>
     </row>
     <row r="1749" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1749">
-        <v>1777</v>
+        <v>1778</v>
       </c>
       <c r="B1749" t="s">
-        <v>4057</v>
+        <v>4058</v>
       </c>
       <c r="C1749" t="s">
         <v>3875</v>
@@ -63862,15 +63885,15 @@
         <v>1353</v>
       </c>
       <c r="M1749" t="s">
-        <v>4558</v>
+        <v>4059</v>
       </c>
     </row>
     <row r="1750" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1750">
-        <v>1778</v>
+        <v>1779</v>
       </c>
       <c r="B1750" t="s">
-        <v>4058</v>
+        <v>4060</v>
       </c>
       <c r="C1750" t="s">
         <v>3875</v>
@@ -63885,15 +63908,15 @@
         <v>1353</v>
       </c>
       <c r="M1750" t="s">
-        <v>4059</v>
+        <v>4559</v>
       </c>
     </row>
     <row r="1751" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1751">
-        <v>1779</v>
+        <v>1780</v>
       </c>
       <c r="B1751" t="s">
-        <v>4060</v>
+        <v>4061</v>
       </c>
       <c r="C1751" t="s">
         <v>3875</v>
@@ -63908,34 +63931,11 @@
         <v>1353</v>
       </c>
       <c r="M1751" t="s">
-        <v>4559</v>
-      </c>
-    </row>
-    <row r="1752" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1752">
-        <v>1780</v>
-      </c>
-      <c r="B1752" t="s">
-        <v>4061</v>
-      </c>
-      <c r="C1752" t="s">
-        <v>3875</v>
-      </c>
-      <c r="D1752">
-        <v>68000</v>
-      </c>
-      <c r="E1752" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1752" t="s">
-        <v>1353</v>
-      </c>
-      <c r="M1752" t="s">
         <v>4062</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M1752"/>
+  <autoFilter ref="A1:M1751"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
036 : added exctsccr driver
</commit_message>
<xml_diff>
--- a/0.36/compatibility.xlsx
+++ b/0.36/compatibility.xlsx
@@ -17,8 +17,8 @@
     <sheet name="GAME_NOT_WORKING FLAG" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ALL!$A$1:$M$1751</definedName>
-    <definedName name="LIST" localSheetId="1">ALL!$B$1:$M$1751</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ALL!$A$1:$M$1747</definedName>
+    <definedName name="LIST" localSheetId="1">ALL!$B$1:$M$1747</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -14078,10 +14078,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P294"/>
+  <dimension ref="A1:P297"/>
   <sheetViews>
     <sheetView topLeftCell="A275" workbookViewId="0">
-      <selection activeCell="A291" sqref="A291:A294"/>
+      <selection activeCell="A292" sqref="A292:A297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20705,6 +20705,84 @@
         <v>3847</v>
       </c>
     </row>
+    <row r="295" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A295">
+        <v>295</v>
+      </c>
+      <c r="B295" t="s">
+        <v>3832</v>
+      </c>
+      <c r="C295" t="s">
+        <v>3833</v>
+      </c>
+      <c r="D295" t="s">
+        <v>14</v>
+      </c>
+      <c r="E295" t="s">
+        <v>14</v>
+      </c>
+      <c r="H295" t="s">
+        <v>1236</v>
+      </c>
+      <c r="I295" t="s">
+        <v>333</v>
+      </c>
+      <c r="M295" t="s">
+        <v>3834</v>
+      </c>
+    </row>
+    <row r="296" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A296">
+        <v>296</v>
+      </c>
+      <c r="B296" t="s">
+        <v>3835</v>
+      </c>
+      <c r="C296" t="s">
+        <v>3833</v>
+      </c>
+      <c r="D296" t="s">
+        <v>14</v>
+      </c>
+      <c r="E296" t="s">
+        <v>14</v>
+      </c>
+      <c r="H296" t="s">
+        <v>1236</v>
+      </c>
+      <c r="I296" t="s">
+        <v>333</v>
+      </c>
+      <c r="M296" t="s">
+        <v>4491</v>
+      </c>
+    </row>
+    <row r="297" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A297">
+        <v>297</v>
+      </c>
+      <c r="B297" t="s">
+        <v>3836</v>
+      </c>
+      <c r="C297" t="s">
+        <v>3833</v>
+      </c>
+      <c r="D297" t="s">
+        <v>14</v>
+      </c>
+      <c r="E297" t="s">
+        <v>14</v>
+      </c>
+      <c r="H297" t="s">
+        <v>71</v>
+      </c>
+      <c r="I297" t="s">
+        <v>166</v>
+      </c>
+      <c r="M297" t="s">
+        <v>4492</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -20713,10 +20791,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1751"/>
+  <dimension ref="A1:M1747"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1601" workbookViewId="0">
-      <selection activeCell="A1616" sqref="A1616:XFD1616"/>
+      <selection activeCell="F1621" sqref="F1621"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -60699,13 +60777,13 @@
     </row>
     <row r="1611" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1611">
-        <v>1638</v>
+        <v>1642</v>
       </c>
       <c r="B1611" t="s">
-        <v>3832</v>
+        <v>3839</v>
       </c>
       <c r="C1611" t="s">
-        <v>3833</v>
+        <v>3840</v>
       </c>
       <c r="D1611" t="s">
         <v>14</v>
@@ -60714,254 +60792,233 @@
         <v>14</v>
       </c>
       <c r="H1611" t="s">
-        <v>1236</v>
-      </c>
-      <c r="I1611" t="s">
-        <v>333</v>
+        <v>349</v>
       </c>
       <c r="M1611" t="s">
-        <v>3834</v>
+        <v>3841</v>
       </c>
     </row>
     <row r="1612" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1612">
-        <v>1639</v>
+        <v>1645</v>
       </c>
       <c r="B1612" t="s">
-        <v>3835</v>
+        <v>3848</v>
       </c>
       <c r="C1612" t="s">
-        <v>3833</v>
-      </c>
-      <c r="D1612" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1612" t="s">
-        <v>14</v>
+        <v>3849</v>
+      </c>
+      <c r="D1612">
+        <v>8080</v>
       </c>
       <c r="H1612" t="s">
-        <v>1236</v>
-      </c>
-      <c r="I1612" t="s">
-        <v>333</v>
+        <v>406</v>
       </c>
       <c r="M1612" t="s">
-        <v>4491</v>
+        <v>3850</v>
       </c>
     </row>
     <row r="1613" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1613">
-        <v>1640</v>
+        <v>1646</v>
       </c>
       <c r="B1613" t="s">
-        <v>3836</v>
+        <v>3851</v>
       </c>
       <c r="C1613" t="s">
-        <v>3833</v>
+        <v>3852</v>
       </c>
       <c r="D1613" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1613" t="s">
-        <v>14</v>
+        <v>1105</v>
       </c>
       <c r="H1613" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1613" t="s">
-        <v>166</v>
+        <v>336</v>
       </c>
       <c r="M1613" t="s">
-        <v>4492</v>
+        <v>3853</v>
       </c>
     </row>
     <row r="1614" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1614">
-        <v>1641</v>
+        <v>1647</v>
       </c>
       <c r="B1614" t="s">
-        <v>3837</v>
+        <v>3854</v>
       </c>
       <c r="C1614" t="s">
-        <v>3833</v>
+        <v>3855</v>
       </c>
       <c r="D1614" t="s">
         <v>14</v>
       </c>
       <c r="E1614" t="s">
-        <v>14</v>
+        <v>154</v>
       </c>
       <c r="H1614" t="s">
-        <v>1236</v>
-      </c>
-      <c r="I1614" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="M1614" t="s">
-        <v>3838</v>
+        <v>3856</v>
       </c>
     </row>
     <row r="1615" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1615">
-        <v>1642</v>
+        <v>1648</v>
       </c>
       <c r="B1615" t="s">
-        <v>3839</v>
+        <v>3857</v>
       </c>
       <c r="C1615" t="s">
-        <v>3840</v>
+        <v>3855</v>
       </c>
       <c r="D1615" t="s">
         <v>14</v>
       </c>
       <c r="E1615" t="s">
-        <v>14</v>
+        <v>154</v>
       </c>
       <c r="H1615" t="s">
-        <v>349</v>
+        <v>336</v>
       </c>
       <c r="M1615" t="s">
-        <v>3841</v>
+        <v>3858</v>
       </c>
     </row>
     <row r="1616" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1616">
-        <v>1645</v>
+        <v>1649</v>
       </c>
       <c r="B1616" t="s">
-        <v>3848</v>
+        <v>3859</v>
       </c>
       <c r="C1616" t="s">
-        <v>3849</v>
-      </c>
-      <c r="D1616">
-        <v>8080</v>
+        <v>3860</v>
+      </c>
+      <c r="D1616" t="s">
+        <v>3861</v>
+      </c>
+      <c r="E1616" t="s">
+        <v>725</v>
       </c>
       <c r="H1616" t="s">
-        <v>406</v>
+        <v>2070</v>
       </c>
       <c r="M1616" t="s">
-        <v>3850</v>
+        <v>3862</v>
       </c>
     </row>
     <row r="1617" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1617">
-        <v>1646</v>
+        <v>1650</v>
       </c>
       <c r="B1617" t="s">
-        <v>3851</v>
+        <v>3863</v>
       </c>
       <c r="C1617" t="s">
-        <v>3852</v>
-      </c>
-      <c r="D1617" t="s">
-        <v>1105</v>
+        <v>3864</v>
+      </c>
+      <c r="D1617">
+        <v>68000</v>
       </c>
       <c r="H1617" t="s">
-        <v>336</v>
+        <v>2375</v>
       </c>
       <c r="M1617" t="s">
-        <v>3853</v>
+        <v>3865</v>
       </c>
     </row>
     <row r="1618" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1618">
-        <v>1647</v>
+        <v>1651</v>
       </c>
       <c r="B1618" t="s">
-        <v>3854</v>
+        <v>3866</v>
       </c>
       <c r="C1618" t="s">
-        <v>3855</v>
-      </c>
-      <c r="D1618" t="s">
-        <v>14</v>
+        <v>3867</v>
+      </c>
+      <c r="D1618">
+        <v>68000</v>
       </c>
       <c r="E1618" t="s">
         <v>154</v>
       </c>
       <c r="H1618" t="s">
-        <v>336</v>
+        <v>1236</v>
       </c>
       <c r="M1618" t="s">
-        <v>3856</v>
+        <v>3868</v>
       </c>
     </row>
     <row r="1619" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1619">
-        <v>1648</v>
+        <v>1652</v>
       </c>
       <c r="B1619" t="s">
-        <v>3857</v>
+        <v>3869</v>
       </c>
       <c r="C1619" t="s">
-        <v>3855</v>
+        <v>3870</v>
       </c>
       <c r="D1619" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1619" t="s">
-        <v>154</v>
+        <v>405</v>
       </c>
       <c r="H1619" t="s">
-        <v>336</v>
+        <v>71</v>
       </c>
       <c r="M1619" t="s">
-        <v>3858</v>
+        <v>3871</v>
       </c>
     </row>
     <row r="1620" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1620">
-        <v>1649</v>
+        <v>1653</v>
       </c>
       <c r="B1620" t="s">
-        <v>3859</v>
+        <v>3872</v>
       </c>
       <c r="C1620" t="s">
-        <v>3860</v>
+        <v>3873</v>
       </c>
       <c r="D1620" t="s">
-        <v>3861</v>
-      </c>
-      <c r="E1620" t="s">
-        <v>725</v>
-      </c>
-      <c r="H1620" t="s">
-        <v>2070</v>
+        <v>14</v>
       </c>
       <c r="M1620" t="s">
-        <v>3862</v>
+        <v>4493</v>
       </c>
     </row>
     <row r="1621" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1621">
-        <v>1650</v>
+        <v>1654</v>
       </c>
       <c r="B1621" t="s">
-        <v>3863</v>
+        <v>3874</v>
       </c>
       <c r="C1621" t="s">
-        <v>3864</v>
+        <v>3875</v>
       </c>
       <c r="D1621">
         <v>68000</v>
       </c>
+      <c r="E1621" t="s">
+        <v>154</v>
+      </c>
       <c r="H1621" t="s">
-        <v>2375</v>
+        <v>1353</v>
       </c>
       <c r="M1621" t="s">
-        <v>3865</v>
+        <v>3876</v>
       </c>
     </row>
     <row r="1622" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1622">
-        <v>1651</v>
+        <v>1655</v>
       </c>
       <c r="B1622" t="s">
-        <v>3866</v>
+        <v>3877</v>
       </c>
       <c r="C1622" t="s">
-        <v>3867</v>
+        <v>3875</v>
       </c>
       <c r="D1622">
         <v>68000</v>
@@ -60970,55 +61027,64 @@
         <v>154</v>
       </c>
       <c r="H1622" t="s">
-        <v>1236</v>
+        <v>1353</v>
       </c>
       <c r="M1622" t="s">
-        <v>3868</v>
+        <v>4494</v>
       </c>
     </row>
     <row r="1623" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1623">
-        <v>1652</v>
+        <v>1656</v>
       </c>
       <c r="B1623" t="s">
-        <v>3869</v>
+        <v>3878</v>
       </c>
       <c r="C1623" t="s">
-        <v>3870</v>
-      </c>
-      <c r="D1623" t="s">
-        <v>405</v>
+        <v>3875</v>
+      </c>
+      <c r="D1623">
+        <v>68000</v>
+      </c>
+      <c r="E1623" t="s">
+        <v>154</v>
       </c>
       <c r="H1623" t="s">
-        <v>71</v>
+        <v>1353</v>
       </c>
       <c r="M1623" t="s">
-        <v>3871</v>
+        <v>3879</v>
       </c>
     </row>
     <row r="1624" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1624">
-        <v>1653</v>
+        <v>1657</v>
       </c>
       <c r="B1624" t="s">
-        <v>3872</v>
+        <v>3880</v>
       </c>
       <c r="C1624" t="s">
-        <v>3873</v>
-      </c>
-      <c r="D1624" t="s">
-        <v>14</v>
+        <v>3875</v>
+      </c>
+      <c r="D1624">
+        <v>68000</v>
+      </c>
+      <c r="E1624" t="s">
+        <v>154</v>
+      </c>
+      <c r="H1624" t="s">
+        <v>1353</v>
       </c>
       <c r="M1624" t="s">
-        <v>4493</v>
+        <v>3881</v>
       </c>
     </row>
     <row r="1625" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1625">
-        <v>1654</v>
+        <v>1658</v>
       </c>
       <c r="B1625" t="s">
-        <v>3874</v>
+        <v>3882</v>
       </c>
       <c r="C1625" t="s">
         <v>3875</v>
@@ -61033,15 +61099,15 @@
         <v>1353</v>
       </c>
       <c r="M1625" t="s">
-        <v>3876</v>
+        <v>3883</v>
       </c>
     </row>
     <row r="1626" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1626">
-        <v>1655</v>
+        <v>1659</v>
       </c>
       <c r="B1626" t="s">
-        <v>3877</v>
+        <v>3884</v>
       </c>
       <c r="C1626" t="s">
         <v>3875</v>
@@ -61056,15 +61122,15 @@
         <v>1353</v>
       </c>
       <c r="M1626" t="s">
-        <v>4494</v>
+        <v>3885</v>
       </c>
     </row>
     <row r="1627" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1627">
-        <v>1656</v>
+        <v>1660</v>
       </c>
       <c r="B1627" t="s">
-        <v>3878</v>
+        <v>3886</v>
       </c>
       <c r="C1627" t="s">
         <v>3875</v>
@@ -61079,15 +61145,15 @@
         <v>1353</v>
       </c>
       <c r="M1627" t="s">
-        <v>3879</v>
+        <v>3887</v>
       </c>
     </row>
     <row r="1628" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1628">
-        <v>1657</v>
+        <v>1661</v>
       </c>
       <c r="B1628" t="s">
-        <v>3880</v>
+        <v>3888</v>
       </c>
       <c r="C1628" t="s">
         <v>3875</v>
@@ -61102,15 +61168,15 @@
         <v>1353</v>
       </c>
       <c r="M1628" t="s">
-        <v>3881</v>
+        <v>4495</v>
       </c>
     </row>
     <row r="1629" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1629">
-        <v>1658</v>
+        <v>1662</v>
       </c>
       <c r="B1629" t="s">
-        <v>3882</v>
+        <v>3889</v>
       </c>
       <c r="C1629" t="s">
         <v>3875</v>
@@ -61125,15 +61191,15 @@
         <v>1353</v>
       </c>
       <c r="M1629" t="s">
-        <v>3883</v>
+        <v>3890</v>
       </c>
     </row>
     <row r="1630" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1630">
-        <v>1659</v>
+        <v>1663</v>
       </c>
       <c r="B1630" t="s">
-        <v>3884</v>
+        <v>3891</v>
       </c>
       <c r="C1630" t="s">
         <v>3875</v>
@@ -61148,15 +61214,15 @@
         <v>1353</v>
       </c>
       <c r="M1630" t="s">
-        <v>3885</v>
+        <v>3892</v>
       </c>
     </row>
     <row r="1631" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1631">
-        <v>1660</v>
+        <v>1664</v>
       </c>
       <c r="B1631" t="s">
-        <v>3886</v>
+        <v>3893</v>
       </c>
       <c r="C1631" t="s">
         <v>3875</v>
@@ -61171,15 +61237,15 @@
         <v>1353</v>
       </c>
       <c r="M1631" t="s">
-        <v>3887</v>
+        <v>3894</v>
       </c>
     </row>
     <row r="1632" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1632">
-        <v>1661</v>
+        <v>1665</v>
       </c>
       <c r="B1632" t="s">
-        <v>3888</v>
+        <v>3895</v>
       </c>
       <c r="C1632" t="s">
         <v>3875</v>
@@ -61194,15 +61260,15 @@
         <v>1353</v>
       </c>
       <c r="M1632" t="s">
-        <v>4495</v>
+        <v>3896</v>
       </c>
     </row>
     <row r="1633" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1633">
-        <v>1662</v>
+        <v>1666</v>
       </c>
       <c r="B1633" t="s">
-        <v>3889</v>
+        <v>3897</v>
       </c>
       <c r="C1633" t="s">
         <v>3875</v>
@@ -61217,15 +61283,15 @@
         <v>1353</v>
       </c>
       <c r="M1633" t="s">
-        <v>3890</v>
+        <v>3898</v>
       </c>
     </row>
     <row r="1634" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1634">
-        <v>1663</v>
+        <v>1667</v>
       </c>
       <c r="B1634" t="s">
-        <v>3891</v>
+        <v>3899</v>
       </c>
       <c r="C1634" t="s">
         <v>3875</v>
@@ -61240,15 +61306,15 @@
         <v>1353</v>
       </c>
       <c r="M1634" t="s">
-        <v>3892</v>
+        <v>4496</v>
       </c>
     </row>
     <row r="1635" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1635">
-        <v>1664</v>
+        <v>1668</v>
       </c>
       <c r="B1635" t="s">
-        <v>3893</v>
+        <v>3900</v>
       </c>
       <c r="C1635" t="s">
         <v>3875</v>
@@ -61263,15 +61329,15 @@
         <v>1353</v>
       </c>
       <c r="M1635" t="s">
-        <v>3894</v>
+        <v>4497</v>
       </c>
     </row>
     <row r="1636" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1636">
-        <v>1665</v>
+        <v>1669</v>
       </c>
       <c r="B1636" t="s">
-        <v>3895</v>
+        <v>3901</v>
       </c>
       <c r="C1636" t="s">
         <v>3875</v>
@@ -61286,15 +61352,15 @@
         <v>1353</v>
       </c>
       <c r="M1636" t="s">
-        <v>3896</v>
+        <v>3902</v>
       </c>
     </row>
     <row r="1637" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1637">
-        <v>1666</v>
+        <v>1670</v>
       </c>
       <c r="B1637" t="s">
-        <v>3897</v>
+        <v>3903</v>
       </c>
       <c r="C1637" t="s">
         <v>3875</v>
@@ -61309,15 +61375,15 @@
         <v>1353</v>
       </c>
       <c r="M1637" t="s">
-        <v>3898</v>
+        <v>3904</v>
       </c>
     </row>
     <row r="1638" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1638">
-        <v>1667</v>
+        <v>1671</v>
       </c>
       <c r="B1638" t="s">
-        <v>3899</v>
+        <v>3905</v>
       </c>
       <c r="C1638" t="s">
         <v>3875</v>
@@ -61332,15 +61398,15 @@
         <v>1353</v>
       </c>
       <c r="M1638" t="s">
-        <v>4496</v>
+        <v>3906</v>
       </c>
     </row>
     <row r="1639" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1639">
-        <v>1668</v>
+        <v>1672</v>
       </c>
       <c r="B1639" t="s">
-        <v>3900</v>
+        <v>3907</v>
       </c>
       <c r="C1639" t="s">
         <v>3875</v>
@@ -61355,15 +61421,15 @@
         <v>1353</v>
       </c>
       <c r="M1639" t="s">
-        <v>4497</v>
+        <v>3908</v>
       </c>
     </row>
     <row r="1640" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1640">
-        <v>1669</v>
+        <v>1673</v>
       </c>
       <c r="B1640" t="s">
-        <v>3901</v>
+        <v>3909</v>
       </c>
       <c r="C1640" t="s">
         <v>3875</v>
@@ -61378,15 +61444,15 @@
         <v>1353</v>
       </c>
       <c r="M1640" t="s">
-        <v>3902</v>
+        <v>3910</v>
       </c>
     </row>
     <row r="1641" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1641">
-        <v>1670</v>
+        <v>1674</v>
       </c>
       <c r="B1641" t="s">
-        <v>3903</v>
+        <v>3911</v>
       </c>
       <c r="C1641" t="s">
         <v>3875</v>
@@ -61401,15 +61467,15 @@
         <v>1353</v>
       </c>
       <c r="M1641" t="s">
-        <v>3904</v>
+        <v>3912</v>
       </c>
     </row>
     <row r="1642" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1642">
-        <v>1671</v>
+        <v>1675</v>
       </c>
       <c r="B1642" t="s">
-        <v>3905</v>
+        <v>3913</v>
       </c>
       <c r="C1642" t="s">
         <v>3875</v>
@@ -61424,15 +61490,15 @@
         <v>1353</v>
       </c>
       <c r="M1642" t="s">
-        <v>3906</v>
+        <v>4498</v>
       </c>
     </row>
     <row r="1643" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1643">
-        <v>1672</v>
+        <v>1676</v>
       </c>
       <c r="B1643" t="s">
-        <v>3907</v>
+        <v>3914</v>
       </c>
       <c r="C1643" t="s">
         <v>3875</v>
@@ -61447,15 +61513,15 @@
         <v>1353</v>
       </c>
       <c r="M1643" t="s">
-        <v>3908</v>
+        <v>3915</v>
       </c>
     </row>
     <row r="1644" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1644">
-        <v>1673</v>
+        <v>1677</v>
       </c>
       <c r="B1644" t="s">
-        <v>3909</v>
+        <v>3916</v>
       </c>
       <c r="C1644" t="s">
         <v>3875</v>
@@ -61470,15 +61536,15 @@
         <v>1353</v>
       </c>
       <c r="M1644" t="s">
-        <v>3910</v>
+        <v>3917</v>
       </c>
     </row>
     <row r="1645" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1645">
-        <v>1674</v>
+        <v>1678</v>
       </c>
       <c r="B1645" t="s">
-        <v>3911</v>
+        <v>3918</v>
       </c>
       <c r="C1645" t="s">
         <v>3875</v>
@@ -61493,15 +61559,15 @@
         <v>1353</v>
       </c>
       <c r="M1645" t="s">
-        <v>3912</v>
+        <v>3919</v>
       </c>
     </row>
     <row r="1646" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1646">
-        <v>1675</v>
+        <v>1679</v>
       </c>
       <c r="B1646" t="s">
-        <v>3913</v>
+        <v>3920</v>
       </c>
       <c r="C1646" t="s">
         <v>3875</v>
@@ -61516,15 +61582,15 @@
         <v>1353</v>
       </c>
       <c r="M1646" t="s">
-        <v>4498</v>
+        <v>4499</v>
       </c>
     </row>
     <row r="1647" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1647">
-        <v>1676</v>
+        <v>1680</v>
       </c>
       <c r="B1647" t="s">
-        <v>3914</v>
+        <v>3921</v>
       </c>
       <c r="C1647" t="s">
         <v>3875</v>
@@ -61539,15 +61605,15 @@
         <v>1353</v>
       </c>
       <c r="M1647" t="s">
-        <v>3915</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="1648" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1648">
-        <v>1677</v>
+        <v>1681</v>
       </c>
       <c r="B1648" t="s">
-        <v>3916</v>
+        <v>3922</v>
       </c>
       <c r="C1648" t="s">
         <v>3875</v>
@@ -61562,15 +61628,15 @@
         <v>1353</v>
       </c>
       <c r="M1648" t="s">
-        <v>3917</v>
+        <v>4501</v>
       </c>
     </row>
     <row r="1649" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1649">
-        <v>1678</v>
+        <v>1682</v>
       </c>
       <c r="B1649" t="s">
-        <v>3918</v>
+        <v>3923</v>
       </c>
       <c r="C1649" t="s">
         <v>3875</v>
@@ -61585,15 +61651,15 @@
         <v>1353</v>
       </c>
       <c r="M1649" t="s">
-        <v>3919</v>
+        <v>3924</v>
       </c>
     </row>
     <row r="1650" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1650">
-        <v>1679</v>
+        <v>1683</v>
       </c>
       <c r="B1650" t="s">
-        <v>3920</v>
+        <v>3925</v>
       </c>
       <c r="C1650" t="s">
         <v>3875</v>
@@ -61608,15 +61674,15 @@
         <v>1353</v>
       </c>
       <c r="M1650" t="s">
-        <v>4499</v>
+        <v>3926</v>
       </c>
     </row>
     <row r="1651" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1651">
-        <v>1680</v>
+        <v>1684</v>
       </c>
       <c r="B1651" t="s">
-        <v>3921</v>
+        <v>3927</v>
       </c>
       <c r="C1651" t="s">
         <v>3875</v>
@@ -61631,15 +61697,15 @@
         <v>1353</v>
       </c>
       <c r="M1651" t="s">
-        <v>4500</v>
+        <v>4502</v>
       </c>
     </row>
     <row r="1652" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1652">
-        <v>1681</v>
+        <v>1685</v>
       </c>
       <c r="B1652" t="s">
-        <v>3922</v>
+        <v>3928</v>
       </c>
       <c r="C1652" t="s">
         <v>3875</v>
@@ -61654,15 +61720,15 @@
         <v>1353</v>
       </c>
       <c r="M1652" t="s">
-        <v>4501</v>
+        <v>3929</v>
       </c>
     </row>
     <row r="1653" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1653">
-        <v>1682</v>
+        <v>1686</v>
       </c>
       <c r="B1653" t="s">
-        <v>3923</v>
+        <v>3930</v>
       </c>
       <c r="C1653" t="s">
         <v>3875</v>
@@ -61677,15 +61743,15 @@
         <v>1353</v>
       </c>
       <c r="M1653" t="s">
-        <v>3924</v>
+        <v>4503</v>
       </c>
     </row>
     <row r="1654" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1654">
-        <v>1683</v>
+        <v>1687</v>
       </c>
       <c r="B1654" t="s">
-        <v>3925</v>
+        <v>3931</v>
       </c>
       <c r="C1654" t="s">
         <v>3875</v>
@@ -61700,15 +61766,15 @@
         <v>1353</v>
       </c>
       <c r="M1654" t="s">
-        <v>3926</v>
+        <v>3932</v>
       </c>
     </row>
     <row r="1655" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1655">
-        <v>1684</v>
+        <v>1688</v>
       </c>
       <c r="B1655" t="s">
-        <v>3927</v>
+        <v>3933</v>
       </c>
       <c r="C1655" t="s">
         <v>3875</v>
@@ -61723,15 +61789,15 @@
         <v>1353</v>
       </c>
       <c r="M1655" t="s">
-        <v>4502</v>
+        <v>3934</v>
       </c>
     </row>
     <row r="1656" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1656">
-        <v>1685</v>
+        <v>1689</v>
       </c>
       <c r="B1656" t="s">
-        <v>3928</v>
+        <v>3935</v>
       </c>
       <c r="C1656" t="s">
         <v>3875</v>
@@ -61746,15 +61812,15 @@
         <v>1353</v>
       </c>
       <c r="M1656" t="s">
-        <v>3929</v>
+        <v>4504</v>
       </c>
     </row>
     <row r="1657" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1657">
-        <v>1686</v>
+        <v>1690</v>
       </c>
       <c r="B1657" t="s">
-        <v>3930</v>
+        <v>3936</v>
       </c>
       <c r="C1657" t="s">
         <v>3875</v>
@@ -61769,15 +61835,15 @@
         <v>1353</v>
       </c>
       <c r="M1657" t="s">
-        <v>4503</v>
+        <v>4505</v>
       </c>
     </row>
     <row r="1658" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1658">
-        <v>1687</v>
+        <v>1691</v>
       </c>
       <c r="B1658" t="s">
-        <v>3931</v>
+        <v>3937</v>
       </c>
       <c r="C1658" t="s">
         <v>3875</v>
@@ -61792,15 +61858,15 @@
         <v>1353</v>
       </c>
       <c r="M1658" t="s">
-        <v>3932</v>
+        <v>3938</v>
       </c>
     </row>
     <row r="1659" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1659">
-        <v>1688</v>
+        <v>1692</v>
       </c>
       <c r="B1659" t="s">
-        <v>3933</v>
+        <v>3939</v>
       </c>
       <c r="C1659" t="s">
         <v>3875</v>
@@ -61815,15 +61881,15 @@
         <v>1353</v>
       </c>
       <c r="M1659" t="s">
-        <v>3934</v>
+        <v>4506</v>
       </c>
     </row>
     <row r="1660" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1660">
-        <v>1689</v>
+        <v>1693</v>
       </c>
       <c r="B1660" t="s">
-        <v>3935</v>
+        <v>3940</v>
       </c>
       <c r="C1660" t="s">
         <v>3875</v>
@@ -61838,15 +61904,15 @@
         <v>1353</v>
       </c>
       <c r="M1660" t="s">
-        <v>4504</v>
+        <v>4507</v>
       </c>
     </row>
     <row r="1661" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1661">
-        <v>1690</v>
+        <v>1694</v>
       </c>
       <c r="B1661" t="s">
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C1661" t="s">
         <v>3875</v>
@@ -61861,15 +61927,15 @@
         <v>1353</v>
       </c>
       <c r="M1661" t="s">
-        <v>4505</v>
+        <v>4508</v>
       </c>
     </row>
     <row r="1662" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1662">
-        <v>1691</v>
+        <v>1695</v>
       </c>
       <c r="B1662" t="s">
-        <v>3937</v>
+        <v>3942</v>
       </c>
       <c r="C1662" t="s">
         <v>3875</v>
@@ -61884,15 +61950,15 @@
         <v>1353</v>
       </c>
       <c r="M1662" t="s">
-        <v>3938</v>
+        <v>4509</v>
       </c>
     </row>
     <row r="1663" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1663">
-        <v>1692</v>
+        <v>1696</v>
       </c>
       <c r="B1663" t="s">
-        <v>3939</v>
+        <v>3943</v>
       </c>
       <c r="C1663" t="s">
         <v>3875</v>
@@ -61907,15 +61973,15 @@
         <v>1353</v>
       </c>
       <c r="M1663" t="s">
-        <v>4506</v>
+        <v>4510</v>
       </c>
     </row>
     <row r="1664" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1664">
-        <v>1693</v>
+        <v>1697</v>
       </c>
       <c r="B1664" t="s">
-        <v>3940</v>
+        <v>3944</v>
       </c>
       <c r="C1664" t="s">
         <v>3875</v>
@@ -61930,15 +61996,15 @@
         <v>1353</v>
       </c>
       <c r="M1664" t="s">
-        <v>4507</v>
+        <v>4511</v>
       </c>
     </row>
     <row r="1665" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1665">
-        <v>1694</v>
+        <v>1698</v>
       </c>
       <c r="B1665" t="s">
-        <v>3941</v>
+        <v>3945</v>
       </c>
       <c r="C1665" t="s">
         <v>3875</v>
@@ -61953,15 +62019,15 @@
         <v>1353</v>
       </c>
       <c r="M1665" t="s">
-        <v>4508</v>
+        <v>4512</v>
       </c>
     </row>
     <row r="1666" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1666">
-        <v>1695</v>
+        <v>1699</v>
       </c>
       <c r="B1666" t="s">
-        <v>3942</v>
+        <v>3946</v>
       </c>
       <c r="C1666" t="s">
         <v>3875</v>
@@ -61976,15 +62042,15 @@
         <v>1353</v>
       </c>
       <c r="M1666" t="s">
-        <v>4509</v>
+        <v>3947</v>
       </c>
     </row>
     <row r="1667" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1667">
-        <v>1696</v>
+        <v>1700</v>
       </c>
       <c r="B1667" t="s">
-        <v>3943</v>
+        <v>3948</v>
       </c>
       <c r="C1667" t="s">
         <v>3875</v>
@@ -61999,15 +62065,15 @@
         <v>1353</v>
       </c>
       <c r="M1667" t="s">
-        <v>4510</v>
+        <v>3949</v>
       </c>
     </row>
     <row r="1668" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1668">
-        <v>1697</v>
+        <v>1701</v>
       </c>
       <c r="B1668" t="s">
-        <v>3944</v>
+        <v>3950</v>
       </c>
       <c r="C1668" t="s">
         <v>3875</v>
@@ -62022,15 +62088,15 @@
         <v>1353</v>
       </c>
       <c r="M1668" t="s">
-        <v>4511</v>
+        <v>3951</v>
       </c>
     </row>
     <row r="1669" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1669">
-        <v>1698</v>
+        <v>1702</v>
       </c>
       <c r="B1669" t="s">
-        <v>3945</v>
+        <v>3952</v>
       </c>
       <c r="C1669" t="s">
         <v>3875</v>
@@ -62045,15 +62111,15 @@
         <v>1353</v>
       </c>
       <c r="M1669" t="s">
-        <v>4512</v>
+        <v>4513</v>
       </c>
     </row>
     <row r="1670" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1670">
-        <v>1699</v>
+        <v>1703</v>
       </c>
       <c r="B1670" t="s">
-        <v>3946</v>
+        <v>3953</v>
       </c>
       <c r="C1670" t="s">
         <v>3875</v>
@@ -62068,15 +62134,15 @@
         <v>1353</v>
       </c>
       <c r="M1670" t="s">
-        <v>3947</v>
+        <v>3954</v>
       </c>
     </row>
     <row r="1671" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1671">
-        <v>1700</v>
+        <v>1704</v>
       </c>
       <c r="B1671" t="s">
-        <v>3948</v>
+        <v>3955</v>
       </c>
       <c r="C1671" t="s">
         <v>3875</v>
@@ -62091,15 +62157,15 @@
         <v>1353</v>
       </c>
       <c r="M1671" t="s">
-        <v>3949</v>
+        <v>3956</v>
       </c>
     </row>
     <row r="1672" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1672">
-        <v>1701</v>
+        <v>1705</v>
       </c>
       <c r="B1672" t="s">
-        <v>3950</v>
+        <v>3957</v>
       </c>
       <c r="C1672" t="s">
         <v>3875</v>
@@ -62114,15 +62180,15 @@
         <v>1353</v>
       </c>
       <c r="M1672" t="s">
-        <v>3951</v>
+        <v>4514</v>
       </c>
     </row>
     <row r="1673" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1673">
-        <v>1702</v>
+        <v>1706</v>
       </c>
       <c r="B1673" t="s">
-        <v>3952</v>
+        <v>3958</v>
       </c>
       <c r="C1673" t="s">
         <v>3875</v>
@@ -62137,15 +62203,15 @@
         <v>1353</v>
       </c>
       <c r="M1673" t="s">
-        <v>4513</v>
+        <v>3959</v>
       </c>
     </row>
     <row r="1674" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1674">
-        <v>1703</v>
+        <v>1707</v>
       </c>
       <c r="B1674" t="s">
-        <v>3953</v>
+        <v>3960</v>
       </c>
       <c r="C1674" t="s">
         <v>3875</v>
@@ -62160,15 +62226,15 @@
         <v>1353</v>
       </c>
       <c r="M1674" t="s">
-        <v>3954</v>
+        <v>4515</v>
       </c>
     </row>
     <row r="1675" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1675">
-        <v>1704</v>
+        <v>1708</v>
       </c>
       <c r="B1675" t="s">
-        <v>3955</v>
+        <v>3961</v>
       </c>
       <c r="C1675" t="s">
         <v>3875</v>
@@ -62183,15 +62249,15 @@
         <v>1353</v>
       </c>
       <c r="M1675" t="s">
-        <v>3956</v>
+        <v>4516</v>
       </c>
     </row>
     <row r="1676" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1676">
-        <v>1705</v>
+        <v>1709</v>
       </c>
       <c r="B1676" t="s">
-        <v>3957</v>
+        <v>3962</v>
       </c>
       <c r="C1676" t="s">
         <v>3875</v>
@@ -62206,15 +62272,15 @@
         <v>1353</v>
       </c>
       <c r="M1676" t="s">
-        <v>4514</v>
+        <v>4517</v>
       </c>
     </row>
     <row r="1677" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1677">
-        <v>1706</v>
+        <v>1710</v>
       </c>
       <c r="B1677" t="s">
-        <v>3958</v>
+        <v>3963</v>
       </c>
       <c r="C1677" t="s">
         <v>3875</v>
@@ -62229,15 +62295,15 @@
         <v>1353</v>
       </c>
       <c r="M1677" t="s">
-        <v>3959</v>
+        <v>4518</v>
       </c>
     </row>
     <row r="1678" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1678">
-        <v>1707</v>
+        <v>1711</v>
       </c>
       <c r="B1678" t="s">
-        <v>3960</v>
+        <v>3964</v>
       </c>
       <c r="C1678" t="s">
         <v>3875</v>
@@ -62252,15 +62318,15 @@
         <v>1353</v>
       </c>
       <c r="M1678" t="s">
-        <v>4515</v>
+        <v>4519</v>
       </c>
     </row>
     <row r="1679" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1679">
-        <v>1708</v>
+        <v>1712</v>
       </c>
       <c r="B1679" t="s">
-        <v>3961</v>
+        <v>3965</v>
       </c>
       <c r="C1679" t="s">
         <v>3875</v>
@@ -62275,15 +62341,15 @@
         <v>1353</v>
       </c>
       <c r="M1679" t="s">
-        <v>4516</v>
+        <v>4520</v>
       </c>
     </row>
     <row r="1680" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1680">
-        <v>1709</v>
+        <v>1713</v>
       </c>
       <c r="B1680" t="s">
-        <v>3962</v>
+        <v>3966</v>
       </c>
       <c r="C1680" t="s">
         <v>3875</v>
@@ -62298,15 +62364,15 @@
         <v>1353</v>
       </c>
       <c r="M1680" t="s">
-        <v>4517</v>
+        <v>3967</v>
       </c>
     </row>
     <row r="1681" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1681">
-        <v>1710</v>
+        <v>1714</v>
       </c>
       <c r="B1681" t="s">
-        <v>3963</v>
+        <v>3968</v>
       </c>
       <c r="C1681" t="s">
         <v>3875</v>
@@ -62321,15 +62387,15 @@
         <v>1353</v>
       </c>
       <c r="M1681" t="s">
-        <v>4518</v>
+        <v>4521</v>
       </c>
     </row>
     <row r="1682" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1682">
-        <v>1711</v>
+        <v>1715</v>
       </c>
       <c r="B1682" t="s">
-        <v>3964</v>
+        <v>3969</v>
       </c>
       <c r="C1682" t="s">
         <v>3875</v>
@@ -62344,15 +62410,15 @@
         <v>1353</v>
       </c>
       <c r="M1682" t="s">
-        <v>4519</v>
+        <v>4522</v>
       </c>
     </row>
     <row r="1683" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1683">
-        <v>1712</v>
+        <v>1716</v>
       </c>
       <c r="B1683" t="s">
-        <v>3965</v>
+        <v>3970</v>
       </c>
       <c r="C1683" t="s">
         <v>3875</v>
@@ -62367,15 +62433,15 @@
         <v>1353</v>
       </c>
       <c r="M1683" t="s">
-        <v>4520</v>
+        <v>3971</v>
       </c>
     </row>
     <row r="1684" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1684">
-        <v>1713</v>
+        <v>1717</v>
       </c>
       <c r="B1684" t="s">
-        <v>3966</v>
+        <v>3972</v>
       </c>
       <c r="C1684" t="s">
         <v>3875</v>
@@ -62390,15 +62456,15 @@
         <v>1353</v>
       </c>
       <c r="M1684" t="s">
-        <v>3967</v>
+        <v>3973</v>
       </c>
     </row>
     <row r="1685" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1685">
-        <v>1714</v>
+        <v>1718</v>
       </c>
       <c r="B1685" t="s">
-        <v>3968</v>
+        <v>3974</v>
       </c>
       <c r="C1685" t="s">
         <v>3875</v>
@@ -62413,15 +62479,15 @@
         <v>1353</v>
       </c>
       <c r="M1685" t="s">
-        <v>4521</v>
+        <v>4523</v>
       </c>
     </row>
     <row r="1686" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1686">
-        <v>1715</v>
+        <v>1719</v>
       </c>
       <c r="B1686" t="s">
-        <v>3969</v>
+        <v>3975</v>
       </c>
       <c r="C1686" t="s">
         <v>3875</v>
@@ -62436,15 +62502,15 @@
         <v>1353</v>
       </c>
       <c r="M1686" t="s">
-        <v>4522</v>
+        <v>3976</v>
       </c>
     </row>
     <row r="1687" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1687">
-        <v>1716</v>
+        <v>1720</v>
       </c>
       <c r="B1687" t="s">
-        <v>3970</v>
+        <v>3977</v>
       </c>
       <c r="C1687" t="s">
         <v>3875</v>
@@ -62459,15 +62525,15 @@
         <v>1353</v>
       </c>
       <c r="M1687" t="s">
-        <v>3971</v>
+        <v>4524</v>
       </c>
     </row>
     <row r="1688" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1688">
-        <v>1717</v>
+        <v>1721</v>
       </c>
       <c r="B1688" t="s">
-        <v>3972</v>
+        <v>3978</v>
       </c>
       <c r="C1688" t="s">
         <v>3875</v>
@@ -62482,15 +62548,15 @@
         <v>1353</v>
       </c>
       <c r="M1688" t="s">
-        <v>3973</v>
+        <v>4525</v>
       </c>
     </row>
     <row r="1689" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1689">
-        <v>1718</v>
+        <v>1722</v>
       </c>
       <c r="B1689" t="s">
-        <v>3974</v>
+        <v>3979</v>
       </c>
       <c r="C1689" t="s">
         <v>3875</v>
@@ -62505,15 +62571,15 @@
         <v>1353</v>
       </c>
       <c r="M1689" t="s">
-        <v>4523</v>
+        <v>4526</v>
       </c>
     </row>
     <row r="1690" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1690">
-        <v>1719</v>
+        <v>1723</v>
       </c>
       <c r="B1690" t="s">
-        <v>3975</v>
+        <v>3980</v>
       </c>
       <c r="C1690" t="s">
         <v>3875</v>
@@ -62528,15 +62594,15 @@
         <v>1353</v>
       </c>
       <c r="M1690" t="s">
-        <v>3976</v>
+        <v>4527</v>
       </c>
     </row>
     <row r="1691" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1691">
-        <v>1720</v>
+        <v>1724</v>
       </c>
       <c r="B1691" t="s">
-        <v>3977</v>
+        <v>3981</v>
       </c>
       <c r="C1691" t="s">
         <v>3875</v>
@@ -62551,15 +62617,15 @@
         <v>1353</v>
       </c>
       <c r="M1691" t="s">
-        <v>4524</v>
+        <v>4528</v>
       </c>
     </row>
     <row r="1692" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1692">
-        <v>1721</v>
+        <v>1725</v>
       </c>
       <c r="B1692" t="s">
-        <v>3978</v>
+        <v>3982</v>
       </c>
       <c r="C1692" t="s">
         <v>3875</v>
@@ -62574,15 +62640,15 @@
         <v>1353</v>
       </c>
       <c r="M1692" t="s">
-        <v>4525</v>
+        <v>3983</v>
       </c>
     </row>
     <row r="1693" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1693">
-        <v>1722</v>
+        <v>1726</v>
       </c>
       <c r="B1693" t="s">
-        <v>3979</v>
+        <v>3984</v>
       </c>
       <c r="C1693" t="s">
         <v>3875</v>
@@ -62597,15 +62663,15 @@
         <v>1353</v>
       </c>
       <c r="M1693" t="s">
-        <v>4526</v>
+        <v>4529</v>
       </c>
     </row>
     <row r="1694" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1694">
-        <v>1723</v>
+        <v>1727</v>
       </c>
       <c r="B1694" t="s">
-        <v>3980</v>
+        <v>3985</v>
       </c>
       <c r="C1694" t="s">
         <v>3875</v>
@@ -62620,15 +62686,15 @@
         <v>1353</v>
       </c>
       <c r="M1694" t="s">
-        <v>4527</v>
+        <v>3986</v>
       </c>
     </row>
     <row r="1695" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1695">
-        <v>1724</v>
+        <v>1728</v>
       </c>
       <c r="B1695" t="s">
-        <v>3981</v>
+        <v>3987</v>
       </c>
       <c r="C1695" t="s">
         <v>3875</v>
@@ -62643,15 +62709,15 @@
         <v>1353</v>
       </c>
       <c r="M1695" t="s">
-        <v>4528</v>
+        <v>4530</v>
       </c>
     </row>
     <row r="1696" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1696">
-        <v>1725</v>
+        <v>1729</v>
       </c>
       <c r="B1696" t="s">
-        <v>3982</v>
+        <v>3988</v>
       </c>
       <c r="C1696" t="s">
         <v>3875</v>
@@ -62666,15 +62732,15 @@
         <v>1353</v>
       </c>
       <c r="M1696" t="s">
-        <v>3983</v>
+        <v>3989</v>
       </c>
     </row>
     <row r="1697" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1697">
-        <v>1726</v>
+        <v>1730</v>
       </c>
       <c r="B1697" t="s">
-        <v>3984</v>
+        <v>3990</v>
       </c>
       <c r="C1697" t="s">
         <v>3875</v>
@@ -62689,15 +62755,15 @@
         <v>1353</v>
       </c>
       <c r="M1697" t="s">
-        <v>4529</v>
+        <v>3991</v>
       </c>
     </row>
     <row r="1698" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1698">
-        <v>1727</v>
+        <v>1731</v>
       </c>
       <c r="B1698" t="s">
-        <v>3985</v>
+        <v>3992</v>
       </c>
       <c r="C1698" t="s">
         <v>3875</v>
@@ -62712,15 +62778,15 @@
         <v>1353</v>
       </c>
       <c r="M1698" t="s">
-        <v>3986</v>
+        <v>4531</v>
       </c>
     </row>
     <row r="1699" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1699">
-        <v>1728</v>
+        <v>1732</v>
       </c>
       <c r="B1699" t="s">
-        <v>3987</v>
+        <v>3993</v>
       </c>
       <c r="C1699" t="s">
         <v>3875</v>
@@ -62735,15 +62801,15 @@
         <v>1353</v>
       </c>
       <c r="M1699" t="s">
-        <v>4530</v>
+        <v>4532</v>
       </c>
     </row>
     <row r="1700" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1700">
-        <v>1729</v>
+        <v>1733</v>
       </c>
       <c r="B1700" t="s">
-        <v>3988</v>
+        <v>3994</v>
       </c>
       <c r="C1700" t="s">
         <v>3875</v>
@@ -62758,15 +62824,15 @@
         <v>1353</v>
       </c>
       <c r="M1700" t="s">
-        <v>3989</v>
+        <v>3995</v>
       </c>
     </row>
     <row r="1701" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1701">
-        <v>1730</v>
+        <v>1734</v>
       </c>
       <c r="B1701" t="s">
-        <v>3990</v>
+        <v>3996</v>
       </c>
       <c r="C1701" t="s">
         <v>3875</v>
@@ -62781,15 +62847,15 @@
         <v>1353</v>
       </c>
       <c r="M1701" t="s">
-        <v>3991</v>
+        <v>3997</v>
       </c>
     </row>
     <row r="1702" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1702">
-        <v>1731</v>
+        <v>1735</v>
       </c>
       <c r="B1702" t="s">
-        <v>3992</v>
+        <v>3998</v>
       </c>
       <c r="C1702" t="s">
         <v>3875</v>
@@ -62804,15 +62870,15 @@
         <v>1353</v>
       </c>
       <c r="M1702" t="s">
-        <v>4531</v>
+        <v>4533</v>
       </c>
     </row>
     <row r="1703" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1703">
-        <v>1732</v>
+        <v>1736</v>
       </c>
       <c r="B1703" t="s">
-        <v>3993</v>
+        <v>3999</v>
       </c>
       <c r="C1703" t="s">
         <v>3875</v>
@@ -62827,15 +62893,15 @@
         <v>1353</v>
       </c>
       <c r="M1703" t="s">
-        <v>4532</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="1704" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1704">
-        <v>1733</v>
+        <v>1737</v>
       </c>
       <c r="B1704" t="s">
-        <v>3994</v>
+        <v>4001</v>
       </c>
       <c r="C1704" t="s">
         <v>3875</v>
@@ -62850,15 +62916,15 @@
         <v>1353</v>
       </c>
       <c r="M1704" t="s">
-        <v>3995</v>
+        <v>4534</v>
       </c>
     </row>
     <row r="1705" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1705">
-        <v>1734</v>
+        <v>1738</v>
       </c>
       <c r="B1705" t="s">
-        <v>3996</v>
+        <v>4002</v>
       </c>
       <c r="C1705" t="s">
         <v>3875</v>
@@ -62873,15 +62939,15 @@
         <v>1353</v>
       </c>
       <c r="M1705" t="s">
-        <v>3997</v>
+        <v>4535</v>
       </c>
     </row>
     <row r="1706" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1706">
-        <v>1735</v>
+        <v>1739</v>
       </c>
       <c r="B1706" t="s">
-        <v>3998</v>
+        <v>4003</v>
       </c>
       <c r="C1706" t="s">
         <v>3875</v>
@@ -62896,15 +62962,15 @@
         <v>1353</v>
       </c>
       <c r="M1706" t="s">
-        <v>4533</v>
+        <v>4536</v>
       </c>
     </row>
     <row r="1707" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1707">
-        <v>1736</v>
+        <v>1740</v>
       </c>
       <c r="B1707" t="s">
-        <v>3999</v>
+        <v>4004</v>
       </c>
       <c r="C1707" t="s">
         <v>3875</v>
@@ -62919,15 +62985,15 @@
         <v>1353</v>
       </c>
       <c r="M1707" t="s">
-        <v>4000</v>
+        <v>4537</v>
       </c>
     </row>
     <row r="1708" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1708">
-        <v>1737</v>
+        <v>1741</v>
       </c>
       <c r="B1708" t="s">
-        <v>4001</v>
+        <v>4005</v>
       </c>
       <c r="C1708" t="s">
         <v>3875</v>
@@ -62942,15 +63008,15 @@
         <v>1353</v>
       </c>
       <c r="M1708" t="s">
-        <v>4534</v>
+        <v>4538</v>
       </c>
     </row>
     <row r="1709" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1709">
-        <v>1738</v>
+        <v>1742</v>
       </c>
       <c r="B1709" t="s">
-        <v>4002</v>
+        <v>4006</v>
       </c>
       <c r="C1709" t="s">
         <v>3875</v>
@@ -62965,15 +63031,15 @@
         <v>1353</v>
       </c>
       <c r="M1709" t="s">
-        <v>4535</v>
+        <v>4539</v>
       </c>
     </row>
     <row r="1710" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1710">
-        <v>1739</v>
+        <v>1743</v>
       </c>
       <c r="B1710" t="s">
-        <v>4003</v>
+        <v>4007</v>
       </c>
       <c r="C1710" t="s">
         <v>3875</v>
@@ -62988,15 +63054,15 @@
         <v>1353</v>
       </c>
       <c r="M1710" t="s">
-        <v>4536</v>
+        <v>4008</v>
       </c>
     </row>
     <row r="1711" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1711">
-        <v>1740</v>
+        <v>1744</v>
       </c>
       <c r="B1711" t="s">
-        <v>4004</v>
+        <v>4009</v>
       </c>
       <c r="C1711" t="s">
         <v>3875</v>
@@ -63011,15 +63077,15 @@
         <v>1353</v>
       </c>
       <c r="M1711" t="s">
-        <v>4537</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="1712" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1712">
-        <v>1741</v>
+        <v>1745</v>
       </c>
       <c r="B1712" t="s">
-        <v>4005</v>
+        <v>4010</v>
       </c>
       <c r="C1712" t="s">
         <v>3875</v>
@@ -63034,15 +63100,15 @@
         <v>1353</v>
       </c>
       <c r="M1712" t="s">
-        <v>4538</v>
+        <v>4541</v>
       </c>
     </row>
     <row r="1713" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1713">
-        <v>1742</v>
+        <v>1746</v>
       </c>
       <c r="B1713" t="s">
-        <v>4006</v>
+        <v>4011</v>
       </c>
       <c r="C1713" t="s">
         <v>3875</v>
@@ -63057,15 +63123,15 @@
         <v>1353</v>
       </c>
       <c r="M1713" t="s">
-        <v>4539</v>
+        <v>4012</v>
       </c>
     </row>
     <row r="1714" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1714">
-        <v>1743</v>
+        <v>1747</v>
       </c>
       <c r="B1714" t="s">
-        <v>4007</v>
+        <v>4013</v>
       </c>
       <c r="C1714" t="s">
         <v>3875</v>
@@ -63080,15 +63146,15 @@
         <v>1353</v>
       </c>
       <c r="M1714" t="s">
-        <v>4008</v>
+        <v>4542</v>
       </c>
     </row>
     <row r="1715" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1715">
-        <v>1744</v>
+        <v>1748</v>
       </c>
       <c r="B1715" t="s">
-        <v>4009</v>
+        <v>4014</v>
       </c>
       <c r="C1715" t="s">
         <v>3875</v>
@@ -63103,15 +63169,15 @@
         <v>1353</v>
       </c>
       <c r="M1715" t="s">
-        <v>4540</v>
+        <v>4015</v>
       </c>
     </row>
     <row r="1716" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1716">
-        <v>1745</v>
+        <v>1749</v>
       </c>
       <c r="B1716" t="s">
-        <v>4010</v>
+        <v>4016</v>
       </c>
       <c r="C1716" t="s">
         <v>3875</v>
@@ -63126,15 +63192,15 @@
         <v>1353</v>
       </c>
       <c r="M1716" t="s">
-        <v>4541</v>
+        <v>4017</v>
       </c>
     </row>
     <row r="1717" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1717">
-        <v>1746</v>
+        <v>1750</v>
       </c>
       <c r="B1717" t="s">
-        <v>4011</v>
+        <v>4018</v>
       </c>
       <c r="C1717" t="s">
         <v>3875</v>
@@ -63149,15 +63215,15 @@
         <v>1353</v>
       </c>
       <c r="M1717" t="s">
-        <v>4012</v>
+        <v>4543</v>
       </c>
     </row>
     <row r="1718" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1718">
-        <v>1747</v>
+        <v>1751</v>
       </c>
       <c r="B1718" t="s">
-        <v>4013</v>
+        <v>4019</v>
       </c>
       <c r="C1718" t="s">
         <v>3875</v>
@@ -63172,15 +63238,15 @@
         <v>1353</v>
       </c>
       <c r="M1718" t="s">
-        <v>4542</v>
+        <v>4020</v>
       </c>
     </row>
     <row r="1719" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1719">
-        <v>1748</v>
+        <v>1752</v>
       </c>
       <c r="B1719" t="s">
-        <v>4014</v>
+        <v>4021</v>
       </c>
       <c r="C1719" t="s">
         <v>3875</v>
@@ -63195,15 +63261,15 @@
         <v>1353</v>
       </c>
       <c r="M1719" t="s">
-        <v>4015</v>
+        <v>4544</v>
       </c>
     </row>
     <row r="1720" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1720">
-        <v>1749</v>
+        <v>1753</v>
       </c>
       <c r="B1720" t="s">
-        <v>4016</v>
+        <v>4022</v>
       </c>
       <c r="C1720" t="s">
         <v>3875</v>
@@ -63218,15 +63284,15 @@
         <v>1353</v>
       </c>
       <c r="M1720" t="s">
-        <v>4017</v>
+        <v>4545</v>
       </c>
     </row>
     <row r="1721" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1721">
-        <v>1750</v>
+        <v>1754</v>
       </c>
       <c r="B1721" t="s">
-        <v>4018</v>
+        <v>4023</v>
       </c>
       <c r="C1721" t="s">
         <v>3875</v>
@@ -63241,15 +63307,15 @@
         <v>1353</v>
       </c>
       <c r="M1721" t="s">
-        <v>4543</v>
+        <v>4546</v>
       </c>
     </row>
     <row r="1722" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1722">
-        <v>1751</v>
+        <v>1755</v>
       </c>
       <c r="B1722" t="s">
-        <v>4019</v>
+        <v>4024</v>
       </c>
       <c r="C1722" t="s">
         <v>3875</v>
@@ -63264,15 +63330,15 @@
         <v>1353</v>
       </c>
       <c r="M1722" t="s">
-        <v>4020</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="1723" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1723">
-        <v>1752</v>
+        <v>1756</v>
       </c>
       <c r="B1723" t="s">
-        <v>4021</v>
+        <v>4025</v>
       </c>
       <c r="C1723" t="s">
         <v>3875</v>
@@ -63287,15 +63353,15 @@
         <v>1353</v>
       </c>
       <c r="M1723" t="s">
-        <v>4544</v>
+        <v>4548</v>
       </c>
     </row>
     <row r="1724" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1724">
-        <v>1753</v>
+        <v>1757</v>
       </c>
       <c r="B1724" t="s">
-        <v>4022</v>
+        <v>4026</v>
       </c>
       <c r="C1724" t="s">
         <v>3875</v>
@@ -63310,15 +63376,15 @@
         <v>1353</v>
       </c>
       <c r="M1724" t="s">
-        <v>4545</v>
+        <v>4027</v>
       </c>
     </row>
     <row r="1725" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1725">
-        <v>1754</v>
+        <v>1758</v>
       </c>
       <c r="B1725" t="s">
-        <v>4023</v>
+        <v>4028</v>
       </c>
       <c r="C1725" t="s">
         <v>3875</v>
@@ -63333,15 +63399,15 @@
         <v>1353</v>
       </c>
       <c r="M1725" t="s">
-        <v>4546</v>
+        <v>4549</v>
       </c>
     </row>
     <row r="1726" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1726">
-        <v>1755</v>
+        <v>1759</v>
       </c>
       <c r="B1726" t="s">
-        <v>4024</v>
+        <v>4029</v>
       </c>
       <c r="C1726" t="s">
         <v>3875</v>
@@ -63356,15 +63422,15 @@
         <v>1353</v>
       </c>
       <c r="M1726" t="s">
-        <v>4547</v>
+        <v>4550</v>
       </c>
     </row>
     <row r="1727" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1727">
-        <v>1756</v>
+        <v>1760</v>
       </c>
       <c r="B1727" t="s">
-        <v>4025</v>
+        <v>4030</v>
       </c>
       <c r="C1727" t="s">
         <v>3875</v>
@@ -63379,15 +63445,15 @@
         <v>1353</v>
       </c>
       <c r="M1727" t="s">
-        <v>4548</v>
+        <v>4031</v>
       </c>
     </row>
     <row r="1728" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1728">
-        <v>1757</v>
+        <v>1761</v>
       </c>
       <c r="B1728" t="s">
-        <v>4026</v>
+        <v>4032</v>
       </c>
       <c r="C1728" t="s">
         <v>3875</v>
@@ -63402,15 +63468,15 @@
         <v>1353</v>
       </c>
       <c r="M1728" t="s">
-        <v>4027</v>
+        <v>4033</v>
       </c>
     </row>
     <row r="1729" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1729">
-        <v>1758</v>
+        <v>1762</v>
       </c>
       <c r="B1729" t="s">
-        <v>4028</v>
+        <v>4034</v>
       </c>
       <c r="C1729" t="s">
         <v>3875</v>
@@ -63425,15 +63491,15 @@
         <v>1353</v>
       </c>
       <c r="M1729" t="s">
-        <v>4549</v>
+        <v>4035</v>
       </c>
     </row>
     <row r="1730" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1730">
-        <v>1759</v>
+        <v>1763</v>
       </c>
       <c r="B1730" t="s">
-        <v>4029</v>
+        <v>4036</v>
       </c>
       <c r="C1730" t="s">
         <v>3875</v>
@@ -63448,15 +63514,15 @@
         <v>1353</v>
       </c>
       <c r="M1730" t="s">
-        <v>4550</v>
+        <v>4037</v>
       </c>
     </row>
     <row r="1731" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1731">
-        <v>1760</v>
+        <v>1764</v>
       </c>
       <c r="B1731" t="s">
-        <v>4030</v>
+        <v>4038</v>
       </c>
       <c r="C1731" t="s">
         <v>3875</v>
@@ -63471,15 +63537,15 @@
         <v>1353</v>
       </c>
       <c r="M1731" t="s">
-        <v>4031</v>
+        <v>4551</v>
       </c>
     </row>
     <row r="1732" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1732">
-        <v>1761</v>
+        <v>1765</v>
       </c>
       <c r="B1732" t="s">
-        <v>4032</v>
+        <v>4039</v>
       </c>
       <c r="C1732" t="s">
         <v>3875</v>
@@ -63494,15 +63560,15 @@
         <v>1353</v>
       </c>
       <c r="M1732" t="s">
-        <v>4033</v>
+        <v>4040</v>
       </c>
     </row>
     <row r="1733" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1733">
-        <v>1762</v>
+        <v>1766</v>
       </c>
       <c r="B1733" t="s">
-        <v>4034</v>
+        <v>4041</v>
       </c>
       <c r="C1733" t="s">
         <v>3875</v>
@@ -63517,15 +63583,15 @@
         <v>1353</v>
       </c>
       <c r="M1733" t="s">
-        <v>4035</v>
+        <v>4042</v>
       </c>
     </row>
     <row r="1734" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1734">
-        <v>1763</v>
+        <v>1767</v>
       </c>
       <c r="B1734" t="s">
-        <v>4036</v>
+        <v>4043</v>
       </c>
       <c r="C1734" t="s">
         <v>3875</v>
@@ -63540,15 +63606,15 @@
         <v>1353</v>
       </c>
       <c r="M1734" t="s">
-        <v>4037</v>
+        <v>4552</v>
       </c>
     </row>
     <row r="1735" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1735">
-        <v>1764</v>
+        <v>1768</v>
       </c>
       <c r="B1735" t="s">
-        <v>4038</v>
+        <v>4044</v>
       </c>
       <c r="C1735" t="s">
         <v>3875</v>
@@ -63563,15 +63629,15 @@
         <v>1353</v>
       </c>
       <c r="M1735" t="s">
-        <v>4551</v>
+        <v>4045</v>
       </c>
     </row>
     <row r="1736" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1736">
-        <v>1765</v>
+        <v>1769</v>
       </c>
       <c r="B1736" t="s">
-        <v>4039</v>
+        <v>4046</v>
       </c>
       <c r="C1736" t="s">
         <v>3875</v>
@@ -63586,15 +63652,15 @@
         <v>1353</v>
       </c>
       <c r="M1736" t="s">
-        <v>4040</v>
+        <v>4553</v>
       </c>
     </row>
     <row r="1737" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1737">
-        <v>1766</v>
+        <v>1770</v>
       </c>
       <c r="B1737" t="s">
-        <v>4041</v>
+        <v>4047</v>
       </c>
       <c r="C1737" t="s">
         <v>3875</v>
@@ -63609,15 +63675,15 @@
         <v>1353</v>
       </c>
       <c r="M1737" t="s">
-        <v>4042</v>
+        <v>4048</v>
       </c>
     </row>
     <row r="1738" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1738">
-        <v>1767</v>
+        <v>1771</v>
       </c>
       <c r="B1738" t="s">
-        <v>4043</v>
+        <v>4049</v>
       </c>
       <c r="C1738" t="s">
         <v>3875</v>
@@ -63632,15 +63698,15 @@
         <v>1353</v>
       </c>
       <c r="M1738" t="s">
-        <v>4552</v>
+        <v>4050</v>
       </c>
     </row>
     <row r="1739" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1739">
-        <v>1768</v>
+        <v>1772</v>
       </c>
       <c r="B1739" t="s">
-        <v>4044</v>
+        <v>4051</v>
       </c>
       <c r="C1739" t="s">
         <v>3875</v>
@@ -63655,15 +63721,15 @@
         <v>1353</v>
       </c>
       <c r="M1739" t="s">
-        <v>4045</v>
+        <v>4052</v>
       </c>
     </row>
     <row r="1740" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1740">
-        <v>1769</v>
+        <v>1773</v>
       </c>
       <c r="B1740" t="s">
-        <v>4046</v>
+        <v>4053</v>
       </c>
       <c r="C1740" t="s">
         <v>3875</v>
@@ -63678,15 +63744,15 @@
         <v>1353</v>
       </c>
       <c r="M1740" t="s">
-        <v>4553</v>
+        <v>4554</v>
       </c>
     </row>
     <row r="1741" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1741">
-        <v>1770</v>
+        <v>1774</v>
       </c>
       <c r="B1741" t="s">
-        <v>4047</v>
+        <v>4054</v>
       </c>
       <c r="C1741" t="s">
         <v>3875</v>
@@ -63701,15 +63767,15 @@
         <v>1353</v>
       </c>
       <c r="M1741" t="s">
-        <v>4048</v>
+        <v>4555</v>
       </c>
     </row>
     <row r="1742" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1742">
-        <v>1771</v>
+        <v>1775</v>
       </c>
       <c r="B1742" t="s">
-        <v>4049</v>
+        <v>4055</v>
       </c>
       <c r="C1742" t="s">
         <v>3875</v>
@@ -63724,15 +63790,15 @@
         <v>1353</v>
       </c>
       <c r="M1742" t="s">
-        <v>4050</v>
+        <v>4556</v>
       </c>
     </row>
     <row r="1743" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1743">
-        <v>1772</v>
+        <v>1776</v>
       </c>
       <c r="B1743" t="s">
-        <v>4051</v>
+        <v>4056</v>
       </c>
       <c r="C1743" t="s">
         <v>3875</v>
@@ -63747,15 +63813,15 @@
         <v>1353</v>
       </c>
       <c r="M1743" t="s">
-        <v>4052</v>
+        <v>4557</v>
       </c>
     </row>
     <row r="1744" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1744">
-        <v>1773</v>
+        <v>1777</v>
       </c>
       <c r="B1744" t="s">
-        <v>4053</v>
+        <v>4057</v>
       </c>
       <c r="C1744" t="s">
         <v>3875</v>
@@ -63770,15 +63836,15 @@
         <v>1353</v>
       </c>
       <c r="M1744" t="s">
-        <v>4554</v>
+        <v>4558</v>
       </c>
     </row>
     <row r="1745" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1745">
-        <v>1774</v>
+        <v>1778</v>
       </c>
       <c r="B1745" t="s">
-        <v>4054</v>
+        <v>4058</v>
       </c>
       <c r="C1745" t="s">
         <v>3875</v>
@@ -63793,15 +63859,15 @@
         <v>1353</v>
       </c>
       <c r="M1745" t="s">
-        <v>4555</v>
+        <v>4059</v>
       </c>
     </row>
     <row r="1746" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1746">
-        <v>1775</v>
+        <v>1779</v>
       </c>
       <c r="B1746" t="s">
-        <v>4055</v>
+        <v>4060</v>
       </c>
       <c r="C1746" t="s">
         <v>3875</v>
@@ -63816,15 +63882,15 @@
         <v>1353</v>
       </c>
       <c r="M1746" t="s">
-        <v>4556</v>
+        <v>4559</v>
       </c>
     </row>
     <row r="1747" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1747">
-        <v>1776</v>
+        <v>1780</v>
       </c>
       <c r="B1747" t="s">
-        <v>4056</v>
+        <v>4061</v>
       </c>
       <c r="C1747" t="s">
         <v>3875</v>
@@ -63839,103 +63905,11 @@
         <v>1353</v>
       </c>
       <c r="M1747" t="s">
-        <v>4557</v>
-      </c>
-    </row>
-    <row r="1748" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1748">
-        <v>1777</v>
-      </c>
-      <c r="B1748" t="s">
-        <v>4057</v>
-      </c>
-      <c r="C1748" t="s">
-        <v>3875</v>
-      </c>
-      <c r="D1748">
-        <v>68000</v>
-      </c>
-      <c r="E1748" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1748" t="s">
-        <v>1353</v>
-      </c>
-      <c r="M1748" t="s">
-        <v>4558</v>
-      </c>
-    </row>
-    <row r="1749" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1749">
-        <v>1778</v>
-      </c>
-      <c r="B1749" t="s">
-        <v>4058</v>
-      </c>
-      <c r="C1749" t="s">
-        <v>3875</v>
-      </c>
-      <c r="D1749">
-        <v>68000</v>
-      </c>
-      <c r="E1749" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1749" t="s">
-        <v>1353</v>
-      </c>
-      <c r="M1749" t="s">
-        <v>4059</v>
-      </c>
-    </row>
-    <row r="1750" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1750">
-        <v>1779</v>
-      </c>
-      <c r="B1750" t="s">
-        <v>4060</v>
-      </c>
-      <c r="C1750" t="s">
-        <v>3875</v>
-      </c>
-      <c r="D1750">
-        <v>68000</v>
-      </c>
-      <c r="E1750" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1750" t="s">
-        <v>1353</v>
-      </c>
-      <c r="M1750" t="s">
-        <v>4559</v>
-      </c>
-    </row>
-    <row r="1751" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1751">
-        <v>1780</v>
-      </c>
-      <c r="B1751" t="s">
-        <v>4061</v>
-      </c>
-      <c r="C1751" t="s">
-        <v>3875</v>
-      </c>
-      <c r="D1751">
-        <v>68000</v>
-      </c>
-      <c r="E1751" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1751" t="s">
-        <v>1353</v>
-      </c>
-      <c r="M1751" t="s">
         <v>4062</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M1751"/>
+  <autoFilter ref="A1:M1747"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -63943,10 +63917,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -64056,6 +64030,32 @@
         <v>2067</v>
       </c>
     </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3837</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3833</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1236</v>
+      </c>
+      <c r="I5" t="s">
+        <v>333</v>
+      </c>
+      <c r="M5" t="s">
+        <v>3838</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
036 : speedbal driver
</commit_message>
<xml_diff>
--- a/0.36/compatibility.xlsx
+++ b/0.36/compatibility.xlsx
@@ -17,8 +17,8 @@
     <sheet name="GAME_NOT_WORKING FLAG" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ALL!$A$1:$M$1737</definedName>
-    <definedName name="LIST" localSheetId="1">ALL!$B$1:$M$1737</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ALL!$A$1:$M$1736</definedName>
+    <definedName name="LIST" localSheetId="1">ALL!$B$1:$M$1736</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -14078,10 +14078,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P307"/>
+  <dimension ref="A1:P308"/>
   <sheetViews>
     <sheetView topLeftCell="A288" workbookViewId="0">
-      <selection activeCell="A301" sqref="A301:A307"/>
+      <selection activeCell="A306" sqref="A306:A308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21025,6 +21025,29 @@
         <v>2470</v>
       </c>
     </row>
+    <row r="308" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A308">
+        <v>308</v>
+      </c>
+      <c r="B308" t="s">
+        <v>3839</v>
+      </c>
+      <c r="C308" t="s">
+        <v>3840</v>
+      </c>
+      <c r="D308" t="s">
+        <v>14</v>
+      </c>
+      <c r="E308" t="s">
+        <v>14</v>
+      </c>
+      <c r="H308" t="s">
+        <v>349</v>
+      </c>
+      <c r="M308" t="s">
+        <v>3841</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -21033,10 +21056,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1737"/>
+  <dimension ref="A1:M1736"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1007" sqref="G1007"/>
+    <sheetView tabSelected="1" topLeftCell="A1346" workbookViewId="0">
+      <selection activeCell="F1609" sqref="F1609"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -60777,73 +60800,73 @@
     </row>
     <row r="1601" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1601">
-        <v>1642</v>
+        <v>1645</v>
       </c>
       <c r="B1601" t="s">
-        <v>3839</v>
+        <v>3848</v>
       </c>
       <c r="C1601" t="s">
-        <v>3840</v>
-      </c>
-      <c r="D1601" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1601" t="s">
-        <v>14</v>
+        <v>3849</v>
+      </c>
+      <c r="D1601">
+        <v>8080</v>
       </c>
       <c r="H1601" t="s">
-        <v>349</v>
+        <v>406</v>
       </c>
       <c r="M1601" t="s">
-        <v>3841</v>
+        <v>3850</v>
       </c>
     </row>
     <row r="1602" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1602">
-        <v>1645</v>
+        <v>1646</v>
       </c>
       <c r="B1602" t="s">
-        <v>3848</v>
+        <v>3851</v>
       </c>
       <c r="C1602" t="s">
-        <v>3849</v>
-      </c>
-      <c r="D1602">
-        <v>8080</v>
+        <v>3852</v>
+      </c>
+      <c r="D1602" t="s">
+        <v>1105</v>
       </c>
       <c r="H1602" t="s">
-        <v>406</v>
+        <v>336</v>
       </c>
       <c r="M1602" t="s">
-        <v>3850</v>
+        <v>3853</v>
       </c>
     </row>
     <row r="1603" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1603">
-        <v>1646</v>
+        <v>1647</v>
       </c>
       <c r="B1603" t="s">
-        <v>3851</v>
+        <v>3854</v>
       </c>
       <c r="C1603" t="s">
-        <v>3852</v>
+        <v>3855</v>
       </c>
       <c r="D1603" t="s">
-        <v>1105</v>
+        <v>14</v>
+      </c>
+      <c r="E1603" t="s">
+        <v>154</v>
       </c>
       <c r="H1603" t="s">
         <v>336</v>
       </c>
       <c r="M1603" t="s">
-        <v>3853</v>
+        <v>3856</v>
       </c>
     </row>
     <row r="1604" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1604">
-        <v>1647</v>
+        <v>1648</v>
       </c>
       <c r="B1604" t="s">
-        <v>3854</v>
+        <v>3857</v>
       </c>
       <c r="C1604" t="s">
         <v>3855</v>
@@ -60858,141 +60881,141 @@
         <v>336</v>
       </c>
       <c r="M1604" t="s">
-        <v>3856</v>
+        <v>3858</v>
       </c>
     </row>
     <row r="1605" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1605">
-        <v>1648</v>
+        <v>1649</v>
       </c>
       <c r="B1605" t="s">
-        <v>3857</v>
+        <v>3859</v>
       </c>
       <c r="C1605" t="s">
-        <v>3855</v>
+        <v>3860</v>
       </c>
       <c r="D1605" t="s">
-        <v>14</v>
+        <v>3861</v>
       </c>
       <c r="E1605" t="s">
-        <v>154</v>
+        <v>725</v>
       </c>
       <c r="H1605" t="s">
-        <v>336</v>
+        <v>2070</v>
       </c>
       <c r="M1605" t="s">
-        <v>3858</v>
+        <v>3862</v>
       </c>
     </row>
     <row r="1606" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1606">
-        <v>1649</v>
+        <v>1650</v>
       </c>
       <c r="B1606" t="s">
-        <v>3859</v>
+        <v>3863</v>
       </c>
       <c r="C1606" t="s">
-        <v>3860</v>
-      </c>
-      <c r="D1606" t="s">
-        <v>3861</v>
-      </c>
-      <c r="E1606" t="s">
-        <v>725</v>
+        <v>3864</v>
+      </c>
+      <c r="D1606">
+        <v>68000</v>
       </c>
       <c r="H1606" t="s">
-        <v>2070</v>
+        <v>2375</v>
       </c>
       <c r="M1606" t="s">
-        <v>3862</v>
+        <v>3865</v>
       </c>
     </row>
     <row r="1607" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1607">
-        <v>1650</v>
+        <v>1651</v>
       </c>
       <c r="B1607" t="s">
-        <v>3863</v>
+        <v>3866</v>
       </c>
       <c r="C1607" t="s">
-        <v>3864</v>
+        <v>3867</v>
       </c>
       <c r="D1607">
         <v>68000</v>
       </c>
+      <c r="E1607" t="s">
+        <v>154</v>
+      </c>
       <c r="H1607" t="s">
-        <v>2375</v>
+        <v>1236</v>
       </c>
       <c r="M1607" t="s">
-        <v>3865</v>
+        <v>3868</v>
       </c>
     </row>
     <row r="1608" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1608">
-        <v>1651</v>
+        <v>1652</v>
       </c>
       <c r="B1608" t="s">
-        <v>3866</v>
+        <v>3869</v>
       </c>
       <c r="C1608" t="s">
-        <v>3867</v>
-      </c>
-      <c r="D1608">
-        <v>68000</v>
-      </c>
-      <c r="E1608" t="s">
-        <v>154</v>
+        <v>3870</v>
+      </c>
+      <c r="D1608" t="s">
+        <v>405</v>
       </c>
       <c r="H1608" t="s">
-        <v>1236</v>
+        <v>71</v>
       </c>
       <c r="M1608" t="s">
-        <v>3868</v>
+        <v>3871</v>
       </c>
     </row>
     <row r="1609" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1609">
-        <v>1652</v>
+        <v>1653</v>
       </c>
       <c r="B1609" t="s">
-        <v>3869</v>
+        <v>3872</v>
       </c>
       <c r="C1609" t="s">
-        <v>3870</v>
+        <v>3873</v>
       </c>
       <c r="D1609" t="s">
-        <v>405</v>
-      </c>
-      <c r="H1609" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="M1609" t="s">
-        <v>3871</v>
+        <v>4493</v>
       </c>
     </row>
     <row r="1610" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1610">
-        <v>1653</v>
+        <v>1654</v>
       </c>
       <c r="B1610" t="s">
-        <v>3872</v>
+        <v>3874</v>
       </c>
       <c r="C1610" t="s">
-        <v>3873</v>
-      </c>
-      <c r="D1610" t="s">
-        <v>14</v>
+        <v>3875</v>
+      </c>
+      <c r="D1610">
+        <v>68000</v>
+      </c>
+      <c r="E1610" t="s">
+        <v>154</v>
+      </c>
+      <c r="H1610" t="s">
+        <v>1353</v>
       </c>
       <c r="M1610" t="s">
-        <v>4493</v>
+        <v>3876</v>
       </c>
     </row>
     <row r="1611" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1611">
-        <v>1654</v>
+        <v>1655</v>
       </c>
       <c r="B1611" t="s">
-        <v>3874</v>
+        <v>3877</v>
       </c>
       <c r="C1611" t="s">
         <v>3875</v>
@@ -61007,15 +61030,15 @@
         <v>1353</v>
       </c>
       <c r="M1611" t="s">
-        <v>3876</v>
+        <v>4494</v>
       </c>
     </row>
     <row r="1612" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1612">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="B1612" t="s">
-        <v>3877</v>
+        <v>3878</v>
       </c>
       <c r="C1612" t="s">
         <v>3875</v>
@@ -61030,15 +61053,15 @@
         <v>1353</v>
       </c>
       <c r="M1612" t="s">
-        <v>4494</v>
+        <v>3879</v>
       </c>
     </row>
     <row r="1613" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1613">
-        <v>1656</v>
+        <v>1657</v>
       </c>
       <c r="B1613" t="s">
-        <v>3878</v>
+        <v>3880</v>
       </c>
       <c r="C1613" t="s">
         <v>3875</v>
@@ -61053,15 +61076,15 @@
         <v>1353</v>
       </c>
       <c r="M1613" t="s">
-        <v>3879</v>
+        <v>3881</v>
       </c>
     </row>
     <row r="1614" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1614">
-        <v>1657</v>
+        <v>1658</v>
       </c>
       <c r="B1614" t="s">
-        <v>3880</v>
+        <v>3882</v>
       </c>
       <c r="C1614" t="s">
         <v>3875</v>
@@ -61076,15 +61099,15 @@
         <v>1353</v>
       </c>
       <c r="M1614" t="s">
-        <v>3881</v>
+        <v>3883</v>
       </c>
     </row>
     <row r="1615" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1615">
-        <v>1658</v>
+        <v>1659</v>
       </c>
       <c r="B1615" t="s">
-        <v>3882</v>
+        <v>3884</v>
       </c>
       <c r="C1615" t="s">
         <v>3875</v>
@@ -61099,15 +61122,15 @@
         <v>1353</v>
       </c>
       <c r="M1615" t="s">
-        <v>3883</v>
+        <v>3885</v>
       </c>
     </row>
     <row r="1616" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1616">
-        <v>1659</v>
+        <v>1660</v>
       </c>
       <c r="B1616" t="s">
-        <v>3884</v>
+        <v>3886</v>
       </c>
       <c r="C1616" t="s">
         <v>3875</v>
@@ -61122,15 +61145,15 @@
         <v>1353</v>
       </c>
       <c r="M1616" t="s">
-        <v>3885</v>
+        <v>3887</v>
       </c>
     </row>
     <row r="1617" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1617">
-        <v>1660</v>
+        <v>1661</v>
       </c>
       <c r="B1617" t="s">
-        <v>3886</v>
+        <v>3888</v>
       </c>
       <c r="C1617" t="s">
         <v>3875</v>
@@ -61145,15 +61168,15 @@
         <v>1353</v>
       </c>
       <c r="M1617" t="s">
-        <v>3887</v>
+        <v>4495</v>
       </c>
     </row>
     <row r="1618" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1618">
-        <v>1661</v>
+        <v>1662</v>
       </c>
       <c r="B1618" t="s">
-        <v>3888</v>
+        <v>3889</v>
       </c>
       <c r="C1618" t="s">
         <v>3875</v>
@@ -61168,15 +61191,15 @@
         <v>1353</v>
       </c>
       <c r="M1618" t="s">
-        <v>4495</v>
+        <v>3890</v>
       </c>
     </row>
     <row r="1619" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1619">
-        <v>1662</v>
+        <v>1663</v>
       </c>
       <c r="B1619" t="s">
-        <v>3889</v>
+        <v>3891</v>
       </c>
       <c r="C1619" t="s">
         <v>3875</v>
@@ -61191,15 +61214,15 @@
         <v>1353</v>
       </c>
       <c r="M1619" t="s">
-        <v>3890</v>
+        <v>3892</v>
       </c>
     </row>
     <row r="1620" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1620">
-        <v>1663</v>
+        <v>1664</v>
       </c>
       <c r="B1620" t="s">
-        <v>3891</v>
+        <v>3893</v>
       </c>
       <c r="C1620" t="s">
         <v>3875</v>
@@ -61214,15 +61237,15 @@
         <v>1353</v>
       </c>
       <c r="M1620" t="s">
-        <v>3892</v>
+        <v>3894</v>
       </c>
     </row>
     <row r="1621" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1621">
-        <v>1664</v>
+        <v>1665</v>
       </c>
       <c r="B1621" t="s">
-        <v>3893</v>
+        <v>3895</v>
       </c>
       <c r="C1621" t="s">
         <v>3875</v>
@@ -61237,15 +61260,15 @@
         <v>1353</v>
       </c>
       <c r="M1621" t="s">
-        <v>3894</v>
+        <v>3896</v>
       </c>
     </row>
     <row r="1622" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1622">
-        <v>1665</v>
+        <v>1666</v>
       </c>
       <c r="B1622" t="s">
-        <v>3895</v>
+        <v>3897</v>
       </c>
       <c r="C1622" t="s">
         <v>3875</v>
@@ -61260,15 +61283,15 @@
         <v>1353</v>
       </c>
       <c r="M1622" t="s">
-        <v>3896</v>
+        <v>3898</v>
       </c>
     </row>
     <row r="1623" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1623">
-        <v>1666</v>
+        <v>1667</v>
       </c>
       <c r="B1623" t="s">
-        <v>3897</v>
+        <v>3899</v>
       </c>
       <c r="C1623" t="s">
         <v>3875</v>
@@ -61283,15 +61306,15 @@
         <v>1353</v>
       </c>
       <c r="M1623" t="s">
-        <v>3898</v>
+        <v>4496</v>
       </c>
     </row>
     <row r="1624" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1624">
-        <v>1667</v>
+        <v>1668</v>
       </c>
       <c r="B1624" t="s">
-        <v>3899</v>
+        <v>3900</v>
       </c>
       <c r="C1624" t="s">
         <v>3875</v>
@@ -61306,15 +61329,15 @@
         <v>1353</v>
       </c>
       <c r="M1624" t="s">
-        <v>4496</v>
+        <v>4497</v>
       </c>
     </row>
     <row r="1625" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1625">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="B1625" t="s">
-        <v>3900</v>
+        <v>3901</v>
       </c>
       <c r="C1625" t="s">
         <v>3875</v>
@@ -61329,15 +61352,15 @@
         <v>1353</v>
       </c>
       <c r="M1625" t="s">
-        <v>4497</v>
+        <v>3902</v>
       </c>
     </row>
     <row r="1626" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1626">
-        <v>1669</v>
+        <v>1670</v>
       </c>
       <c r="B1626" t="s">
-        <v>3901</v>
+        <v>3903</v>
       </c>
       <c r="C1626" t="s">
         <v>3875</v>
@@ -61352,15 +61375,15 @@
         <v>1353</v>
       </c>
       <c r="M1626" t="s">
-        <v>3902</v>
+        <v>3904</v>
       </c>
     </row>
     <row r="1627" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1627">
-        <v>1670</v>
+        <v>1671</v>
       </c>
       <c r="B1627" t="s">
-        <v>3903</v>
+        <v>3905</v>
       </c>
       <c r="C1627" t="s">
         <v>3875</v>
@@ -61375,15 +61398,15 @@
         <v>1353</v>
       </c>
       <c r="M1627" t="s">
-        <v>3904</v>
+        <v>3906</v>
       </c>
     </row>
     <row r="1628" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1628">
-        <v>1671</v>
+        <v>1672</v>
       </c>
       <c r="B1628" t="s">
-        <v>3905</v>
+        <v>3907</v>
       </c>
       <c r="C1628" t="s">
         <v>3875</v>
@@ -61398,15 +61421,15 @@
         <v>1353</v>
       </c>
       <c r="M1628" t="s">
-        <v>3906</v>
+        <v>3908</v>
       </c>
     </row>
     <row r="1629" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1629">
-        <v>1672</v>
+        <v>1673</v>
       </c>
       <c r="B1629" t="s">
-        <v>3907</v>
+        <v>3909</v>
       </c>
       <c r="C1629" t="s">
         <v>3875</v>
@@ -61421,15 +61444,15 @@
         <v>1353</v>
       </c>
       <c r="M1629" t="s">
-        <v>3908</v>
+        <v>3910</v>
       </c>
     </row>
     <row r="1630" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1630">
-        <v>1673</v>
+        <v>1674</v>
       </c>
       <c r="B1630" t="s">
-        <v>3909</v>
+        <v>3911</v>
       </c>
       <c r="C1630" t="s">
         <v>3875</v>
@@ -61444,15 +61467,15 @@
         <v>1353</v>
       </c>
       <c r="M1630" t="s">
-        <v>3910</v>
+        <v>3912</v>
       </c>
     </row>
     <row r="1631" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1631">
-        <v>1674</v>
+        <v>1675</v>
       </c>
       <c r="B1631" t="s">
-        <v>3911</v>
+        <v>3913</v>
       </c>
       <c r="C1631" t="s">
         <v>3875</v>
@@ -61467,15 +61490,15 @@
         <v>1353</v>
       </c>
       <c r="M1631" t="s">
-        <v>3912</v>
+        <v>4498</v>
       </c>
     </row>
     <row r="1632" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1632">
-        <v>1675</v>
+        <v>1676</v>
       </c>
       <c r="B1632" t="s">
-        <v>3913</v>
+        <v>3914</v>
       </c>
       <c r="C1632" t="s">
         <v>3875</v>
@@ -61490,15 +61513,15 @@
         <v>1353</v>
       </c>
       <c r="M1632" t="s">
-        <v>4498</v>
+        <v>3915</v>
       </c>
     </row>
     <row r="1633" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1633">
-        <v>1676</v>
+        <v>1677</v>
       </c>
       <c r="B1633" t="s">
-        <v>3914</v>
+        <v>3916</v>
       </c>
       <c r="C1633" t="s">
         <v>3875</v>
@@ -61513,15 +61536,15 @@
         <v>1353</v>
       </c>
       <c r="M1633" t="s">
-        <v>3915</v>
+        <v>3917</v>
       </c>
     </row>
     <row r="1634" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1634">
-        <v>1677</v>
+        <v>1678</v>
       </c>
       <c r="B1634" t="s">
-        <v>3916</v>
+        <v>3918</v>
       </c>
       <c r="C1634" t="s">
         <v>3875</v>
@@ -61536,15 +61559,15 @@
         <v>1353</v>
       </c>
       <c r="M1634" t="s">
-        <v>3917</v>
+        <v>3919</v>
       </c>
     </row>
     <row r="1635" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1635">
-        <v>1678</v>
+        <v>1679</v>
       </c>
       <c r="B1635" t="s">
-        <v>3918</v>
+        <v>3920</v>
       </c>
       <c r="C1635" t="s">
         <v>3875</v>
@@ -61559,15 +61582,15 @@
         <v>1353</v>
       </c>
       <c r="M1635" t="s">
-        <v>3919</v>
+        <v>4499</v>
       </c>
     </row>
     <row r="1636" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1636">
-        <v>1679</v>
+        <v>1680</v>
       </c>
       <c r="B1636" t="s">
-        <v>3920</v>
+        <v>3921</v>
       </c>
       <c r="C1636" t="s">
         <v>3875</v>
@@ -61582,15 +61605,15 @@
         <v>1353</v>
       </c>
       <c r="M1636" t="s">
-        <v>4499</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="1637" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1637">
-        <v>1680</v>
+        <v>1681</v>
       </c>
       <c r="B1637" t="s">
-        <v>3921</v>
+        <v>3922</v>
       </c>
       <c r="C1637" t="s">
         <v>3875</v>
@@ -61605,15 +61628,15 @@
         <v>1353</v>
       </c>
       <c r="M1637" t="s">
-        <v>4500</v>
+        <v>4501</v>
       </c>
     </row>
     <row r="1638" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1638">
-        <v>1681</v>
+        <v>1682</v>
       </c>
       <c r="B1638" t="s">
-        <v>3922</v>
+        <v>3923</v>
       </c>
       <c r="C1638" t="s">
         <v>3875</v>
@@ -61628,15 +61651,15 @@
         <v>1353</v>
       </c>
       <c r="M1638" t="s">
-        <v>4501</v>
+        <v>3924</v>
       </c>
     </row>
     <row r="1639" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1639">
-        <v>1682</v>
+        <v>1683</v>
       </c>
       <c r="B1639" t="s">
-        <v>3923</v>
+        <v>3925</v>
       </c>
       <c r="C1639" t="s">
         <v>3875</v>
@@ -61651,15 +61674,15 @@
         <v>1353</v>
       </c>
       <c r="M1639" t="s">
-        <v>3924</v>
+        <v>3926</v>
       </c>
     </row>
     <row r="1640" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1640">
-        <v>1683</v>
+        <v>1684</v>
       </c>
       <c r="B1640" t="s">
-        <v>3925</v>
+        <v>3927</v>
       </c>
       <c r="C1640" t="s">
         <v>3875</v>
@@ -61674,15 +61697,15 @@
         <v>1353</v>
       </c>
       <c r="M1640" t="s">
-        <v>3926</v>
+        <v>4502</v>
       </c>
     </row>
     <row r="1641" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1641">
-        <v>1684</v>
+        <v>1685</v>
       </c>
       <c r="B1641" t="s">
-        <v>3927</v>
+        <v>3928</v>
       </c>
       <c r="C1641" t="s">
         <v>3875</v>
@@ -61697,15 +61720,15 @@
         <v>1353</v>
       </c>
       <c r="M1641" t="s">
-        <v>4502</v>
+        <v>3929</v>
       </c>
     </row>
     <row r="1642" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1642">
-        <v>1685</v>
+        <v>1686</v>
       </c>
       <c r="B1642" t="s">
-        <v>3928</v>
+        <v>3930</v>
       </c>
       <c r="C1642" t="s">
         <v>3875</v>
@@ -61720,15 +61743,15 @@
         <v>1353</v>
       </c>
       <c r="M1642" t="s">
-        <v>3929</v>
+        <v>4503</v>
       </c>
     </row>
     <row r="1643" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1643">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="B1643" t="s">
-        <v>3930</v>
+        <v>3931</v>
       </c>
       <c r="C1643" t="s">
         <v>3875</v>
@@ -61743,15 +61766,15 @@
         <v>1353</v>
       </c>
       <c r="M1643" t="s">
-        <v>4503</v>
+        <v>3932</v>
       </c>
     </row>
     <row r="1644" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1644">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="B1644" t="s">
-        <v>3931</v>
+        <v>3933</v>
       </c>
       <c r="C1644" t="s">
         <v>3875</v>
@@ -61766,15 +61789,15 @@
         <v>1353</v>
       </c>
       <c r="M1644" t="s">
-        <v>3932</v>
+        <v>3934</v>
       </c>
     </row>
     <row r="1645" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1645">
-        <v>1688</v>
+        <v>1689</v>
       </c>
       <c r="B1645" t="s">
-        <v>3933</v>
+        <v>3935</v>
       </c>
       <c r="C1645" t="s">
         <v>3875</v>
@@ -61789,15 +61812,15 @@
         <v>1353</v>
       </c>
       <c r="M1645" t="s">
-        <v>3934</v>
+        <v>4504</v>
       </c>
     </row>
     <row r="1646" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1646">
-        <v>1689</v>
+        <v>1690</v>
       </c>
       <c r="B1646" t="s">
-        <v>3935</v>
+        <v>3936</v>
       </c>
       <c r="C1646" t="s">
         <v>3875</v>
@@ -61812,15 +61835,15 @@
         <v>1353</v>
       </c>
       <c r="M1646" t="s">
-        <v>4504</v>
+        <v>4505</v>
       </c>
     </row>
     <row r="1647" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1647">
-        <v>1690</v>
+        <v>1691</v>
       </c>
       <c r="B1647" t="s">
-        <v>3936</v>
+        <v>3937</v>
       </c>
       <c r="C1647" t="s">
         <v>3875</v>
@@ -61835,15 +61858,15 @@
         <v>1353</v>
       </c>
       <c r="M1647" t="s">
-        <v>4505</v>
+        <v>3938</v>
       </c>
     </row>
     <row r="1648" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1648">
-        <v>1691</v>
+        <v>1692</v>
       </c>
       <c r="B1648" t="s">
-        <v>3937</v>
+        <v>3939</v>
       </c>
       <c r="C1648" t="s">
         <v>3875</v>
@@ -61858,15 +61881,15 @@
         <v>1353</v>
       </c>
       <c r="M1648" t="s">
-        <v>3938</v>
+        <v>4506</v>
       </c>
     </row>
     <row r="1649" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1649">
-        <v>1692</v>
+        <v>1693</v>
       </c>
       <c r="B1649" t="s">
-        <v>3939</v>
+        <v>3940</v>
       </c>
       <c r="C1649" t="s">
         <v>3875</v>
@@ -61881,15 +61904,15 @@
         <v>1353</v>
       </c>
       <c r="M1649" t="s">
-        <v>4506</v>
+        <v>4507</v>
       </c>
     </row>
     <row r="1650" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1650">
-        <v>1693</v>
+        <v>1694</v>
       </c>
       <c r="B1650" t="s">
-        <v>3940</v>
+        <v>3941</v>
       </c>
       <c r="C1650" t="s">
         <v>3875</v>
@@ -61904,15 +61927,15 @@
         <v>1353</v>
       </c>
       <c r="M1650" t="s">
-        <v>4507</v>
+        <v>4508</v>
       </c>
     </row>
     <row r="1651" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1651">
-        <v>1694</v>
+        <v>1695</v>
       </c>
       <c r="B1651" t="s">
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C1651" t="s">
         <v>3875</v>
@@ -61927,15 +61950,15 @@
         <v>1353</v>
       </c>
       <c r="M1651" t="s">
-        <v>4508</v>
+        <v>4509</v>
       </c>
     </row>
     <row r="1652" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1652">
-        <v>1695</v>
+        <v>1696</v>
       </c>
       <c r="B1652" t="s">
-        <v>3942</v>
+        <v>3943</v>
       </c>
       <c r="C1652" t="s">
         <v>3875</v>
@@ -61950,15 +61973,15 @@
         <v>1353</v>
       </c>
       <c r="M1652" t="s">
-        <v>4509</v>
+        <v>4510</v>
       </c>
     </row>
     <row r="1653" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1653">
-        <v>1696</v>
+        <v>1697</v>
       </c>
       <c r="B1653" t="s">
-        <v>3943</v>
+        <v>3944</v>
       </c>
       <c r="C1653" t="s">
         <v>3875</v>
@@ -61973,15 +61996,15 @@
         <v>1353</v>
       </c>
       <c r="M1653" t="s">
-        <v>4510</v>
+        <v>4511</v>
       </c>
     </row>
     <row r="1654" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1654">
-        <v>1697</v>
+        <v>1698</v>
       </c>
       <c r="B1654" t="s">
-        <v>3944</v>
+        <v>3945</v>
       </c>
       <c r="C1654" t="s">
         <v>3875</v>
@@ -61996,15 +62019,15 @@
         <v>1353</v>
       </c>
       <c r="M1654" t="s">
-        <v>4511</v>
+        <v>4512</v>
       </c>
     </row>
     <row r="1655" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1655">
-        <v>1698</v>
+        <v>1699</v>
       </c>
       <c r="B1655" t="s">
-        <v>3945</v>
+        <v>3946</v>
       </c>
       <c r="C1655" t="s">
         <v>3875</v>
@@ -62019,15 +62042,15 @@
         <v>1353</v>
       </c>
       <c r="M1655" t="s">
-        <v>4512</v>
+        <v>3947</v>
       </c>
     </row>
     <row r="1656" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1656">
-        <v>1699</v>
+        <v>1700</v>
       </c>
       <c r="B1656" t="s">
-        <v>3946</v>
+        <v>3948</v>
       </c>
       <c r="C1656" t="s">
         <v>3875</v>
@@ -62042,15 +62065,15 @@
         <v>1353</v>
       </c>
       <c r="M1656" t="s">
-        <v>3947</v>
+        <v>3949</v>
       </c>
     </row>
     <row r="1657" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1657">
-        <v>1700</v>
+        <v>1701</v>
       </c>
       <c r="B1657" t="s">
-        <v>3948</v>
+        <v>3950</v>
       </c>
       <c r="C1657" t="s">
         <v>3875</v>
@@ -62065,15 +62088,15 @@
         <v>1353</v>
       </c>
       <c r="M1657" t="s">
-        <v>3949</v>
+        <v>3951</v>
       </c>
     </row>
     <row r="1658" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1658">
-        <v>1701</v>
+        <v>1702</v>
       </c>
       <c r="B1658" t="s">
-        <v>3950</v>
+        <v>3952</v>
       </c>
       <c r="C1658" t="s">
         <v>3875</v>
@@ -62088,15 +62111,15 @@
         <v>1353</v>
       </c>
       <c r="M1658" t="s">
-        <v>3951</v>
+        <v>4513</v>
       </c>
     </row>
     <row r="1659" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1659">
-        <v>1702</v>
+        <v>1703</v>
       </c>
       <c r="B1659" t="s">
-        <v>3952</v>
+        <v>3953</v>
       </c>
       <c r="C1659" t="s">
         <v>3875</v>
@@ -62111,15 +62134,15 @@
         <v>1353</v>
       </c>
       <c r="M1659" t="s">
-        <v>4513</v>
+        <v>3954</v>
       </c>
     </row>
     <row r="1660" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1660">
-        <v>1703</v>
+        <v>1704</v>
       </c>
       <c r="B1660" t="s">
-        <v>3953</v>
+        <v>3955</v>
       </c>
       <c r="C1660" t="s">
         <v>3875</v>
@@ -62134,15 +62157,15 @@
         <v>1353</v>
       </c>
       <c r="M1660" t="s">
-        <v>3954</v>
+        <v>3956</v>
       </c>
     </row>
     <row r="1661" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1661">
-        <v>1704</v>
+        <v>1705</v>
       </c>
       <c r="B1661" t="s">
-        <v>3955</v>
+        <v>3957</v>
       </c>
       <c r="C1661" t="s">
         <v>3875</v>
@@ -62157,15 +62180,15 @@
         <v>1353</v>
       </c>
       <c r="M1661" t="s">
-        <v>3956</v>
+        <v>4514</v>
       </c>
     </row>
     <row r="1662" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1662">
-        <v>1705</v>
+        <v>1706</v>
       </c>
       <c r="B1662" t="s">
-        <v>3957</v>
+        <v>3958</v>
       </c>
       <c r="C1662" t="s">
         <v>3875</v>
@@ -62180,15 +62203,15 @@
         <v>1353</v>
       </c>
       <c r="M1662" t="s">
-        <v>4514</v>
+        <v>3959</v>
       </c>
     </row>
     <row r="1663" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1663">
-        <v>1706</v>
+        <v>1707</v>
       </c>
       <c r="B1663" t="s">
-        <v>3958</v>
+        <v>3960</v>
       </c>
       <c r="C1663" t="s">
         <v>3875</v>
@@ -62203,15 +62226,15 @@
         <v>1353</v>
       </c>
       <c r="M1663" t="s">
-        <v>3959</v>
+        <v>4515</v>
       </c>
     </row>
     <row r="1664" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1664">
-        <v>1707</v>
+        <v>1708</v>
       </c>
       <c r="B1664" t="s">
-        <v>3960</v>
+        <v>3961</v>
       </c>
       <c r="C1664" t="s">
         <v>3875</v>
@@ -62226,15 +62249,15 @@
         <v>1353</v>
       </c>
       <c r="M1664" t="s">
-        <v>4515</v>
+        <v>4516</v>
       </c>
     </row>
     <row r="1665" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1665">
-        <v>1708</v>
+        <v>1709</v>
       </c>
       <c r="B1665" t="s">
-        <v>3961</v>
+        <v>3962</v>
       </c>
       <c r="C1665" t="s">
         <v>3875</v>
@@ -62249,15 +62272,15 @@
         <v>1353</v>
       </c>
       <c r="M1665" t="s">
-        <v>4516</v>
+        <v>4517</v>
       </c>
     </row>
     <row r="1666" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1666">
-        <v>1709</v>
+        <v>1710</v>
       </c>
       <c r="B1666" t="s">
-        <v>3962</v>
+        <v>3963</v>
       </c>
       <c r="C1666" t="s">
         <v>3875</v>
@@ -62272,15 +62295,15 @@
         <v>1353</v>
       </c>
       <c r="M1666" t="s">
-        <v>4517</v>
+        <v>4518</v>
       </c>
     </row>
     <row r="1667" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1667">
-        <v>1710</v>
+        <v>1711</v>
       </c>
       <c r="B1667" t="s">
-        <v>3963</v>
+        <v>3964</v>
       </c>
       <c r="C1667" t="s">
         <v>3875</v>
@@ -62295,15 +62318,15 @@
         <v>1353</v>
       </c>
       <c r="M1667" t="s">
-        <v>4518</v>
+        <v>4519</v>
       </c>
     </row>
     <row r="1668" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1668">
-        <v>1711</v>
+        <v>1712</v>
       </c>
       <c r="B1668" t="s">
-        <v>3964</v>
+        <v>3965</v>
       </c>
       <c r="C1668" t="s">
         <v>3875</v>
@@ -62318,15 +62341,15 @@
         <v>1353</v>
       </c>
       <c r="M1668" t="s">
-        <v>4519</v>
+        <v>4520</v>
       </c>
     </row>
     <row r="1669" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1669">
-        <v>1712</v>
+        <v>1713</v>
       </c>
       <c r="B1669" t="s">
-        <v>3965</v>
+        <v>3966</v>
       </c>
       <c r="C1669" t="s">
         <v>3875</v>
@@ -62341,15 +62364,15 @@
         <v>1353</v>
       </c>
       <c r="M1669" t="s">
-        <v>4520</v>
+        <v>3967</v>
       </c>
     </row>
     <row r="1670" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1670">
-        <v>1713</v>
+        <v>1714</v>
       </c>
       <c r="B1670" t="s">
-        <v>3966</v>
+        <v>3968</v>
       </c>
       <c r="C1670" t="s">
         <v>3875</v>
@@ -62364,15 +62387,15 @@
         <v>1353</v>
       </c>
       <c r="M1670" t="s">
-        <v>3967</v>
+        <v>4521</v>
       </c>
     </row>
     <row r="1671" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1671">
-        <v>1714</v>
+        <v>1715</v>
       </c>
       <c r="B1671" t="s">
-        <v>3968</v>
+        <v>3969</v>
       </c>
       <c r="C1671" t="s">
         <v>3875</v>
@@ -62387,15 +62410,15 @@
         <v>1353</v>
       </c>
       <c r="M1671" t="s">
-        <v>4521</v>
+        <v>4522</v>
       </c>
     </row>
     <row r="1672" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1672">
-        <v>1715</v>
+        <v>1716</v>
       </c>
       <c r="B1672" t="s">
-        <v>3969</v>
+        <v>3970</v>
       </c>
       <c r="C1672" t="s">
         <v>3875</v>
@@ -62410,15 +62433,15 @@
         <v>1353</v>
       </c>
       <c r="M1672" t="s">
-        <v>4522</v>
+        <v>3971</v>
       </c>
     </row>
     <row r="1673" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1673">
-        <v>1716</v>
+        <v>1717</v>
       </c>
       <c r="B1673" t="s">
-        <v>3970</v>
+        <v>3972</v>
       </c>
       <c r="C1673" t="s">
         <v>3875</v>
@@ -62433,15 +62456,15 @@
         <v>1353</v>
       </c>
       <c r="M1673" t="s">
-        <v>3971</v>
+        <v>3973</v>
       </c>
     </row>
     <row r="1674" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1674">
-        <v>1717</v>
+        <v>1718</v>
       </c>
       <c r="B1674" t="s">
-        <v>3972</v>
+        <v>3974</v>
       </c>
       <c r="C1674" t="s">
         <v>3875</v>
@@ -62456,15 +62479,15 @@
         <v>1353</v>
       </c>
       <c r="M1674" t="s">
-        <v>3973</v>
+        <v>4523</v>
       </c>
     </row>
     <row r="1675" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1675">
-        <v>1718</v>
+        <v>1719</v>
       </c>
       <c r="B1675" t="s">
-        <v>3974</v>
+        <v>3975</v>
       </c>
       <c r="C1675" t="s">
         <v>3875</v>
@@ -62479,15 +62502,15 @@
         <v>1353</v>
       </c>
       <c r="M1675" t="s">
-        <v>4523</v>
+        <v>3976</v>
       </c>
     </row>
     <row r="1676" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1676">
-        <v>1719</v>
+        <v>1720</v>
       </c>
       <c r="B1676" t="s">
-        <v>3975</v>
+        <v>3977</v>
       </c>
       <c r="C1676" t="s">
         <v>3875</v>
@@ -62502,15 +62525,15 @@
         <v>1353</v>
       </c>
       <c r="M1676" t="s">
-        <v>3976</v>
+        <v>4524</v>
       </c>
     </row>
     <row r="1677" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1677">
-        <v>1720</v>
+        <v>1721</v>
       </c>
       <c r="B1677" t="s">
-        <v>3977</v>
+        <v>3978</v>
       </c>
       <c r="C1677" t="s">
         <v>3875</v>
@@ -62525,15 +62548,15 @@
         <v>1353</v>
       </c>
       <c r="M1677" t="s">
-        <v>4524</v>
+        <v>4525</v>
       </c>
     </row>
     <row r="1678" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1678">
-        <v>1721</v>
+        <v>1722</v>
       </c>
       <c r="B1678" t="s">
-        <v>3978</v>
+        <v>3979</v>
       </c>
       <c r="C1678" t="s">
         <v>3875</v>
@@ -62548,15 +62571,15 @@
         <v>1353</v>
       </c>
       <c r="M1678" t="s">
-        <v>4525</v>
+        <v>4526</v>
       </c>
     </row>
     <row r="1679" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1679">
-        <v>1722</v>
+        <v>1723</v>
       </c>
       <c r="B1679" t="s">
-        <v>3979</v>
+        <v>3980</v>
       </c>
       <c r="C1679" t="s">
         <v>3875</v>
@@ -62571,15 +62594,15 @@
         <v>1353</v>
       </c>
       <c r="M1679" t="s">
-        <v>4526</v>
+        <v>4527</v>
       </c>
     </row>
     <row r="1680" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1680">
-        <v>1723</v>
+        <v>1724</v>
       </c>
       <c r="B1680" t="s">
-        <v>3980</v>
+        <v>3981</v>
       </c>
       <c r="C1680" t="s">
         <v>3875</v>
@@ -62594,15 +62617,15 @@
         <v>1353</v>
       </c>
       <c r="M1680" t="s">
-        <v>4527</v>
+        <v>4528</v>
       </c>
     </row>
     <row r="1681" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1681">
-        <v>1724</v>
+        <v>1725</v>
       </c>
       <c r="B1681" t="s">
-        <v>3981</v>
+        <v>3982</v>
       </c>
       <c r="C1681" t="s">
         <v>3875</v>
@@ -62617,15 +62640,15 @@
         <v>1353</v>
       </c>
       <c r="M1681" t="s">
-        <v>4528</v>
+        <v>3983</v>
       </c>
     </row>
     <row r="1682" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1682">
-        <v>1725</v>
+        <v>1726</v>
       </c>
       <c r="B1682" t="s">
-        <v>3982</v>
+        <v>3984</v>
       </c>
       <c r="C1682" t="s">
         <v>3875</v>
@@ -62640,15 +62663,15 @@
         <v>1353</v>
       </c>
       <c r="M1682" t="s">
-        <v>3983</v>
+        <v>4529</v>
       </c>
     </row>
     <row r="1683" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1683">
-        <v>1726</v>
+        <v>1727</v>
       </c>
       <c r="B1683" t="s">
-        <v>3984</v>
+        <v>3985</v>
       </c>
       <c r="C1683" t="s">
         <v>3875</v>
@@ -62663,15 +62686,15 @@
         <v>1353</v>
       </c>
       <c r="M1683" t="s">
-        <v>4529</v>
+        <v>3986</v>
       </c>
     </row>
     <row r="1684" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1684">
-        <v>1727</v>
+        <v>1728</v>
       </c>
       <c r="B1684" t="s">
-        <v>3985</v>
+        <v>3987</v>
       </c>
       <c r="C1684" t="s">
         <v>3875</v>
@@ -62686,15 +62709,15 @@
         <v>1353</v>
       </c>
       <c r="M1684" t="s">
-        <v>3986</v>
+        <v>4530</v>
       </c>
     </row>
     <row r="1685" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1685">
-        <v>1728</v>
+        <v>1729</v>
       </c>
       <c r="B1685" t="s">
-        <v>3987</v>
+        <v>3988</v>
       </c>
       <c r="C1685" t="s">
         <v>3875</v>
@@ -62709,15 +62732,15 @@
         <v>1353</v>
       </c>
       <c r="M1685" t="s">
-        <v>4530</v>
+        <v>3989</v>
       </c>
     </row>
     <row r="1686" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1686">
-        <v>1729</v>
+        <v>1730</v>
       </c>
       <c r="B1686" t="s">
-        <v>3988</v>
+        <v>3990</v>
       </c>
       <c r="C1686" t="s">
         <v>3875</v>
@@ -62732,15 +62755,15 @@
         <v>1353</v>
       </c>
       <c r="M1686" t="s">
-        <v>3989</v>
+        <v>3991</v>
       </c>
     </row>
     <row r="1687" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1687">
-        <v>1730</v>
+        <v>1731</v>
       </c>
       <c r="B1687" t="s">
-        <v>3990</v>
+        <v>3992</v>
       </c>
       <c r="C1687" t="s">
         <v>3875</v>
@@ -62755,15 +62778,15 @@
         <v>1353</v>
       </c>
       <c r="M1687" t="s">
-        <v>3991</v>
+        <v>4531</v>
       </c>
     </row>
     <row r="1688" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1688">
-        <v>1731</v>
+        <v>1732</v>
       </c>
       <c r="B1688" t="s">
-        <v>3992</v>
+        <v>3993</v>
       </c>
       <c r="C1688" t="s">
         <v>3875</v>
@@ -62778,15 +62801,15 @@
         <v>1353</v>
       </c>
       <c r="M1688" t="s">
-        <v>4531</v>
+        <v>4532</v>
       </c>
     </row>
     <row r="1689" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1689">
-        <v>1732</v>
+        <v>1733</v>
       </c>
       <c r="B1689" t="s">
-        <v>3993</v>
+        <v>3994</v>
       </c>
       <c r="C1689" t="s">
         <v>3875</v>
@@ -62801,15 +62824,15 @@
         <v>1353</v>
       </c>
       <c r="M1689" t="s">
-        <v>4532</v>
+        <v>3995</v>
       </c>
     </row>
     <row r="1690" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1690">
-        <v>1733</v>
+        <v>1734</v>
       </c>
       <c r="B1690" t="s">
-        <v>3994</v>
+        <v>3996</v>
       </c>
       <c r="C1690" t="s">
         <v>3875</v>
@@ -62824,15 +62847,15 @@
         <v>1353</v>
       </c>
       <c r="M1690" t="s">
-        <v>3995</v>
+        <v>3997</v>
       </c>
     </row>
     <row r="1691" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1691">
-        <v>1734</v>
+        <v>1735</v>
       </c>
       <c r="B1691" t="s">
-        <v>3996</v>
+        <v>3998</v>
       </c>
       <c r="C1691" t="s">
         <v>3875</v>
@@ -62847,15 +62870,15 @@
         <v>1353</v>
       </c>
       <c r="M1691" t="s">
-        <v>3997</v>
+        <v>4533</v>
       </c>
     </row>
     <row r="1692" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1692">
-        <v>1735</v>
+        <v>1736</v>
       </c>
       <c r="B1692" t="s">
-        <v>3998</v>
+        <v>3999</v>
       </c>
       <c r="C1692" t="s">
         <v>3875</v>
@@ -62870,15 +62893,15 @@
         <v>1353</v>
       </c>
       <c r="M1692" t="s">
-        <v>4533</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="1693" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1693">
-        <v>1736</v>
+        <v>1737</v>
       </c>
       <c r="B1693" t="s">
-        <v>3999</v>
+        <v>4001</v>
       </c>
       <c r="C1693" t="s">
         <v>3875</v>
@@ -62893,15 +62916,15 @@
         <v>1353</v>
       </c>
       <c r="M1693" t="s">
-        <v>4000</v>
+        <v>4534</v>
       </c>
     </row>
     <row r="1694" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1694">
-        <v>1737</v>
+        <v>1738</v>
       </c>
       <c r="B1694" t="s">
-        <v>4001</v>
+        <v>4002</v>
       </c>
       <c r="C1694" t="s">
         <v>3875</v>
@@ -62916,15 +62939,15 @@
         <v>1353</v>
       </c>
       <c r="M1694" t="s">
-        <v>4534</v>
+        <v>4535</v>
       </c>
     </row>
     <row r="1695" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1695">
-        <v>1738</v>
+        <v>1739</v>
       </c>
       <c r="B1695" t="s">
-        <v>4002</v>
+        <v>4003</v>
       </c>
       <c r="C1695" t="s">
         <v>3875</v>
@@ -62939,15 +62962,15 @@
         <v>1353</v>
       </c>
       <c r="M1695" t="s">
-        <v>4535</v>
+        <v>4536</v>
       </c>
     </row>
     <row r="1696" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1696">
-        <v>1739</v>
+        <v>1740</v>
       </c>
       <c r="B1696" t="s">
-        <v>4003</v>
+        <v>4004</v>
       </c>
       <c r="C1696" t="s">
         <v>3875</v>
@@ -62962,15 +62985,15 @@
         <v>1353</v>
       </c>
       <c r="M1696" t="s">
-        <v>4536</v>
+        <v>4537</v>
       </c>
     </row>
     <row r="1697" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1697">
-        <v>1740</v>
+        <v>1741</v>
       </c>
       <c r="B1697" t="s">
-        <v>4004</v>
+        <v>4005</v>
       </c>
       <c r="C1697" t="s">
         <v>3875</v>
@@ -62985,15 +63008,15 @@
         <v>1353</v>
       </c>
       <c r="M1697" t="s">
-        <v>4537</v>
+        <v>4538</v>
       </c>
     </row>
     <row r="1698" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1698">
-        <v>1741</v>
+        <v>1742</v>
       </c>
       <c r="B1698" t="s">
-        <v>4005</v>
+        <v>4006</v>
       </c>
       <c r="C1698" t="s">
         <v>3875</v>
@@ -63008,15 +63031,15 @@
         <v>1353</v>
       </c>
       <c r="M1698" t="s">
-        <v>4538</v>
+        <v>4539</v>
       </c>
     </row>
     <row r="1699" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1699">
-        <v>1742</v>
+        <v>1743</v>
       </c>
       <c r="B1699" t="s">
-        <v>4006</v>
+        <v>4007</v>
       </c>
       <c r="C1699" t="s">
         <v>3875</v>
@@ -63031,15 +63054,15 @@
         <v>1353</v>
       </c>
       <c r="M1699" t="s">
-        <v>4539</v>
+        <v>4008</v>
       </c>
     </row>
     <row r="1700" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1700">
-        <v>1743</v>
+        <v>1744</v>
       </c>
       <c r="B1700" t="s">
-        <v>4007</v>
+        <v>4009</v>
       </c>
       <c r="C1700" t="s">
         <v>3875</v>
@@ -63054,15 +63077,15 @@
         <v>1353</v>
       </c>
       <c r="M1700" t="s">
-        <v>4008</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="1701" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1701">
-        <v>1744</v>
+        <v>1745</v>
       </c>
       <c r="B1701" t="s">
-        <v>4009</v>
+        <v>4010</v>
       </c>
       <c r="C1701" t="s">
         <v>3875</v>
@@ -63077,15 +63100,15 @@
         <v>1353</v>
       </c>
       <c r="M1701" t="s">
-        <v>4540</v>
+        <v>4541</v>
       </c>
     </row>
     <row r="1702" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1702">
-        <v>1745</v>
+        <v>1746</v>
       </c>
       <c r="B1702" t="s">
-        <v>4010</v>
+        <v>4011</v>
       </c>
       <c r="C1702" t="s">
         <v>3875</v>
@@ -63100,15 +63123,15 @@
         <v>1353</v>
       </c>
       <c r="M1702" t="s">
-        <v>4541</v>
+        <v>4012</v>
       </c>
     </row>
     <row r="1703" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1703">
-        <v>1746</v>
+        <v>1747</v>
       </c>
       <c r="B1703" t="s">
-        <v>4011</v>
+        <v>4013</v>
       </c>
       <c r="C1703" t="s">
         <v>3875</v>
@@ -63123,15 +63146,15 @@
         <v>1353</v>
       </c>
       <c r="M1703" t="s">
-        <v>4012</v>
+        <v>4542</v>
       </c>
     </row>
     <row r="1704" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1704">
-        <v>1747</v>
+        <v>1748</v>
       </c>
       <c r="B1704" t="s">
-        <v>4013</v>
+        <v>4014</v>
       </c>
       <c r="C1704" t="s">
         <v>3875</v>
@@ -63146,15 +63169,15 @@
         <v>1353</v>
       </c>
       <c r="M1704" t="s">
-        <v>4542</v>
+        <v>4015</v>
       </c>
     </row>
     <row r="1705" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1705">
-        <v>1748</v>
+        <v>1749</v>
       </c>
       <c r="B1705" t="s">
-        <v>4014</v>
+        <v>4016</v>
       </c>
       <c r="C1705" t="s">
         <v>3875</v>
@@ -63169,15 +63192,15 @@
         <v>1353</v>
       </c>
       <c r="M1705" t="s">
-        <v>4015</v>
+        <v>4017</v>
       </c>
     </row>
     <row r="1706" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1706">
-        <v>1749</v>
+        <v>1750</v>
       </c>
       <c r="B1706" t="s">
-        <v>4016</v>
+        <v>4018</v>
       </c>
       <c r="C1706" t="s">
         <v>3875</v>
@@ -63192,15 +63215,15 @@
         <v>1353</v>
       </c>
       <c r="M1706" t="s">
-        <v>4017</v>
+        <v>4543</v>
       </c>
     </row>
     <row r="1707" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1707">
-        <v>1750</v>
+        <v>1751</v>
       </c>
       <c r="B1707" t="s">
-        <v>4018</v>
+        <v>4019</v>
       </c>
       <c r="C1707" t="s">
         <v>3875</v>
@@ -63215,15 +63238,15 @@
         <v>1353</v>
       </c>
       <c r="M1707" t="s">
-        <v>4543</v>
+        <v>4020</v>
       </c>
     </row>
     <row r="1708" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1708">
-        <v>1751</v>
+        <v>1752</v>
       </c>
       <c r="B1708" t="s">
-        <v>4019</v>
+        <v>4021</v>
       </c>
       <c r="C1708" t="s">
         <v>3875</v>
@@ -63238,15 +63261,15 @@
         <v>1353</v>
       </c>
       <c r="M1708" t="s">
-        <v>4020</v>
+        <v>4544</v>
       </c>
     </row>
     <row r="1709" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1709">
-        <v>1752</v>
+        <v>1753</v>
       </c>
       <c r="B1709" t="s">
-        <v>4021</v>
+        <v>4022</v>
       </c>
       <c r="C1709" t="s">
         <v>3875</v>
@@ -63261,15 +63284,15 @@
         <v>1353</v>
       </c>
       <c r="M1709" t="s">
-        <v>4544</v>
+        <v>4545</v>
       </c>
     </row>
     <row r="1710" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1710">
-        <v>1753</v>
+        <v>1754</v>
       </c>
       <c r="B1710" t="s">
-        <v>4022</v>
+        <v>4023</v>
       </c>
       <c r="C1710" t="s">
         <v>3875</v>
@@ -63284,15 +63307,15 @@
         <v>1353</v>
       </c>
       <c r="M1710" t="s">
-        <v>4545</v>
+        <v>4546</v>
       </c>
     </row>
     <row r="1711" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1711">
-        <v>1754</v>
+        <v>1755</v>
       </c>
       <c r="B1711" t="s">
-        <v>4023</v>
+        <v>4024</v>
       </c>
       <c r="C1711" t="s">
         <v>3875</v>
@@ -63307,15 +63330,15 @@
         <v>1353</v>
       </c>
       <c r="M1711" t="s">
-        <v>4546</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="1712" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1712">
-        <v>1755</v>
+        <v>1756</v>
       </c>
       <c r="B1712" t="s">
-        <v>4024</v>
+        <v>4025</v>
       </c>
       <c r="C1712" t="s">
         <v>3875</v>
@@ -63330,15 +63353,15 @@
         <v>1353</v>
       </c>
       <c r="M1712" t="s">
-        <v>4547</v>
+        <v>4548</v>
       </c>
     </row>
     <row r="1713" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1713">
-        <v>1756</v>
+        <v>1757</v>
       </c>
       <c r="B1713" t="s">
-        <v>4025</v>
+        <v>4026</v>
       </c>
       <c r="C1713" t="s">
         <v>3875</v>
@@ -63353,15 +63376,15 @@
         <v>1353</v>
       </c>
       <c r="M1713" t="s">
-        <v>4548</v>
+        <v>4027</v>
       </c>
     </row>
     <row r="1714" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1714">
-        <v>1757</v>
+        <v>1758</v>
       </c>
       <c r="B1714" t="s">
-        <v>4026</v>
+        <v>4028</v>
       </c>
       <c r="C1714" t="s">
         <v>3875</v>
@@ -63376,15 +63399,15 @@
         <v>1353</v>
       </c>
       <c r="M1714" t="s">
-        <v>4027</v>
+        <v>4549</v>
       </c>
     </row>
     <row r="1715" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1715">
-        <v>1758</v>
+        <v>1759</v>
       </c>
       <c r="B1715" t="s">
-        <v>4028</v>
+        <v>4029</v>
       </c>
       <c r="C1715" t="s">
         <v>3875</v>
@@ -63399,15 +63422,15 @@
         <v>1353</v>
       </c>
       <c r="M1715" t="s">
-        <v>4549</v>
+        <v>4550</v>
       </c>
     </row>
     <row r="1716" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1716">
-        <v>1759</v>
+        <v>1760</v>
       </c>
       <c r="B1716" t="s">
-        <v>4029</v>
+        <v>4030</v>
       </c>
       <c r="C1716" t="s">
         <v>3875</v>
@@ -63422,15 +63445,15 @@
         <v>1353</v>
       </c>
       <c r="M1716" t="s">
-        <v>4550</v>
+        <v>4031</v>
       </c>
     </row>
     <row r="1717" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1717">
-        <v>1760</v>
+        <v>1761</v>
       </c>
       <c r="B1717" t="s">
-        <v>4030</v>
+        <v>4032</v>
       </c>
       <c r="C1717" t="s">
         <v>3875</v>
@@ -63445,15 +63468,15 @@
         <v>1353</v>
       </c>
       <c r="M1717" t="s">
-        <v>4031</v>
+        <v>4033</v>
       </c>
     </row>
     <row r="1718" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1718">
-        <v>1761</v>
+        <v>1762</v>
       </c>
       <c r="B1718" t="s">
-        <v>4032</v>
+        <v>4034</v>
       </c>
       <c r="C1718" t="s">
         <v>3875</v>
@@ -63468,15 +63491,15 @@
         <v>1353</v>
       </c>
       <c r="M1718" t="s">
-        <v>4033</v>
+        <v>4035</v>
       </c>
     </row>
     <row r="1719" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1719">
-        <v>1762</v>
+        <v>1763</v>
       </c>
       <c r="B1719" t="s">
-        <v>4034</v>
+        <v>4036</v>
       </c>
       <c r="C1719" t="s">
         <v>3875</v>
@@ -63491,15 +63514,15 @@
         <v>1353</v>
       </c>
       <c r="M1719" t="s">
-        <v>4035</v>
+        <v>4037</v>
       </c>
     </row>
     <row r="1720" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1720">
-        <v>1763</v>
+        <v>1764</v>
       </c>
       <c r="B1720" t="s">
-        <v>4036</v>
+        <v>4038</v>
       </c>
       <c r="C1720" t="s">
         <v>3875</v>
@@ -63514,15 +63537,15 @@
         <v>1353</v>
       </c>
       <c r="M1720" t="s">
-        <v>4037</v>
+        <v>4551</v>
       </c>
     </row>
     <row r="1721" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1721">
-        <v>1764</v>
+        <v>1765</v>
       </c>
       <c r="B1721" t="s">
-        <v>4038</v>
+        <v>4039</v>
       </c>
       <c r="C1721" t="s">
         <v>3875</v>
@@ -63537,15 +63560,15 @@
         <v>1353</v>
       </c>
       <c r="M1721" t="s">
-        <v>4551</v>
+        <v>4040</v>
       </c>
     </row>
     <row r="1722" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1722">
-        <v>1765</v>
+        <v>1766</v>
       </c>
       <c r="B1722" t="s">
-        <v>4039</v>
+        <v>4041</v>
       </c>
       <c r="C1722" t="s">
         <v>3875</v>
@@ -63560,15 +63583,15 @@
         <v>1353</v>
       </c>
       <c r="M1722" t="s">
-        <v>4040</v>
+        <v>4042</v>
       </c>
     </row>
     <row r="1723" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1723">
-        <v>1766</v>
+        <v>1767</v>
       </c>
       <c r="B1723" t="s">
-        <v>4041</v>
+        <v>4043</v>
       </c>
       <c r="C1723" t="s">
         <v>3875</v>
@@ -63583,15 +63606,15 @@
         <v>1353</v>
       </c>
       <c r="M1723" t="s">
-        <v>4042</v>
+        <v>4552</v>
       </c>
     </row>
     <row r="1724" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1724">
-        <v>1767</v>
+        <v>1768</v>
       </c>
       <c r="B1724" t="s">
-        <v>4043</v>
+        <v>4044</v>
       </c>
       <c r="C1724" t="s">
         <v>3875</v>
@@ -63606,15 +63629,15 @@
         <v>1353</v>
       </c>
       <c r="M1724" t="s">
-        <v>4552</v>
+        <v>4045</v>
       </c>
     </row>
     <row r="1725" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1725">
-        <v>1768</v>
+        <v>1769</v>
       </c>
       <c r="B1725" t="s">
-        <v>4044</v>
+        <v>4046</v>
       </c>
       <c r="C1725" t="s">
         <v>3875</v>
@@ -63629,15 +63652,15 @@
         <v>1353</v>
       </c>
       <c r="M1725" t="s">
-        <v>4045</v>
+        <v>4553</v>
       </c>
     </row>
     <row r="1726" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1726">
-        <v>1769</v>
+        <v>1770</v>
       </c>
       <c r="B1726" t="s">
-        <v>4046</v>
+        <v>4047</v>
       </c>
       <c r="C1726" t="s">
         <v>3875</v>
@@ -63652,15 +63675,15 @@
         <v>1353</v>
       </c>
       <c r="M1726" t="s">
-        <v>4553</v>
+        <v>4048</v>
       </c>
     </row>
     <row r="1727" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1727">
-        <v>1770</v>
+        <v>1771</v>
       </c>
       <c r="B1727" t="s">
-        <v>4047</v>
+        <v>4049</v>
       </c>
       <c r="C1727" t="s">
         <v>3875</v>
@@ -63675,15 +63698,15 @@
         <v>1353</v>
       </c>
       <c r="M1727" t="s">
-        <v>4048</v>
+        <v>4050</v>
       </c>
     </row>
     <row r="1728" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1728">
-        <v>1771</v>
+        <v>1772</v>
       </c>
       <c r="B1728" t="s">
-        <v>4049</v>
+        <v>4051</v>
       </c>
       <c r="C1728" t="s">
         <v>3875</v>
@@ -63698,15 +63721,15 @@
         <v>1353</v>
       </c>
       <c r="M1728" t="s">
-        <v>4050</v>
+        <v>4052</v>
       </c>
     </row>
     <row r="1729" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1729">
-        <v>1772</v>
+        <v>1773</v>
       </c>
       <c r="B1729" t="s">
-        <v>4051</v>
+        <v>4053</v>
       </c>
       <c r="C1729" t="s">
         <v>3875</v>
@@ -63721,15 +63744,15 @@
         <v>1353</v>
       </c>
       <c r="M1729" t="s">
-        <v>4052</v>
+        <v>4554</v>
       </c>
     </row>
     <row r="1730" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1730">
-        <v>1773</v>
+        <v>1774</v>
       </c>
       <c r="B1730" t="s">
-        <v>4053</v>
+        <v>4054</v>
       </c>
       <c r="C1730" t="s">
         <v>3875</v>
@@ -63744,15 +63767,15 @@
         <v>1353</v>
       </c>
       <c r="M1730" t="s">
-        <v>4554</v>
+        <v>4555</v>
       </c>
     </row>
     <row r="1731" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1731">
-        <v>1774</v>
+        <v>1775</v>
       </c>
       <c r="B1731" t="s">
-        <v>4054</v>
+        <v>4055</v>
       </c>
       <c r="C1731" t="s">
         <v>3875</v>
@@ -63767,15 +63790,15 @@
         <v>1353</v>
       </c>
       <c r="M1731" t="s">
-        <v>4555</v>
+        <v>4556</v>
       </c>
     </row>
     <row r="1732" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1732">
-        <v>1775</v>
+        <v>1776</v>
       </c>
       <c r="B1732" t="s">
-        <v>4055</v>
+        <v>4056</v>
       </c>
       <c r="C1732" t="s">
         <v>3875</v>
@@ -63790,15 +63813,15 @@
         <v>1353</v>
       </c>
       <c r="M1732" t="s">
-        <v>4556</v>
+        <v>4557</v>
       </c>
     </row>
     <row r="1733" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1733">
-        <v>1776</v>
+        <v>1777</v>
       </c>
       <c r="B1733" t="s">
-        <v>4056</v>
+        <v>4057</v>
       </c>
       <c r="C1733" t="s">
         <v>3875</v>
@@ -63813,15 +63836,15 @@
         <v>1353</v>
       </c>
       <c r="M1733" t="s">
-        <v>4557</v>
+        <v>4558</v>
       </c>
     </row>
     <row r="1734" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1734">
-        <v>1777</v>
+        <v>1778</v>
       </c>
       <c r="B1734" t="s">
-        <v>4057</v>
+        <v>4058</v>
       </c>
       <c r="C1734" t="s">
         <v>3875</v>
@@ -63836,15 +63859,15 @@
         <v>1353</v>
       </c>
       <c r="M1734" t="s">
-        <v>4558</v>
+        <v>4059</v>
       </c>
     </row>
     <row r="1735" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1735">
-        <v>1778</v>
+        <v>1779</v>
       </c>
       <c r="B1735" t="s">
-        <v>4058</v>
+        <v>4060</v>
       </c>
       <c r="C1735" t="s">
         <v>3875</v>
@@ -63859,15 +63882,15 @@
         <v>1353</v>
       </c>
       <c r="M1735" t="s">
-        <v>4059</v>
+        <v>4559</v>
       </c>
     </row>
     <row r="1736" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1736">
-        <v>1779</v>
+        <v>1780</v>
       </c>
       <c r="B1736" t="s">
-        <v>4060</v>
+        <v>4061</v>
       </c>
       <c r="C1736" t="s">
         <v>3875</v>
@@ -63882,34 +63905,11 @@
         <v>1353</v>
       </c>
       <c r="M1736" t="s">
-        <v>4559</v>
-      </c>
-    </row>
-    <row r="1737" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1737">
-        <v>1780</v>
-      </c>
-      <c r="B1737" t="s">
-        <v>4061</v>
-      </c>
-      <c r="C1737" t="s">
-        <v>3875</v>
-      </c>
-      <c r="D1737">
-        <v>68000</v>
-      </c>
-      <c r="E1737" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1737" t="s">
-        <v>1353</v>
-      </c>
-      <c r="M1737" t="s">
         <v>4062</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M1737"/>
+  <autoFilter ref="A1:M1736"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
036 : airbustr driver
</commit_message>
<xml_diff>
--- a/0.36/compatibility.xlsx
+++ b/0.36/compatibility.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Playable (untested)" sheetId="4" r:id="rId1"/>
@@ -17,8 +17,8 @@
     <sheet name="GAME_NOT_WORKING FLAG" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ALL!$A$1:$M$1686</definedName>
-    <definedName name="LIST" localSheetId="1">ALL!$B$1:$M$1686</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ALL!$A$1:$M$1685</definedName>
+    <definedName name="LIST" localSheetId="1">ALL!$B$1:$M$1685</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12448" uniqueCount="4567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12449" uniqueCount="4567">
   <si>
     <t>romname</t>
   </si>
@@ -14081,10 +14081,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P356"/>
+  <dimension ref="A1:P357"/>
   <sheetViews>
-    <sheetView topLeftCell="A340" workbookViewId="0">
-      <selection activeCell="A357" sqref="A357"/>
+    <sheetView tabSelected="1" topLeftCell="A334" workbookViewId="0">
+      <selection activeCell="N357" sqref="N357"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22180,7 +22180,7 @@
         <v>2447</v>
       </c>
     </row>
-    <row r="353" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A353">
         <v>353</v>
       </c>
@@ -22206,7 +22206,7 @@
         <v>2449</v>
       </c>
     </row>
-    <row r="354" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A354">
         <v>354</v>
       </c>
@@ -22232,7 +22232,7 @@
         <v>2451</v>
       </c>
     </row>
-    <row r="355" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A355">
         <v>355</v>
       </c>
@@ -22258,7 +22258,7 @@
         <v>2453</v>
       </c>
     </row>
-    <row r="356" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A356">
         <v>356</v>
       </c>
@@ -22282,6 +22282,38 @@
       </c>
       <c r="M356" t="s">
         <v>2455</v>
+      </c>
+    </row>
+    <row r="357" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A357">
+        <v>357</v>
+      </c>
+      <c r="B357" t="s">
+        <v>3754</v>
+      </c>
+      <c r="C357" t="s">
+        <v>3755</v>
+      </c>
+      <c r="D357" t="s">
+        <v>14</v>
+      </c>
+      <c r="E357" t="s">
+        <v>14</v>
+      </c>
+      <c r="F357" t="s">
+        <v>14</v>
+      </c>
+      <c r="H357" t="s">
+        <v>336</v>
+      </c>
+      <c r="I357" t="s">
+        <v>1492</v>
+      </c>
+      <c r="M357" t="s">
+        <v>3756</v>
+      </c>
+      <c r="N357" t="s">
+        <v>4566</v>
       </c>
     </row>
   </sheetData>
@@ -22292,10 +22324,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1686"/>
+  <dimension ref="A1:M1685"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1406" workbookViewId="0">
-      <selection activeCell="F980" sqref="F980"/>
+    <sheetView topLeftCell="A1513" workbookViewId="0">
+      <selection activeCell="A1528" sqref="A1528:XFD1528"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -60300,39 +60332,33 @@
     </row>
     <row r="1528" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1528">
-        <v>1611</v>
+        <v>1612</v>
       </c>
       <c r="B1528" t="s">
-        <v>3754</v>
+        <v>3757</v>
       </c>
       <c r="C1528" t="s">
-        <v>3755</v>
+        <v>3758</v>
       </c>
       <c r="D1528" t="s">
         <v>14</v>
       </c>
       <c r="E1528" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1528" t="s">
-        <v>14</v>
+        <v>725</v>
       </c>
       <c r="H1528" t="s">
-        <v>336</v>
-      </c>
-      <c r="I1528" t="s">
-        <v>1492</v>
+        <v>166</v>
       </c>
       <c r="M1528" t="s">
-        <v>3756</v>
+        <v>4490</v>
       </c>
     </row>
     <row r="1529" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1529">
-        <v>1612</v>
+        <v>1613</v>
       </c>
       <c r="B1529" t="s">
-        <v>3757</v>
+        <v>3759</v>
       </c>
       <c r="C1529" t="s">
         <v>3758</v>
@@ -60347,15 +60373,15 @@
         <v>166</v>
       </c>
       <c r="M1529" t="s">
-        <v>4490</v>
+        <v>3760</v>
       </c>
     </row>
     <row r="1530" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1530">
-        <v>1613</v>
+        <v>1614</v>
       </c>
       <c r="B1530" t="s">
-        <v>3759</v>
+        <v>3761</v>
       </c>
       <c r="C1530" t="s">
         <v>3758</v>
@@ -60370,15 +60396,15 @@
         <v>166</v>
       </c>
       <c r="M1530" t="s">
-        <v>3760</v>
+        <v>3762</v>
       </c>
     </row>
     <row r="1531" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1531">
-        <v>1614</v>
+        <v>1615</v>
       </c>
       <c r="B1531" t="s">
-        <v>3761</v>
+        <v>3763</v>
       </c>
       <c r="C1531" t="s">
         <v>3758</v>
@@ -60393,15 +60419,15 @@
         <v>166</v>
       </c>
       <c r="M1531" t="s">
-        <v>3762</v>
+        <v>3764</v>
       </c>
     </row>
     <row r="1532" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1532">
-        <v>1615</v>
+        <v>1616</v>
       </c>
       <c r="B1532" t="s">
-        <v>3763</v>
+        <v>3765</v>
       </c>
       <c r="C1532" t="s">
         <v>3758</v>
@@ -60416,61 +60442,58 @@
         <v>166</v>
       </c>
       <c r="M1532" t="s">
-        <v>3764</v>
+        <v>3766</v>
       </c>
     </row>
     <row r="1533" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1533">
-        <v>1616</v>
+        <v>1617</v>
       </c>
       <c r="B1533" t="s">
-        <v>3765</v>
+        <v>3774</v>
       </c>
       <c r="C1533" t="s">
-        <v>3758</v>
+        <v>3775</v>
       </c>
       <c r="D1533" t="s">
         <v>14</v>
       </c>
       <c r="E1533" t="s">
-        <v>725</v>
+        <v>154</v>
       </c>
       <c r="H1533" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="M1533" t="s">
-        <v>3766</v>
+        <v>3776</v>
       </c>
     </row>
     <row r="1534" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1534">
-        <v>1617</v>
+        <v>1618</v>
       </c>
       <c r="B1534" t="s">
-        <v>3774</v>
+        <v>3777</v>
       </c>
       <c r="C1534" t="s">
-        <v>3775</v>
+        <v>3778</v>
       </c>
       <c r="D1534" t="s">
         <v>14</v>
-      </c>
-      <c r="E1534" t="s">
-        <v>154</v>
       </c>
       <c r="H1534" t="s">
         <v>172</v>
       </c>
       <c r="M1534" t="s">
-        <v>3776</v>
+        <v>3779</v>
       </c>
     </row>
     <row r="1535" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1535">
-        <v>1618</v>
+        <v>1619</v>
       </c>
       <c r="B1535" t="s">
-        <v>3777</v>
+        <v>3780</v>
       </c>
       <c r="C1535" t="s">
         <v>3778</v>
@@ -60482,35 +60505,38 @@
         <v>172</v>
       </c>
       <c r="M1535" t="s">
-        <v>3779</v>
+        <v>3781</v>
       </c>
     </row>
     <row r="1536" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1536">
-        <v>1619</v>
+        <v>1624</v>
       </c>
       <c r="B1536" t="s">
-        <v>3780</v>
+        <v>3791</v>
       </c>
       <c r="C1536" t="s">
-        <v>3778</v>
+        <v>3792</v>
       </c>
       <c r="D1536" t="s">
-        <v>14</v>
+        <v>405</v>
+      </c>
+      <c r="E1536" t="s">
+        <v>1184</v>
       </c>
       <c r="H1536" t="s">
-        <v>172</v>
+        <v>71</v>
       </c>
       <c r="M1536" t="s">
-        <v>3781</v>
+        <v>3793</v>
       </c>
     </row>
     <row r="1537" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1537">
-        <v>1624</v>
+        <v>1625</v>
       </c>
       <c r="B1537" t="s">
-        <v>3791</v>
+        <v>3794</v>
       </c>
       <c r="C1537" t="s">
         <v>3792</v>
@@ -60525,18 +60551,18 @@
         <v>71</v>
       </c>
       <c r="M1537" t="s">
-        <v>3793</v>
+        <v>3795</v>
       </c>
     </row>
     <row r="1538" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1538">
-        <v>1625</v>
+        <v>1626</v>
       </c>
       <c r="B1538" t="s">
-        <v>3794</v>
+        <v>3799</v>
       </c>
       <c r="C1538" t="s">
-        <v>3792</v>
+        <v>3800</v>
       </c>
       <c r="D1538" t="s">
         <v>405</v>
@@ -60544,65 +60570,59 @@
       <c r="E1538" t="s">
         <v>1184</v>
       </c>
+      <c r="F1538" t="s">
+        <v>3801</v>
+      </c>
       <c r="H1538" t="s">
         <v>71</v>
       </c>
       <c r="M1538" t="s">
-        <v>3795</v>
+        <v>3802</v>
       </c>
     </row>
     <row r="1539" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1539">
-        <v>1626</v>
+        <v>1627</v>
       </c>
       <c r="B1539" t="s">
-        <v>3799</v>
+        <v>3803</v>
       </c>
       <c r="C1539" t="s">
-        <v>3800</v>
+        <v>3804</v>
       </c>
       <c r="D1539" t="s">
-        <v>405</v>
-      </c>
-      <c r="E1539" t="s">
-        <v>1184</v>
-      </c>
-      <c r="F1539" t="s">
-        <v>3801</v>
+        <v>473</v>
       </c>
       <c r="H1539" t="s">
-        <v>71</v>
+        <v>2936</v>
       </c>
       <c r="M1539" t="s">
-        <v>3802</v>
+        <v>3805</v>
       </c>
     </row>
     <row r="1540" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1540">
-        <v>1627</v>
+        <v>1628</v>
       </c>
       <c r="B1540" t="s">
-        <v>3803</v>
+        <v>3806</v>
       </c>
       <c r="C1540" t="s">
-        <v>3804</v>
+        <v>3807</v>
       </c>
       <c r="D1540" t="s">
         <v>473</v>
       </c>
-      <c r="H1540" t="s">
-        <v>2936</v>
-      </c>
       <c r="M1540" t="s">
-        <v>3805</v>
+        <v>3808</v>
       </c>
     </row>
     <row r="1541" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1541">
-        <v>1628</v>
+        <v>1629</v>
       </c>
       <c r="B1541" t="s">
-        <v>3806</v>
+        <v>3809</v>
       </c>
       <c r="C1541" t="s">
         <v>3807</v>
@@ -60611,101 +60631,116 @@
         <v>473</v>
       </c>
       <c r="M1541" t="s">
-        <v>3808</v>
+        <v>3810</v>
       </c>
     </row>
     <row r="1542" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1542">
-        <v>1629</v>
+        <v>1630</v>
       </c>
       <c r="B1542" t="s">
-        <v>3809</v>
+        <v>3811</v>
       </c>
       <c r="C1542" t="s">
-        <v>3807</v>
-      </c>
-      <c r="D1542" t="s">
-        <v>473</v>
+        <v>3812</v>
+      </c>
+      <c r="D1542">
+        <v>8080</v>
       </c>
       <c r="M1542" t="s">
-        <v>3810</v>
+        <v>3813</v>
       </c>
     </row>
     <row r="1543" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1543">
-        <v>1630</v>
+        <v>1631</v>
       </c>
       <c r="B1543" t="s">
-        <v>3811</v>
+        <v>3814</v>
       </c>
       <c r="C1543" t="s">
-        <v>3812</v>
-      </c>
-      <c r="D1543">
-        <v>8080</v>
+        <v>3815</v>
+      </c>
+      <c r="D1543" t="s">
+        <v>3436</v>
+      </c>
+      <c r="E1543" t="s">
+        <v>3436</v>
+      </c>
+      <c r="F1543" t="s">
+        <v>1184</v>
+      </c>
+      <c r="G1543" t="s">
+        <v>1184</v>
+      </c>
+      <c r="H1543" t="s">
+        <v>333</v>
+      </c>
+      <c r="I1543" t="s">
+        <v>551</v>
       </c>
       <c r="M1543" t="s">
-        <v>3813</v>
+        <v>3816</v>
       </c>
     </row>
     <row r="1544" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1544">
-        <v>1631</v>
+        <v>1632</v>
       </c>
       <c r="B1544" t="s">
-        <v>3814</v>
+        <v>3817</v>
       </c>
       <c r="C1544" t="s">
-        <v>3815</v>
+        <v>3818</v>
       </c>
       <c r="D1544" t="s">
-        <v>3436</v>
-      </c>
-      <c r="E1544" t="s">
-        <v>3436</v>
-      </c>
-      <c r="F1544" t="s">
-        <v>1184</v>
-      </c>
-      <c r="G1544" t="s">
-        <v>1184</v>
+        <v>14</v>
       </c>
       <c r="H1544" t="s">
-        <v>333</v>
-      </c>
-      <c r="I1544" t="s">
-        <v>551</v>
+        <v>172</v>
       </c>
       <c r="M1544" t="s">
-        <v>3816</v>
+        <v>3819</v>
       </c>
     </row>
     <row r="1545" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1545">
-        <v>1632</v>
+        <v>1633</v>
       </c>
       <c r="B1545" t="s">
-        <v>3817</v>
+        <v>3820</v>
       </c>
       <c r="C1545" t="s">
-        <v>3818</v>
+        <v>3821</v>
       </c>
       <c r="D1545" t="s">
         <v>14</v>
       </c>
+      <c r="E1545" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1545" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1545" t="s">
+        <v>154</v>
+      </c>
       <c r="H1545" t="s">
-        <v>172</v>
+        <v>71</v>
+      </c>
+      <c r="I1545" t="s">
+        <v>166</v>
       </c>
       <c r="M1545" t="s">
-        <v>3819</v>
+        <v>3822</v>
       </c>
     </row>
     <row r="1546" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1546">
-        <v>1633</v>
+        <v>1634</v>
       </c>
       <c r="B1546" t="s">
-        <v>3820</v>
+        <v>3823</v>
       </c>
       <c r="C1546" t="s">
         <v>3821</v>
@@ -60729,15 +60764,15 @@
         <v>166</v>
       </c>
       <c r="M1546" t="s">
-        <v>3822</v>
+        <v>3824</v>
       </c>
     </row>
     <row r="1547" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1547">
-        <v>1634</v>
+        <v>1635</v>
       </c>
       <c r="B1547" t="s">
-        <v>3823</v>
+        <v>3825</v>
       </c>
       <c r="C1547" t="s">
         <v>3821</v>
@@ -60761,15 +60796,15 @@
         <v>166</v>
       </c>
       <c r="M1547" t="s">
-        <v>3824</v>
+        <v>3826</v>
       </c>
     </row>
     <row r="1548" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1548">
-        <v>1635</v>
+        <v>1636</v>
       </c>
       <c r="B1548" t="s">
-        <v>3825</v>
+        <v>3827</v>
       </c>
       <c r="C1548" t="s">
         <v>3821</v>
@@ -60793,110 +60828,101 @@
         <v>166</v>
       </c>
       <c r="M1548" t="s">
-        <v>3826</v>
+        <v>3828</v>
       </c>
     </row>
     <row r="1549" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1549">
-        <v>1636</v>
+        <v>1637</v>
       </c>
       <c r="B1549" t="s">
-        <v>3827</v>
+        <v>3829</v>
       </c>
       <c r="C1549" t="s">
-        <v>3821</v>
-      </c>
-      <c r="D1549" t="s">
-        <v>14</v>
+        <v>3830</v>
+      </c>
+      <c r="D1549">
+        <v>68000</v>
       </c>
       <c r="E1549" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1549" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1549" t="s">
         <v>154</v>
       </c>
       <c r="H1549" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1549" t="s">
-        <v>166</v>
+        <v>1492</v>
       </c>
       <c r="M1549" t="s">
-        <v>3828</v>
+        <v>3831</v>
       </c>
     </row>
     <row r="1550" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1550">
-        <v>1637</v>
+        <v>1645</v>
       </c>
       <c r="B1550" t="s">
-        <v>3829</v>
+        <v>3848</v>
       </c>
       <c r="C1550" t="s">
-        <v>3830</v>
+        <v>3849</v>
       </c>
       <c r="D1550">
-        <v>68000</v>
-      </c>
-      <c r="E1550" t="s">
-        <v>154</v>
+        <v>8080</v>
       </c>
       <c r="H1550" t="s">
-        <v>1492</v>
+        <v>406</v>
       </c>
       <c r="M1550" t="s">
-        <v>3831</v>
+        <v>3850</v>
       </c>
     </row>
     <row r="1551" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1551">
-        <v>1645</v>
+        <v>1646</v>
       </c>
       <c r="B1551" t="s">
-        <v>3848</v>
+        <v>3851</v>
       </c>
       <c r="C1551" t="s">
-        <v>3849</v>
-      </c>
-      <c r="D1551">
-        <v>8080</v>
+        <v>3852</v>
+      </c>
+      <c r="D1551" t="s">
+        <v>1105</v>
       </c>
       <c r="H1551" t="s">
-        <v>406</v>
+        <v>336</v>
       </c>
       <c r="M1551" t="s">
-        <v>3850</v>
+        <v>3853</v>
       </c>
     </row>
     <row r="1552" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1552">
-        <v>1646</v>
+        <v>1647</v>
       </c>
       <c r="B1552" t="s">
-        <v>3851</v>
+        <v>3854</v>
       </c>
       <c r="C1552" t="s">
-        <v>3852</v>
+        <v>3855</v>
       </c>
       <c r="D1552" t="s">
-        <v>1105</v>
+        <v>14</v>
+      </c>
+      <c r="E1552" t="s">
+        <v>154</v>
       </c>
       <c r="H1552" t="s">
         <v>336</v>
       </c>
       <c r="M1552" t="s">
-        <v>3853</v>
+        <v>3856</v>
       </c>
     </row>
     <row r="1553" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1553">
-        <v>1647</v>
+        <v>1648</v>
       </c>
       <c r="B1553" t="s">
-        <v>3854</v>
+        <v>3857</v>
       </c>
       <c r="C1553" t="s">
         <v>3855</v>
@@ -60911,141 +60937,141 @@
         <v>336</v>
       </c>
       <c r="M1553" t="s">
-        <v>3856</v>
+        <v>3858</v>
       </c>
     </row>
     <row r="1554" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1554">
-        <v>1648</v>
+        <v>1649</v>
       </c>
       <c r="B1554" t="s">
-        <v>3857</v>
+        <v>3859</v>
       </c>
       <c r="C1554" t="s">
-        <v>3855</v>
+        <v>3860</v>
       </c>
       <c r="D1554" t="s">
-        <v>14</v>
+        <v>3861</v>
       </c>
       <c r="E1554" t="s">
-        <v>154</v>
+        <v>725</v>
       </c>
       <c r="H1554" t="s">
-        <v>336</v>
+        <v>2070</v>
       </c>
       <c r="M1554" t="s">
-        <v>3858</v>
+        <v>3862</v>
       </c>
     </row>
     <row r="1555" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1555">
-        <v>1649</v>
+        <v>1650</v>
       </c>
       <c r="B1555" t="s">
-        <v>3859</v>
+        <v>3863</v>
       </c>
       <c r="C1555" t="s">
-        <v>3860</v>
-      </c>
-      <c r="D1555" t="s">
-        <v>3861</v>
-      </c>
-      <c r="E1555" t="s">
-        <v>725</v>
+        <v>3864</v>
+      </c>
+      <c r="D1555">
+        <v>68000</v>
       </c>
       <c r="H1555" t="s">
-        <v>2070</v>
+        <v>2375</v>
       </c>
       <c r="M1555" t="s">
-        <v>3862</v>
+        <v>3865</v>
       </c>
     </row>
     <row r="1556" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1556">
-        <v>1650</v>
+        <v>1651</v>
       </c>
       <c r="B1556" t="s">
-        <v>3863</v>
+        <v>3866</v>
       </c>
       <c r="C1556" t="s">
-        <v>3864</v>
+        <v>3867</v>
       </c>
       <c r="D1556">
         <v>68000</v>
       </c>
+      <c r="E1556" t="s">
+        <v>154</v>
+      </c>
       <c r="H1556" t="s">
-        <v>2375</v>
+        <v>1236</v>
       </c>
       <c r="M1556" t="s">
-        <v>3865</v>
+        <v>3868</v>
       </c>
     </row>
     <row r="1557" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1557">
-        <v>1651</v>
+        <v>1652</v>
       </c>
       <c r="B1557" t="s">
-        <v>3866</v>
+        <v>3869</v>
       </c>
       <c r="C1557" t="s">
-        <v>3867</v>
-      </c>
-      <c r="D1557">
-        <v>68000</v>
-      </c>
-      <c r="E1557" t="s">
-        <v>154</v>
+        <v>3870</v>
+      </c>
+      <c r="D1557" t="s">
+        <v>405</v>
       </c>
       <c r="H1557" t="s">
-        <v>1236</v>
+        <v>71</v>
       </c>
       <c r="M1557" t="s">
-        <v>3868</v>
+        <v>3871</v>
       </c>
     </row>
     <row r="1558" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1558">
-        <v>1652</v>
+        <v>1653</v>
       </c>
       <c r="B1558" t="s">
-        <v>3869</v>
+        <v>3872</v>
       </c>
       <c r="C1558" t="s">
-        <v>3870</v>
+        <v>3873</v>
       </c>
       <c r="D1558" t="s">
-        <v>405</v>
-      </c>
-      <c r="H1558" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="M1558" t="s">
-        <v>3871</v>
+        <v>4493</v>
       </c>
     </row>
     <row r="1559" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1559">
-        <v>1653</v>
+        <v>1654</v>
       </c>
       <c r="B1559" t="s">
-        <v>3872</v>
+        <v>3874</v>
       </c>
       <c r="C1559" t="s">
-        <v>3873</v>
-      </c>
-      <c r="D1559" t="s">
-        <v>14</v>
+        <v>3875</v>
+      </c>
+      <c r="D1559">
+        <v>68000</v>
+      </c>
+      <c r="E1559" t="s">
+        <v>154</v>
+      </c>
+      <c r="H1559" t="s">
+        <v>1353</v>
       </c>
       <c r="M1559" t="s">
-        <v>4493</v>
+        <v>3876</v>
       </c>
     </row>
     <row r="1560" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1560">
-        <v>1654</v>
+        <v>1655</v>
       </c>
       <c r="B1560" t="s">
-        <v>3874</v>
+        <v>3877</v>
       </c>
       <c r="C1560" t="s">
         <v>3875</v>
@@ -61060,15 +61086,15 @@
         <v>1353</v>
       </c>
       <c r="M1560" t="s">
-        <v>3876</v>
+        <v>4494</v>
       </c>
     </row>
     <row r="1561" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1561">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="B1561" t="s">
-        <v>3877</v>
+        <v>3878</v>
       </c>
       <c r="C1561" t="s">
         <v>3875</v>
@@ -61083,15 +61109,15 @@
         <v>1353</v>
       </c>
       <c r="M1561" t="s">
-        <v>4494</v>
+        <v>3879</v>
       </c>
     </row>
     <row r="1562" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1562">
-        <v>1656</v>
+        <v>1657</v>
       </c>
       <c r="B1562" t="s">
-        <v>3878</v>
+        <v>3880</v>
       </c>
       <c r="C1562" t="s">
         <v>3875</v>
@@ -61106,15 +61132,15 @@
         <v>1353</v>
       </c>
       <c r="M1562" t="s">
-        <v>3879</v>
+        <v>3881</v>
       </c>
     </row>
     <row r="1563" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1563">
-        <v>1657</v>
+        <v>1658</v>
       </c>
       <c r="B1563" t="s">
-        <v>3880</v>
+        <v>3882</v>
       </c>
       <c r="C1563" t="s">
         <v>3875</v>
@@ -61129,15 +61155,15 @@
         <v>1353</v>
       </c>
       <c r="M1563" t="s">
-        <v>3881</v>
+        <v>3883</v>
       </c>
     </row>
     <row r="1564" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1564">
-        <v>1658</v>
+        <v>1659</v>
       </c>
       <c r="B1564" t="s">
-        <v>3882</v>
+        <v>3884</v>
       </c>
       <c r="C1564" t="s">
         <v>3875</v>
@@ -61152,15 +61178,15 @@
         <v>1353</v>
       </c>
       <c r="M1564" t="s">
-        <v>3883</v>
+        <v>3885</v>
       </c>
     </row>
     <row r="1565" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1565">
-        <v>1659</v>
+        <v>1660</v>
       </c>
       <c r="B1565" t="s">
-        <v>3884</v>
+        <v>3886</v>
       </c>
       <c r="C1565" t="s">
         <v>3875</v>
@@ -61175,15 +61201,15 @@
         <v>1353</v>
       </c>
       <c r="M1565" t="s">
-        <v>3885</v>
+        <v>3887</v>
       </c>
     </row>
     <row r="1566" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1566">
-        <v>1660</v>
+        <v>1661</v>
       </c>
       <c r="B1566" t="s">
-        <v>3886</v>
+        <v>3888</v>
       </c>
       <c r="C1566" t="s">
         <v>3875</v>
@@ -61198,15 +61224,15 @@
         <v>1353</v>
       </c>
       <c r="M1566" t="s">
-        <v>3887</v>
+        <v>4495</v>
       </c>
     </row>
     <row r="1567" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1567">
-        <v>1661</v>
+        <v>1662</v>
       </c>
       <c r="B1567" t="s">
-        <v>3888</v>
+        <v>3889</v>
       </c>
       <c r="C1567" t="s">
         <v>3875</v>
@@ -61221,15 +61247,15 @@
         <v>1353</v>
       </c>
       <c r="M1567" t="s">
-        <v>4495</v>
+        <v>3890</v>
       </c>
     </row>
     <row r="1568" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1568">
-        <v>1662</v>
+        <v>1663</v>
       </c>
       <c r="B1568" t="s">
-        <v>3889</v>
+        <v>3891</v>
       </c>
       <c r="C1568" t="s">
         <v>3875</v>
@@ -61244,15 +61270,15 @@
         <v>1353</v>
       </c>
       <c r="M1568" t="s">
-        <v>3890</v>
+        <v>3892</v>
       </c>
     </row>
     <row r="1569" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1569">
-        <v>1663</v>
+        <v>1664</v>
       </c>
       <c r="B1569" t="s">
-        <v>3891</v>
+        <v>3893</v>
       </c>
       <c r="C1569" t="s">
         <v>3875</v>
@@ -61267,15 +61293,15 @@
         <v>1353</v>
       </c>
       <c r="M1569" t="s">
-        <v>3892</v>
+        <v>3894</v>
       </c>
     </row>
     <row r="1570" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1570">
-        <v>1664</v>
+        <v>1665</v>
       </c>
       <c r="B1570" t="s">
-        <v>3893</v>
+        <v>3895</v>
       </c>
       <c r="C1570" t="s">
         <v>3875</v>
@@ -61290,15 +61316,15 @@
         <v>1353</v>
       </c>
       <c r="M1570" t="s">
-        <v>3894</v>
+        <v>3896</v>
       </c>
     </row>
     <row r="1571" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1571">
-        <v>1665</v>
+        <v>1666</v>
       </c>
       <c r="B1571" t="s">
-        <v>3895</v>
+        <v>3897</v>
       </c>
       <c r="C1571" t="s">
         <v>3875</v>
@@ -61313,15 +61339,15 @@
         <v>1353</v>
       </c>
       <c r="M1571" t="s">
-        <v>3896</v>
+        <v>3898</v>
       </c>
     </row>
     <row r="1572" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1572">
-        <v>1666</v>
+        <v>1667</v>
       </c>
       <c r="B1572" t="s">
-        <v>3897</v>
+        <v>3899</v>
       </c>
       <c r="C1572" t="s">
         <v>3875</v>
@@ -61336,15 +61362,15 @@
         <v>1353</v>
       </c>
       <c r="M1572" t="s">
-        <v>3898</v>
+        <v>4496</v>
       </c>
     </row>
     <row r="1573" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1573">
-        <v>1667</v>
+        <v>1668</v>
       </c>
       <c r="B1573" t="s">
-        <v>3899</v>
+        <v>3900</v>
       </c>
       <c r="C1573" t="s">
         <v>3875</v>
@@ -61359,15 +61385,15 @@
         <v>1353</v>
       </c>
       <c r="M1573" t="s">
-        <v>4496</v>
+        <v>4497</v>
       </c>
     </row>
     <row r="1574" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1574">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="B1574" t="s">
-        <v>3900</v>
+        <v>3901</v>
       </c>
       <c r="C1574" t="s">
         <v>3875</v>
@@ -61382,15 +61408,15 @@
         <v>1353</v>
       </c>
       <c r="M1574" t="s">
-        <v>4497</v>
+        <v>3902</v>
       </c>
     </row>
     <row r="1575" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1575">
-        <v>1669</v>
+        <v>1670</v>
       </c>
       <c r="B1575" t="s">
-        <v>3901</v>
+        <v>3903</v>
       </c>
       <c r="C1575" t="s">
         <v>3875</v>
@@ -61405,15 +61431,15 @@
         <v>1353</v>
       </c>
       <c r="M1575" t="s">
-        <v>3902</v>
+        <v>3904</v>
       </c>
     </row>
     <row r="1576" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1576">
-        <v>1670</v>
+        <v>1671</v>
       </c>
       <c r="B1576" t="s">
-        <v>3903</v>
+        <v>3905</v>
       </c>
       <c r="C1576" t="s">
         <v>3875</v>
@@ -61428,15 +61454,15 @@
         <v>1353</v>
       </c>
       <c r="M1576" t="s">
-        <v>3904</v>
+        <v>3906</v>
       </c>
     </row>
     <row r="1577" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1577">
-        <v>1671</v>
+        <v>1672</v>
       </c>
       <c r="B1577" t="s">
-        <v>3905</v>
+        <v>3907</v>
       </c>
       <c r="C1577" t="s">
         <v>3875</v>
@@ -61451,15 +61477,15 @@
         <v>1353</v>
       </c>
       <c r="M1577" t="s">
-        <v>3906</v>
+        <v>3908</v>
       </c>
     </row>
     <row r="1578" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1578">
-        <v>1672</v>
+        <v>1673</v>
       </c>
       <c r="B1578" t="s">
-        <v>3907</v>
+        <v>3909</v>
       </c>
       <c r="C1578" t="s">
         <v>3875</v>
@@ -61474,15 +61500,15 @@
         <v>1353</v>
       </c>
       <c r="M1578" t="s">
-        <v>3908</v>
+        <v>3910</v>
       </c>
     </row>
     <row r="1579" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1579">
-        <v>1673</v>
+        <v>1674</v>
       </c>
       <c r="B1579" t="s">
-        <v>3909</v>
+        <v>3911</v>
       </c>
       <c r="C1579" t="s">
         <v>3875</v>
@@ -61497,15 +61523,15 @@
         <v>1353</v>
       </c>
       <c r="M1579" t="s">
-        <v>3910</v>
+        <v>3912</v>
       </c>
     </row>
     <row r="1580" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1580">
-        <v>1674</v>
+        <v>1675</v>
       </c>
       <c r="B1580" t="s">
-        <v>3911</v>
+        <v>3913</v>
       </c>
       <c r="C1580" t="s">
         <v>3875</v>
@@ -61520,15 +61546,15 @@
         <v>1353</v>
       </c>
       <c r="M1580" t="s">
-        <v>3912</v>
+        <v>4498</v>
       </c>
     </row>
     <row r="1581" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1581">
-        <v>1675</v>
+        <v>1676</v>
       </c>
       <c r="B1581" t="s">
-        <v>3913</v>
+        <v>3914</v>
       </c>
       <c r="C1581" t="s">
         <v>3875</v>
@@ -61543,15 +61569,15 @@
         <v>1353</v>
       </c>
       <c r="M1581" t="s">
-        <v>4498</v>
+        <v>3915</v>
       </c>
     </row>
     <row r="1582" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1582">
-        <v>1676</v>
+        <v>1677</v>
       </c>
       <c r="B1582" t="s">
-        <v>3914</v>
+        <v>3916</v>
       </c>
       <c r="C1582" t="s">
         <v>3875</v>
@@ -61566,15 +61592,15 @@
         <v>1353</v>
       </c>
       <c r="M1582" t="s">
-        <v>3915</v>
+        <v>3917</v>
       </c>
     </row>
     <row r="1583" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1583">
-        <v>1677</v>
+        <v>1678</v>
       </c>
       <c r="B1583" t="s">
-        <v>3916</v>
+        <v>3918</v>
       </c>
       <c r="C1583" t="s">
         <v>3875</v>
@@ -61589,15 +61615,15 @@
         <v>1353</v>
       </c>
       <c r="M1583" t="s">
-        <v>3917</v>
+        <v>3919</v>
       </c>
     </row>
     <row r="1584" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1584">
-        <v>1678</v>
+        <v>1679</v>
       </c>
       <c r="B1584" t="s">
-        <v>3918</v>
+        <v>3920</v>
       </c>
       <c r="C1584" t="s">
         <v>3875</v>
@@ -61612,15 +61638,15 @@
         <v>1353</v>
       </c>
       <c r="M1584" t="s">
-        <v>3919</v>
+        <v>4499</v>
       </c>
     </row>
     <row r="1585" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1585">
-        <v>1679</v>
+        <v>1680</v>
       </c>
       <c r="B1585" t="s">
-        <v>3920</v>
+        <v>3921</v>
       </c>
       <c r="C1585" t="s">
         <v>3875</v>
@@ -61635,15 +61661,15 @@
         <v>1353</v>
       </c>
       <c r="M1585" t="s">
-        <v>4499</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="1586" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1586">
-        <v>1680</v>
+        <v>1681</v>
       </c>
       <c r="B1586" t="s">
-        <v>3921</v>
+        <v>3922</v>
       </c>
       <c r="C1586" t="s">
         <v>3875</v>
@@ -61658,15 +61684,15 @@
         <v>1353</v>
       </c>
       <c r="M1586" t="s">
-        <v>4500</v>
+        <v>4501</v>
       </c>
     </row>
     <row r="1587" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1587">
-        <v>1681</v>
+        <v>1682</v>
       </c>
       <c r="B1587" t="s">
-        <v>3922</v>
+        <v>3923</v>
       </c>
       <c r="C1587" t="s">
         <v>3875</v>
@@ -61681,15 +61707,15 @@
         <v>1353</v>
       </c>
       <c r="M1587" t="s">
-        <v>4501</v>
+        <v>3924</v>
       </c>
     </row>
     <row r="1588" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1588">
-        <v>1682</v>
+        <v>1683</v>
       </c>
       <c r="B1588" t="s">
-        <v>3923</v>
+        <v>3925</v>
       </c>
       <c r="C1588" t="s">
         <v>3875</v>
@@ -61704,15 +61730,15 @@
         <v>1353</v>
       </c>
       <c r="M1588" t="s">
-        <v>3924</v>
+        <v>3926</v>
       </c>
     </row>
     <row r="1589" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1589">
-        <v>1683</v>
+        <v>1684</v>
       </c>
       <c r="B1589" t="s">
-        <v>3925</v>
+        <v>3927</v>
       </c>
       <c r="C1589" t="s">
         <v>3875</v>
@@ -61727,15 +61753,15 @@
         <v>1353</v>
       </c>
       <c r="M1589" t="s">
-        <v>3926</v>
+        <v>4502</v>
       </c>
     </row>
     <row r="1590" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1590">
-        <v>1684</v>
+        <v>1685</v>
       </c>
       <c r="B1590" t="s">
-        <v>3927</v>
+        <v>3928</v>
       </c>
       <c r="C1590" t="s">
         <v>3875</v>
@@ -61750,15 +61776,15 @@
         <v>1353</v>
       </c>
       <c r="M1590" t="s">
-        <v>4502</v>
+        <v>3929</v>
       </c>
     </row>
     <row r="1591" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1591">
-        <v>1685</v>
+        <v>1686</v>
       </c>
       <c r="B1591" t="s">
-        <v>3928</v>
+        <v>3930</v>
       </c>
       <c r="C1591" t="s">
         <v>3875</v>
@@ -61773,15 +61799,15 @@
         <v>1353</v>
       </c>
       <c r="M1591" t="s">
-        <v>3929</v>
+        <v>4503</v>
       </c>
     </row>
     <row r="1592" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1592">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="B1592" t="s">
-        <v>3930</v>
+        <v>3931</v>
       </c>
       <c r="C1592" t="s">
         <v>3875</v>
@@ -61796,15 +61822,15 @@
         <v>1353</v>
       </c>
       <c r="M1592" t="s">
-        <v>4503</v>
+        <v>3932</v>
       </c>
     </row>
     <row r="1593" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1593">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="B1593" t="s">
-        <v>3931</v>
+        <v>3933</v>
       </c>
       <c r="C1593" t="s">
         <v>3875</v>
@@ -61819,15 +61845,15 @@
         <v>1353</v>
       </c>
       <c r="M1593" t="s">
-        <v>3932</v>
+        <v>3934</v>
       </c>
     </row>
     <row r="1594" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1594">
-        <v>1688</v>
+        <v>1689</v>
       </c>
       <c r="B1594" t="s">
-        <v>3933</v>
+        <v>3935</v>
       </c>
       <c r="C1594" t="s">
         <v>3875</v>
@@ -61842,15 +61868,15 @@
         <v>1353</v>
       </c>
       <c r="M1594" t="s">
-        <v>3934</v>
+        <v>4504</v>
       </c>
     </row>
     <row r="1595" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1595">
-        <v>1689</v>
+        <v>1690</v>
       </c>
       <c r="B1595" t="s">
-        <v>3935</v>
+        <v>3936</v>
       </c>
       <c r="C1595" t="s">
         <v>3875</v>
@@ -61865,15 +61891,15 @@
         <v>1353</v>
       </c>
       <c r="M1595" t="s">
-        <v>4504</v>
+        <v>4505</v>
       </c>
     </row>
     <row r="1596" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1596">
-        <v>1690</v>
+        <v>1691</v>
       </c>
       <c r="B1596" t="s">
-        <v>3936</v>
+        <v>3937</v>
       </c>
       <c r="C1596" t="s">
         <v>3875</v>
@@ -61888,15 +61914,15 @@
         <v>1353</v>
       </c>
       <c r="M1596" t="s">
-        <v>4505</v>
+        <v>3938</v>
       </c>
     </row>
     <row r="1597" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1597">
-        <v>1691</v>
+        <v>1692</v>
       </c>
       <c r="B1597" t="s">
-        <v>3937</v>
+        <v>3939</v>
       </c>
       <c r="C1597" t="s">
         <v>3875</v>
@@ -61911,15 +61937,15 @@
         <v>1353</v>
       </c>
       <c r="M1597" t="s">
-        <v>3938</v>
+        <v>4506</v>
       </c>
     </row>
     <row r="1598" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1598">
-        <v>1692</v>
+        <v>1693</v>
       </c>
       <c r="B1598" t="s">
-        <v>3939</v>
+        <v>3940</v>
       </c>
       <c r="C1598" t="s">
         <v>3875</v>
@@ -61934,15 +61960,15 @@
         <v>1353</v>
       </c>
       <c r="M1598" t="s">
-        <v>4506</v>
+        <v>4507</v>
       </c>
     </row>
     <row r="1599" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1599">
-        <v>1693</v>
+        <v>1694</v>
       </c>
       <c r="B1599" t="s">
-        <v>3940</v>
+        <v>3941</v>
       </c>
       <c r="C1599" t="s">
         <v>3875</v>
@@ -61957,15 +61983,15 @@
         <v>1353</v>
       </c>
       <c r="M1599" t="s">
-        <v>4507</v>
+        <v>4508</v>
       </c>
     </row>
     <row r="1600" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1600">
-        <v>1694</v>
+        <v>1695</v>
       </c>
       <c r="B1600" t="s">
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C1600" t="s">
         <v>3875</v>
@@ -61980,15 +62006,15 @@
         <v>1353</v>
       </c>
       <c r="M1600" t="s">
-        <v>4508</v>
+        <v>4509</v>
       </c>
     </row>
     <row r="1601" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1601">
-        <v>1695</v>
+        <v>1696</v>
       </c>
       <c r="B1601" t="s">
-        <v>3942</v>
+        <v>3943</v>
       </c>
       <c r="C1601" t="s">
         <v>3875</v>
@@ -62003,15 +62029,15 @@
         <v>1353</v>
       </c>
       <c r="M1601" t="s">
-        <v>4509</v>
+        <v>4510</v>
       </c>
     </row>
     <row r="1602" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1602">
-        <v>1696</v>
+        <v>1697</v>
       </c>
       <c r="B1602" t="s">
-        <v>3943</v>
+        <v>3944</v>
       </c>
       <c r="C1602" t="s">
         <v>3875</v>
@@ -62026,15 +62052,15 @@
         <v>1353</v>
       </c>
       <c r="M1602" t="s">
-        <v>4510</v>
+        <v>4511</v>
       </c>
     </row>
     <row r="1603" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1603">
-        <v>1697</v>
+        <v>1698</v>
       </c>
       <c r="B1603" t="s">
-        <v>3944</v>
+        <v>3945</v>
       </c>
       <c r="C1603" t="s">
         <v>3875</v>
@@ -62049,15 +62075,15 @@
         <v>1353</v>
       </c>
       <c r="M1603" t="s">
-        <v>4511</v>
+        <v>4512</v>
       </c>
     </row>
     <row r="1604" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1604">
-        <v>1698</v>
+        <v>1699</v>
       </c>
       <c r="B1604" t="s">
-        <v>3945</v>
+        <v>3946</v>
       </c>
       <c r="C1604" t="s">
         <v>3875</v>
@@ -62072,15 +62098,15 @@
         <v>1353</v>
       </c>
       <c r="M1604" t="s">
-        <v>4512</v>
+        <v>3947</v>
       </c>
     </row>
     <row r="1605" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1605">
-        <v>1699</v>
+        <v>1700</v>
       </c>
       <c r="B1605" t="s">
-        <v>3946</v>
+        <v>3948</v>
       </c>
       <c r="C1605" t="s">
         <v>3875</v>
@@ -62095,15 +62121,15 @@
         <v>1353</v>
       </c>
       <c r="M1605" t="s">
-        <v>3947</v>
+        <v>3949</v>
       </c>
     </row>
     <row r="1606" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1606">
-        <v>1700</v>
+        <v>1701</v>
       </c>
       <c r="B1606" t="s">
-        <v>3948</v>
+        <v>3950</v>
       </c>
       <c r="C1606" t="s">
         <v>3875</v>
@@ -62118,15 +62144,15 @@
         <v>1353</v>
       </c>
       <c r="M1606" t="s">
-        <v>3949</v>
+        <v>3951</v>
       </c>
     </row>
     <row r="1607" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1607">
-        <v>1701</v>
+        <v>1702</v>
       </c>
       <c r="B1607" t="s">
-        <v>3950</v>
+        <v>3952</v>
       </c>
       <c r="C1607" t="s">
         <v>3875</v>
@@ -62141,15 +62167,15 @@
         <v>1353</v>
       </c>
       <c r="M1607" t="s">
-        <v>3951</v>
+        <v>4513</v>
       </c>
     </row>
     <row r="1608" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1608">
-        <v>1702</v>
+        <v>1703</v>
       </c>
       <c r="B1608" t="s">
-        <v>3952</v>
+        <v>3953</v>
       </c>
       <c r="C1608" t="s">
         <v>3875</v>
@@ -62164,15 +62190,15 @@
         <v>1353</v>
       </c>
       <c r="M1608" t="s">
-        <v>4513</v>
+        <v>3954</v>
       </c>
     </row>
     <row r="1609" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1609">
-        <v>1703</v>
+        <v>1704</v>
       </c>
       <c r="B1609" t="s">
-        <v>3953</v>
+        <v>3955</v>
       </c>
       <c r="C1609" t="s">
         <v>3875</v>
@@ -62187,15 +62213,15 @@
         <v>1353</v>
       </c>
       <c r="M1609" t="s">
-        <v>3954</v>
+        <v>3956</v>
       </c>
     </row>
     <row r="1610" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1610">
-        <v>1704</v>
+        <v>1705</v>
       </c>
       <c r="B1610" t="s">
-        <v>3955</v>
+        <v>3957</v>
       </c>
       <c r="C1610" t="s">
         <v>3875</v>
@@ -62210,15 +62236,15 @@
         <v>1353</v>
       </c>
       <c r="M1610" t="s">
-        <v>3956</v>
+        <v>4514</v>
       </c>
     </row>
     <row r="1611" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1611">
-        <v>1705</v>
+        <v>1706</v>
       </c>
       <c r="B1611" t="s">
-        <v>3957</v>
+        <v>3958</v>
       </c>
       <c r="C1611" t="s">
         <v>3875</v>
@@ -62233,15 +62259,15 @@
         <v>1353</v>
       </c>
       <c r="M1611" t="s">
-        <v>4514</v>
+        <v>3959</v>
       </c>
     </row>
     <row r="1612" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1612">
-        <v>1706</v>
+        <v>1707</v>
       </c>
       <c r="B1612" t="s">
-        <v>3958</v>
+        <v>3960</v>
       </c>
       <c r="C1612" t="s">
         <v>3875</v>
@@ -62256,15 +62282,15 @@
         <v>1353</v>
       </c>
       <c r="M1612" t="s">
-        <v>3959</v>
+        <v>4515</v>
       </c>
     </row>
     <row r="1613" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1613">
-        <v>1707</v>
+        <v>1708</v>
       </c>
       <c r="B1613" t="s">
-        <v>3960</v>
+        <v>3961</v>
       </c>
       <c r="C1613" t="s">
         <v>3875</v>
@@ -62279,15 +62305,15 @@
         <v>1353</v>
       </c>
       <c r="M1613" t="s">
-        <v>4515</v>
+        <v>4516</v>
       </c>
     </row>
     <row r="1614" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1614">
-        <v>1708</v>
+        <v>1709</v>
       </c>
       <c r="B1614" t="s">
-        <v>3961</v>
+        <v>3962</v>
       </c>
       <c r="C1614" t="s">
         <v>3875</v>
@@ -62302,15 +62328,15 @@
         <v>1353</v>
       </c>
       <c r="M1614" t="s">
-        <v>4516</v>
+        <v>4517</v>
       </c>
     </row>
     <row r="1615" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1615">
-        <v>1709</v>
+        <v>1710</v>
       </c>
       <c r="B1615" t="s">
-        <v>3962</v>
+        <v>3963</v>
       </c>
       <c r="C1615" t="s">
         <v>3875</v>
@@ -62325,15 +62351,15 @@
         <v>1353</v>
       </c>
       <c r="M1615" t="s">
-        <v>4517</v>
+        <v>4518</v>
       </c>
     </row>
     <row r="1616" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1616">
-        <v>1710</v>
+        <v>1711</v>
       </c>
       <c r="B1616" t="s">
-        <v>3963</v>
+        <v>3964</v>
       </c>
       <c r="C1616" t="s">
         <v>3875</v>
@@ -62348,15 +62374,15 @@
         <v>1353</v>
       </c>
       <c r="M1616" t="s">
-        <v>4518</v>
+        <v>4519</v>
       </c>
     </row>
     <row r="1617" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1617">
-        <v>1711</v>
+        <v>1712</v>
       </c>
       <c r="B1617" t="s">
-        <v>3964</v>
+        <v>3965</v>
       </c>
       <c r="C1617" t="s">
         <v>3875</v>
@@ -62371,15 +62397,15 @@
         <v>1353</v>
       </c>
       <c r="M1617" t="s">
-        <v>4519</v>
+        <v>4520</v>
       </c>
     </row>
     <row r="1618" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1618">
-        <v>1712</v>
+        <v>1713</v>
       </c>
       <c r="B1618" t="s">
-        <v>3965</v>
+        <v>3966</v>
       </c>
       <c r="C1618" t="s">
         <v>3875</v>
@@ -62394,15 +62420,15 @@
         <v>1353</v>
       </c>
       <c r="M1618" t="s">
-        <v>4520</v>
+        <v>3967</v>
       </c>
     </row>
     <row r="1619" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1619">
-        <v>1713</v>
+        <v>1714</v>
       </c>
       <c r="B1619" t="s">
-        <v>3966</v>
+        <v>3968</v>
       </c>
       <c r="C1619" t="s">
         <v>3875</v>
@@ -62417,15 +62443,15 @@
         <v>1353</v>
       </c>
       <c r="M1619" t="s">
-        <v>3967</v>
+        <v>4521</v>
       </c>
     </row>
     <row r="1620" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1620">
-        <v>1714</v>
+        <v>1715</v>
       </c>
       <c r="B1620" t="s">
-        <v>3968</v>
+        <v>3969</v>
       </c>
       <c r="C1620" t="s">
         <v>3875</v>
@@ -62440,15 +62466,15 @@
         <v>1353</v>
       </c>
       <c r="M1620" t="s">
-        <v>4521</v>
+        <v>4522</v>
       </c>
     </row>
     <row r="1621" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1621">
-        <v>1715</v>
+        <v>1716</v>
       </c>
       <c r="B1621" t="s">
-        <v>3969</v>
+        <v>3970</v>
       </c>
       <c r="C1621" t="s">
         <v>3875</v>
@@ -62463,15 +62489,15 @@
         <v>1353</v>
       </c>
       <c r="M1621" t="s">
-        <v>4522</v>
+        <v>3971</v>
       </c>
     </row>
     <row r="1622" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1622">
-        <v>1716</v>
+        <v>1717</v>
       </c>
       <c r="B1622" t="s">
-        <v>3970</v>
+        <v>3972</v>
       </c>
       <c r="C1622" t="s">
         <v>3875</v>
@@ -62486,15 +62512,15 @@
         <v>1353</v>
       </c>
       <c r="M1622" t="s">
-        <v>3971</v>
+        <v>3973</v>
       </c>
     </row>
     <row r="1623" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1623">
-        <v>1717</v>
+        <v>1718</v>
       </c>
       <c r="B1623" t="s">
-        <v>3972</v>
+        <v>3974</v>
       </c>
       <c r="C1623" t="s">
         <v>3875</v>
@@ -62509,15 +62535,15 @@
         <v>1353</v>
       </c>
       <c r="M1623" t="s">
-        <v>3973</v>
+        <v>4523</v>
       </c>
     </row>
     <row r="1624" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1624">
-        <v>1718</v>
+        <v>1719</v>
       </c>
       <c r="B1624" t="s">
-        <v>3974</v>
+        <v>3975</v>
       </c>
       <c r="C1624" t="s">
         <v>3875</v>
@@ -62532,15 +62558,15 @@
         <v>1353</v>
       </c>
       <c r="M1624" t="s">
-        <v>4523</v>
+        <v>3976</v>
       </c>
     </row>
     <row r="1625" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1625">
-        <v>1719</v>
+        <v>1720</v>
       </c>
       <c r="B1625" t="s">
-        <v>3975</v>
+        <v>3977</v>
       </c>
       <c r="C1625" t="s">
         <v>3875</v>
@@ -62555,15 +62581,15 @@
         <v>1353</v>
       </c>
       <c r="M1625" t="s">
-        <v>3976</v>
+        <v>4524</v>
       </c>
     </row>
     <row r="1626" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1626">
-        <v>1720</v>
+        <v>1721</v>
       </c>
       <c r="B1626" t="s">
-        <v>3977</v>
+        <v>3978</v>
       </c>
       <c r="C1626" t="s">
         <v>3875</v>
@@ -62578,15 +62604,15 @@
         <v>1353</v>
       </c>
       <c r="M1626" t="s">
-        <v>4524</v>
+        <v>4525</v>
       </c>
     </row>
     <row r="1627" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1627">
-        <v>1721</v>
+        <v>1722</v>
       </c>
       <c r="B1627" t="s">
-        <v>3978</v>
+        <v>3979</v>
       </c>
       <c r="C1627" t="s">
         <v>3875</v>
@@ -62601,15 +62627,15 @@
         <v>1353</v>
       </c>
       <c r="M1627" t="s">
-        <v>4525</v>
+        <v>4526</v>
       </c>
     </row>
     <row r="1628" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1628">
-        <v>1722</v>
+        <v>1723</v>
       </c>
       <c r="B1628" t="s">
-        <v>3979</v>
+        <v>3980</v>
       </c>
       <c r="C1628" t="s">
         <v>3875</v>
@@ -62624,15 +62650,15 @@
         <v>1353</v>
       </c>
       <c r="M1628" t="s">
-        <v>4526</v>
+        <v>4527</v>
       </c>
     </row>
     <row r="1629" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1629">
-        <v>1723</v>
+        <v>1724</v>
       </c>
       <c r="B1629" t="s">
-        <v>3980</v>
+        <v>3981</v>
       </c>
       <c r="C1629" t="s">
         <v>3875</v>
@@ -62647,15 +62673,15 @@
         <v>1353</v>
       </c>
       <c r="M1629" t="s">
-        <v>4527</v>
+        <v>4528</v>
       </c>
     </row>
     <row r="1630" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1630">
-        <v>1724</v>
+        <v>1725</v>
       </c>
       <c r="B1630" t="s">
-        <v>3981</v>
+        <v>3982</v>
       </c>
       <c r="C1630" t="s">
         <v>3875</v>
@@ -62670,15 +62696,15 @@
         <v>1353</v>
       </c>
       <c r="M1630" t="s">
-        <v>4528</v>
+        <v>3983</v>
       </c>
     </row>
     <row r="1631" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1631">
-        <v>1725</v>
+        <v>1726</v>
       </c>
       <c r="B1631" t="s">
-        <v>3982</v>
+        <v>3984</v>
       </c>
       <c r="C1631" t="s">
         <v>3875</v>
@@ -62693,15 +62719,15 @@
         <v>1353</v>
       </c>
       <c r="M1631" t="s">
-        <v>3983</v>
+        <v>4529</v>
       </c>
     </row>
     <row r="1632" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1632">
-        <v>1726</v>
+        <v>1727</v>
       </c>
       <c r="B1632" t="s">
-        <v>3984</v>
+        <v>3985</v>
       </c>
       <c r="C1632" t="s">
         <v>3875</v>
@@ -62716,15 +62742,15 @@
         <v>1353</v>
       </c>
       <c r="M1632" t="s">
-        <v>4529</v>
+        <v>3986</v>
       </c>
     </row>
     <row r="1633" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1633">
-        <v>1727</v>
+        <v>1728</v>
       </c>
       <c r="B1633" t="s">
-        <v>3985</v>
+        <v>3987</v>
       </c>
       <c r="C1633" t="s">
         <v>3875</v>
@@ -62739,15 +62765,15 @@
         <v>1353</v>
       </c>
       <c r="M1633" t="s">
-        <v>3986</v>
+        <v>4530</v>
       </c>
     </row>
     <row r="1634" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1634">
-        <v>1728</v>
+        <v>1729</v>
       </c>
       <c r="B1634" t="s">
-        <v>3987</v>
+        <v>3988</v>
       </c>
       <c r="C1634" t="s">
         <v>3875</v>
@@ -62762,15 +62788,15 @@
         <v>1353</v>
       </c>
       <c r="M1634" t="s">
-        <v>4530</v>
+        <v>3989</v>
       </c>
     </row>
     <row r="1635" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1635">
-        <v>1729</v>
+        <v>1730</v>
       </c>
       <c r="B1635" t="s">
-        <v>3988</v>
+        <v>3990</v>
       </c>
       <c r="C1635" t="s">
         <v>3875</v>
@@ -62785,15 +62811,15 @@
         <v>1353</v>
       </c>
       <c r="M1635" t="s">
-        <v>3989</v>
+        <v>3991</v>
       </c>
     </row>
     <row r="1636" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1636">
-        <v>1730</v>
+        <v>1731</v>
       </c>
       <c r="B1636" t="s">
-        <v>3990</v>
+        <v>3992</v>
       </c>
       <c r="C1636" t="s">
         <v>3875</v>
@@ -62808,15 +62834,15 @@
         <v>1353</v>
       </c>
       <c r="M1636" t="s">
-        <v>3991</v>
+        <v>4531</v>
       </c>
     </row>
     <row r="1637" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1637">
-        <v>1731</v>
+        <v>1732</v>
       </c>
       <c r="B1637" t="s">
-        <v>3992</v>
+        <v>3993</v>
       </c>
       <c r="C1637" t="s">
         <v>3875</v>
@@ -62831,15 +62857,15 @@
         <v>1353</v>
       </c>
       <c r="M1637" t="s">
-        <v>4531</v>
+        <v>4532</v>
       </c>
     </row>
     <row r="1638" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1638">
-        <v>1732</v>
+        <v>1733</v>
       </c>
       <c r="B1638" t="s">
-        <v>3993</v>
+        <v>3994</v>
       </c>
       <c r="C1638" t="s">
         <v>3875</v>
@@ -62854,15 +62880,15 @@
         <v>1353</v>
       </c>
       <c r="M1638" t="s">
-        <v>4532</v>
+        <v>3995</v>
       </c>
     </row>
     <row r="1639" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1639">
-        <v>1733</v>
+        <v>1734</v>
       </c>
       <c r="B1639" t="s">
-        <v>3994</v>
+        <v>3996</v>
       </c>
       <c r="C1639" t="s">
         <v>3875</v>
@@ -62877,15 +62903,15 @@
         <v>1353</v>
       </c>
       <c r="M1639" t="s">
-        <v>3995</v>
+        <v>3997</v>
       </c>
     </row>
     <row r="1640" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1640">
-        <v>1734</v>
+        <v>1735</v>
       </c>
       <c r="B1640" t="s">
-        <v>3996</v>
+        <v>3998</v>
       </c>
       <c r="C1640" t="s">
         <v>3875</v>
@@ -62900,15 +62926,15 @@
         <v>1353</v>
       </c>
       <c r="M1640" t="s">
-        <v>3997</v>
+        <v>4533</v>
       </c>
     </row>
     <row r="1641" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1641">
-        <v>1735</v>
+        <v>1736</v>
       </c>
       <c r="B1641" t="s">
-        <v>3998</v>
+        <v>3999</v>
       </c>
       <c r="C1641" t="s">
         <v>3875</v>
@@ -62923,15 +62949,15 @@
         <v>1353</v>
       </c>
       <c r="M1641" t="s">
-        <v>4533</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="1642" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1642">
-        <v>1736</v>
+        <v>1737</v>
       </c>
       <c r="B1642" t="s">
-        <v>3999</v>
+        <v>4001</v>
       </c>
       <c r="C1642" t="s">
         <v>3875</v>
@@ -62946,15 +62972,15 @@
         <v>1353</v>
       </c>
       <c r="M1642" t="s">
-        <v>4000</v>
+        <v>4534</v>
       </c>
     </row>
     <row r="1643" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1643">
-        <v>1737</v>
+        <v>1738</v>
       </c>
       <c r="B1643" t="s">
-        <v>4001</v>
+        <v>4002</v>
       </c>
       <c r="C1643" t="s">
         <v>3875</v>
@@ -62969,15 +62995,15 @@
         <v>1353</v>
       </c>
       <c r="M1643" t="s">
-        <v>4534</v>
+        <v>4535</v>
       </c>
     </row>
     <row r="1644" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1644">
-        <v>1738</v>
+        <v>1739</v>
       </c>
       <c r="B1644" t="s">
-        <v>4002</v>
+        <v>4003</v>
       </c>
       <c r="C1644" t="s">
         <v>3875</v>
@@ -62992,15 +63018,15 @@
         <v>1353</v>
       </c>
       <c r="M1644" t="s">
-        <v>4535</v>
+        <v>4536</v>
       </c>
     </row>
     <row r="1645" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1645">
-        <v>1739</v>
+        <v>1740</v>
       </c>
       <c r="B1645" t="s">
-        <v>4003</v>
+        <v>4004</v>
       </c>
       <c r="C1645" t="s">
         <v>3875</v>
@@ -63015,15 +63041,15 @@
         <v>1353</v>
       </c>
       <c r="M1645" t="s">
-        <v>4536</v>
+        <v>4537</v>
       </c>
     </row>
     <row r="1646" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1646">
-        <v>1740</v>
+        <v>1741</v>
       </c>
       <c r="B1646" t="s">
-        <v>4004</v>
+        <v>4005</v>
       </c>
       <c r="C1646" t="s">
         <v>3875</v>
@@ -63038,15 +63064,15 @@
         <v>1353</v>
       </c>
       <c r="M1646" t="s">
-        <v>4537</v>
+        <v>4538</v>
       </c>
     </row>
     <row r="1647" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1647">
-        <v>1741</v>
+        <v>1742</v>
       </c>
       <c r="B1647" t="s">
-        <v>4005</v>
+        <v>4006</v>
       </c>
       <c r="C1647" t="s">
         <v>3875</v>
@@ -63061,15 +63087,15 @@
         <v>1353</v>
       </c>
       <c r="M1647" t="s">
-        <v>4538</v>
+        <v>4539</v>
       </c>
     </row>
     <row r="1648" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1648">
-        <v>1742</v>
+        <v>1743</v>
       </c>
       <c r="B1648" t="s">
-        <v>4006</v>
+        <v>4007</v>
       </c>
       <c r="C1648" t="s">
         <v>3875</v>
@@ -63084,15 +63110,15 @@
         <v>1353</v>
       </c>
       <c r="M1648" t="s">
-        <v>4539</v>
+        <v>4008</v>
       </c>
     </row>
     <row r="1649" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1649">
-        <v>1743</v>
+        <v>1744</v>
       </c>
       <c r="B1649" t="s">
-        <v>4007</v>
+        <v>4009</v>
       </c>
       <c r="C1649" t="s">
         <v>3875</v>
@@ -63107,15 +63133,15 @@
         <v>1353</v>
       </c>
       <c r="M1649" t="s">
-        <v>4008</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="1650" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1650">
-        <v>1744</v>
+        <v>1745</v>
       </c>
       <c r="B1650" t="s">
-        <v>4009</v>
+        <v>4010</v>
       </c>
       <c r="C1650" t="s">
         <v>3875</v>
@@ -63130,15 +63156,15 @@
         <v>1353</v>
       </c>
       <c r="M1650" t="s">
-        <v>4540</v>
+        <v>4541</v>
       </c>
     </row>
     <row r="1651" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1651">
-        <v>1745</v>
+        <v>1746</v>
       </c>
       <c r="B1651" t="s">
-        <v>4010</v>
+        <v>4011</v>
       </c>
       <c r="C1651" t="s">
         <v>3875</v>
@@ -63153,15 +63179,15 @@
         <v>1353</v>
       </c>
       <c r="M1651" t="s">
-        <v>4541</v>
+        <v>4012</v>
       </c>
     </row>
     <row r="1652" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1652">
-        <v>1746</v>
+        <v>1747</v>
       </c>
       <c r="B1652" t="s">
-        <v>4011</v>
+        <v>4013</v>
       </c>
       <c r="C1652" t="s">
         <v>3875</v>
@@ -63176,15 +63202,15 @@
         <v>1353</v>
       </c>
       <c r="M1652" t="s">
-        <v>4012</v>
+        <v>4542</v>
       </c>
     </row>
     <row r="1653" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1653">
-        <v>1747</v>
+        <v>1748</v>
       </c>
       <c r="B1653" t="s">
-        <v>4013</v>
+        <v>4014</v>
       </c>
       <c r="C1653" t="s">
         <v>3875</v>
@@ -63199,15 +63225,15 @@
         <v>1353</v>
       </c>
       <c r="M1653" t="s">
-        <v>4542</v>
+        <v>4015</v>
       </c>
     </row>
     <row r="1654" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1654">
-        <v>1748</v>
+        <v>1749</v>
       </c>
       <c r="B1654" t="s">
-        <v>4014</v>
+        <v>4016</v>
       </c>
       <c r="C1654" t="s">
         <v>3875</v>
@@ -63222,15 +63248,15 @@
         <v>1353</v>
       </c>
       <c r="M1654" t="s">
-        <v>4015</v>
+        <v>4017</v>
       </c>
     </row>
     <row r="1655" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1655">
-        <v>1749</v>
+        <v>1750</v>
       </c>
       <c r="B1655" t="s">
-        <v>4016</v>
+        <v>4018</v>
       </c>
       <c r="C1655" t="s">
         <v>3875</v>
@@ -63245,15 +63271,15 @@
         <v>1353</v>
       </c>
       <c r="M1655" t="s">
-        <v>4017</v>
+        <v>4543</v>
       </c>
     </row>
     <row r="1656" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1656">
-        <v>1750</v>
+        <v>1751</v>
       </c>
       <c r="B1656" t="s">
-        <v>4018</v>
+        <v>4019</v>
       </c>
       <c r="C1656" t="s">
         <v>3875</v>
@@ -63268,15 +63294,15 @@
         <v>1353</v>
       </c>
       <c r="M1656" t="s">
-        <v>4543</v>
+        <v>4020</v>
       </c>
     </row>
     <row r="1657" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1657">
-        <v>1751</v>
+        <v>1752</v>
       </c>
       <c r="B1657" t="s">
-        <v>4019</v>
+        <v>4021</v>
       </c>
       <c r="C1657" t="s">
         <v>3875</v>
@@ -63291,15 +63317,15 @@
         <v>1353</v>
       </c>
       <c r="M1657" t="s">
-        <v>4020</v>
+        <v>4544</v>
       </c>
     </row>
     <row r="1658" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1658">
-        <v>1752</v>
+        <v>1753</v>
       </c>
       <c r="B1658" t="s">
-        <v>4021</v>
+        <v>4022</v>
       </c>
       <c r="C1658" t="s">
         <v>3875</v>
@@ -63314,15 +63340,15 @@
         <v>1353</v>
       </c>
       <c r="M1658" t="s">
-        <v>4544</v>
+        <v>4545</v>
       </c>
     </row>
     <row r="1659" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1659">
-        <v>1753</v>
+        <v>1754</v>
       </c>
       <c r="B1659" t="s">
-        <v>4022</v>
+        <v>4023</v>
       </c>
       <c r="C1659" t="s">
         <v>3875</v>
@@ -63337,15 +63363,15 @@
         <v>1353</v>
       </c>
       <c r="M1659" t="s">
-        <v>4545</v>
+        <v>4546</v>
       </c>
     </row>
     <row r="1660" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1660">
-        <v>1754</v>
+        <v>1755</v>
       </c>
       <c r="B1660" t="s">
-        <v>4023</v>
+        <v>4024</v>
       </c>
       <c r="C1660" t="s">
         <v>3875</v>
@@ -63360,15 +63386,15 @@
         <v>1353</v>
       </c>
       <c r="M1660" t="s">
-        <v>4546</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="1661" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1661">
-        <v>1755</v>
+        <v>1756</v>
       </c>
       <c r="B1661" t="s">
-        <v>4024</v>
+        <v>4025</v>
       </c>
       <c r="C1661" t="s">
         <v>3875</v>
@@ -63383,15 +63409,15 @@
         <v>1353</v>
       </c>
       <c r="M1661" t="s">
-        <v>4547</v>
+        <v>4548</v>
       </c>
     </row>
     <row r="1662" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1662">
-        <v>1756</v>
+        <v>1757</v>
       </c>
       <c r="B1662" t="s">
-        <v>4025</v>
+        <v>4026</v>
       </c>
       <c r="C1662" t="s">
         <v>3875</v>
@@ -63406,15 +63432,15 @@
         <v>1353</v>
       </c>
       <c r="M1662" t="s">
-        <v>4548</v>
+        <v>4027</v>
       </c>
     </row>
     <row r="1663" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1663">
-        <v>1757</v>
+        <v>1758</v>
       </c>
       <c r="B1663" t="s">
-        <v>4026</v>
+        <v>4028</v>
       </c>
       <c r="C1663" t="s">
         <v>3875</v>
@@ -63429,15 +63455,15 @@
         <v>1353</v>
       </c>
       <c r="M1663" t="s">
-        <v>4027</v>
+        <v>4549</v>
       </c>
     </row>
     <row r="1664" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1664">
-        <v>1758</v>
+        <v>1759</v>
       </c>
       <c r="B1664" t="s">
-        <v>4028</v>
+        <v>4029</v>
       </c>
       <c r="C1664" t="s">
         <v>3875</v>
@@ -63452,15 +63478,15 @@
         <v>1353</v>
       </c>
       <c r="M1664" t="s">
-        <v>4549</v>
+        <v>4550</v>
       </c>
     </row>
     <row r="1665" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1665">
-        <v>1759</v>
+        <v>1760</v>
       </c>
       <c r="B1665" t="s">
-        <v>4029</v>
+        <v>4030</v>
       </c>
       <c r="C1665" t="s">
         <v>3875</v>
@@ -63475,15 +63501,15 @@
         <v>1353</v>
       </c>
       <c r="M1665" t="s">
-        <v>4550</v>
+        <v>4031</v>
       </c>
     </row>
     <row r="1666" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1666">
-        <v>1760</v>
+        <v>1761</v>
       </c>
       <c r="B1666" t="s">
-        <v>4030</v>
+        <v>4032</v>
       </c>
       <c r="C1666" t="s">
         <v>3875</v>
@@ -63498,15 +63524,15 @@
         <v>1353</v>
       </c>
       <c r="M1666" t="s">
-        <v>4031</v>
+        <v>4033</v>
       </c>
     </row>
     <row r="1667" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1667">
-        <v>1761</v>
+        <v>1762</v>
       </c>
       <c r="B1667" t="s">
-        <v>4032</v>
+        <v>4034</v>
       </c>
       <c r="C1667" t="s">
         <v>3875</v>
@@ -63521,15 +63547,15 @@
         <v>1353</v>
       </c>
       <c r="M1667" t="s">
-        <v>4033</v>
+        <v>4035</v>
       </c>
     </row>
     <row r="1668" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1668">
-        <v>1762</v>
+        <v>1763</v>
       </c>
       <c r="B1668" t="s">
-        <v>4034</v>
+        <v>4036</v>
       </c>
       <c r="C1668" t="s">
         <v>3875</v>
@@ -63544,15 +63570,15 @@
         <v>1353</v>
       </c>
       <c r="M1668" t="s">
-        <v>4035</v>
+        <v>4037</v>
       </c>
     </row>
     <row r="1669" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1669">
-        <v>1763</v>
+        <v>1764</v>
       </c>
       <c r="B1669" t="s">
-        <v>4036</v>
+        <v>4038</v>
       </c>
       <c r="C1669" t="s">
         <v>3875</v>
@@ -63567,15 +63593,15 @@
         <v>1353</v>
       </c>
       <c r="M1669" t="s">
-        <v>4037</v>
+        <v>4551</v>
       </c>
     </row>
     <row r="1670" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1670">
-        <v>1764</v>
+        <v>1765</v>
       </c>
       <c r="B1670" t="s">
-        <v>4038</v>
+        <v>4039</v>
       </c>
       <c r="C1670" t="s">
         <v>3875</v>
@@ -63590,15 +63616,15 @@
         <v>1353</v>
       </c>
       <c r="M1670" t="s">
-        <v>4551</v>
+        <v>4040</v>
       </c>
     </row>
     <row r="1671" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1671">
-        <v>1765</v>
+        <v>1766</v>
       </c>
       <c r="B1671" t="s">
-        <v>4039</v>
+        <v>4041</v>
       </c>
       <c r="C1671" t="s">
         <v>3875</v>
@@ -63613,15 +63639,15 @@
         <v>1353</v>
       </c>
       <c r="M1671" t="s">
-        <v>4040</v>
+        <v>4042</v>
       </c>
     </row>
     <row r="1672" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1672">
-        <v>1766</v>
+        <v>1767</v>
       </c>
       <c r="B1672" t="s">
-        <v>4041</v>
+        <v>4043</v>
       </c>
       <c r="C1672" t="s">
         <v>3875</v>
@@ -63636,15 +63662,15 @@
         <v>1353</v>
       </c>
       <c r="M1672" t="s">
-        <v>4042</v>
+        <v>4552</v>
       </c>
     </row>
     <row r="1673" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1673">
-        <v>1767</v>
+        <v>1768</v>
       </c>
       <c r="B1673" t="s">
-        <v>4043</v>
+        <v>4044</v>
       </c>
       <c r="C1673" t="s">
         <v>3875</v>
@@ -63659,15 +63685,15 @@
         <v>1353</v>
       </c>
       <c r="M1673" t="s">
-        <v>4552</v>
+        <v>4045</v>
       </c>
     </row>
     <row r="1674" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1674">
-        <v>1768</v>
+        <v>1769</v>
       </c>
       <c r="B1674" t="s">
-        <v>4044</v>
+        <v>4046</v>
       </c>
       <c r="C1674" t="s">
         <v>3875</v>
@@ -63682,15 +63708,15 @@
         <v>1353</v>
       </c>
       <c r="M1674" t="s">
-        <v>4045</v>
+        <v>4553</v>
       </c>
     </row>
     <row r="1675" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1675">
-        <v>1769</v>
+        <v>1770</v>
       </c>
       <c r="B1675" t="s">
-        <v>4046</v>
+        <v>4047</v>
       </c>
       <c r="C1675" t="s">
         <v>3875</v>
@@ -63705,15 +63731,15 @@
         <v>1353</v>
       </c>
       <c r="M1675" t="s">
-        <v>4553</v>
+        <v>4048</v>
       </c>
     </row>
     <row r="1676" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1676">
-        <v>1770</v>
+        <v>1771</v>
       </c>
       <c r="B1676" t="s">
-        <v>4047</v>
+        <v>4049</v>
       </c>
       <c r="C1676" t="s">
         <v>3875</v>
@@ -63728,15 +63754,15 @@
         <v>1353</v>
       </c>
       <c r="M1676" t="s">
-        <v>4048</v>
+        <v>4050</v>
       </c>
     </row>
     <row r="1677" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1677">
-        <v>1771</v>
+        <v>1772</v>
       </c>
       <c r="B1677" t="s">
-        <v>4049</v>
+        <v>4051</v>
       </c>
       <c r="C1677" t="s">
         <v>3875</v>
@@ -63751,15 +63777,15 @@
         <v>1353</v>
       </c>
       <c r="M1677" t="s">
-        <v>4050</v>
+        <v>4052</v>
       </c>
     </row>
     <row r="1678" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1678">
-        <v>1772</v>
+        <v>1773</v>
       </c>
       <c r="B1678" t="s">
-        <v>4051</v>
+        <v>4053</v>
       </c>
       <c r="C1678" t="s">
         <v>3875</v>
@@ -63774,15 +63800,15 @@
         <v>1353</v>
       </c>
       <c r="M1678" t="s">
-        <v>4052</v>
+        <v>4554</v>
       </c>
     </row>
     <row r="1679" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1679">
-        <v>1773</v>
+        <v>1774</v>
       </c>
       <c r="B1679" t="s">
-        <v>4053</v>
+        <v>4054</v>
       </c>
       <c r="C1679" t="s">
         <v>3875</v>
@@ -63797,15 +63823,15 @@
         <v>1353</v>
       </c>
       <c r="M1679" t="s">
-        <v>4554</v>
+        <v>4555</v>
       </c>
     </row>
     <row r="1680" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1680">
-        <v>1774</v>
+        <v>1775</v>
       </c>
       <c r="B1680" t="s">
-        <v>4054</v>
+        <v>4055</v>
       </c>
       <c r="C1680" t="s">
         <v>3875</v>
@@ -63820,15 +63846,15 @@
         <v>1353</v>
       </c>
       <c r="M1680" t="s">
-        <v>4555</v>
+        <v>4556</v>
       </c>
     </row>
     <row r="1681" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1681">
-        <v>1775</v>
+        <v>1776</v>
       </c>
       <c r="B1681" t="s">
-        <v>4055</v>
+        <v>4056</v>
       </c>
       <c r="C1681" t="s">
         <v>3875</v>
@@ -63843,15 +63869,15 @@
         <v>1353</v>
       </c>
       <c r="M1681" t="s">
-        <v>4556</v>
+        <v>4557</v>
       </c>
     </row>
     <row r="1682" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1682">
-        <v>1776</v>
+        <v>1777</v>
       </c>
       <c r="B1682" t="s">
-        <v>4056</v>
+        <v>4057</v>
       </c>
       <c r="C1682" t="s">
         <v>3875</v>
@@ -63866,15 +63892,15 @@
         <v>1353</v>
       </c>
       <c r="M1682" t="s">
-        <v>4557</v>
+        <v>4558</v>
       </c>
     </row>
     <row r="1683" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1683">
-        <v>1777</v>
+        <v>1778</v>
       </c>
       <c r="B1683" t="s">
-        <v>4057</v>
+        <v>4058</v>
       </c>
       <c r="C1683" t="s">
         <v>3875</v>
@@ -63889,15 +63915,15 @@
         <v>1353</v>
       </c>
       <c r="M1683" t="s">
-        <v>4558</v>
+        <v>4059</v>
       </c>
     </row>
     <row r="1684" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1684">
-        <v>1778</v>
+        <v>1779</v>
       </c>
       <c r="B1684" t="s">
-        <v>4058</v>
+        <v>4060</v>
       </c>
       <c r="C1684" t="s">
         <v>3875</v>
@@ -63912,15 +63938,15 @@
         <v>1353</v>
       </c>
       <c r="M1684" t="s">
-        <v>4059</v>
+        <v>4559</v>
       </c>
     </row>
     <row r="1685" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1685">
-        <v>1779</v>
+        <v>1780</v>
       </c>
       <c r="B1685" t="s">
-        <v>4060</v>
+        <v>4061</v>
       </c>
       <c r="C1685" t="s">
         <v>3875</v>
@@ -63935,34 +63961,11 @@
         <v>1353</v>
       </c>
       <c r="M1685" t="s">
-        <v>4559</v>
-      </c>
-    </row>
-    <row r="1686" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1686">
-        <v>1780</v>
-      </c>
-      <c r="B1686" t="s">
-        <v>4061</v>
-      </c>
-      <c r="C1686" t="s">
-        <v>3875</v>
-      </c>
-      <c r="D1686">
-        <v>68000</v>
-      </c>
-      <c r="E1686" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1686" t="s">
-        <v>1353</v>
-      </c>
-      <c r="M1686" t="s">
         <v>4062</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M1686"/>
+  <autoFilter ref="A1:M1685"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
036 : Added spacefb driver
</commit_message>
<xml_diff>
--- a/0.36/compatibility.xlsx
+++ b/0.36/compatibility.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Playable (untested)" sheetId="4" r:id="rId1"/>
@@ -17,8 +17,8 @@
     <sheet name="GAME_NOT_WORKING FLAG" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ALL!$A$1:$M$1633</definedName>
-    <definedName name="LIST" localSheetId="1">ALL!$B$1:$M$1633</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ALL!$A$1:$M$1628</definedName>
+    <definedName name="LIST" localSheetId="1">ALL!$B$1:$M$1628</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -14084,10 +14084,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P408"/>
+  <dimension ref="A1:P413"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A393" workbookViewId="0">
-      <selection activeCell="O422" sqref="O422"/>
+    <sheetView topLeftCell="A393" workbookViewId="0">
+      <selection activeCell="A414" sqref="A414"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23639,6 +23639,121 @@
         <v>4567</v>
       </c>
     </row>
+    <row r="409" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A409">
+        <v>409</v>
+      </c>
+      <c r="B409" t="s">
+        <v>3757</v>
+      </c>
+      <c r="C409" t="s">
+        <v>3758</v>
+      </c>
+      <c r="D409" t="s">
+        <v>14</v>
+      </c>
+      <c r="E409" t="s">
+        <v>725</v>
+      </c>
+      <c r="H409" t="s">
+        <v>166</v>
+      </c>
+      <c r="M409" t="s">
+        <v>4490</v>
+      </c>
+    </row>
+    <row r="410" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A410">
+        <v>410</v>
+      </c>
+      <c r="B410" t="s">
+        <v>3759</v>
+      </c>
+      <c r="C410" t="s">
+        <v>3758</v>
+      </c>
+      <c r="D410" t="s">
+        <v>14</v>
+      </c>
+      <c r="E410" t="s">
+        <v>725</v>
+      </c>
+      <c r="H410" t="s">
+        <v>166</v>
+      </c>
+      <c r="M410" t="s">
+        <v>3760</v>
+      </c>
+    </row>
+    <row r="411" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A411">
+        <v>411</v>
+      </c>
+      <c r="B411" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C411" t="s">
+        <v>3758</v>
+      </c>
+      <c r="D411" t="s">
+        <v>14</v>
+      </c>
+      <c r="E411" t="s">
+        <v>725</v>
+      </c>
+      <c r="H411" t="s">
+        <v>166</v>
+      </c>
+      <c r="M411" t="s">
+        <v>3762</v>
+      </c>
+    </row>
+    <row r="412" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A412">
+        <v>412</v>
+      </c>
+      <c r="B412" t="s">
+        <v>3763</v>
+      </c>
+      <c r="C412" t="s">
+        <v>3758</v>
+      </c>
+      <c r="D412" t="s">
+        <v>14</v>
+      </c>
+      <c r="E412" t="s">
+        <v>725</v>
+      </c>
+      <c r="H412" t="s">
+        <v>166</v>
+      </c>
+      <c r="M412" t="s">
+        <v>3764</v>
+      </c>
+    </row>
+    <row r="413" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A413">
+        <v>413</v>
+      </c>
+      <c r="B413" t="s">
+        <v>3765</v>
+      </c>
+      <c r="C413" t="s">
+        <v>3758</v>
+      </c>
+      <c r="D413" t="s">
+        <v>14</v>
+      </c>
+      <c r="E413" t="s">
+        <v>725</v>
+      </c>
+      <c r="H413" t="s">
+        <v>166</v>
+      </c>
+      <c r="M413" t="s">
+        <v>3766</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -23647,10 +23762,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1633"/>
+  <dimension ref="A1:M1628"/>
   <sheetViews>
-    <sheetView topLeftCell="A1613" workbookViewId="0">
-      <selection activeCell="A962" sqref="A962:XFD964"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E695" sqref="E695"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -60318,666 +60433,657 @@
     </row>
     <row r="1476" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1476">
-        <v>1612</v>
+        <v>1617</v>
       </c>
       <c r="B1476" t="s">
-        <v>3757</v>
+        <v>3774</v>
       </c>
       <c r="C1476" t="s">
-        <v>3758</v>
+        <v>3775</v>
       </c>
       <c r="D1476" t="s">
         <v>14</v>
       </c>
       <c r="E1476" t="s">
-        <v>725</v>
+        <v>154</v>
       </c>
       <c r="H1476" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="M1476" t="s">
-        <v>4490</v>
+        <v>3776</v>
       </c>
     </row>
     <row r="1477" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1477">
-        <v>1613</v>
+        <v>1618</v>
       </c>
       <c r="B1477" t="s">
-        <v>3759</v>
+        <v>3777</v>
       </c>
       <c r="C1477" t="s">
-        <v>3758</v>
+        <v>3778</v>
       </c>
       <c r="D1477" t="s">
         <v>14</v>
       </c>
-      <c r="E1477" t="s">
-        <v>725</v>
-      </c>
       <c r="H1477" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="M1477" t="s">
-        <v>3760</v>
+        <v>3779</v>
       </c>
     </row>
     <row r="1478" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1478">
-        <v>1614</v>
+        <v>1619</v>
       </c>
       <c r="B1478" t="s">
-        <v>3761</v>
+        <v>3780</v>
       </c>
       <c r="C1478" t="s">
-        <v>3758</v>
+        <v>3778</v>
       </c>
       <c r="D1478" t="s">
         <v>14</v>
       </c>
-      <c r="E1478" t="s">
-        <v>725</v>
-      </c>
       <c r="H1478" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="M1478" t="s">
-        <v>3762</v>
+        <v>3781</v>
       </c>
     </row>
     <row r="1479" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1479">
-        <v>1615</v>
+        <v>1624</v>
       </c>
       <c r="B1479" t="s">
-        <v>3763</v>
+        <v>3791</v>
       </c>
       <c r="C1479" t="s">
-        <v>3758</v>
+        <v>3792</v>
       </c>
       <c r="D1479" t="s">
-        <v>14</v>
+        <v>405</v>
       </c>
       <c r="E1479" t="s">
-        <v>725</v>
+        <v>1184</v>
       </c>
       <c r="H1479" t="s">
-        <v>166</v>
+        <v>71</v>
       </c>
       <c r="M1479" t="s">
-        <v>3764</v>
+        <v>3793</v>
       </c>
     </row>
     <row r="1480" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1480">
-        <v>1616</v>
+        <v>1625</v>
       </c>
       <c r="B1480" t="s">
-        <v>3765</v>
+        <v>3794</v>
       </c>
       <c r="C1480" t="s">
-        <v>3758</v>
+        <v>3792</v>
       </c>
       <c r="D1480" t="s">
-        <v>14</v>
+        <v>405</v>
       </c>
       <c r="E1480" t="s">
-        <v>725</v>
+        <v>1184</v>
       </c>
       <c r="H1480" t="s">
-        <v>166</v>
+        <v>71</v>
       </c>
       <c r="M1480" t="s">
-        <v>3766</v>
+        <v>3795</v>
       </c>
     </row>
     <row r="1481" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1481">
-        <v>1617</v>
+        <v>1626</v>
       </c>
       <c r="B1481" t="s">
-        <v>3774</v>
+        <v>3799</v>
       </c>
       <c r="C1481" t="s">
-        <v>3775</v>
+        <v>3800</v>
       </c>
       <c r="D1481" t="s">
-        <v>14</v>
+        <v>405</v>
       </c>
       <c r="E1481" t="s">
-        <v>154</v>
+        <v>1184</v>
+      </c>
+      <c r="F1481" t="s">
+        <v>3801</v>
       </c>
       <c r="H1481" t="s">
-        <v>172</v>
+        <v>71</v>
       </c>
       <c r="M1481" t="s">
-        <v>3776</v>
+        <v>3802</v>
       </c>
     </row>
     <row r="1482" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1482">
-        <v>1618</v>
+        <v>1627</v>
       </c>
       <c r="B1482" t="s">
-        <v>3777</v>
+        <v>3803</v>
       </c>
       <c r="C1482" t="s">
-        <v>3778</v>
+        <v>3804</v>
       </c>
       <c r="D1482" t="s">
-        <v>14</v>
+        <v>473</v>
       </c>
       <c r="H1482" t="s">
-        <v>172</v>
+        <v>2936</v>
       </c>
       <c r="M1482" t="s">
-        <v>3779</v>
+        <v>3805</v>
       </c>
     </row>
     <row r="1483" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1483">
-        <v>1619</v>
+        <v>1628</v>
       </c>
       <c r="B1483" t="s">
-        <v>3780</v>
+        <v>3806</v>
       </c>
       <c r="C1483" t="s">
-        <v>3778</v>
+        <v>3807</v>
       </c>
       <c r="D1483" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1483" t="s">
-        <v>172</v>
+        <v>473</v>
       </c>
       <c r="M1483" t="s">
-        <v>3781</v>
+        <v>3808</v>
       </c>
     </row>
     <row r="1484" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1484">
-        <v>1624</v>
+        <v>1629</v>
       </c>
       <c r="B1484" t="s">
-        <v>3791</v>
+        <v>3809</v>
       </c>
       <c r="C1484" t="s">
-        <v>3792</v>
+        <v>3807</v>
       </c>
       <c r="D1484" t="s">
-        <v>405</v>
-      </c>
-      <c r="E1484" t="s">
-        <v>1184</v>
-      </c>
-      <c r="H1484" t="s">
-        <v>71</v>
+        <v>473</v>
       </c>
       <c r="M1484" t="s">
-        <v>3793</v>
+        <v>3810</v>
       </c>
     </row>
     <row r="1485" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1485">
-        <v>1625</v>
+        <v>1630</v>
       </c>
       <c r="B1485" t="s">
-        <v>3794</v>
+        <v>3811</v>
       </c>
       <c r="C1485" t="s">
-        <v>3792</v>
-      </c>
-      <c r="D1485" t="s">
-        <v>405</v>
-      </c>
-      <c r="E1485" t="s">
-        <v>1184</v>
-      </c>
-      <c r="H1485" t="s">
-        <v>71</v>
+        <v>3812</v>
+      </c>
+      <c r="D1485">
+        <v>8080</v>
       </c>
       <c r="M1485" t="s">
-        <v>3795</v>
+        <v>3813</v>
       </c>
     </row>
     <row r="1486" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1486">
-        <v>1626</v>
+        <v>1631</v>
       </c>
       <c r="B1486" t="s">
-        <v>3799</v>
+        <v>3814</v>
       </c>
       <c r="C1486" t="s">
-        <v>3800</v>
+        <v>3815</v>
       </c>
       <c r="D1486" t="s">
-        <v>405</v>
+        <v>3436</v>
       </c>
       <c r="E1486" t="s">
+        <v>3436</v>
+      </c>
+      <c r="F1486" t="s">
         <v>1184</v>
       </c>
-      <c r="F1486" t="s">
-        <v>3801</v>
+      <c r="G1486" t="s">
+        <v>1184</v>
       </c>
       <c r="H1486" t="s">
-        <v>71</v>
+        <v>333</v>
+      </c>
+      <c r="I1486" t="s">
+        <v>551</v>
       </c>
       <c r="M1486" t="s">
-        <v>3802</v>
+        <v>3816</v>
       </c>
     </row>
     <row r="1487" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1487">
-        <v>1627</v>
+        <v>1632</v>
       </c>
       <c r="B1487" t="s">
-        <v>3803</v>
+        <v>3817</v>
       </c>
       <c r="C1487" t="s">
-        <v>3804</v>
+        <v>3818</v>
       </c>
       <c r="D1487" t="s">
-        <v>473</v>
+        <v>14</v>
       </c>
       <c r="H1487" t="s">
-        <v>2936</v>
+        <v>172</v>
       </c>
       <c r="M1487" t="s">
-        <v>3805</v>
+        <v>3819</v>
       </c>
     </row>
     <row r="1488" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1488">
-        <v>1628</v>
+        <v>1633</v>
       </c>
       <c r="B1488" t="s">
-        <v>3806</v>
+        <v>3820</v>
       </c>
       <c r="C1488" t="s">
-        <v>3807</v>
+        <v>3821</v>
       </c>
       <c r="D1488" t="s">
-        <v>473</v>
+        <v>14</v>
+      </c>
+      <c r="E1488" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1488" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1488" t="s">
+        <v>154</v>
+      </c>
+      <c r="H1488" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1488" t="s">
+        <v>166</v>
       </c>
       <c r="M1488" t="s">
-        <v>3808</v>
+        <v>3822</v>
       </c>
     </row>
     <row r="1489" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1489">
-        <v>1629</v>
+        <v>1634</v>
       </c>
       <c r="B1489" t="s">
-        <v>3809</v>
+        <v>3823</v>
       </c>
       <c r="C1489" t="s">
-        <v>3807</v>
+        <v>3821</v>
       </c>
       <c r="D1489" t="s">
-        <v>473</v>
+        <v>14</v>
+      </c>
+      <c r="E1489" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1489" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1489" t="s">
+        <v>154</v>
+      </c>
+      <c r="H1489" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1489" t="s">
+        <v>166</v>
       </c>
       <c r="M1489" t="s">
-        <v>3810</v>
+        <v>3824</v>
       </c>
     </row>
     <row r="1490" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1490">
-        <v>1630</v>
+        <v>1635</v>
       </c>
       <c r="B1490" t="s">
-        <v>3811</v>
+        <v>3825</v>
       </c>
       <c r="C1490" t="s">
-        <v>3812</v>
-      </c>
-      <c r="D1490">
-        <v>8080</v>
+        <v>3821</v>
+      </c>
+      <c r="D1490" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1490" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1490" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1490" t="s">
+        <v>154</v>
+      </c>
+      <c r="H1490" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1490" t="s">
+        <v>166</v>
       </c>
       <c r="M1490" t="s">
-        <v>3813</v>
+        <v>3826</v>
       </c>
     </row>
     <row r="1491" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1491">
-        <v>1631</v>
+        <v>1636</v>
       </c>
       <c r="B1491" t="s">
-        <v>3814</v>
+        <v>3827</v>
       </c>
       <c r="C1491" t="s">
-        <v>3815</v>
+        <v>3821</v>
       </c>
       <c r="D1491" t="s">
-        <v>3436</v>
+        <v>14</v>
       </c>
       <c r="E1491" t="s">
-        <v>3436</v>
+        <v>14</v>
       </c>
       <c r="F1491" t="s">
-        <v>1184</v>
+        <v>14</v>
       </c>
       <c r="G1491" t="s">
-        <v>1184</v>
+        <v>154</v>
       </c>
       <c r="H1491" t="s">
-        <v>333</v>
+        <v>71</v>
       </c>
       <c r="I1491" t="s">
-        <v>551</v>
+        <v>166</v>
       </c>
       <c r="M1491" t="s">
-        <v>3816</v>
+        <v>3828</v>
       </c>
     </row>
     <row r="1492" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1492">
-        <v>1632</v>
+        <v>1637</v>
       </c>
       <c r="B1492" t="s">
-        <v>3817</v>
+        <v>3829</v>
       </c>
       <c r="C1492" t="s">
-        <v>3818</v>
-      </c>
-      <c r="D1492" t="s">
-        <v>14</v>
+        <v>3830</v>
+      </c>
+      <c r="D1492">
+        <v>68000</v>
+      </c>
+      <c r="E1492" t="s">
+        <v>154</v>
       </c>
       <c r="H1492" t="s">
-        <v>172</v>
+        <v>1492</v>
       </c>
       <c r="M1492" t="s">
-        <v>3819</v>
+        <v>3831</v>
       </c>
     </row>
     <row r="1493" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1493">
-        <v>1633</v>
+        <v>1645</v>
       </c>
       <c r="B1493" t="s">
-        <v>3820</v>
+        <v>3848</v>
       </c>
       <c r="C1493" t="s">
-        <v>3821</v>
-      </c>
-      <c r="D1493" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1493" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1493" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1493" t="s">
-        <v>154</v>
+        <v>3849</v>
+      </c>
+      <c r="D1493">
+        <v>8080</v>
       </c>
       <c r="H1493" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1493" t="s">
-        <v>166</v>
+        <v>406</v>
       </c>
       <c r="M1493" t="s">
-        <v>3822</v>
+        <v>3850</v>
       </c>
     </row>
     <row r="1494" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1494">
-        <v>1634</v>
+        <v>1646</v>
       </c>
       <c r="B1494" t="s">
-        <v>3823</v>
+        <v>3851</v>
       </c>
       <c r="C1494" t="s">
-        <v>3821</v>
+        <v>3852</v>
       </c>
       <c r="D1494" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1494" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1494" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1494" t="s">
-        <v>154</v>
+        <v>1105</v>
       </c>
       <c r="H1494" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1494" t="s">
-        <v>166</v>
+        <v>336</v>
       </c>
       <c r="M1494" t="s">
-        <v>3824</v>
+        <v>3853</v>
       </c>
     </row>
     <row r="1495" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1495">
-        <v>1635</v>
+        <v>1647</v>
       </c>
       <c r="B1495" t="s">
-        <v>3825</v>
+        <v>3854</v>
       </c>
       <c r="C1495" t="s">
-        <v>3821</v>
+        <v>3855</v>
       </c>
       <c r="D1495" t="s">
         <v>14</v>
       </c>
       <c r="E1495" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1495" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1495" t="s">
         <v>154</v>
       </c>
       <c r="H1495" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1495" t="s">
-        <v>166</v>
+        <v>336</v>
       </c>
       <c r="M1495" t="s">
-        <v>3826</v>
+        <v>3856</v>
       </c>
     </row>
     <row r="1496" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1496">
-        <v>1636</v>
+        <v>1648</v>
       </c>
       <c r="B1496" t="s">
-        <v>3827</v>
+        <v>3857</v>
       </c>
       <c r="C1496" t="s">
-        <v>3821</v>
+        <v>3855</v>
       </c>
       <c r="D1496" t="s">
         <v>14</v>
       </c>
       <c r="E1496" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1496" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1496" t="s">
         <v>154</v>
       </c>
       <c r="H1496" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1496" t="s">
-        <v>166</v>
+        <v>336</v>
       </c>
       <c r="M1496" t="s">
-        <v>3828</v>
+        <v>3858</v>
       </c>
     </row>
     <row r="1497" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1497">
-        <v>1637</v>
+        <v>1649</v>
       </c>
       <c r="B1497" t="s">
-        <v>3829</v>
+        <v>3859</v>
       </c>
       <c r="C1497" t="s">
-        <v>3830</v>
-      </c>
-      <c r="D1497">
-        <v>68000</v>
+        <v>3860</v>
+      </c>
+      <c r="D1497" t="s">
+        <v>3861</v>
       </c>
       <c r="E1497" t="s">
-        <v>154</v>
+        <v>725</v>
       </c>
       <c r="H1497" t="s">
-        <v>1492</v>
+        <v>2070</v>
       </c>
       <c r="M1497" t="s">
-        <v>3831</v>
+        <v>3862</v>
       </c>
     </row>
     <row r="1498" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1498">
-        <v>1645</v>
+        <v>1650</v>
       </c>
       <c r="B1498" t="s">
-        <v>3848</v>
+        <v>3863</v>
       </c>
       <c r="C1498" t="s">
-        <v>3849</v>
+        <v>3864</v>
       </c>
       <c r="D1498">
-        <v>8080</v>
+        <v>68000</v>
       </c>
       <c r="H1498" t="s">
-        <v>406</v>
+        <v>2375</v>
       </c>
       <c r="M1498" t="s">
-        <v>3850</v>
+        <v>3865</v>
       </c>
     </row>
     <row r="1499" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1499">
-        <v>1646</v>
+        <v>1651</v>
       </c>
       <c r="B1499" t="s">
-        <v>3851</v>
+        <v>3866</v>
       </c>
       <c r="C1499" t="s">
-        <v>3852</v>
-      </c>
-      <c r="D1499" t="s">
-        <v>1105</v>
+        <v>3867</v>
+      </c>
+      <c r="D1499">
+        <v>68000</v>
+      </c>
+      <c r="E1499" t="s">
+        <v>154</v>
       </c>
       <c r="H1499" t="s">
-        <v>336</v>
+        <v>1236</v>
       </c>
       <c r="M1499" t="s">
-        <v>3853</v>
+        <v>3868</v>
       </c>
     </row>
     <row r="1500" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1500">
-        <v>1647</v>
+        <v>1652</v>
       </c>
       <c r="B1500" t="s">
-        <v>3854</v>
+        <v>3869</v>
       </c>
       <c r="C1500" t="s">
-        <v>3855</v>
+        <v>3870</v>
       </c>
       <c r="D1500" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1500" t="s">
-        <v>154</v>
+        <v>405</v>
       </c>
       <c r="H1500" t="s">
-        <v>336</v>
+        <v>71</v>
       </c>
       <c r="M1500" t="s">
-        <v>3856</v>
+        <v>3871</v>
       </c>
     </row>
     <row r="1501" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1501">
-        <v>1648</v>
+        <v>1653</v>
       </c>
       <c r="B1501" t="s">
-        <v>3857</v>
+        <v>3872</v>
       </c>
       <c r="C1501" t="s">
-        <v>3855</v>
+        <v>3873</v>
       </c>
       <c r="D1501" t="s">
         <v>14</v>
       </c>
-      <c r="E1501" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1501" t="s">
-        <v>336</v>
-      </c>
       <c r="M1501" t="s">
-        <v>3858</v>
+        <v>4493</v>
       </c>
     </row>
     <row r="1502" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1502">
-        <v>1649</v>
+        <v>1654</v>
       </c>
       <c r="B1502" t="s">
-        <v>3859</v>
+        <v>3874</v>
       </c>
       <c r="C1502" t="s">
-        <v>3860</v>
-      </c>
-      <c r="D1502" t="s">
-        <v>3861</v>
+        <v>3875</v>
+      </c>
+      <c r="D1502">
+        <v>68000</v>
       </c>
       <c r="E1502" t="s">
-        <v>725</v>
+        <v>154</v>
       </c>
       <c r="H1502" t="s">
-        <v>2070</v>
+        <v>1353</v>
       </c>
       <c r="M1502" t="s">
-        <v>3862</v>
+        <v>3876</v>
       </c>
     </row>
     <row r="1503" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1503">
-        <v>1650</v>
+        <v>1655</v>
       </c>
       <c r="B1503" t="s">
-        <v>3863</v>
+        <v>3877</v>
       </c>
       <c r="C1503" t="s">
-        <v>3864</v>
+        <v>3875</v>
       </c>
       <c r="D1503">
         <v>68000</v>
       </c>
+      <c r="E1503" t="s">
+        <v>154</v>
+      </c>
       <c r="H1503" t="s">
-        <v>2375</v>
+        <v>1353</v>
       </c>
       <c r="M1503" t="s">
-        <v>3865</v>
+        <v>4494</v>
       </c>
     </row>
     <row r="1504" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1504">
-        <v>1651</v>
+        <v>1656</v>
       </c>
       <c r="B1504" t="s">
-        <v>3866</v>
+        <v>3878</v>
       </c>
       <c r="C1504" t="s">
-        <v>3867</v>
+        <v>3875</v>
       </c>
       <c r="D1504">
         <v>68000</v>
@@ -60986,55 +61092,64 @@
         <v>154</v>
       </c>
       <c r="H1504" t="s">
-        <v>1236</v>
+        <v>1353</v>
       </c>
       <c r="M1504" t="s">
-        <v>3868</v>
+        <v>3879</v>
       </c>
     </row>
     <row r="1505" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1505">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="B1505" t="s">
-        <v>3869</v>
+        <v>3880</v>
       </c>
       <c r="C1505" t="s">
-        <v>3870</v>
-      </c>
-      <c r="D1505" t="s">
-        <v>405</v>
+        <v>3875</v>
+      </c>
+      <c r="D1505">
+        <v>68000</v>
+      </c>
+      <c r="E1505" t="s">
+        <v>154</v>
       </c>
       <c r="H1505" t="s">
-        <v>71</v>
+        <v>1353</v>
       </c>
       <c r="M1505" t="s">
-        <v>3871</v>
+        <v>3881</v>
       </c>
     </row>
     <row r="1506" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1506">
-        <v>1653</v>
+        <v>1658</v>
       </c>
       <c r="B1506" t="s">
-        <v>3872</v>
+        <v>3882</v>
       </c>
       <c r="C1506" t="s">
-        <v>3873</v>
-      </c>
-      <c r="D1506" t="s">
-        <v>14</v>
+        <v>3875</v>
+      </c>
+      <c r="D1506">
+        <v>68000</v>
+      </c>
+      <c r="E1506" t="s">
+        <v>154</v>
+      </c>
+      <c r="H1506" t="s">
+        <v>1353</v>
       </c>
       <c r="M1506" t="s">
-        <v>4493</v>
+        <v>3883</v>
       </c>
     </row>
     <row r="1507" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1507">
-        <v>1654</v>
+        <v>1659</v>
       </c>
       <c r="B1507" t="s">
-        <v>3874</v>
+        <v>3884</v>
       </c>
       <c r="C1507" t="s">
         <v>3875</v>
@@ -61049,15 +61164,15 @@
         <v>1353</v>
       </c>
       <c r="M1507" t="s">
-        <v>3876</v>
+        <v>3885</v>
       </c>
     </row>
     <row r="1508" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1508">
-        <v>1655</v>
+        <v>1660</v>
       </c>
       <c r="B1508" t="s">
-        <v>3877</v>
+        <v>3886</v>
       </c>
       <c r="C1508" t="s">
         <v>3875</v>
@@ -61072,15 +61187,15 @@
         <v>1353</v>
       </c>
       <c r="M1508" t="s">
-        <v>4494</v>
+        <v>3887</v>
       </c>
     </row>
     <row r="1509" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1509">
-        <v>1656</v>
+        <v>1661</v>
       </c>
       <c r="B1509" t="s">
-        <v>3878</v>
+        <v>3888</v>
       </c>
       <c r="C1509" t="s">
         <v>3875</v>
@@ -61095,15 +61210,15 @@
         <v>1353</v>
       </c>
       <c r="M1509" t="s">
-        <v>3879</v>
+        <v>4495</v>
       </c>
     </row>
     <row r="1510" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1510">
-        <v>1657</v>
+        <v>1662</v>
       </c>
       <c r="B1510" t="s">
-        <v>3880</v>
+        <v>3889</v>
       </c>
       <c r="C1510" t="s">
         <v>3875</v>
@@ -61118,15 +61233,15 @@
         <v>1353</v>
       </c>
       <c r="M1510" t="s">
-        <v>3881</v>
+        <v>3890</v>
       </c>
     </row>
     <row r="1511" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1511">
-        <v>1658</v>
+        <v>1663</v>
       </c>
       <c r="B1511" t="s">
-        <v>3882</v>
+        <v>3891</v>
       </c>
       <c r="C1511" t="s">
         <v>3875</v>
@@ -61141,15 +61256,15 @@
         <v>1353</v>
       </c>
       <c r="M1511" t="s">
-        <v>3883</v>
+        <v>3892</v>
       </c>
     </row>
     <row r="1512" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1512">
-        <v>1659</v>
+        <v>1664</v>
       </c>
       <c r="B1512" t="s">
-        <v>3884</v>
+        <v>3893</v>
       </c>
       <c r="C1512" t="s">
         <v>3875</v>
@@ -61164,15 +61279,15 @@
         <v>1353</v>
       </c>
       <c r="M1512" t="s">
-        <v>3885</v>
+        <v>3894</v>
       </c>
     </row>
     <row r="1513" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1513">
-        <v>1660</v>
+        <v>1665</v>
       </c>
       <c r="B1513" t="s">
-        <v>3886</v>
+        <v>3895</v>
       </c>
       <c r="C1513" t="s">
         <v>3875</v>
@@ -61187,15 +61302,15 @@
         <v>1353</v>
       </c>
       <c r="M1513" t="s">
-        <v>3887</v>
+        <v>3896</v>
       </c>
     </row>
     <row r="1514" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1514">
-        <v>1661</v>
+        <v>1666</v>
       </c>
       <c r="B1514" t="s">
-        <v>3888</v>
+        <v>3897</v>
       </c>
       <c r="C1514" t="s">
         <v>3875</v>
@@ -61210,15 +61325,15 @@
         <v>1353</v>
       </c>
       <c r="M1514" t="s">
-        <v>4495</v>
+        <v>3898</v>
       </c>
     </row>
     <row r="1515" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1515">
-        <v>1662</v>
+        <v>1667</v>
       </c>
       <c r="B1515" t="s">
-        <v>3889</v>
+        <v>3899</v>
       </c>
       <c r="C1515" t="s">
         <v>3875</v>
@@ -61233,15 +61348,15 @@
         <v>1353</v>
       </c>
       <c r="M1515" t="s">
-        <v>3890</v>
+        <v>4496</v>
       </c>
     </row>
     <row r="1516" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1516">
-        <v>1663</v>
+        <v>1668</v>
       </c>
       <c r="B1516" t="s">
-        <v>3891</v>
+        <v>3900</v>
       </c>
       <c r="C1516" t="s">
         <v>3875</v>
@@ -61256,15 +61371,15 @@
         <v>1353</v>
       </c>
       <c r="M1516" t="s">
-        <v>3892</v>
+        <v>4497</v>
       </c>
     </row>
     <row r="1517" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1517">
-        <v>1664</v>
+        <v>1669</v>
       </c>
       <c r="B1517" t="s">
-        <v>3893</v>
+        <v>3901</v>
       </c>
       <c r="C1517" t="s">
         <v>3875</v>
@@ -61279,15 +61394,15 @@
         <v>1353</v>
       </c>
       <c r="M1517" t="s">
-        <v>3894</v>
+        <v>3902</v>
       </c>
     </row>
     <row r="1518" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1518">
-        <v>1665</v>
+        <v>1670</v>
       </c>
       <c r="B1518" t="s">
-        <v>3895</v>
+        <v>3903</v>
       </c>
       <c r="C1518" t="s">
         <v>3875</v>
@@ -61302,15 +61417,15 @@
         <v>1353</v>
       </c>
       <c r="M1518" t="s">
-        <v>3896</v>
+        <v>3904</v>
       </c>
     </row>
     <row r="1519" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1519">
-        <v>1666</v>
+        <v>1671</v>
       </c>
       <c r="B1519" t="s">
-        <v>3897</v>
+        <v>3905</v>
       </c>
       <c r="C1519" t="s">
         <v>3875</v>
@@ -61325,15 +61440,15 @@
         <v>1353</v>
       </c>
       <c r="M1519" t="s">
-        <v>3898</v>
+        <v>3906</v>
       </c>
     </row>
     <row r="1520" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1520">
-        <v>1667</v>
+        <v>1672</v>
       </c>
       <c r="B1520" t="s">
-        <v>3899</v>
+        <v>3907</v>
       </c>
       <c r="C1520" t="s">
         <v>3875</v>
@@ -61348,15 +61463,15 @@
         <v>1353</v>
       </c>
       <c r="M1520" t="s">
-        <v>4496</v>
+        <v>3908</v>
       </c>
     </row>
     <row r="1521" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1521">
-        <v>1668</v>
+        <v>1673</v>
       </c>
       <c r="B1521" t="s">
-        <v>3900</v>
+        <v>3909</v>
       </c>
       <c r="C1521" t="s">
         <v>3875</v>
@@ -61371,15 +61486,15 @@
         <v>1353</v>
       </c>
       <c r="M1521" t="s">
-        <v>4497</v>
+        <v>3910</v>
       </c>
     </row>
     <row r="1522" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1522">
-        <v>1669</v>
+        <v>1674</v>
       </c>
       <c r="B1522" t="s">
-        <v>3901</v>
+        <v>3911</v>
       </c>
       <c r="C1522" t="s">
         <v>3875</v>
@@ -61394,15 +61509,15 @@
         <v>1353</v>
       </c>
       <c r="M1522" t="s">
-        <v>3902</v>
+        <v>3912</v>
       </c>
     </row>
     <row r="1523" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1523">
-        <v>1670</v>
+        <v>1675</v>
       </c>
       <c r="B1523" t="s">
-        <v>3903</v>
+        <v>3913</v>
       </c>
       <c r="C1523" t="s">
         <v>3875</v>
@@ -61417,15 +61532,15 @@
         <v>1353</v>
       </c>
       <c r="M1523" t="s">
-        <v>3904</v>
+        <v>4498</v>
       </c>
     </row>
     <row r="1524" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1524">
-        <v>1671</v>
+        <v>1676</v>
       </c>
       <c r="B1524" t="s">
-        <v>3905</v>
+        <v>3914</v>
       </c>
       <c r="C1524" t="s">
         <v>3875</v>
@@ -61440,15 +61555,15 @@
         <v>1353</v>
       </c>
       <c r="M1524" t="s">
-        <v>3906</v>
+        <v>3915</v>
       </c>
     </row>
     <row r="1525" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1525">
-        <v>1672</v>
+        <v>1677</v>
       </c>
       <c r="B1525" t="s">
-        <v>3907</v>
+        <v>3916</v>
       </c>
       <c r="C1525" t="s">
         <v>3875</v>
@@ -61463,15 +61578,15 @@
         <v>1353</v>
       </c>
       <c r="M1525" t="s">
-        <v>3908</v>
+        <v>3917</v>
       </c>
     </row>
     <row r="1526" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1526">
-        <v>1673</v>
+        <v>1678</v>
       </c>
       <c r="B1526" t="s">
-        <v>3909</v>
+        <v>3918</v>
       </c>
       <c r="C1526" t="s">
         <v>3875</v>
@@ -61486,15 +61601,15 @@
         <v>1353</v>
       </c>
       <c r="M1526" t="s">
-        <v>3910</v>
+        <v>3919</v>
       </c>
     </row>
     <row r="1527" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1527">
-        <v>1674</v>
+        <v>1679</v>
       </c>
       <c r="B1527" t="s">
-        <v>3911</v>
+        <v>3920</v>
       </c>
       <c r="C1527" t="s">
         <v>3875</v>
@@ -61509,15 +61624,15 @@
         <v>1353</v>
       </c>
       <c r="M1527" t="s">
-        <v>3912</v>
+        <v>4499</v>
       </c>
     </row>
     <row r="1528" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1528">
-        <v>1675</v>
+        <v>1680</v>
       </c>
       <c r="B1528" t="s">
-        <v>3913</v>
+        <v>3921</v>
       </c>
       <c r="C1528" t="s">
         <v>3875</v>
@@ -61532,15 +61647,15 @@
         <v>1353</v>
       </c>
       <c r="M1528" t="s">
-        <v>4498</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="1529" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1529">
-        <v>1676</v>
+        <v>1681</v>
       </c>
       <c r="B1529" t="s">
-        <v>3914</v>
+        <v>3922</v>
       </c>
       <c r="C1529" t="s">
         <v>3875</v>
@@ -61555,15 +61670,15 @@
         <v>1353</v>
       </c>
       <c r="M1529" t="s">
-        <v>3915</v>
+        <v>4501</v>
       </c>
     </row>
     <row r="1530" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1530">
-        <v>1677</v>
+        <v>1682</v>
       </c>
       <c r="B1530" t="s">
-        <v>3916</v>
+        <v>3923</v>
       </c>
       <c r="C1530" t="s">
         <v>3875</v>
@@ -61578,15 +61693,15 @@
         <v>1353</v>
       </c>
       <c r="M1530" t="s">
-        <v>3917</v>
+        <v>3924</v>
       </c>
     </row>
     <row r="1531" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1531">
-        <v>1678</v>
+        <v>1683</v>
       </c>
       <c r="B1531" t="s">
-        <v>3918</v>
+        <v>3925</v>
       </c>
       <c r="C1531" t="s">
         <v>3875</v>
@@ -61601,15 +61716,15 @@
         <v>1353</v>
       </c>
       <c r="M1531" t="s">
-        <v>3919</v>
+        <v>3926</v>
       </c>
     </row>
     <row r="1532" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1532">
-        <v>1679</v>
+        <v>1684</v>
       </c>
       <c r="B1532" t="s">
-        <v>3920</v>
+        <v>3927</v>
       </c>
       <c r="C1532" t="s">
         <v>3875</v>
@@ -61624,15 +61739,15 @@
         <v>1353</v>
       </c>
       <c r="M1532" t="s">
-        <v>4499</v>
+        <v>4502</v>
       </c>
     </row>
     <row r="1533" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1533">
-        <v>1680</v>
+        <v>1685</v>
       </c>
       <c r="B1533" t="s">
-        <v>3921</v>
+        <v>3928</v>
       </c>
       <c r="C1533" t="s">
         <v>3875</v>
@@ -61647,15 +61762,15 @@
         <v>1353</v>
       </c>
       <c r="M1533" t="s">
-        <v>4500</v>
+        <v>3929</v>
       </c>
     </row>
     <row r="1534" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1534">
-        <v>1681</v>
+        <v>1686</v>
       </c>
       <c r="B1534" t="s">
-        <v>3922</v>
+        <v>3930</v>
       </c>
       <c r="C1534" t="s">
         <v>3875</v>
@@ -61670,15 +61785,15 @@
         <v>1353</v>
       </c>
       <c r="M1534" t="s">
-        <v>4501</v>
+        <v>4503</v>
       </c>
     </row>
     <row r="1535" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1535">
-        <v>1682</v>
+        <v>1687</v>
       </c>
       <c r="B1535" t="s">
-        <v>3923</v>
+        <v>3931</v>
       </c>
       <c r="C1535" t="s">
         <v>3875</v>
@@ -61693,15 +61808,15 @@
         <v>1353</v>
       </c>
       <c r="M1535" t="s">
-        <v>3924</v>
+        <v>3932</v>
       </c>
     </row>
     <row r="1536" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1536">
-        <v>1683</v>
+        <v>1688</v>
       </c>
       <c r="B1536" t="s">
-        <v>3925</v>
+        <v>3933</v>
       </c>
       <c r="C1536" t="s">
         <v>3875</v>
@@ -61716,15 +61831,15 @@
         <v>1353</v>
       </c>
       <c r="M1536" t="s">
-        <v>3926</v>
+        <v>3934</v>
       </c>
     </row>
     <row r="1537" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1537">
-        <v>1684</v>
+        <v>1689</v>
       </c>
       <c r="B1537" t="s">
-        <v>3927</v>
+        <v>3935</v>
       </c>
       <c r="C1537" t="s">
         <v>3875</v>
@@ -61739,15 +61854,15 @@
         <v>1353</v>
       </c>
       <c r="M1537" t="s">
-        <v>4502</v>
+        <v>4504</v>
       </c>
     </row>
     <row r="1538" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1538">
-        <v>1685</v>
+        <v>1690</v>
       </c>
       <c r="B1538" t="s">
-        <v>3928</v>
+        <v>3936</v>
       </c>
       <c r="C1538" t="s">
         <v>3875</v>
@@ -61762,15 +61877,15 @@
         <v>1353</v>
       </c>
       <c r="M1538" t="s">
-        <v>3929</v>
+        <v>4505</v>
       </c>
     </row>
     <row r="1539" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1539">
-        <v>1686</v>
+        <v>1691</v>
       </c>
       <c r="B1539" t="s">
-        <v>3930</v>
+        <v>3937</v>
       </c>
       <c r="C1539" t="s">
         <v>3875</v>
@@ -61785,15 +61900,15 @@
         <v>1353</v>
       </c>
       <c r="M1539" t="s">
-        <v>4503</v>
+        <v>3938</v>
       </c>
     </row>
     <row r="1540" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1540">
-        <v>1687</v>
+        <v>1692</v>
       </c>
       <c r="B1540" t="s">
-        <v>3931</v>
+        <v>3939</v>
       </c>
       <c r="C1540" t="s">
         <v>3875</v>
@@ -61808,15 +61923,15 @@
         <v>1353</v>
       </c>
       <c r="M1540" t="s">
-        <v>3932</v>
+        <v>4506</v>
       </c>
     </row>
     <row r="1541" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1541">
-        <v>1688</v>
+        <v>1693</v>
       </c>
       <c r="B1541" t="s">
-        <v>3933</v>
+        <v>3940</v>
       </c>
       <c r="C1541" t="s">
         <v>3875</v>
@@ -61831,15 +61946,15 @@
         <v>1353</v>
       </c>
       <c r="M1541" t="s">
-        <v>3934</v>
+        <v>4507</v>
       </c>
     </row>
     <row r="1542" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1542">
-        <v>1689</v>
+        <v>1694</v>
       </c>
       <c r="B1542" t="s">
-        <v>3935</v>
+        <v>3941</v>
       </c>
       <c r="C1542" t="s">
         <v>3875</v>
@@ -61854,15 +61969,15 @@
         <v>1353</v>
       </c>
       <c r="M1542" t="s">
-        <v>4504</v>
+        <v>4508</v>
       </c>
     </row>
     <row r="1543" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1543">
-        <v>1690</v>
+        <v>1695</v>
       </c>
       <c r="B1543" t="s">
-        <v>3936</v>
+        <v>3942</v>
       </c>
       <c r="C1543" t="s">
         <v>3875</v>
@@ -61877,15 +61992,15 @@
         <v>1353</v>
       </c>
       <c r="M1543" t="s">
-        <v>4505</v>
+        <v>4509</v>
       </c>
     </row>
     <row r="1544" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1544">
-        <v>1691</v>
+        <v>1696</v>
       </c>
       <c r="B1544" t="s">
-        <v>3937</v>
+        <v>3943</v>
       </c>
       <c r="C1544" t="s">
         <v>3875</v>
@@ -61900,15 +62015,15 @@
         <v>1353</v>
       </c>
       <c r="M1544" t="s">
-        <v>3938</v>
+        <v>4510</v>
       </c>
     </row>
     <row r="1545" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1545">
-        <v>1692</v>
+        <v>1697</v>
       </c>
       <c r="B1545" t="s">
-        <v>3939</v>
+        <v>3944</v>
       </c>
       <c r="C1545" t="s">
         <v>3875</v>
@@ -61923,15 +62038,15 @@
         <v>1353</v>
       </c>
       <c r="M1545" t="s">
-        <v>4506</v>
+        <v>4511</v>
       </c>
     </row>
     <row r="1546" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1546">
-        <v>1693</v>
+        <v>1698</v>
       </c>
       <c r="B1546" t="s">
-        <v>3940</v>
+        <v>3945</v>
       </c>
       <c r="C1546" t="s">
         <v>3875</v>
@@ -61946,15 +62061,15 @@
         <v>1353</v>
       </c>
       <c r="M1546" t="s">
-        <v>4507</v>
+        <v>4512</v>
       </c>
     </row>
     <row r="1547" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1547">
-        <v>1694</v>
+        <v>1699</v>
       </c>
       <c r="B1547" t="s">
-        <v>3941</v>
+        <v>3946</v>
       </c>
       <c r="C1547" t="s">
         <v>3875</v>
@@ -61969,15 +62084,15 @@
         <v>1353</v>
       </c>
       <c r="M1547" t="s">
-        <v>4508</v>
+        <v>3947</v>
       </c>
     </row>
     <row r="1548" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1548">
-        <v>1695</v>
+        <v>1700</v>
       </c>
       <c r="B1548" t="s">
-        <v>3942</v>
+        <v>3948</v>
       </c>
       <c r="C1548" t="s">
         <v>3875</v>
@@ -61992,15 +62107,15 @@
         <v>1353</v>
       </c>
       <c r="M1548" t="s">
-        <v>4509</v>
+        <v>3949</v>
       </c>
     </row>
     <row r="1549" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1549">
-        <v>1696</v>
+        <v>1701</v>
       </c>
       <c r="B1549" t="s">
-        <v>3943</v>
+        <v>3950</v>
       </c>
       <c r="C1549" t="s">
         <v>3875</v>
@@ -62015,15 +62130,15 @@
         <v>1353</v>
       </c>
       <c r="M1549" t="s">
-        <v>4510</v>
+        <v>3951</v>
       </c>
     </row>
     <row r="1550" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1550">
-        <v>1697</v>
+        <v>1702</v>
       </c>
       <c r="B1550" t="s">
-        <v>3944</v>
+        <v>3952</v>
       </c>
       <c r="C1550" t="s">
         <v>3875</v>
@@ -62038,15 +62153,15 @@
         <v>1353</v>
       </c>
       <c r="M1550" t="s">
-        <v>4511</v>
+        <v>4513</v>
       </c>
     </row>
     <row r="1551" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1551">
-        <v>1698</v>
+        <v>1703</v>
       </c>
       <c r="B1551" t="s">
-        <v>3945</v>
+        <v>3953</v>
       </c>
       <c r="C1551" t="s">
         <v>3875</v>
@@ -62061,15 +62176,15 @@
         <v>1353</v>
       </c>
       <c r="M1551" t="s">
-        <v>4512</v>
+        <v>3954</v>
       </c>
     </row>
     <row r="1552" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1552">
-        <v>1699</v>
+        <v>1704</v>
       </c>
       <c r="B1552" t="s">
-        <v>3946</v>
+        <v>3955</v>
       </c>
       <c r="C1552" t="s">
         <v>3875</v>
@@ -62084,15 +62199,15 @@
         <v>1353</v>
       </c>
       <c r="M1552" t="s">
-        <v>3947</v>
+        <v>3956</v>
       </c>
     </row>
     <row r="1553" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1553">
-        <v>1700</v>
+        <v>1705</v>
       </c>
       <c r="B1553" t="s">
-        <v>3948</v>
+        <v>3957</v>
       </c>
       <c r="C1553" t="s">
         <v>3875</v>
@@ -62107,15 +62222,15 @@
         <v>1353</v>
       </c>
       <c r="M1553" t="s">
-        <v>3949</v>
+        <v>4514</v>
       </c>
     </row>
     <row r="1554" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1554">
-        <v>1701</v>
+        <v>1706</v>
       </c>
       <c r="B1554" t="s">
-        <v>3950</v>
+        <v>3958</v>
       </c>
       <c r="C1554" t="s">
         <v>3875</v>
@@ -62130,15 +62245,15 @@
         <v>1353</v>
       </c>
       <c r="M1554" t="s">
-        <v>3951</v>
+        <v>3959</v>
       </c>
     </row>
     <row r="1555" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1555">
-        <v>1702</v>
+        <v>1707</v>
       </c>
       <c r="B1555" t="s">
-        <v>3952</v>
+        <v>3960</v>
       </c>
       <c r="C1555" t="s">
         <v>3875</v>
@@ -62153,15 +62268,15 @@
         <v>1353</v>
       </c>
       <c r="M1555" t="s">
-        <v>4513</v>
+        <v>4515</v>
       </c>
     </row>
     <row r="1556" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1556">
-        <v>1703</v>
+        <v>1708</v>
       </c>
       <c r="B1556" t="s">
-        <v>3953</v>
+        <v>3961</v>
       </c>
       <c r="C1556" t="s">
         <v>3875</v>
@@ -62176,15 +62291,15 @@
         <v>1353</v>
       </c>
       <c r="M1556" t="s">
-        <v>3954</v>
+        <v>4516</v>
       </c>
     </row>
     <row r="1557" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1557">
-        <v>1704</v>
+        <v>1709</v>
       </c>
       <c r="B1557" t="s">
-        <v>3955</v>
+        <v>3962</v>
       </c>
       <c r="C1557" t="s">
         <v>3875</v>
@@ -62199,15 +62314,15 @@
         <v>1353</v>
       </c>
       <c r="M1557" t="s">
-        <v>3956</v>
+        <v>4517</v>
       </c>
     </row>
     <row r="1558" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1558">
-        <v>1705</v>
+        <v>1710</v>
       </c>
       <c r="B1558" t="s">
-        <v>3957</v>
+        <v>3963</v>
       </c>
       <c r="C1558" t="s">
         <v>3875</v>
@@ -62222,15 +62337,15 @@
         <v>1353</v>
       </c>
       <c r="M1558" t="s">
-        <v>4514</v>
+        <v>4518</v>
       </c>
     </row>
     <row r="1559" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1559">
-        <v>1706</v>
+        <v>1711</v>
       </c>
       <c r="B1559" t="s">
-        <v>3958</v>
+        <v>3964</v>
       </c>
       <c r="C1559" t="s">
         <v>3875</v>
@@ -62245,15 +62360,15 @@
         <v>1353</v>
       </c>
       <c r="M1559" t="s">
-        <v>3959</v>
+        <v>4519</v>
       </c>
     </row>
     <row r="1560" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1560">
-        <v>1707</v>
+        <v>1712</v>
       </c>
       <c r="B1560" t="s">
-        <v>3960</v>
+        <v>3965</v>
       </c>
       <c r="C1560" t="s">
         <v>3875</v>
@@ -62268,15 +62383,15 @@
         <v>1353</v>
       </c>
       <c r="M1560" t="s">
-        <v>4515</v>
+        <v>4520</v>
       </c>
     </row>
     <row r="1561" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1561">
-        <v>1708</v>
+        <v>1713</v>
       </c>
       <c r="B1561" t="s">
-        <v>3961</v>
+        <v>3966</v>
       </c>
       <c r="C1561" t="s">
         <v>3875</v>
@@ -62291,15 +62406,15 @@
         <v>1353</v>
       </c>
       <c r="M1561" t="s">
-        <v>4516</v>
+        <v>3967</v>
       </c>
     </row>
     <row r="1562" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1562">
-        <v>1709</v>
+        <v>1714</v>
       </c>
       <c r="B1562" t="s">
-        <v>3962</v>
+        <v>3968</v>
       </c>
       <c r="C1562" t="s">
         <v>3875</v>
@@ -62314,15 +62429,15 @@
         <v>1353</v>
       </c>
       <c r="M1562" t="s">
-        <v>4517</v>
+        <v>4521</v>
       </c>
     </row>
     <row r="1563" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1563">
-        <v>1710</v>
+        <v>1715</v>
       </c>
       <c r="B1563" t="s">
-        <v>3963</v>
+        <v>3969</v>
       </c>
       <c r="C1563" t="s">
         <v>3875</v>
@@ -62337,15 +62452,15 @@
         <v>1353</v>
       </c>
       <c r="M1563" t="s">
-        <v>4518</v>
+        <v>4522</v>
       </c>
     </row>
     <row r="1564" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1564">
-        <v>1711</v>
+        <v>1716</v>
       </c>
       <c r="B1564" t="s">
-        <v>3964</v>
+        <v>3970</v>
       </c>
       <c r="C1564" t="s">
         <v>3875</v>
@@ -62360,15 +62475,15 @@
         <v>1353</v>
       </c>
       <c r="M1564" t="s">
-        <v>4519</v>
+        <v>3971</v>
       </c>
     </row>
     <row r="1565" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1565">
-        <v>1712</v>
+        <v>1717</v>
       </c>
       <c r="B1565" t="s">
-        <v>3965</v>
+        <v>3972</v>
       </c>
       <c r="C1565" t="s">
         <v>3875</v>
@@ -62383,15 +62498,15 @@
         <v>1353</v>
       </c>
       <c r="M1565" t="s">
-        <v>4520</v>
+        <v>3973</v>
       </c>
     </row>
     <row r="1566" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1566">
-        <v>1713</v>
+        <v>1718</v>
       </c>
       <c r="B1566" t="s">
-        <v>3966</v>
+        <v>3974</v>
       </c>
       <c r="C1566" t="s">
         <v>3875</v>
@@ -62406,15 +62521,15 @@
         <v>1353</v>
       </c>
       <c r="M1566" t="s">
-        <v>3967</v>
+        <v>4523</v>
       </c>
     </row>
     <row r="1567" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1567">
-        <v>1714</v>
+        <v>1719</v>
       </c>
       <c r="B1567" t="s">
-        <v>3968</v>
+        <v>3975</v>
       </c>
       <c r="C1567" t="s">
         <v>3875</v>
@@ -62429,15 +62544,15 @@
         <v>1353</v>
       </c>
       <c r="M1567" t="s">
-        <v>4521</v>
+        <v>3976</v>
       </c>
     </row>
     <row r="1568" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1568">
-        <v>1715</v>
+        <v>1720</v>
       </c>
       <c r="B1568" t="s">
-        <v>3969</v>
+        <v>3977</v>
       </c>
       <c r="C1568" t="s">
         <v>3875</v>
@@ -62452,15 +62567,15 @@
         <v>1353</v>
       </c>
       <c r="M1568" t="s">
-        <v>4522</v>
+        <v>4524</v>
       </c>
     </row>
     <row r="1569" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1569">
-        <v>1716</v>
+        <v>1721</v>
       </c>
       <c r="B1569" t="s">
-        <v>3970</v>
+        <v>3978</v>
       </c>
       <c r="C1569" t="s">
         <v>3875</v>
@@ -62475,15 +62590,15 @@
         <v>1353</v>
       </c>
       <c r="M1569" t="s">
-        <v>3971</v>
+        <v>4525</v>
       </c>
     </row>
     <row r="1570" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1570">
-        <v>1717</v>
+        <v>1722</v>
       </c>
       <c r="B1570" t="s">
-        <v>3972</v>
+        <v>3979</v>
       </c>
       <c r="C1570" t="s">
         <v>3875</v>
@@ -62498,15 +62613,15 @@
         <v>1353</v>
       </c>
       <c r="M1570" t="s">
-        <v>3973</v>
+        <v>4526</v>
       </c>
     </row>
     <row r="1571" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1571">
-        <v>1718</v>
+        <v>1723</v>
       </c>
       <c r="B1571" t="s">
-        <v>3974</v>
+        <v>3980</v>
       </c>
       <c r="C1571" t="s">
         <v>3875</v>
@@ -62521,15 +62636,15 @@
         <v>1353</v>
       </c>
       <c r="M1571" t="s">
-        <v>4523</v>
+        <v>4527</v>
       </c>
     </row>
     <row r="1572" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1572">
-        <v>1719</v>
+        <v>1724</v>
       </c>
       <c r="B1572" t="s">
-        <v>3975</v>
+        <v>3981</v>
       </c>
       <c r="C1572" t="s">
         <v>3875</v>
@@ -62544,15 +62659,15 @@
         <v>1353</v>
       </c>
       <c r="M1572" t="s">
-        <v>3976</v>
+        <v>4528</v>
       </c>
     </row>
     <row r="1573" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1573">
-        <v>1720</v>
+        <v>1725</v>
       </c>
       <c r="B1573" t="s">
-        <v>3977</v>
+        <v>3982</v>
       </c>
       <c r="C1573" t="s">
         <v>3875</v>
@@ -62567,15 +62682,15 @@
         <v>1353</v>
       </c>
       <c r="M1573" t="s">
-        <v>4524</v>
+        <v>3983</v>
       </c>
     </row>
     <row r="1574" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1574">
-        <v>1721</v>
+        <v>1726</v>
       </c>
       <c r="B1574" t="s">
-        <v>3978</v>
+        <v>3984</v>
       </c>
       <c r="C1574" t="s">
         <v>3875</v>
@@ -62590,15 +62705,15 @@
         <v>1353</v>
       </c>
       <c r="M1574" t="s">
-        <v>4525</v>
+        <v>4529</v>
       </c>
     </row>
     <row r="1575" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1575">
-        <v>1722</v>
+        <v>1727</v>
       </c>
       <c r="B1575" t="s">
-        <v>3979</v>
+        <v>3985</v>
       </c>
       <c r="C1575" t="s">
         <v>3875</v>
@@ -62613,15 +62728,15 @@
         <v>1353</v>
       </c>
       <c r="M1575" t="s">
-        <v>4526</v>
+        <v>3986</v>
       </c>
     </row>
     <row r="1576" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1576">
-        <v>1723</v>
+        <v>1728</v>
       </c>
       <c r="B1576" t="s">
-        <v>3980</v>
+        <v>3987</v>
       </c>
       <c r="C1576" t="s">
         <v>3875</v>
@@ -62636,15 +62751,15 @@
         <v>1353</v>
       </c>
       <c r="M1576" t="s">
-        <v>4527</v>
+        <v>4530</v>
       </c>
     </row>
     <row r="1577" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1577">
-        <v>1724</v>
+        <v>1729</v>
       </c>
       <c r="B1577" t="s">
-        <v>3981</v>
+        <v>3988</v>
       </c>
       <c r="C1577" t="s">
         <v>3875</v>
@@ -62659,15 +62774,15 @@
         <v>1353</v>
       </c>
       <c r="M1577" t="s">
-        <v>4528</v>
+        <v>3989</v>
       </c>
     </row>
     <row r="1578" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1578">
-        <v>1725</v>
+        <v>1730</v>
       </c>
       <c r="B1578" t="s">
-        <v>3982</v>
+        <v>3990</v>
       </c>
       <c r="C1578" t="s">
         <v>3875</v>
@@ -62682,15 +62797,15 @@
         <v>1353</v>
       </c>
       <c r="M1578" t="s">
-        <v>3983</v>
+        <v>3991</v>
       </c>
     </row>
     <row r="1579" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1579">
-        <v>1726</v>
+        <v>1731</v>
       </c>
       <c r="B1579" t="s">
-        <v>3984</v>
+        <v>3992</v>
       </c>
       <c r="C1579" t="s">
         <v>3875</v>
@@ -62705,15 +62820,15 @@
         <v>1353</v>
       </c>
       <c r="M1579" t="s">
-        <v>4529</v>
+        <v>4531</v>
       </c>
     </row>
     <row r="1580" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1580">
-        <v>1727</v>
+        <v>1732</v>
       </c>
       <c r="B1580" t="s">
-        <v>3985</v>
+        <v>3993</v>
       </c>
       <c r="C1580" t="s">
         <v>3875</v>
@@ -62728,15 +62843,15 @@
         <v>1353</v>
       </c>
       <c r="M1580" t="s">
-        <v>3986</v>
+        <v>4532</v>
       </c>
     </row>
     <row r="1581" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1581">
-        <v>1728</v>
+        <v>1733</v>
       </c>
       <c r="B1581" t="s">
-        <v>3987</v>
+        <v>3994</v>
       </c>
       <c r="C1581" t="s">
         <v>3875</v>
@@ -62751,15 +62866,15 @@
         <v>1353</v>
       </c>
       <c r="M1581" t="s">
-        <v>4530</v>
+        <v>3995</v>
       </c>
     </row>
     <row r="1582" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1582">
-        <v>1729</v>
+        <v>1734</v>
       </c>
       <c r="B1582" t="s">
-        <v>3988</v>
+        <v>3996</v>
       </c>
       <c r="C1582" t="s">
         <v>3875</v>
@@ -62774,15 +62889,15 @@
         <v>1353</v>
       </c>
       <c r="M1582" t="s">
-        <v>3989</v>
+        <v>3997</v>
       </c>
     </row>
     <row r="1583" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1583">
-        <v>1730</v>
+        <v>1735</v>
       </c>
       <c r="B1583" t="s">
-        <v>3990</v>
+        <v>3998</v>
       </c>
       <c r="C1583" t="s">
         <v>3875</v>
@@ -62797,15 +62912,15 @@
         <v>1353</v>
       </c>
       <c r="M1583" t="s">
-        <v>3991</v>
+        <v>4533</v>
       </c>
     </row>
     <row r="1584" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1584">
-        <v>1731</v>
+        <v>1736</v>
       </c>
       <c r="B1584" t="s">
-        <v>3992</v>
+        <v>3999</v>
       </c>
       <c r="C1584" t="s">
         <v>3875</v>
@@ -62820,15 +62935,15 @@
         <v>1353</v>
       </c>
       <c r="M1584" t="s">
-        <v>4531</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="1585" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1585">
-        <v>1732</v>
+        <v>1737</v>
       </c>
       <c r="B1585" t="s">
-        <v>3993</v>
+        <v>4001</v>
       </c>
       <c r="C1585" t="s">
         <v>3875</v>
@@ -62843,15 +62958,15 @@
         <v>1353</v>
       </c>
       <c r="M1585" t="s">
-        <v>4532</v>
+        <v>4534</v>
       </c>
     </row>
     <row r="1586" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1586">
-        <v>1733</v>
+        <v>1738</v>
       </c>
       <c r="B1586" t="s">
-        <v>3994</v>
+        <v>4002</v>
       </c>
       <c r="C1586" t="s">
         <v>3875</v>
@@ -62866,15 +62981,15 @@
         <v>1353</v>
       </c>
       <c r="M1586" t="s">
-        <v>3995</v>
+        <v>4535</v>
       </c>
     </row>
     <row r="1587" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1587">
-        <v>1734</v>
+        <v>1739</v>
       </c>
       <c r="B1587" t="s">
-        <v>3996</v>
+        <v>4003</v>
       </c>
       <c r="C1587" t="s">
         <v>3875</v>
@@ -62889,15 +63004,15 @@
         <v>1353</v>
       </c>
       <c r="M1587" t="s">
-        <v>3997</v>
+        <v>4536</v>
       </c>
     </row>
     <row r="1588" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1588">
-        <v>1735</v>
+        <v>1740</v>
       </c>
       <c r="B1588" t="s">
-        <v>3998</v>
+        <v>4004</v>
       </c>
       <c r="C1588" t="s">
         <v>3875</v>
@@ -62912,15 +63027,15 @@
         <v>1353</v>
       </c>
       <c r="M1588" t="s">
-        <v>4533</v>
+        <v>4537</v>
       </c>
     </row>
     <row r="1589" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1589">
-        <v>1736</v>
+        <v>1741</v>
       </c>
       <c r="B1589" t="s">
-        <v>3999</v>
+        <v>4005</v>
       </c>
       <c r="C1589" t="s">
         <v>3875</v>
@@ -62935,15 +63050,15 @@
         <v>1353</v>
       </c>
       <c r="M1589" t="s">
-        <v>4000</v>
+        <v>4538</v>
       </c>
     </row>
     <row r="1590" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1590">
-        <v>1737</v>
+        <v>1742</v>
       </c>
       <c r="B1590" t="s">
-        <v>4001</v>
+        <v>4006</v>
       </c>
       <c r="C1590" t="s">
         <v>3875</v>
@@ -62958,15 +63073,15 @@
         <v>1353</v>
       </c>
       <c r="M1590" t="s">
-        <v>4534</v>
+        <v>4539</v>
       </c>
     </row>
     <row r="1591" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1591">
-        <v>1738</v>
+        <v>1743</v>
       </c>
       <c r="B1591" t="s">
-        <v>4002</v>
+        <v>4007</v>
       </c>
       <c r="C1591" t="s">
         <v>3875</v>
@@ -62981,15 +63096,15 @@
         <v>1353</v>
       </c>
       <c r="M1591" t="s">
-        <v>4535</v>
+        <v>4008</v>
       </c>
     </row>
     <row r="1592" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1592">
-        <v>1739</v>
+        <v>1744</v>
       </c>
       <c r="B1592" t="s">
-        <v>4003</v>
+        <v>4009</v>
       </c>
       <c r="C1592" t="s">
         <v>3875</v>
@@ -63004,15 +63119,15 @@
         <v>1353</v>
       </c>
       <c r="M1592" t="s">
-        <v>4536</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="1593" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1593">
-        <v>1740</v>
+        <v>1745</v>
       </c>
       <c r="B1593" t="s">
-        <v>4004</v>
+        <v>4010</v>
       </c>
       <c r="C1593" t="s">
         <v>3875</v>
@@ -63027,15 +63142,15 @@
         <v>1353</v>
       </c>
       <c r="M1593" t="s">
-        <v>4537</v>
+        <v>4541</v>
       </c>
     </row>
     <row r="1594" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1594">
-        <v>1741</v>
+        <v>1746</v>
       </c>
       <c r="B1594" t="s">
-        <v>4005</v>
+        <v>4011</v>
       </c>
       <c r="C1594" t="s">
         <v>3875</v>
@@ -63050,15 +63165,15 @@
         <v>1353</v>
       </c>
       <c r="M1594" t="s">
-        <v>4538</v>
+        <v>4012</v>
       </c>
     </row>
     <row r="1595" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1595">
-        <v>1742</v>
+        <v>1747</v>
       </c>
       <c r="B1595" t="s">
-        <v>4006</v>
+        <v>4013</v>
       </c>
       <c r="C1595" t="s">
         <v>3875</v>
@@ -63073,15 +63188,15 @@
         <v>1353</v>
       </c>
       <c r="M1595" t="s">
-        <v>4539</v>
+        <v>4542</v>
       </c>
     </row>
     <row r="1596" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1596">
-        <v>1743</v>
+        <v>1748</v>
       </c>
       <c r="B1596" t="s">
-        <v>4007</v>
+        <v>4014</v>
       </c>
       <c r="C1596" t="s">
         <v>3875</v>
@@ -63096,15 +63211,15 @@
         <v>1353</v>
       </c>
       <c r="M1596" t="s">
-        <v>4008</v>
+        <v>4015</v>
       </c>
     </row>
     <row r="1597" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1597">
-        <v>1744</v>
+        <v>1749</v>
       </c>
       <c r="B1597" t="s">
-        <v>4009</v>
+        <v>4016</v>
       </c>
       <c r="C1597" t="s">
         <v>3875</v>
@@ -63119,15 +63234,15 @@
         <v>1353</v>
       </c>
       <c r="M1597" t="s">
-        <v>4540</v>
+        <v>4017</v>
       </c>
     </row>
     <row r="1598" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1598">
-        <v>1745</v>
+        <v>1750</v>
       </c>
       <c r="B1598" t="s">
-        <v>4010</v>
+        <v>4018</v>
       </c>
       <c r="C1598" t="s">
         <v>3875</v>
@@ -63142,15 +63257,15 @@
         <v>1353</v>
       </c>
       <c r="M1598" t="s">
-        <v>4541</v>
+        <v>4543</v>
       </c>
     </row>
     <row r="1599" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1599">
-        <v>1746</v>
+        <v>1751</v>
       </c>
       <c r="B1599" t="s">
-        <v>4011</v>
+        <v>4019</v>
       </c>
       <c r="C1599" t="s">
         <v>3875</v>
@@ -63165,15 +63280,15 @@
         <v>1353</v>
       </c>
       <c r="M1599" t="s">
-        <v>4012</v>
+        <v>4020</v>
       </c>
     </row>
     <row r="1600" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1600">
-        <v>1747</v>
+        <v>1752</v>
       </c>
       <c r="B1600" t="s">
-        <v>4013</v>
+        <v>4021</v>
       </c>
       <c r="C1600" t="s">
         <v>3875</v>
@@ -63188,15 +63303,15 @@
         <v>1353</v>
       </c>
       <c r="M1600" t="s">
-        <v>4542</v>
+        <v>4544</v>
       </c>
     </row>
     <row r="1601" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1601">
-        <v>1748</v>
+        <v>1753</v>
       </c>
       <c r="B1601" t="s">
-        <v>4014</v>
+        <v>4022</v>
       </c>
       <c r="C1601" t="s">
         <v>3875</v>
@@ -63211,15 +63326,15 @@
         <v>1353</v>
       </c>
       <c r="M1601" t="s">
-        <v>4015</v>
+        <v>4545</v>
       </c>
     </row>
     <row r="1602" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1602">
-        <v>1749</v>
+        <v>1754</v>
       </c>
       <c r="B1602" t="s">
-        <v>4016</v>
+        <v>4023</v>
       </c>
       <c r="C1602" t="s">
         <v>3875</v>
@@ -63234,15 +63349,15 @@
         <v>1353</v>
       </c>
       <c r="M1602" t="s">
-        <v>4017</v>
+        <v>4546</v>
       </c>
     </row>
     <row r="1603" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1603">
-        <v>1750</v>
+        <v>1755</v>
       </c>
       <c r="B1603" t="s">
-        <v>4018</v>
+        <v>4024</v>
       </c>
       <c r="C1603" t="s">
         <v>3875</v>
@@ -63257,15 +63372,15 @@
         <v>1353</v>
       </c>
       <c r="M1603" t="s">
-        <v>4543</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="1604" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1604">
-        <v>1751</v>
+        <v>1756</v>
       </c>
       <c r="B1604" t="s">
-        <v>4019</v>
+        <v>4025</v>
       </c>
       <c r="C1604" t="s">
         <v>3875</v>
@@ -63280,15 +63395,15 @@
         <v>1353</v>
       </c>
       <c r="M1604" t="s">
-        <v>4020</v>
+        <v>4548</v>
       </c>
     </row>
     <row r="1605" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1605">
-        <v>1752</v>
+        <v>1757</v>
       </c>
       <c r="B1605" t="s">
-        <v>4021</v>
+        <v>4026</v>
       </c>
       <c r="C1605" t="s">
         <v>3875</v>
@@ -63303,15 +63418,15 @@
         <v>1353</v>
       </c>
       <c r="M1605" t="s">
-        <v>4544</v>
+        <v>4027</v>
       </c>
     </row>
     <row r="1606" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1606">
-        <v>1753</v>
+        <v>1758</v>
       </c>
       <c r="B1606" t="s">
-        <v>4022</v>
+        <v>4028</v>
       </c>
       <c r="C1606" t="s">
         <v>3875</v>
@@ -63326,15 +63441,15 @@
         <v>1353</v>
       </c>
       <c r="M1606" t="s">
-        <v>4545</v>
+        <v>4549</v>
       </c>
     </row>
     <row r="1607" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1607">
-        <v>1754</v>
+        <v>1759</v>
       </c>
       <c r="B1607" t="s">
-        <v>4023</v>
+        <v>4029</v>
       </c>
       <c r="C1607" t="s">
         <v>3875</v>
@@ -63349,15 +63464,15 @@
         <v>1353</v>
       </c>
       <c r="M1607" t="s">
-        <v>4546</v>
+        <v>4550</v>
       </c>
     </row>
     <row r="1608" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1608">
-        <v>1755</v>
+        <v>1760</v>
       </c>
       <c r="B1608" t="s">
-        <v>4024</v>
+        <v>4030</v>
       </c>
       <c r="C1608" t="s">
         <v>3875</v>
@@ -63372,15 +63487,15 @@
         <v>1353</v>
       </c>
       <c r="M1608" t="s">
-        <v>4547</v>
+        <v>4031</v>
       </c>
     </row>
     <row r="1609" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1609">
-        <v>1756</v>
+        <v>1761</v>
       </c>
       <c r="B1609" t="s">
-        <v>4025</v>
+        <v>4032</v>
       </c>
       <c r="C1609" t="s">
         <v>3875</v>
@@ -63395,15 +63510,15 @@
         <v>1353</v>
       </c>
       <c r="M1609" t="s">
-        <v>4548</v>
+        <v>4033</v>
       </c>
     </row>
     <row r="1610" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1610">
-        <v>1757</v>
+        <v>1762</v>
       </c>
       <c r="B1610" t="s">
-        <v>4026</v>
+        <v>4034</v>
       </c>
       <c r="C1610" t="s">
         <v>3875</v>
@@ -63418,15 +63533,15 @@
         <v>1353</v>
       </c>
       <c r="M1610" t="s">
-        <v>4027</v>
+        <v>4035</v>
       </c>
     </row>
     <row r="1611" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1611">
-        <v>1758</v>
+        <v>1763</v>
       </c>
       <c r="B1611" t="s">
-        <v>4028</v>
+        <v>4036</v>
       </c>
       <c r="C1611" t="s">
         <v>3875</v>
@@ -63441,15 +63556,15 @@
         <v>1353</v>
       </c>
       <c r="M1611" t="s">
-        <v>4549</v>
+        <v>4037</v>
       </c>
     </row>
     <row r="1612" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1612">
-        <v>1759</v>
+        <v>1764</v>
       </c>
       <c r="B1612" t="s">
-        <v>4029</v>
+        <v>4038</v>
       </c>
       <c r="C1612" t="s">
         <v>3875</v>
@@ -63464,15 +63579,15 @@
         <v>1353</v>
       </c>
       <c r="M1612" t="s">
-        <v>4550</v>
+        <v>4551</v>
       </c>
     </row>
     <row r="1613" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1613">
-        <v>1760</v>
+        <v>1765</v>
       </c>
       <c r="B1613" t="s">
-        <v>4030</v>
+        <v>4039</v>
       </c>
       <c r="C1613" t="s">
         <v>3875</v>
@@ -63487,15 +63602,15 @@
         <v>1353</v>
       </c>
       <c r="M1613" t="s">
-        <v>4031</v>
+        <v>4040</v>
       </c>
     </row>
     <row r="1614" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1614">
-        <v>1761</v>
+        <v>1766</v>
       </c>
       <c r="B1614" t="s">
-        <v>4032</v>
+        <v>4041</v>
       </c>
       <c r="C1614" t="s">
         <v>3875</v>
@@ -63510,15 +63625,15 @@
         <v>1353</v>
       </c>
       <c r="M1614" t="s">
-        <v>4033</v>
+        <v>4042</v>
       </c>
     </row>
     <row r="1615" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1615">
-        <v>1762</v>
+        <v>1767</v>
       </c>
       <c r="B1615" t="s">
-        <v>4034</v>
+        <v>4043</v>
       </c>
       <c r="C1615" t="s">
         <v>3875</v>
@@ -63533,15 +63648,15 @@
         <v>1353</v>
       </c>
       <c r="M1615" t="s">
-        <v>4035</v>
+        <v>4552</v>
       </c>
     </row>
     <row r="1616" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1616">
-        <v>1763</v>
+        <v>1768</v>
       </c>
       <c r="B1616" t="s">
-        <v>4036</v>
+        <v>4044</v>
       </c>
       <c r="C1616" t="s">
         <v>3875</v>
@@ -63556,15 +63671,15 @@
         <v>1353</v>
       </c>
       <c r="M1616" t="s">
-        <v>4037</v>
+        <v>4045</v>
       </c>
     </row>
     <row r="1617" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1617">
-        <v>1764</v>
+        <v>1769</v>
       </c>
       <c r="B1617" t="s">
-        <v>4038</v>
+        <v>4046</v>
       </c>
       <c r="C1617" t="s">
         <v>3875</v>
@@ -63579,15 +63694,15 @@
         <v>1353</v>
       </c>
       <c r="M1617" t="s">
-        <v>4551</v>
+        <v>4553</v>
       </c>
     </row>
     <row r="1618" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1618">
-        <v>1765</v>
+        <v>1770</v>
       </c>
       <c r="B1618" t="s">
-        <v>4039</v>
+        <v>4047</v>
       </c>
       <c r="C1618" t="s">
         <v>3875</v>
@@ -63602,15 +63717,15 @@
         <v>1353</v>
       </c>
       <c r="M1618" t="s">
-        <v>4040</v>
+        <v>4048</v>
       </c>
     </row>
     <row r="1619" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1619">
-        <v>1766</v>
+        <v>1771</v>
       </c>
       <c r="B1619" t="s">
-        <v>4041</v>
+        <v>4049</v>
       </c>
       <c r="C1619" t="s">
         <v>3875</v>
@@ -63625,15 +63740,15 @@
         <v>1353</v>
       </c>
       <c r="M1619" t="s">
-        <v>4042</v>
+        <v>4050</v>
       </c>
     </row>
     <row r="1620" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1620">
-        <v>1767</v>
+        <v>1772</v>
       </c>
       <c r="B1620" t="s">
-        <v>4043</v>
+        <v>4051</v>
       </c>
       <c r="C1620" t="s">
         <v>3875</v>
@@ -63648,15 +63763,15 @@
         <v>1353</v>
       </c>
       <c r="M1620" t="s">
-        <v>4552</v>
+        <v>4052</v>
       </c>
     </row>
     <row r="1621" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1621">
-        <v>1768</v>
+        <v>1773</v>
       </c>
       <c r="B1621" t="s">
-        <v>4044</v>
+        <v>4053</v>
       </c>
       <c r="C1621" t="s">
         <v>3875</v>
@@ -63671,15 +63786,15 @@
         <v>1353</v>
       </c>
       <c r="M1621" t="s">
-        <v>4045</v>
+        <v>4554</v>
       </c>
     </row>
     <row r="1622" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1622">
-        <v>1769</v>
+        <v>1774</v>
       </c>
       <c r="B1622" t="s">
-        <v>4046</v>
+        <v>4054</v>
       </c>
       <c r="C1622" t="s">
         <v>3875</v>
@@ -63694,15 +63809,15 @@
         <v>1353</v>
       </c>
       <c r="M1622" t="s">
-        <v>4553</v>
+        <v>4555</v>
       </c>
     </row>
     <row r="1623" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1623">
-        <v>1770</v>
+        <v>1775</v>
       </c>
       <c r="B1623" t="s">
-        <v>4047</v>
+        <v>4055</v>
       </c>
       <c r="C1623" t="s">
         <v>3875</v>
@@ -63717,15 +63832,15 @@
         <v>1353</v>
       </c>
       <c r="M1623" t="s">
-        <v>4048</v>
+        <v>4556</v>
       </c>
     </row>
     <row r="1624" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1624">
-        <v>1771</v>
+        <v>1776</v>
       </c>
       <c r="B1624" t="s">
-        <v>4049</v>
+        <v>4056</v>
       </c>
       <c r="C1624" t="s">
         <v>3875</v>
@@ -63740,15 +63855,15 @@
         <v>1353</v>
       </c>
       <c r="M1624" t="s">
-        <v>4050</v>
+        <v>4557</v>
       </c>
     </row>
     <row r="1625" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1625">
-        <v>1772</v>
+        <v>1777</v>
       </c>
       <c r="B1625" t="s">
-        <v>4051</v>
+        <v>4057</v>
       </c>
       <c r="C1625" t="s">
         <v>3875</v>
@@ -63763,15 +63878,15 @@
         <v>1353</v>
       </c>
       <c r="M1625" t="s">
-        <v>4052</v>
+        <v>4558</v>
       </c>
     </row>
     <row r="1626" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1626">
-        <v>1773</v>
+        <v>1778</v>
       </c>
       <c r="B1626" t="s">
-        <v>4053</v>
+        <v>4058</v>
       </c>
       <c r="C1626" t="s">
         <v>3875</v>
@@ -63786,15 +63901,15 @@
         <v>1353</v>
       </c>
       <c r="M1626" t="s">
-        <v>4554</v>
+        <v>4059</v>
       </c>
     </row>
     <row r="1627" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1627">
-        <v>1774</v>
+        <v>1779</v>
       </c>
       <c r="B1627" t="s">
-        <v>4054</v>
+        <v>4060</v>
       </c>
       <c r="C1627" t="s">
         <v>3875</v>
@@ -63809,15 +63924,15 @@
         <v>1353</v>
       </c>
       <c r="M1627" t="s">
-        <v>4555</v>
+        <v>4559</v>
       </c>
     </row>
     <row r="1628" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1628">
-        <v>1775</v>
+        <v>1780</v>
       </c>
       <c r="B1628" t="s">
-        <v>4055</v>
+        <v>4061</v>
       </c>
       <c r="C1628" t="s">
         <v>3875</v>
@@ -63832,126 +63947,11 @@
         <v>1353</v>
       </c>
       <c r="M1628" t="s">
-        <v>4556</v>
-      </c>
-    </row>
-    <row r="1629" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1629">
-        <v>1776</v>
-      </c>
-      <c r="B1629" t="s">
-        <v>4056</v>
-      </c>
-      <c r="C1629" t="s">
-        <v>3875</v>
-      </c>
-      <c r="D1629">
-        <v>68000</v>
-      </c>
-      <c r="E1629" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1629" t="s">
-        <v>1353</v>
-      </c>
-      <c r="M1629" t="s">
-        <v>4557</v>
-      </c>
-    </row>
-    <row r="1630" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1630">
-        <v>1777</v>
-      </c>
-      <c r="B1630" t="s">
-        <v>4057</v>
-      </c>
-      <c r="C1630" t="s">
-        <v>3875</v>
-      </c>
-      <c r="D1630">
-        <v>68000</v>
-      </c>
-      <c r="E1630" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1630" t="s">
-        <v>1353</v>
-      </c>
-      <c r="M1630" t="s">
-        <v>4558</v>
-      </c>
-    </row>
-    <row r="1631" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1631">
-        <v>1778</v>
-      </c>
-      <c r="B1631" t="s">
-        <v>4058</v>
-      </c>
-      <c r="C1631" t="s">
-        <v>3875</v>
-      </c>
-      <c r="D1631">
-        <v>68000</v>
-      </c>
-      <c r="E1631" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1631" t="s">
-        <v>1353</v>
-      </c>
-      <c r="M1631" t="s">
-        <v>4059</v>
-      </c>
-    </row>
-    <row r="1632" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1632">
-        <v>1779</v>
-      </c>
-      <c r="B1632" t="s">
-        <v>4060</v>
-      </c>
-      <c r="C1632" t="s">
-        <v>3875</v>
-      </c>
-      <c r="D1632">
-        <v>68000</v>
-      </c>
-      <c r="E1632" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1632" t="s">
-        <v>1353</v>
-      </c>
-      <c r="M1632" t="s">
-        <v>4559</v>
-      </c>
-    </row>
-    <row r="1633" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1633">
-        <v>1780</v>
-      </c>
-      <c r="B1633" t="s">
-        <v>4061</v>
-      </c>
-      <c r="C1633" t="s">
-        <v>3875</v>
-      </c>
-      <c r="D1633">
-        <v>68000</v>
-      </c>
-      <c r="E1633" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1633" t="s">
-        <v>1353</v>
-      </c>
-      <c r="M1633" t="s">
         <v>4062</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M1633"/>
+  <autoFilter ref="A1:M1628"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
036 : simpsons driver
</commit_message>
<xml_diff>
--- a/0.36/compatibility.xlsx
+++ b/0.36/compatibility.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Playable(tested)" sheetId="6" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12459" uniqueCount="4570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12468" uniqueCount="4571">
   <si>
     <t>romname</t>
   </si>
@@ -13768,6 +13768,9 @@
   </si>
   <si>
     <t>konamiic</t>
+  </si>
+  <si>
+    <t>eeprom machine</t>
   </si>
 </sst>
 </file>
@@ -14091,10 +14094,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14103,9 +14106,10 @@
     <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="35.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -14134,7 +14138,7 @@
         <v>4568</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -14163,7 +14167,7 @@
         <v>4568</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -14195,7 +14199,7 @@
         <v>4569</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -14227,7 +14231,7 @@
         <v>4569</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
@@ -14259,7 +14263,7 @@
         <v>4569</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
@@ -14288,7 +14292,7 @@
         <v>4569</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7</v>
       </c>
@@ -14315,6 +14319,111 @@
       </c>
       <c r="N7" t="s">
         <v>4569</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2729</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2730</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2652</v>
+      </c>
+      <c r="E8" t="s">
+        <v>154</v>
+      </c>
+      <c r="H8" t="s">
+        <v>551</v>
+      </c>
+      <c r="I8">
+        <v>53260</v>
+      </c>
+      <c r="M8" t="s">
+        <v>2731</v>
+      </c>
+      <c r="N8" t="s">
+        <v>4569</v>
+      </c>
+      <c r="O8" t="s">
+        <v>4567</v>
+      </c>
+      <c r="P8" t="s">
+        <v>4570</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2732</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2730</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2652</v>
+      </c>
+      <c r="E9" t="s">
+        <v>154</v>
+      </c>
+      <c r="H9" t="s">
+        <v>551</v>
+      </c>
+      <c r="I9">
+        <v>53260</v>
+      </c>
+      <c r="M9" t="s">
+        <v>2733</v>
+      </c>
+      <c r="N9" t="s">
+        <v>4569</v>
+      </c>
+      <c r="O9" t="s">
+        <v>4567</v>
+      </c>
+      <c r="P9" t="s">
+        <v>4570</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2734</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2730</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2652</v>
+      </c>
+      <c r="E10" t="s">
+        <v>154</v>
+      </c>
+      <c r="H10" t="s">
+        <v>551</v>
+      </c>
+      <c r="I10">
+        <v>53260</v>
+      </c>
+      <c r="M10" t="s">
+        <v>4378</v>
+      </c>
+      <c r="N10" t="s">
+        <v>4569</v>
+      </c>
+      <c r="O10" t="s">
+        <v>4567</v>
+      </c>
+      <c r="P10" t="s">
+        <v>4570</v>
       </c>
     </row>
   </sheetData>
@@ -26960,8 +27069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1499"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A885" workbookViewId="0">
-      <selection activeCell="F904" sqref="F904"/>
+    <sheetView topLeftCell="A921" workbookViewId="0">
+      <selection activeCell="A944" sqref="A944:XFD946"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -50360,84 +50469,6 @@
       </c>
       <c r="M943" t="s">
         <v>2728</v>
-      </c>
-    </row>
-    <row r="944" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A944">
-        <v>1029</v>
-      </c>
-      <c r="B944" t="s">
-        <v>2729</v>
-      </c>
-      <c r="C944" t="s">
-        <v>2730</v>
-      </c>
-      <c r="D944" t="s">
-        <v>2652</v>
-      </c>
-      <c r="E944" t="s">
-        <v>154</v>
-      </c>
-      <c r="H944" t="s">
-        <v>551</v>
-      </c>
-      <c r="I944">
-        <v>53260</v>
-      </c>
-      <c r="M944" t="s">
-        <v>2731</v>
-      </c>
-    </row>
-    <row r="945" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A945">
-        <v>1030</v>
-      </c>
-      <c r="B945" t="s">
-        <v>2732</v>
-      </c>
-      <c r="C945" t="s">
-        <v>2730</v>
-      </c>
-      <c r="D945" t="s">
-        <v>2652</v>
-      </c>
-      <c r="E945" t="s">
-        <v>154</v>
-      </c>
-      <c r="H945" t="s">
-        <v>551</v>
-      </c>
-      <c r="I945">
-        <v>53260</v>
-      </c>
-      <c r="M945" t="s">
-        <v>2733</v>
-      </c>
-    </row>
-    <row r="946" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A946">
-        <v>1031</v>
-      </c>
-      <c r="B946" t="s">
-        <v>2734</v>
-      </c>
-      <c r="C946" t="s">
-        <v>2730</v>
-      </c>
-      <c r="D946" t="s">
-        <v>2652</v>
-      </c>
-      <c r="E946" t="s">
-        <v>154</v>
-      </c>
-      <c r="H946" t="s">
-        <v>551</v>
-      </c>
-      <c r="I946">
-        <v>53260</v>
-      </c>
-      <c r="M946" t="s">
-        <v>4378</v>
       </c>
     </row>
     <row r="947" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
036 : mystston driver
</commit_message>
<xml_diff>
--- a/0.36/compatibility.xlsx
+++ b/0.36/compatibility.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Playable(tested)" sheetId="6" r:id="rId1"/>
@@ -14107,10 +14107,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14723,6 +14723,26 @@
       </c>
       <c r="M20" t="s">
         <v>3329</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3324</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3325</v>
+      </c>
+      <c r="D21" t="s">
+        <v>405</v>
+      </c>
+      <c r="H21" t="s">
+        <v>172</v>
+      </c>
+      <c r="M21" t="s">
+        <v>3326</v>
       </c>
     </row>
   </sheetData>
@@ -30000,8 +30020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1373"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1065" workbookViewId="0">
-      <selection activeCell="A1080" sqref="A1080:XFD1080"/>
+    <sheetView topLeftCell="A1065" workbookViewId="0">
+      <selection activeCell="A1079" sqref="A1079:XFD1079"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -56850,26 +56870,6 @@
       </c>
       <c r="M1078" t="s">
         <v>3323</v>
-      </c>
-    </row>
-    <row r="1079" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1079">
-        <v>1286</v>
-      </c>
-      <c r="B1079" t="s">
-        <v>3324</v>
-      </c>
-      <c r="C1079" t="s">
-        <v>3325</v>
-      </c>
-      <c r="D1079" t="s">
-        <v>405</v>
-      </c>
-      <c r="H1079" t="s">
-        <v>172</v>
-      </c>
-      <c r="M1079" t="s">
-        <v>3326</v>
       </c>
     </row>
     <row r="1080" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
036 : updated compatibility list
</commit_message>
<xml_diff>
--- a/0.36/compatibility.xlsx
+++ b/0.36/compatibility.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Playable(tested)" sheetId="6" r:id="rId1"/>
@@ -14753,10 +14753,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P654"/>
+  <dimension ref="A1:P660"/>
   <sheetViews>
-    <sheetView topLeftCell="A634" workbookViewId="0">
-      <selection activeCell="A648" sqref="A648:A654"/>
+    <sheetView tabSelected="1" topLeftCell="A634" workbookViewId="0">
+      <selection activeCell="A655" sqref="A655:A660"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30548,6 +30548,135 @@
         <v>318</v>
       </c>
     </row>
+    <row r="655" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A655">
+        <v>655</v>
+      </c>
+      <c r="B655" t="s">
+        <v>1335</v>
+      </c>
+      <c r="C655" t="s">
+        <v>1336</v>
+      </c>
+      <c r="D655" t="s">
+        <v>14</v>
+      </c>
+      <c r="E655" t="s">
+        <v>1220</v>
+      </c>
+      <c r="H655" t="s">
+        <v>71</v>
+      </c>
+      <c r="M655" t="s">
+        <v>1337</v>
+      </c>
+    </row>
+    <row r="656" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A656">
+        <v>656</v>
+      </c>
+      <c r="B656" t="s">
+        <v>1338</v>
+      </c>
+      <c r="C656" t="s">
+        <v>1336</v>
+      </c>
+      <c r="D656" t="s">
+        <v>14</v>
+      </c>
+      <c r="E656" t="s">
+        <v>1220</v>
+      </c>
+      <c r="H656" t="s">
+        <v>71</v>
+      </c>
+      <c r="M656" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="657" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A657">
+        <v>657</v>
+      </c>
+      <c r="B657" t="s">
+        <v>1340</v>
+      </c>
+      <c r="C657" t="s">
+        <v>1336</v>
+      </c>
+      <c r="D657" t="s">
+        <v>14</v>
+      </c>
+      <c r="E657" t="s">
+        <v>1220</v>
+      </c>
+      <c r="H657" t="s">
+        <v>71</v>
+      </c>
+      <c r="M657" t="s">
+        <v>1341</v>
+      </c>
+    </row>
+    <row r="658" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A658">
+        <v>658</v>
+      </c>
+      <c r="B658" t="s">
+        <v>1343</v>
+      </c>
+      <c r="C658" t="s">
+        <v>1336</v>
+      </c>
+      <c r="D658" t="s">
+        <v>14</v>
+      </c>
+      <c r="H658" t="s">
+        <v>71</v>
+      </c>
+      <c r="M658" t="s">
+        <v>4190</v>
+      </c>
+    </row>
+    <row r="659" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A659">
+        <v>659</v>
+      </c>
+      <c r="B659" t="s">
+        <v>1344</v>
+      </c>
+      <c r="C659" t="s">
+        <v>1336</v>
+      </c>
+      <c r="D659" t="s">
+        <v>14</v>
+      </c>
+      <c r="H659" t="s">
+        <v>71</v>
+      </c>
+      <c r="M659" t="s">
+        <v>4191</v>
+      </c>
+    </row>
+    <row r="660" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A660">
+        <v>660</v>
+      </c>
+      <c r="B660" t="s">
+        <v>1345</v>
+      </c>
+      <c r="C660" t="s">
+        <v>1336</v>
+      </c>
+      <c r="D660" t="s">
+        <v>14</v>
+      </c>
+      <c r="H660" t="s">
+        <v>71</v>
+      </c>
+      <c r="M660" t="s">
+        <v>4192</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -30558,8 +30687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1349"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1014" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD7"/>
+    <sheetView topLeftCell="A356" workbookViewId="0">
+      <selection activeCell="A371" sqref="A371:XFD377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39798,158 +39927,6 @@
       </c>
       <c r="M370" t="s">
         <v>1334</v>
-      </c>
-    </row>
-    <row r="371" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A371">
-        <v>418</v>
-      </c>
-      <c r="B371" t="s">
-        <v>1335</v>
-      </c>
-      <c r="C371" t="s">
-        <v>1336</v>
-      </c>
-      <c r="D371" t="s">
-        <v>14</v>
-      </c>
-      <c r="E371" t="s">
-        <v>1220</v>
-      </c>
-      <c r="H371" t="s">
-        <v>71</v>
-      </c>
-      <c r="M371" t="s">
-        <v>1337</v>
-      </c>
-    </row>
-    <row r="372" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A372">
-        <v>419</v>
-      </c>
-      <c r="B372" t="s">
-        <v>1338</v>
-      </c>
-      <c r="C372" t="s">
-        <v>1336</v>
-      </c>
-      <c r="D372" t="s">
-        <v>14</v>
-      </c>
-      <c r="E372" t="s">
-        <v>1220</v>
-      </c>
-      <c r="H372" t="s">
-        <v>71</v>
-      </c>
-      <c r="M372" t="s">
-        <v>1339</v>
-      </c>
-    </row>
-    <row r="373" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A373">
-        <v>420</v>
-      </c>
-      <c r="B373" t="s">
-        <v>1340</v>
-      </c>
-      <c r="C373" t="s">
-        <v>1336</v>
-      </c>
-      <c r="D373" t="s">
-        <v>14</v>
-      </c>
-      <c r="E373" t="s">
-        <v>1220</v>
-      </c>
-      <c r="H373" t="s">
-        <v>71</v>
-      </c>
-      <c r="M373" t="s">
-        <v>1341</v>
-      </c>
-    </row>
-    <row r="374" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A374">
-        <v>421</v>
-      </c>
-      <c r="B374" t="s">
-        <v>1342</v>
-      </c>
-      <c r="C374" t="s">
-        <v>1336</v>
-      </c>
-      <c r="D374" t="s">
-        <v>14</v>
-      </c>
-      <c r="E374" t="s">
-        <v>1220</v>
-      </c>
-      <c r="H374" t="s">
-        <v>71</v>
-      </c>
-      <c r="M374" t="s">
-        <v>4189</v>
-      </c>
-    </row>
-    <row r="375" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A375">
-        <v>422</v>
-      </c>
-      <c r="B375" t="s">
-        <v>1343</v>
-      </c>
-      <c r="C375" t="s">
-        <v>1336</v>
-      </c>
-      <c r="D375" t="s">
-        <v>14</v>
-      </c>
-      <c r="H375" t="s">
-        <v>71</v>
-      </c>
-      <c r="M375" t="s">
-        <v>4190</v>
-      </c>
-    </row>
-    <row r="376" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A376">
-        <v>423</v>
-      </c>
-      <c r="B376" t="s">
-        <v>1344</v>
-      </c>
-      <c r="C376" t="s">
-        <v>1336</v>
-      </c>
-      <c r="D376" t="s">
-        <v>14</v>
-      </c>
-      <c r="H376" t="s">
-        <v>71</v>
-      </c>
-      <c r="M376" t="s">
-        <v>4191</v>
-      </c>
-    </row>
-    <row r="377" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A377">
-        <v>424</v>
-      </c>
-      <c r="B377" t="s">
-        <v>1345</v>
-      </c>
-      <c r="C377" t="s">
-        <v>1336</v>
-      </c>
-      <c r="D377" t="s">
-        <v>14</v>
-      </c>
-      <c r="H377" t="s">
-        <v>71</v>
-      </c>
-      <c r="M377" t="s">
-        <v>4192</v>
       </c>
     </row>
     <row r="378" spans="1:13" x14ac:dyDescent="0.3">
@@ -64029,10 +64006,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A24"/>
+      <selection activeCell="A23" sqref="A23:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -64623,6 +64600,29 @@
         <v>2052</v>
       </c>
     </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1342</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1336</v>
+      </c>
+      <c r="D25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1220</v>
+      </c>
+      <c r="H25" t="s">
+        <v>71</v>
+      </c>
+      <c r="M25" t="s">
+        <v>4189</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>